<commit_message>
blanchard et al 2006 extraction
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96748D7E-ADCE-E446-9475-7F1536B4C111}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC42994-87BA-004C-A2A0-CCCFE48217A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4400" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="300" yWindow="460" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="50">
   <si>
     <t>study_id</t>
   </si>
@@ -33,9 +33,6 @@
     <t>org_level</t>
   </si>
   <si>
-    <t>flux_type</t>
-  </si>
-  <si>
     <t>flux_pattern</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>BL * s^-1</t>
   </si>
   <si>
-    <t>temp_exposed</t>
-  </si>
-  <si>
     <t>period_flux</t>
   </si>
   <si>
@@ -138,10 +132,49 @@
     <t>bartheld2017</t>
   </si>
   <si>
-    <t>table 1</t>
-  </si>
-  <si>
     <t>blanchard2006</t>
+  </si>
+  <si>
+    <t>flux_treatment</t>
+  </si>
+  <si>
+    <t>temp_measured</t>
+  </si>
+  <si>
+    <t>20-14</t>
+  </si>
+  <si>
+    <t>23-17</t>
+  </si>
+  <si>
+    <t>26-14</t>
+  </si>
+  <si>
+    <t>26-20</t>
+  </si>
+  <si>
+    <t>29-17</t>
+  </si>
+  <si>
+    <t>29-23</t>
+  </si>
+  <si>
+    <t>visible inflorescence percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent </t>
+  </si>
+  <si>
+    <t>Phalaenopsis</t>
+  </si>
+  <si>
+    <t>Brother Goldsmith ‘720’</t>
+  </si>
+  <si>
+    <t>20 weeks</t>
+  </si>
+  <si>
+    <t>Miva Smartissimo x Canberra ‘450’</t>
   </si>
 </sst>
 </file>
@@ -507,107 +540,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AE14"/>
+  <dimension ref="A1:AE37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>20</v>
-      </c>
       <c r="Z1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>25</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -615,19 +649,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
       <c r="G2">
         <v>20</v>
@@ -648,10 +679,10 @@
         <v>5</v>
       </c>
       <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
         <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
       </c>
       <c r="O2" s="1">
         <v>1.1297709899999999</v>
@@ -669,10 +700,10 @@
         <v>8.0152669999999995E-2</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V2" s="2">
         <v>1</v>
@@ -689,19 +720,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
       </c>
       <c r="G3">
         <v>20</v>
@@ -722,10 +750,10 @@
         <v>12</v>
       </c>
       <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
         <v>27</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
       </c>
       <c r="O3" s="1">
         <v>3.29770992</v>
@@ -743,10 +771,10 @@
         <v>0.17557252000000001</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V3" s="2">
         <v>1</v>
@@ -763,19 +791,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
       </c>
       <c r="G4">
         <v>20</v>
@@ -796,10 +821,10 @@
         <v>20</v>
       </c>
       <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s">
         <v>27</v>
-      </c>
-      <c r="N4" t="s">
-        <v>28</v>
       </c>
       <c r="O4" s="1">
         <v>4.19847328</v>
@@ -817,10 +842,10 @@
         <v>0.17938931</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V4" s="2">
         <v>1</v>
@@ -837,19 +862,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -870,10 +892,10 @@
         <v>25</v>
       </c>
       <c r="M5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" t="s">
         <v>27</v>
-      </c>
-      <c r="N5" t="s">
-        <v>28</v>
       </c>
       <c r="O5" s="1">
         <v>3.4961832099999999</v>
@@ -891,10 +913,10 @@
         <v>0.22900762999999999</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V5" s="2">
         <v>1</v>
@@ -911,19 +933,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
         <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -944,10 +963,10 @@
         <v>30</v>
       </c>
       <c r="M6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" t="s">
         <v>27</v>
-      </c>
-      <c r="N6" t="s">
-        <v>28</v>
       </c>
       <c r="O6" s="1">
         <v>2.7938931299999998</v>
@@ -965,10 +984,10 @@
         <v>0.15648855</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V6" s="2">
         <v>1</v>
@@ -985,19 +1004,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
       </c>
       <c r="G7">
         <v>20</v>
@@ -1018,10 +1034,10 @@
         <v>35</v>
       </c>
       <c r="M7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" t="s">
         <v>27</v>
-      </c>
-      <c r="N7" t="s">
-        <v>28</v>
       </c>
       <c r="O7" s="1">
         <v>1.6106870200000001</v>
@@ -1039,10 +1055,10 @@
         <v>0.17557252000000001</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V7" s="2">
         <v>1</v>
@@ -1059,16 +1075,16 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1080,10 +1096,10 @@
         <v>20</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>18.5</v>
       </c>
       <c r="J8">
-        <v>20</v>
+        <v>21.5</v>
       </c>
       <c r="K8">
         <v>24</v>
@@ -1092,10 +1108,10 @@
         <v>5</v>
       </c>
       <c r="M8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" t="s">
         <v>27</v>
-      </c>
-      <c r="N8" t="s">
-        <v>28</v>
       </c>
       <c r="O8" s="1">
         <v>0.93129770999999995</v>
@@ -1113,10 +1129,10 @@
         <v>6.1068699999999997E-2</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V8" s="2">
         <v>1</v>
@@ -1133,16 +1149,16 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1154,10 +1170,10 @@
         <v>20</v>
       </c>
       <c r="I9">
-        <v>20</v>
+        <v>18.5</v>
       </c>
       <c r="J9">
-        <v>20</v>
+        <v>21.5</v>
       </c>
       <c r="K9">
         <v>24</v>
@@ -1166,10 +1182,10 @@
         <v>12</v>
       </c>
       <c r="M9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" t="s">
         <v>27</v>
-      </c>
-      <c r="N9" t="s">
-        <v>28</v>
       </c>
       <c r="O9" s="1">
         <v>2.6259541999999998</v>
@@ -1187,10 +1203,10 @@
         <v>0.11832061000000001</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V9" s="2">
         <v>1</v>
@@ -1207,16 +1223,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1228,10 +1244,10 @@
         <v>20</v>
       </c>
       <c r="I10">
-        <v>20</v>
+        <v>18.5</v>
       </c>
       <c r="J10">
-        <v>20</v>
+        <v>21.5</v>
       </c>
       <c r="K10">
         <v>24</v>
@@ -1240,10 +1256,10 @@
         <v>20</v>
       </c>
       <c r="M10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" t="s">
         <v>27</v>
-      </c>
-      <c r="N10" t="s">
-        <v>28</v>
       </c>
       <c r="O10" s="1">
         <v>3.3893129800000001</v>
@@ -1261,10 +1277,10 @@
         <v>0.12977099</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V10" s="2">
         <v>1</v>
@@ -1281,16 +1297,16 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1302,10 +1318,10 @@
         <v>20</v>
       </c>
       <c r="I11">
-        <v>20</v>
+        <v>18.5</v>
       </c>
       <c r="J11">
-        <v>20</v>
+        <v>21.5</v>
       </c>
       <c r="K11">
         <v>24</v>
@@ -1314,10 +1330,10 @@
         <v>25</v>
       </c>
       <c r="M11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" t="s">
         <v>27</v>
-      </c>
-      <c r="N11" t="s">
-        <v>28</v>
       </c>
       <c r="O11" s="1">
         <v>3.2061068700000002</v>
@@ -1335,10 +1351,10 @@
         <v>0.13740458</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V11" s="2">
         <v>1</v>
@@ -1355,16 +1371,16 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1376,10 +1392,10 @@
         <v>20</v>
       </c>
       <c r="I12">
-        <v>20</v>
+        <v>18.5</v>
       </c>
       <c r="J12">
-        <v>20</v>
+        <v>21.5</v>
       </c>
       <c r="K12">
         <v>24</v>
@@ -1388,10 +1404,10 @@
         <v>30</v>
       </c>
       <c r="M12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" t="s">
         <v>27</v>
-      </c>
-      <c r="N12" t="s">
-        <v>28</v>
       </c>
       <c r="O12" s="1">
         <v>2.53435115</v>
@@ -1409,10 +1425,10 @@
         <v>0.15267175999999999</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V12" s="2">
         <v>1</v>
@@ -1429,16 +1445,16 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1450,10 +1466,10 @@
         <v>20</v>
       </c>
       <c r="I13">
-        <v>20</v>
+        <v>18.5</v>
       </c>
       <c r="J13">
-        <v>20</v>
+        <v>21.5</v>
       </c>
       <c r="K13">
         <v>24</v>
@@ -1462,10 +1478,10 @@
         <v>35</v>
       </c>
       <c r="M13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" t="s">
         <v>27</v>
-      </c>
-      <c r="N13" t="s">
-        <v>28</v>
       </c>
       <c r="O13" s="1">
         <v>1.6793893099999999</v>
@@ -1483,10 +1499,10 @@
         <v>0.11450382000000001</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="V13" s="2">
         <v>1</v>
@@ -1503,13 +1519,1655 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>29</v>
+      </c>
+      <c r="H14">
+        <v>14</v>
+      </c>
+      <c r="I14">
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <v>14</v>
+      </c>
+      <c r="K14">
+        <v>24</v>
+      </c>
+      <c r="L14">
+        <v>14</v>
+      </c>
+      <c r="M14" t="s">
+        <v>44</v>
+      </c>
+      <c r="N14" t="s">
+        <v>45</v>
+      </c>
+      <c r="O14">
+        <v>94.982490801278004</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>10</v>
+      </c>
+      <c r="T14" t="s">
+        <v>46</v>
+      </c>
+      <c r="U14" t="s">
+        <v>47</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0</v>
+      </c>
+      <c r="W14" s="2">
+        <v>2</v>
+      </c>
+      <c r="X14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>29</v>
+      </c>
+      <c r="H15">
+        <v>17</v>
+      </c>
+      <c r="I15">
+        <v>17</v>
+      </c>
+      <c r="J15">
+        <v>17</v>
+      </c>
+      <c r="L15">
+        <v>17</v>
+      </c>
+      <c r="M15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N15" t="s">
+        <v>45</v>
+      </c>
+      <c r="O15">
+        <v>94.957189268920303</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>10</v>
+      </c>
+      <c r="T15" t="s">
+        <v>46</v>
+      </c>
+      <c r="U15" t="s">
+        <v>47</v>
+      </c>
+      <c r="V15" s="2">
+        <v>0</v>
+      </c>
+      <c r="W15" s="2">
+        <v>2</v>
+      </c>
+      <c r="X15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>29</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+      <c r="I16">
+        <v>20</v>
+      </c>
+      <c r="J16">
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <v>20</v>
+      </c>
+      <c r="M16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N16" t="s">
+        <v>45</v>
+      </c>
+      <c r="O16">
+        <v>84.793240722547097</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>10</v>
+      </c>
+      <c r="T16" t="s">
+        <v>46</v>
+      </c>
+      <c r="U16" t="s">
+        <v>47</v>
+      </c>
+      <c r="V16" s="2">
+        <v>0</v>
+      </c>
+      <c r="W16" s="2">
+        <v>2</v>
+      </c>
+      <c r="X16" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>29</v>
+      </c>
+      <c r="H17">
+        <v>23</v>
+      </c>
+      <c r="I17">
+        <v>23</v>
+      </c>
+      <c r="J17">
+        <v>23</v>
+      </c>
+      <c r="L17">
+        <v>23</v>
+      </c>
+      <c r="M17" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" t="s">
+        <v>45</v>
+      </c>
+      <c r="O17">
+        <v>89.906572745942995</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>10</v>
+      </c>
+      <c r="T17" t="s">
+        <v>46</v>
+      </c>
+      <c r="U17" t="s">
+        <v>47</v>
+      </c>
+      <c r="V17" s="2">
+        <v>0</v>
+      </c>
+      <c r="W17" s="2">
+        <v>2</v>
+      </c>
+      <c r="X17" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>29</v>
+      </c>
+      <c r="H18">
+        <v>26</v>
+      </c>
+      <c r="I18">
+        <v>26</v>
+      </c>
+      <c r="J18">
+        <v>26</v>
+      </c>
+      <c r="L18">
+        <v>26</v>
+      </c>
+      <c r="M18" t="s">
+        <v>44</v>
+      </c>
+      <c r="N18" t="s">
+        <v>45</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>10</v>
+      </c>
+      <c r="T18" t="s">
+        <v>46</v>
+      </c>
+      <c r="U18" t="s">
+        <v>47</v>
+      </c>
+      <c r="V18" s="2">
+        <v>0</v>
+      </c>
+      <c r="W18" s="2">
+        <v>2</v>
+      </c>
+      <c r="X18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>29</v>
+      </c>
+      <c r="H19">
+        <v>29</v>
+      </c>
+      <c r="I19">
+        <v>29</v>
+      </c>
+      <c r="J19">
+        <v>29</v>
+      </c>
+      <c r="L19">
+        <v>29</v>
+      </c>
+      <c r="M19" t="s">
+        <v>44</v>
+      </c>
+      <c r="N19" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>10</v>
+      </c>
+      <c r="T19" t="s">
+        <v>46</v>
+      </c>
+      <c r="U19" t="s">
+        <v>47</v>
+      </c>
+      <c r="V19" s="2">
+        <v>0</v>
+      </c>
+      <c r="W19" s="2">
+        <v>2</v>
+      </c>
+      <c r="X19" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>29</v>
+      </c>
+      <c r="H20">
+        <f>AVERAGE(I20:J20)</f>
+        <v>17</v>
+      </c>
+      <c r="I20">
+        <v>14</v>
+      </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
+      <c r="K20">
+        <v>24</v>
+      </c>
+      <c r="L20" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
-        <v>37</v>
+      <c r="M20" t="s">
+        <v>44</v>
+      </c>
+      <c r="N20" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20">
+        <v>94.8312199376075</v>
+      </c>
+      <c r="P20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>10</v>
+      </c>
+      <c r="T20" t="s">
+        <v>46</v>
+      </c>
+      <c r="U20" t="s">
+        <v>47</v>
+      </c>
+      <c r="V20" s="2">
+        <v>0</v>
+      </c>
+      <c r="W20" s="2">
+        <v>2</v>
+      </c>
+      <c r="X20" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>29</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ref="H21:H25" si="0">AVERAGE(I21:J21)</f>
+        <v>20</v>
+      </c>
+      <c r="I21">
+        <v>17</v>
+      </c>
+      <c r="J21">
+        <v>23</v>
+      </c>
+      <c r="K21">
+        <v>24</v>
+      </c>
+      <c r="L21" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N21" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21">
+        <v>79.806147195701897</v>
+      </c>
+      <c r="P21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>10</v>
+      </c>
+      <c r="T21" t="s">
+        <v>46</v>
+      </c>
+      <c r="U21" t="s">
+        <v>47</v>
+      </c>
+      <c r="V21" s="2">
+        <v>0</v>
+      </c>
+      <c r="W21" s="2">
+        <v>2</v>
+      </c>
+      <c r="X21" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>29</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I22">
+        <v>14</v>
+      </c>
+      <c r="J22">
+        <v>26</v>
+      </c>
+      <c r="K22">
+        <v>24</v>
+      </c>
+      <c r="L22" t="s">
+        <v>40</v>
+      </c>
+      <c r="M22" t="s">
+        <v>44</v>
+      </c>
+      <c r="N22" t="s">
+        <v>45</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>10</v>
+      </c>
+      <c r="T22" t="s">
+        <v>46</v>
+      </c>
+      <c r="U22" t="s">
+        <v>47</v>
+      </c>
+      <c r="V22" s="2">
+        <v>0</v>
+      </c>
+      <c r="W22" s="2">
+        <v>2</v>
+      </c>
+      <c r="X22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>29</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="I23">
+        <v>20</v>
+      </c>
+      <c r="J23">
+        <v>26</v>
+      </c>
+      <c r="K23">
+        <v>24</v>
+      </c>
+      <c r="L23" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" t="s">
+        <v>44</v>
+      </c>
+      <c r="N23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>10</v>
+      </c>
+      <c r="T23" t="s">
+        <v>46</v>
+      </c>
+      <c r="U23" t="s">
+        <v>47</v>
+      </c>
+      <c r="V23" s="2">
+        <v>0</v>
+      </c>
+      <c r="W23" s="2">
+        <v>2</v>
+      </c>
+      <c r="X23" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>29</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="I24">
+        <v>17</v>
+      </c>
+      <c r="J24">
+        <v>29</v>
+      </c>
+      <c r="K24">
+        <v>24</v>
+      </c>
+      <c r="L24" t="s">
+        <v>42</v>
+      </c>
+      <c r="M24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N24" t="s">
+        <v>45</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>10</v>
+      </c>
+      <c r="T24" t="s">
+        <v>46</v>
+      </c>
+      <c r="U24" t="s">
+        <v>47</v>
+      </c>
+      <c r="V24" s="2">
+        <v>0</v>
+      </c>
+      <c r="W24" s="2">
+        <v>2</v>
+      </c>
+      <c r="X24" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>29</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="I25">
+        <v>23</v>
+      </c>
+      <c r="J25">
+        <v>29</v>
+      </c>
+      <c r="K25">
+        <v>24</v>
+      </c>
+      <c r="L25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M25" t="s">
+        <v>44</v>
+      </c>
+      <c r="N25" t="s">
+        <v>45</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>10</v>
+      </c>
+      <c r="T25" t="s">
+        <v>46</v>
+      </c>
+      <c r="U25" t="s">
+        <v>47</v>
+      </c>
+      <c r="V25" s="2">
+        <v>0</v>
+      </c>
+      <c r="W25" s="2">
+        <v>2</v>
+      </c>
+      <c r="X25" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>29</v>
+      </c>
+      <c r="H26">
+        <v>14</v>
+      </c>
+      <c r="I26">
+        <v>14</v>
+      </c>
+      <c r="J26">
+        <v>14</v>
+      </c>
+      <c r="K26">
+        <v>24</v>
+      </c>
+      <c r="L26">
+        <v>14</v>
+      </c>
+      <c r="M26" t="s">
+        <v>44</v>
+      </c>
+      <c r="N26" t="s">
+        <v>45</v>
+      </c>
+      <c r="O26">
+        <v>99.991410583503097</v>
+      </c>
+      <c r="P26" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>10</v>
+      </c>
+      <c r="T26" t="s">
+        <v>46</v>
+      </c>
+      <c r="U26" t="s">
+        <v>49</v>
+      </c>
+      <c r="V26" s="2">
+        <v>0</v>
+      </c>
+      <c r="W26" s="2">
+        <v>2</v>
+      </c>
+      <c r="X26" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>29</v>
+      </c>
+      <c r="H27">
+        <v>17</v>
+      </c>
+      <c r="I27">
+        <v>17</v>
+      </c>
+      <c r="J27">
+        <v>17</v>
+      </c>
+      <c r="L27">
+        <v>17</v>
+      </c>
+      <c r="M27" t="s">
+        <v>44</v>
+      </c>
+      <c r="N27" t="s">
+        <v>45</v>
+      </c>
+      <c r="O27">
+        <v>99.978929087656297</v>
+      </c>
+      <c r="P27" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>10</v>
+      </c>
+      <c r="T27" t="s">
+        <v>46</v>
+      </c>
+      <c r="U27" t="s">
+        <v>49</v>
+      </c>
+      <c r="V27" s="2">
+        <v>0</v>
+      </c>
+      <c r="W27" s="2">
+        <v>2</v>
+      </c>
+      <c r="X27" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>29</v>
+      </c>
+      <c r="H28">
+        <v>20</v>
+      </c>
+      <c r="I28">
+        <v>20</v>
+      </c>
+      <c r="J28">
+        <v>20</v>
+      </c>
+      <c r="L28">
+        <v>20</v>
+      </c>
+      <c r="M28" t="s">
+        <v>44</v>
+      </c>
+      <c r="N28" t="s">
+        <v>45</v>
+      </c>
+      <c r="O28">
+        <v>99.966447591809398</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>10</v>
+      </c>
+      <c r="T28" t="s">
+        <v>46</v>
+      </c>
+      <c r="U28" t="s">
+        <v>49</v>
+      </c>
+      <c r="V28" s="2">
+        <v>0</v>
+      </c>
+      <c r="W28" s="2">
+        <v>2</v>
+      </c>
+      <c r="X28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>29</v>
+      </c>
+      <c r="H29">
+        <v>23</v>
+      </c>
+      <c r="I29">
+        <v>23</v>
+      </c>
+      <c r="J29">
+        <v>23</v>
+      </c>
+      <c r="L29">
+        <v>23</v>
+      </c>
+      <c r="M29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N29" t="s">
+        <v>45</v>
+      </c>
+      <c r="O29">
+        <v>99.953697676697004</v>
+      </c>
+      <c r="P29" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>10</v>
+      </c>
+      <c r="T29" t="s">
+        <v>46</v>
+      </c>
+      <c r="U29" t="s">
+        <v>49</v>
+      </c>
+      <c r="V29" s="2">
+        <v>0</v>
+      </c>
+      <c r="W29" s="2">
+        <v>2</v>
+      </c>
+      <c r="X29" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>29</v>
+      </c>
+      <c r="H30">
+        <v>26</v>
+      </c>
+      <c r="I30">
+        <v>26</v>
+      </c>
+      <c r="J30">
+        <v>26</v>
+      </c>
+      <c r="L30">
+        <v>26</v>
+      </c>
+      <c r="M30" t="s">
+        <v>44</v>
+      </c>
+      <c r="N30" t="s">
+        <v>45</v>
+      </c>
+      <c r="O30">
+        <v>9.9132603143457594</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>10</v>
+      </c>
+      <c r="T30" t="s">
+        <v>46</v>
+      </c>
+      <c r="U30" t="s">
+        <v>49</v>
+      </c>
+      <c r="V30" s="2">
+        <v>0</v>
+      </c>
+      <c r="W30" s="2">
+        <v>2</v>
+      </c>
+      <c r="X30" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>29</v>
+      </c>
+      <c r="H31">
+        <v>29</v>
+      </c>
+      <c r="I31">
+        <v>29</v>
+      </c>
+      <c r="J31">
+        <v>29</v>
+      </c>
+      <c r="L31">
+        <v>29</v>
+      </c>
+      <c r="M31" t="s">
+        <v>44</v>
+      </c>
+      <c r="N31" t="s">
+        <v>45</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>10</v>
+      </c>
+      <c r="T31" t="s">
+        <v>46</v>
+      </c>
+      <c r="U31" t="s">
+        <v>49</v>
+      </c>
+      <c r="V31" s="2">
+        <v>0</v>
+      </c>
+      <c r="W31" s="2">
+        <v>2</v>
+      </c>
+      <c r="X31" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>29</v>
+      </c>
+      <c r="H32">
+        <f>AVERAGE(I32:J32)</f>
+        <v>17</v>
+      </c>
+      <c r="I32">
+        <v>14</v>
+      </c>
+      <c r="J32">
+        <v>20</v>
+      </c>
+      <c r="K32">
+        <v>24</v>
+      </c>
+      <c r="L32" t="s">
+        <v>38</v>
+      </c>
+      <c r="M32" t="s">
+        <v>44</v>
+      </c>
+      <c r="N32" t="s">
+        <v>45</v>
+      </c>
+      <c r="O32">
+        <v>99.916118979523603</v>
+      </c>
+      <c r="P32" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>10</v>
+      </c>
+      <c r="T32" t="s">
+        <v>46</v>
+      </c>
+      <c r="U32" t="s">
+        <v>49</v>
+      </c>
+      <c r="V32" s="2">
+        <v>0</v>
+      </c>
+      <c r="W32" s="2">
+        <v>2</v>
+      </c>
+      <c r="X32" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>29</v>
+      </c>
+      <c r="H33">
+        <f t="shared" ref="H33:H37" si="1">AVERAGE(I33:J33)</f>
+        <v>20</v>
+      </c>
+      <c r="I33">
+        <v>17</v>
+      </c>
+      <c r="J33">
+        <v>23</v>
+      </c>
+      <c r="K33">
+        <v>24</v>
+      </c>
+      <c r="L33" t="s">
+        <v>39</v>
+      </c>
+      <c r="M33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N33" t="s">
+        <v>45</v>
+      </c>
+      <c r="O33">
+        <v>99.903503274043899</v>
+      </c>
+      <c r="P33" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>10</v>
+      </c>
+      <c r="T33" t="s">
+        <v>46</v>
+      </c>
+      <c r="U33" t="s">
+        <v>49</v>
+      </c>
+      <c r="V33" s="2">
+        <v>0</v>
+      </c>
+      <c r="W33" s="2">
+        <v>2</v>
+      </c>
+      <c r="X33" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>29</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I34">
+        <v>14</v>
+      </c>
+      <c r="J34">
+        <v>26</v>
+      </c>
+      <c r="K34">
+        <v>24</v>
+      </c>
+      <c r="L34" t="s">
+        <v>40</v>
+      </c>
+      <c r="M34" t="s">
+        <v>44</v>
+      </c>
+      <c r="N34" t="s">
+        <v>45</v>
+      </c>
+      <c r="O34">
+        <v>54.738472399117903</v>
+      </c>
+      <c r="P34" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>10</v>
+      </c>
+      <c r="T34" t="s">
+        <v>46</v>
+      </c>
+      <c r="U34" t="s">
+        <v>49</v>
+      </c>
+      <c r="V34" s="2">
+        <v>0</v>
+      </c>
+      <c r="W34" s="2">
+        <v>2</v>
+      </c>
+      <c r="X34" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>29</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I35">
+        <v>20</v>
+      </c>
+      <c r="J35">
+        <v>26</v>
+      </c>
+      <c r="K35">
+        <v>24</v>
+      </c>
+      <c r="L35" t="s">
+        <v>41</v>
+      </c>
+      <c r="M35" t="s">
+        <v>44</v>
+      </c>
+      <c r="N35" t="s">
+        <v>45</v>
+      </c>
+      <c r="O35">
+        <v>74.947356271548998</v>
+      </c>
+      <c r="P35" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>10</v>
+      </c>
+      <c r="T35" t="s">
+        <v>46</v>
+      </c>
+      <c r="U35" t="s">
+        <v>49</v>
+      </c>
+      <c r="V35" s="2">
+        <v>0</v>
+      </c>
+      <c r="W35" s="2">
+        <v>2</v>
+      </c>
+      <c r="X35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>29</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I36">
+        <v>17</v>
+      </c>
+      <c r="J36">
+        <v>29</v>
+      </c>
+      <c r="K36">
+        <v>24</v>
+      </c>
+      <c r="L36" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" t="s">
+        <v>44</v>
+      </c>
+      <c r="N36" t="s">
+        <v>45</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>10</v>
+      </c>
+      <c r="T36" t="s">
+        <v>46</v>
+      </c>
+      <c r="U36" t="s">
+        <v>49</v>
+      </c>
+      <c r="V36" s="2">
+        <v>0</v>
+      </c>
+      <c r="W36" s="2">
+        <v>2</v>
+      </c>
+      <c r="X36" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>29</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I37">
+        <v>23</v>
+      </c>
+      <c r="J37">
+        <v>29</v>
+      </c>
+      <c r="K37">
+        <v>24</v>
+      </c>
+      <c r="L37" t="s">
+        <v>43</v>
+      </c>
+      <c r="M37" t="s">
+        <v>44</v>
+      </c>
+      <c r="N37" t="s">
+        <v>45</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>10</v>
+      </c>
+      <c r="T37" t="s">
+        <v>46</v>
+      </c>
+      <c r="U37" t="s">
+        <v>49</v>
+      </c>
+      <c r="V37" s="2">
+        <v>0</v>
+      </c>
+      <c r="W37" s="2">
+        <v>2</v>
+      </c>
+      <c r="X37" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="H20:H25" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
du et al 2009 extraction
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC42994-87BA-004C-A2A0-CCCFE48217A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DD9028-148A-2C4E-AAD4-997E4468E8F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="460" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="63">
   <si>
     <t>study_id</t>
   </si>
@@ -176,12 +176,51 @@
   <si>
     <t>Miva Smartissimo x Canberra ‘450’</t>
   </si>
+  <si>
+    <t>du2009</t>
+  </si>
+  <si>
+    <t>figure 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carapace width </t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>body mass</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>carapace height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chinemys </t>
+  </si>
+  <si>
+    <t>reevesii</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>figure 4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +239,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,10 +268,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,11 +587,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AE37"/>
+  <dimension ref="A1:AE91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N43" sqref="N43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3164,6 +3211,3984 @@
         <v>48</v>
       </c>
     </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>28</v>
+      </c>
+      <c r="I38">
+        <v>28</v>
+      </c>
+      <c r="J38">
+        <v>28</v>
+      </c>
+      <c r="M38" t="s">
+        <v>54</v>
+      </c>
+      <c r="N38" t="s">
+        <v>55</v>
+      </c>
+      <c r="O38">
+        <v>5.6285077951002203</v>
+      </c>
+      <c r="P38" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <v>24</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0.12828507795099986</v>
+      </c>
+      <c r="T38" t="s">
+        <v>57</v>
+      </c>
+      <c r="U38" t="s">
+        <v>58</v>
+      </c>
+      <c r="V38" s="2">
+        <v>1</v>
+      </c>
+      <c r="W38" s="2">
+        <v>0</v>
+      </c>
+      <c r="X38" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>28</v>
+      </c>
+      <c r="I39">
+        <v>25</v>
+      </c>
+      <c r="J39">
+        <v>31</v>
+      </c>
+      <c r="K39">
+        <v>24</v>
+      </c>
+      <c r="M39" t="s">
+        <v>54</v>
+      </c>
+      <c r="N39" t="s">
+        <v>55</v>
+      </c>
+      <c r="O39">
+        <v>5.2489977728285</v>
+      </c>
+      <c r="P39" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>25</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0.16035634743875038</v>
+      </c>
+      <c r="T39" t="s">
+        <v>57</v>
+      </c>
+      <c r="U39" t="s">
+        <v>58</v>
+      </c>
+      <c r="V39" s="2">
+        <v>1</v>
+      </c>
+      <c r="W39" s="2">
+        <v>0</v>
+      </c>
+      <c r="X39" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>28</v>
+      </c>
+      <c r="I40">
+        <v>22</v>
+      </c>
+      <c r="J40">
+        <v>34</v>
+      </c>
+      <c r="K40">
+        <v>24</v>
+      </c>
+      <c r="M40" t="s">
+        <v>54</v>
+      </c>
+      <c r="N40" t="s">
+        <v>55</v>
+      </c>
+      <c r="O40">
+        <v>5.3238307349665899</v>
+      </c>
+      <c r="P40" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>25</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0.27795100222717473</v>
+      </c>
+      <c r="T40" t="s">
+        <v>57</v>
+      </c>
+      <c r="U40" t="s">
+        <v>58</v>
+      </c>
+      <c r="V40" s="2">
+        <v>1</v>
+      </c>
+      <c r="W40" s="2">
+        <v>0</v>
+      </c>
+      <c r="X40" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>28</v>
+      </c>
+      <c r="I41">
+        <v>28</v>
+      </c>
+      <c r="J41">
+        <v>28</v>
+      </c>
+      <c r="M41" t="s">
+        <v>54</v>
+      </c>
+      <c r="N41" t="s">
+        <v>55</v>
+      </c>
+      <c r="O41">
+        <v>5.6285077951002203</v>
+      </c>
+      <c r="P41" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q41">
+        <v>14</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>9.8886414253899879E-2</v>
+      </c>
+      <c r="T41" t="s">
+        <v>57</v>
+      </c>
+      <c r="U41" t="s">
+        <v>58</v>
+      </c>
+      <c r="V41" s="2">
+        <v>1</v>
+      </c>
+      <c r="W41" s="2">
+        <v>0</v>
+      </c>
+      <c r="X41" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>28</v>
+      </c>
+      <c r="I42">
+        <v>25</v>
+      </c>
+      <c r="J42">
+        <v>31</v>
+      </c>
+      <c r="K42">
+        <v>24</v>
+      </c>
+      <c r="M42" t="s">
+        <v>54</v>
+      </c>
+      <c r="N42" t="s">
+        <v>55</v>
+      </c>
+      <c r="O42">
+        <v>5.2489977728285</v>
+      </c>
+      <c r="P42" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q42">
+        <v>9</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>9.8886414253894994E-2</v>
+      </c>
+      <c r="T42" t="s">
+        <v>57</v>
+      </c>
+      <c r="U42" t="s">
+        <v>58</v>
+      </c>
+      <c r="V42" s="2">
+        <v>1</v>
+      </c>
+      <c r="W42" s="2">
+        <v>0</v>
+      </c>
+      <c r="X42" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>28</v>
+      </c>
+      <c r="I43">
+        <v>22</v>
+      </c>
+      <c r="J43">
+        <v>34</v>
+      </c>
+      <c r="K43">
+        <v>24</v>
+      </c>
+      <c r="M43" t="s">
+        <v>54</v>
+      </c>
+      <c r="N43" t="s">
+        <v>55</v>
+      </c>
+      <c r="O43">
+        <v>5.2596881959910897</v>
+      </c>
+      <c r="P43" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q43">
+        <v>3</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>9.6213808463255113E-2</v>
+      </c>
+      <c r="T43" t="s">
+        <v>57</v>
+      </c>
+      <c r="U43" t="s">
+        <v>58</v>
+      </c>
+      <c r="V43" s="2">
+        <v>1</v>
+      </c>
+      <c r="W43" s="2">
+        <v>0</v>
+      </c>
+      <c r="X43" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>28</v>
+      </c>
+      <c r="I44">
+        <v>28</v>
+      </c>
+      <c r="J44">
+        <v>28</v>
+      </c>
+      <c r="M44" t="s">
+        <v>56</v>
+      </c>
+      <c r="N44" t="s">
+        <v>53</v>
+      </c>
+      <c r="O44">
+        <v>28.113333333333301</v>
+      </c>
+      <c r="P44" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>24</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0.24000000000000021</v>
+      </c>
+      <c r="T44" t="s">
+        <v>57</v>
+      </c>
+      <c r="U44" t="s">
+        <v>58</v>
+      </c>
+      <c r="V44" s="2">
+        <v>1</v>
+      </c>
+      <c r="W44" s="2">
+        <v>0</v>
+      </c>
+      <c r="X44" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>28</v>
+      </c>
+      <c r="I45">
+        <v>25</v>
+      </c>
+      <c r="J45">
+        <v>31</v>
+      </c>
+      <c r="K45">
+        <v>24</v>
+      </c>
+      <c r="M45" t="s">
+        <v>56</v>
+      </c>
+      <c r="N45" t="s">
+        <v>53</v>
+      </c>
+      <c r="O45">
+        <v>27.26</v>
+      </c>
+      <c r="P45" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="3">
+        <v>25</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0.30666666666670039</v>
+      </c>
+      <c r="T45" t="s">
+        <v>57</v>
+      </c>
+      <c r="U45" t="s">
+        <v>58</v>
+      </c>
+      <c r="V45" s="2">
+        <v>1</v>
+      </c>
+      <c r="W45" s="2">
+        <v>0</v>
+      </c>
+      <c r="X45" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>28</v>
+      </c>
+      <c r="I46">
+        <v>22</v>
+      </c>
+      <c r="J46">
+        <v>34</v>
+      </c>
+      <c r="K46">
+        <v>24</v>
+      </c>
+      <c r="M46" t="s">
+        <v>56</v>
+      </c>
+      <c r="N46" t="s">
+        <v>53</v>
+      </c>
+      <c r="O46">
+        <v>27.3666666666666</v>
+      </c>
+      <c r="P46" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>25</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0.52666666666664952</v>
+      </c>
+      <c r="T46" t="s">
+        <v>57</v>
+      </c>
+      <c r="U46" t="s">
+        <v>58</v>
+      </c>
+      <c r="V46" s="2">
+        <v>1</v>
+      </c>
+      <c r="W46" s="2">
+        <v>0</v>
+      </c>
+      <c r="X46" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>28</v>
+      </c>
+      <c r="I47">
+        <v>28</v>
+      </c>
+      <c r="J47">
+        <v>28</v>
+      </c>
+      <c r="M47" t="s">
+        <v>56</v>
+      </c>
+      <c r="N47" t="s">
+        <v>53</v>
+      </c>
+      <c r="O47">
+        <v>28.108888888888799</v>
+      </c>
+      <c r="P47" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>14</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0.18666666666665144</v>
+      </c>
+      <c r="T47" t="s">
+        <v>57</v>
+      </c>
+      <c r="U47" t="s">
+        <v>58</v>
+      </c>
+      <c r="V47" s="2">
+        <v>1</v>
+      </c>
+      <c r="W47" s="2">
+        <v>0</v>
+      </c>
+      <c r="X47" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>28</v>
+      </c>
+      <c r="I48">
+        <v>25</v>
+      </c>
+      <c r="J48">
+        <v>31</v>
+      </c>
+      <c r="K48">
+        <v>24</v>
+      </c>
+      <c r="M48" t="s">
+        <v>56</v>
+      </c>
+      <c r="N48" t="s">
+        <v>53</v>
+      </c>
+      <c r="O48">
+        <v>27.704444444444398</v>
+      </c>
+      <c r="P48" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>9</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0.18444444444445018</v>
+      </c>
+      <c r="T48" t="s">
+        <v>57</v>
+      </c>
+      <c r="U48" t="s">
+        <v>58</v>
+      </c>
+      <c r="V48" s="2">
+        <v>1</v>
+      </c>
+      <c r="W48" s="2">
+        <v>0</v>
+      </c>
+      <c r="X48" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>28</v>
+      </c>
+      <c r="I49">
+        <v>22</v>
+      </c>
+      <c r="J49">
+        <v>34</v>
+      </c>
+      <c r="K49">
+        <v>24</v>
+      </c>
+      <c r="M49" t="s">
+        <v>56</v>
+      </c>
+      <c r="N49" t="s">
+        <v>53</v>
+      </c>
+      <c r="O49">
+        <v>27.8466666666666</v>
+      </c>
+      <c r="P49" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>3</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0.17777777777779846</v>
+      </c>
+      <c r="T49" t="s">
+        <v>57</v>
+      </c>
+      <c r="U49" t="s">
+        <v>58</v>
+      </c>
+      <c r="V49" s="2">
+        <v>1</v>
+      </c>
+      <c r="W49" s="2">
+        <v>0</v>
+      </c>
+      <c r="X49" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>28</v>
+      </c>
+      <c r="I50">
+        <v>28</v>
+      </c>
+      <c r="J50">
+        <v>28</v>
+      </c>
+      <c r="M50" t="s">
+        <v>52</v>
+      </c>
+      <c r="N50" t="s">
+        <v>53</v>
+      </c>
+      <c r="O50">
+        <v>22.706467391304301</v>
+      </c>
+      <c r="P50" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>24</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>0.29461956521740085</v>
+      </c>
+      <c r="T50" t="s">
+        <v>57</v>
+      </c>
+      <c r="U50" t="s">
+        <v>58</v>
+      </c>
+      <c r="V50" s="2">
+        <v>1</v>
+      </c>
+      <c r="W50" s="2">
+        <v>0</v>
+      </c>
+      <c r="X50" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>28</v>
+      </c>
+      <c r="I51">
+        <v>25</v>
+      </c>
+      <c r="J51">
+        <v>31</v>
+      </c>
+      <c r="K51">
+        <v>24</v>
+      </c>
+      <c r="M51" t="s">
+        <v>52</v>
+      </c>
+      <c r="N51" t="s">
+        <v>53</v>
+      </c>
+      <c r="O51">
+        <v>21.534604037266998</v>
+      </c>
+      <c r="P51" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>25</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>0.37834821428569931</v>
+      </c>
+      <c r="T51" t="s">
+        <v>57</v>
+      </c>
+      <c r="U51" t="s">
+        <v>58</v>
+      </c>
+      <c r="V51" s="2">
+        <v>1</v>
+      </c>
+      <c r="W51" s="2">
+        <v>0</v>
+      </c>
+      <c r="X51" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>28</v>
+      </c>
+      <c r="I52">
+        <v>22</v>
+      </c>
+      <c r="J52">
+        <v>34</v>
+      </c>
+      <c r="K52">
+        <v>24</v>
+      </c>
+      <c r="M52" t="s">
+        <v>52</v>
+      </c>
+      <c r="N52" t="s">
+        <v>53</v>
+      </c>
+      <c r="O52">
+        <v>21.983253105589998</v>
+      </c>
+      <c r="P52" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>25</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>0.64955357142860137</v>
+      </c>
+      <c r="T52" t="s">
+        <v>57</v>
+      </c>
+      <c r="U52" t="s">
+        <v>58</v>
+      </c>
+      <c r="V52" s="2">
+        <v>1</v>
+      </c>
+      <c r="W52" s="2">
+        <v>0</v>
+      </c>
+      <c r="X52" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>28</v>
+      </c>
+      <c r="I53">
+        <v>28</v>
+      </c>
+      <c r="J53">
+        <v>28</v>
+      </c>
+      <c r="M53" t="s">
+        <v>52</v>
+      </c>
+      <c r="N53" t="s">
+        <v>53</v>
+      </c>
+      <c r="O53">
+        <v>22.639503105589998</v>
+      </c>
+      <c r="P53" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>14</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>0.22095885093165002</v>
+      </c>
+      <c r="T53" t="s">
+        <v>57</v>
+      </c>
+      <c r="U53" t="s">
+        <v>58</v>
+      </c>
+      <c r="V53" s="2">
+        <v>1</v>
+      </c>
+      <c r="W53" s="2">
+        <v>0</v>
+      </c>
+      <c r="X53" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>28</v>
+      </c>
+      <c r="I54">
+        <v>25</v>
+      </c>
+      <c r="J54">
+        <v>31</v>
+      </c>
+      <c r="K54">
+        <v>24</v>
+      </c>
+      <c r="M54" t="s">
+        <v>52</v>
+      </c>
+      <c r="N54" t="s">
+        <v>53</v>
+      </c>
+      <c r="O54">
+        <v>21.789068322981301</v>
+      </c>
+      <c r="P54" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>9</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0.23102678571425095</v>
+      </c>
+      <c r="T54" t="s">
+        <v>57</v>
+      </c>
+      <c r="U54" t="s">
+        <v>58</v>
+      </c>
+      <c r="V54" s="2">
+        <v>1</v>
+      </c>
+      <c r="W54" s="2">
+        <v>0</v>
+      </c>
+      <c r="X54" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>28</v>
+      </c>
+      <c r="I55">
+        <v>22</v>
+      </c>
+      <c r="J55">
+        <v>34</v>
+      </c>
+      <c r="K55">
+        <v>24</v>
+      </c>
+      <c r="M55" t="s">
+        <v>52</v>
+      </c>
+      <c r="N55" t="s">
+        <v>53</v>
+      </c>
+      <c r="O55">
+        <v>22.2109316770186</v>
+      </c>
+      <c r="P55" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="3">
+        <v>3</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>0.234375</v>
+      </c>
+      <c r="T55" t="s">
+        <v>57</v>
+      </c>
+      <c r="U55" t="s">
+        <v>58</v>
+      </c>
+      <c r="V55" s="2">
+        <v>1</v>
+      </c>
+      <c r="W55" s="2">
+        <v>0</v>
+      </c>
+      <c r="X55" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" t="s">
+        <v>62</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>28</v>
+      </c>
+      <c r="I56">
+        <v>28</v>
+      </c>
+      <c r="J56">
+        <v>28</v>
+      </c>
+      <c r="M56" t="s">
+        <v>54</v>
+      </c>
+      <c r="N56" t="s">
+        <v>55</v>
+      </c>
+      <c r="O56">
+        <v>270.77363896848101</v>
+      </c>
+      <c r="P56" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="3">
+        <v>23</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <v>15.042979942693492</v>
+      </c>
+      <c r="T56" t="s">
+        <v>57</v>
+      </c>
+      <c r="U56" t="s">
+        <v>58</v>
+      </c>
+      <c r="V56" s="2">
+        <v>1</v>
+      </c>
+      <c r="W56" s="2">
+        <v>1</v>
+      </c>
+      <c r="X56" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE56">
+        <v>455.83529832288798</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>28</v>
+      </c>
+      <c r="I57">
+        <v>28</v>
+      </c>
+      <c r="J57">
+        <v>28</v>
+      </c>
+      <c r="M57" t="s">
+        <v>54</v>
+      </c>
+      <c r="N57" t="s">
+        <v>55</v>
+      </c>
+      <c r="O57">
+        <v>238.681948424068</v>
+      </c>
+      <c r="P57" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="3">
+        <v>23</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57">
+        <v>13.538681948423999</v>
+      </c>
+      <c r="T57" t="s">
+        <v>57</v>
+      </c>
+      <c r="U57" t="s">
+        <v>58</v>
+      </c>
+      <c r="V57" s="2">
+        <v>1</v>
+      </c>
+      <c r="W57" s="2">
+        <v>1</v>
+      </c>
+      <c r="X57" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE57">
+        <v>389.52915198929901</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>28</v>
+      </c>
+      <c r="I58">
+        <v>28</v>
+      </c>
+      <c r="J58">
+        <v>28</v>
+      </c>
+      <c r="M58" t="s">
+        <v>54</v>
+      </c>
+      <c r="N58" t="s">
+        <v>55</v>
+      </c>
+      <c r="O58">
+        <v>153.438395415472</v>
+      </c>
+      <c r="P58" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q58" s="3">
+        <v>23</v>
+      </c>
+      <c r="R58">
+        <v>0</v>
+      </c>
+      <c r="S58">
+        <v>5.5157593123209949</v>
+      </c>
+      <c r="T58" t="s">
+        <v>57</v>
+      </c>
+      <c r="U58" t="s">
+        <v>58</v>
+      </c>
+      <c r="V58" s="2">
+        <v>1</v>
+      </c>
+      <c r="W58" s="2">
+        <v>1</v>
+      </c>
+      <c r="X58" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE58">
+        <v>270.055865277625</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" t="s">
+        <v>62</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>28</v>
+      </c>
+      <c r="I59">
+        <v>28</v>
+      </c>
+      <c r="J59">
+        <v>28</v>
+      </c>
+      <c r="M59" t="s">
+        <v>54</v>
+      </c>
+      <c r="N59" t="s">
+        <v>55</v>
+      </c>
+      <c r="O59">
+        <v>68.194842406876703</v>
+      </c>
+      <c r="P59" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="3">
+        <v>23</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <v>3.7607449856733055</v>
+      </c>
+      <c r="T59" t="s">
+        <v>57</v>
+      </c>
+      <c r="U59" t="s">
+        <v>58</v>
+      </c>
+      <c r="V59" s="2">
+        <v>1</v>
+      </c>
+      <c r="W59" s="2">
+        <v>1</v>
+      </c>
+      <c r="X59" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE59">
+        <v>179.75762886776201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>28</v>
+      </c>
+      <c r="I60">
+        <v>28</v>
+      </c>
+      <c r="J60">
+        <v>28</v>
+      </c>
+      <c r="M60" t="s">
+        <v>54</v>
+      </c>
+      <c r="N60" t="s">
+        <v>55</v>
+      </c>
+      <c r="O60">
+        <v>34.097421203438302</v>
+      </c>
+      <c r="P60" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="3">
+        <v>23</v>
+      </c>
+      <c r="R60">
+        <v>0</v>
+      </c>
+      <c r="S60">
+        <v>3.7607449856733517</v>
+      </c>
+      <c r="T60" t="s">
+        <v>57</v>
+      </c>
+      <c r="U60" t="s">
+        <v>58</v>
+      </c>
+      <c r="V60" s="2">
+        <v>1</v>
+      </c>
+      <c r="W60" s="2">
+        <v>1</v>
+      </c>
+      <c r="X60" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC60" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE60">
+        <v>89.312378569410697</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>50</v>
+      </c>
+      <c r="C61" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>28</v>
+      </c>
+      <c r="I61">
+        <v>28</v>
+      </c>
+      <c r="J61">
+        <v>28</v>
+      </c>
+      <c r="M61" t="s">
+        <v>54</v>
+      </c>
+      <c r="N61" t="s">
+        <v>55</v>
+      </c>
+      <c r="O61">
+        <v>6.0171919770773403</v>
+      </c>
+      <c r="P61" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="3">
+        <v>23</v>
+      </c>
+      <c r="R61">
+        <v>0</v>
+      </c>
+      <c r="T61" t="s">
+        <v>57</v>
+      </c>
+      <c r="U61" t="s">
+        <v>58</v>
+      </c>
+      <c r="V61" s="2">
+        <v>1</v>
+      </c>
+      <c r="W61" s="2">
+        <v>1</v>
+      </c>
+      <c r="X61" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC61" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>11</v>
+      </c>
+      <c r="B62" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>28</v>
+      </c>
+      <c r="I62">
+        <v>25</v>
+      </c>
+      <c r="J62">
+        <v>31</v>
+      </c>
+      <c r="K62">
+        <v>24</v>
+      </c>
+      <c r="M62" t="s">
+        <v>54</v>
+      </c>
+      <c r="N62" t="s">
+        <v>55</v>
+      </c>
+      <c r="O62">
+        <v>309.88538681948398</v>
+      </c>
+      <c r="P62" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q62" s="3">
+        <v>24</v>
+      </c>
+      <c r="R62">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <v>21.060171919771022</v>
+      </c>
+      <c r="T62" t="s">
+        <v>57</v>
+      </c>
+      <c r="U62" t="s">
+        <v>58</v>
+      </c>
+      <c r="V62" s="2">
+        <v>1</v>
+      </c>
+      <c r="W62" s="2">
+        <v>1</v>
+      </c>
+      <c r="X62" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC62" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE62">
+        <v>455.72287593757301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>11</v>
+      </c>
+      <c r="B63" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" t="s">
+        <v>62</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>28</v>
+      </c>
+      <c r="I63">
+        <v>25</v>
+      </c>
+      <c r="J63">
+        <v>31</v>
+      </c>
+      <c r="K63">
+        <v>24</v>
+      </c>
+      <c r="M63" t="s">
+        <v>54</v>
+      </c>
+      <c r="N63" t="s">
+        <v>55</v>
+      </c>
+      <c r="O63">
+        <v>252.722063037249</v>
+      </c>
+      <c r="P63" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q63" s="3">
+        <v>24</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>13.037249283667506</v>
+      </c>
+      <c r="T63" t="s">
+        <v>57</v>
+      </c>
+      <c r="U63" t="s">
+        <v>58</v>
+      </c>
+      <c r="V63" s="2">
+        <v>1</v>
+      </c>
+      <c r="W63" s="2">
+        <v>1</v>
+      </c>
+      <c r="X63" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC63" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE63">
+        <v>389.48879523559702</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>11</v>
+      </c>
+      <c r="B64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" t="s">
+        <v>62</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>28</v>
+      </c>
+      <c r="I64">
+        <v>25</v>
+      </c>
+      <c r="J64">
+        <v>31</v>
+      </c>
+      <c r="K64">
+        <v>24</v>
+      </c>
+      <c r="M64" t="s">
+        <v>54</v>
+      </c>
+      <c r="N64" t="s">
+        <v>55</v>
+      </c>
+      <c r="O64">
+        <v>153.438395415472</v>
+      </c>
+      <c r="P64" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="3">
+        <v>24</v>
+      </c>
+      <c r="R64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>5.5157593123209949</v>
+      </c>
+      <c r="T64" t="s">
+        <v>57</v>
+      </c>
+      <c r="U64" t="s">
+        <v>58</v>
+      </c>
+      <c r="V64" s="2">
+        <v>1</v>
+      </c>
+      <c r="W64" s="2">
+        <v>1</v>
+      </c>
+      <c r="X64" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC64" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE64">
+        <v>269.04982906032097</v>
+      </c>
+    </row>
+    <row r="65" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>11</v>
+      </c>
+      <c r="B65" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" t="s">
+        <v>62</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>28</v>
+      </c>
+      <c r="I65">
+        <v>25</v>
+      </c>
+      <c r="J65">
+        <v>31</v>
+      </c>
+      <c r="K65">
+        <v>24</v>
+      </c>
+      <c r="M65" t="s">
+        <v>54</v>
+      </c>
+      <c r="N65" t="s">
+        <v>55</v>
+      </c>
+      <c r="O65">
+        <v>71.203438395415404</v>
+      </c>
+      <c r="P65" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q65" s="3">
+        <v>24</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>5.0143266475644026</v>
+      </c>
+      <c r="T65" t="s">
+        <v>57</v>
+      </c>
+      <c r="U65" t="s">
+        <v>58</v>
+      </c>
+      <c r="V65" s="2">
+        <v>1</v>
+      </c>
+      <c r="W65" s="2">
+        <v>1</v>
+      </c>
+      <c r="X65" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC65" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE65">
+        <v>178.74294477466501</v>
+      </c>
+    </row>
+    <row r="66" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>11</v>
+      </c>
+      <c r="B66" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>28</v>
+      </c>
+      <c r="I66">
+        <v>25</v>
+      </c>
+      <c r="J66">
+        <v>31</v>
+      </c>
+      <c r="K66">
+        <v>24</v>
+      </c>
+      <c r="M66" t="s">
+        <v>54</v>
+      </c>
+      <c r="N66" t="s">
+        <v>55</v>
+      </c>
+      <c r="O66">
+        <v>34.097421203438302</v>
+      </c>
+      <c r="P66" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q66" s="3">
+        <v>24</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="S66">
+        <v>5.0143266475644488</v>
+      </c>
+      <c r="T66" t="s">
+        <v>57</v>
+      </c>
+      <c r="U66" t="s">
+        <v>58</v>
+      </c>
+      <c r="V66" s="2">
+        <v>1</v>
+      </c>
+      <c r="W66" s="2">
+        <v>1</v>
+      </c>
+      <c r="X66" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC66" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE66">
+        <v>89.312378569410697</v>
+      </c>
+    </row>
+    <row r="67" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>11</v>
+      </c>
+      <c r="B67" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" t="s">
+        <v>62</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>28</v>
+      </c>
+      <c r="I67">
+        <v>25</v>
+      </c>
+      <c r="J67">
+        <v>31</v>
+      </c>
+      <c r="K67">
+        <v>24</v>
+      </c>
+      <c r="M67" t="s">
+        <v>54</v>
+      </c>
+      <c r="N67" t="s">
+        <v>55</v>
+      </c>
+      <c r="O67">
+        <v>6.0171919770773403</v>
+      </c>
+      <c r="P67" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q67" s="3">
+        <v>24</v>
+      </c>
+      <c r="R67">
+        <v>0</v>
+      </c>
+      <c r="T67" t="s">
+        <v>57</v>
+      </c>
+      <c r="U67" t="s">
+        <v>58</v>
+      </c>
+      <c r="V67" s="2">
+        <v>1</v>
+      </c>
+      <c r="W67" s="2">
+        <v>1</v>
+      </c>
+      <c r="X67" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB67" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC67" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>12</v>
+      </c>
+      <c r="B68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" t="s">
+        <v>62</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>28</v>
+      </c>
+      <c r="I68">
+        <v>22</v>
+      </c>
+      <c r="J68">
+        <v>34</v>
+      </c>
+      <c r="K68">
+        <v>24</v>
+      </c>
+      <c r="M68" t="s">
+        <v>54</v>
+      </c>
+      <c r="N68" t="s">
+        <v>55</v>
+      </c>
+      <c r="O68">
+        <v>300.85959885386802</v>
+      </c>
+      <c r="P68" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q68" s="3">
+        <v>24</v>
+      </c>
+      <c r="R68">
+        <v>0</v>
+      </c>
+      <c r="S68">
+        <v>16.045845272206492</v>
+      </c>
+      <c r="T68" t="s">
+        <v>57</v>
+      </c>
+      <c r="U68" t="s">
+        <v>58</v>
+      </c>
+      <c r="V68" s="2">
+        <v>1</v>
+      </c>
+      <c r="W68" s="2">
+        <v>1</v>
+      </c>
+      <c r="X68" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB68" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC68" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE68">
+        <v>455.74881956495398</v>
+      </c>
+    </row>
+    <row r="69" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>12</v>
+      </c>
+      <c r="B69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C69" t="s">
+        <v>62</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>28</v>
+      </c>
+      <c r="I69">
+        <v>22</v>
+      </c>
+      <c r="J69">
+        <v>34</v>
+      </c>
+      <c r="K69">
+        <v>24</v>
+      </c>
+      <c r="M69" t="s">
+        <v>54</v>
+      </c>
+      <c r="N69" t="s">
+        <v>55</v>
+      </c>
+      <c r="O69">
+        <v>263.25214899713399</v>
+      </c>
+      <c r="P69" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q69" s="3">
+        <v>24</v>
+      </c>
+      <c r="R69">
+        <v>0</v>
+      </c>
+      <c r="S69">
+        <v>13.287965616045511</v>
+      </c>
+      <c r="T69" t="s">
+        <v>57</v>
+      </c>
+      <c r="U69" t="s">
+        <v>58</v>
+      </c>
+      <c r="V69" s="2">
+        <v>1</v>
+      </c>
+      <c r="W69" s="2">
+        <v>1</v>
+      </c>
+      <c r="X69" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE69">
+        <v>389.45852767032</v>
+      </c>
+    </row>
+    <row r="70" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>12</v>
+      </c>
+      <c r="B70" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" t="s">
+        <v>62</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>28</v>
+      </c>
+      <c r="I70">
+        <v>22</v>
+      </c>
+      <c r="J70">
+        <v>34</v>
+      </c>
+      <c r="K70">
+        <v>24</v>
+      </c>
+      <c r="M70" t="s">
+        <v>54</v>
+      </c>
+      <c r="N70" t="s">
+        <v>55</v>
+      </c>
+      <c r="O70">
+        <v>165.47277936962701</v>
+      </c>
+      <c r="P70" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q70" s="3">
+        <v>24</v>
+      </c>
+      <c r="R70">
+        <v>0</v>
+      </c>
+      <c r="S70">
+        <v>6.5186246418334974</v>
+      </c>
+      <c r="T70" t="s">
+        <v>57</v>
+      </c>
+      <c r="U70" t="s">
+        <v>58</v>
+      </c>
+      <c r="V70" s="2">
+        <v>1</v>
+      </c>
+      <c r="W70" s="2">
+        <v>1</v>
+      </c>
+      <c r="X70" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC70" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE70">
+        <v>269.015237557148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>12</v>
+      </c>
+      <c r="B71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C71" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>28</v>
+      </c>
+      <c r="I71">
+        <v>22</v>
+      </c>
+      <c r="J71">
+        <v>34</v>
+      </c>
+      <c r="K71">
+        <v>24</v>
+      </c>
+      <c r="M71" t="s">
+        <v>54</v>
+      </c>
+      <c r="N71" t="s">
+        <v>55</v>
+      </c>
+      <c r="O71">
+        <v>80.229226361031394</v>
+      </c>
+      <c r="P71" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q71" s="3">
+        <v>24</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>5.5157593123209452</v>
+      </c>
+      <c r="T71" t="s">
+        <v>57</v>
+      </c>
+      <c r="U71" t="s">
+        <v>58</v>
+      </c>
+      <c r="V71" s="2">
+        <v>1</v>
+      </c>
+      <c r="W71" s="2">
+        <v>1</v>
+      </c>
+      <c r="X71" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB71" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC71" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE71">
+        <v>179.72303736458801</v>
+      </c>
+    </row>
+    <row r="72" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>12</v>
+      </c>
+      <c r="B72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" t="s">
+        <v>62</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>28</v>
+      </c>
+      <c r="I72">
+        <v>22</v>
+      </c>
+      <c r="J72">
+        <v>34</v>
+      </c>
+      <c r="K72">
+        <v>24</v>
+      </c>
+      <c r="M72" t="s">
+        <v>54</v>
+      </c>
+      <c r="N72" t="s">
+        <v>55</v>
+      </c>
+      <c r="O72">
+        <v>40.114613180515597</v>
+      </c>
+      <c r="P72" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q72" s="3">
+        <v>24</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
+        <v>3.0085959885386977</v>
+      </c>
+      <c r="T72" t="s">
+        <v>57</v>
+      </c>
+      <c r="U72" t="s">
+        <v>58</v>
+      </c>
+      <c r="V72" s="2">
+        <v>1</v>
+      </c>
+      <c r="W72" s="2">
+        <v>1</v>
+      </c>
+      <c r="X72" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB72" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC72" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE72">
+        <v>89.295082817823896</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>12</v>
+      </c>
+      <c r="B73" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73" t="s">
+        <v>62</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>28</v>
+      </c>
+      <c r="I73">
+        <v>22</v>
+      </c>
+      <c r="J73">
+        <v>34</v>
+      </c>
+      <c r="K73">
+        <v>24</v>
+      </c>
+      <c r="M73" t="s">
+        <v>54</v>
+      </c>
+      <c r="N73" t="s">
+        <v>55</v>
+      </c>
+      <c r="O73">
+        <v>5.0143266475644701</v>
+      </c>
+      <c r="P73" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="3">
+        <v>24</v>
+      </c>
+      <c r="R73">
+        <v>0</v>
+      </c>
+      <c r="T73" t="s">
+        <v>57</v>
+      </c>
+      <c r="U73" t="s">
+        <v>58</v>
+      </c>
+      <c r="V73" s="2">
+        <v>1</v>
+      </c>
+      <c r="W73" s="2">
+        <v>1</v>
+      </c>
+      <c r="X73" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB73" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC73" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>13</v>
+      </c>
+      <c r="B74" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" t="s">
+        <v>62</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>28</v>
+      </c>
+      <c r="I74">
+        <v>28</v>
+      </c>
+      <c r="J74">
+        <v>28</v>
+      </c>
+      <c r="M74" t="s">
+        <v>54</v>
+      </c>
+      <c r="N74" t="s">
+        <v>55</v>
+      </c>
+      <c r="O74">
+        <v>129.36962750716299</v>
+      </c>
+      <c r="P74" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="3">
+        <v>14</v>
+      </c>
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74">
+        <v>25.071633237822496</v>
+      </c>
+      <c r="T74" t="s">
+        <v>57</v>
+      </c>
+      <c r="U74" t="s">
+        <v>58</v>
+      </c>
+      <c r="V74" s="2">
+        <v>1</v>
+      </c>
+      <c r="W74" s="2">
+        <v>1</v>
+      </c>
+      <c r="X74" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB74" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE74">
+        <v>455.23571226787601</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>13</v>
+      </c>
+      <c r="B75" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>28</v>
+      </c>
+      <c r="I75">
+        <v>28</v>
+      </c>
+      <c r="J75">
+        <v>28</v>
+      </c>
+      <c r="M75" t="s">
+        <v>54</v>
+      </c>
+      <c r="N75" t="s">
+        <v>55</v>
+      </c>
+      <c r="O75">
+        <v>111.31805157593099</v>
+      </c>
+      <c r="P75" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="3">
+        <v>14</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>38.108882521489946</v>
+      </c>
+      <c r="T75" t="s">
+        <v>57</v>
+      </c>
+      <c r="U75" t="s">
+        <v>58</v>
+      </c>
+      <c r="V75" s="2">
+        <v>1</v>
+      </c>
+      <c r="W75" s="2">
+        <v>1</v>
+      </c>
+      <c r="X75" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC75" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE75">
+        <v>388.88920918058398</v>
+      </c>
+    </row>
+    <row r="76" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>13</v>
+      </c>
+      <c r="B76" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>28</v>
+      </c>
+      <c r="I76">
+        <v>28</v>
+      </c>
+      <c r="J76">
+        <v>28</v>
+      </c>
+      <c r="M76" t="s">
+        <v>54</v>
+      </c>
+      <c r="N76" t="s">
+        <v>55</v>
+      </c>
+      <c r="O76">
+        <v>103.295128939828</v>
+      </c>
+      <c r="P76" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="3">
+        <v>14</v>
+      </c>
+      <c r="R76">
+        <v>0</v>
+      </c>
+      <c r="S76">
+        <v>18.051575931232101</v>
+      </c>
+      <c r="T76" t="s">
+        <v>57</v>
+      </c>
+      <c r="U76" t="s">
+        <v>58</v>
+      </c>
+      <c r="V76" s="2">
+        <v>1</v>
+      </c>
+      <c r="W76" s="2">
+        <v>1</v>
+      </c>
+      <c r="X76" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB76" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC76" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE76">
+        <v>270.19999654084899</v>
+      </c>
+    </row>
+    <row r="77" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>13</v>
+      </c>
+      <c r="B77" t="s">
+        <v>50</v>
+      </c>
+      <c r="C77" t="s">
+        <v>62</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>28</v>
+      </c>
+      <c r="I77">
+        <v>28</v>
+      </c>
+      <c r="J77">
+        <v>28</v>
+      </c>
+      <c r="M77" t="s">
+        <v>54</v>
+      </c>
+      <c r="N77" t="s">
+        <v>55</v>
+      </c>
+      <c r="O77">
+        <v>63.1805157593123</v>
+      </c>
+      <c r="P77" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q77" s="3">
+        <v>14</v>
+      </c>
+      <c r="R77">
+        <v>0</v>
+      </c>
+      <c r="S77">
+        <v>7.0200573065902532</v>
+      </c>
+      <c r="T77" t="s">
+        <v>57</v>
+      </c>
+      <c r="U77" t="s">
+        <v>58</v>
+      </c>
+      <c r="V77" s="2">
+        <v>1</v>
+      </c>
+      <c r="W77" s="2">
+        <v>1</v>
+      </c>
+      <c r="X77" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC77" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE77">
+        <v>179.77204199408399</v>
+      </c>
+    </row>
+    <row r="78" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>13</v>
+      </c>
+      <c r="B78" t="s">
+        <v>50</v>
+      </c>
+      <c r="C78" t="s">
+        <v>62</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>28</v>
+      </c>
+      <c r="I78">
+        <v>28</v>
+      </c>
+      <c r="J78">
+        <v>28</v>
+      </c>
+      <c r="M78" t="s">
+        <v>54</v>
+      </c>
+      <c r="N78" t="s">
+        <v>55</v>
+      </c>
+      <c r="O78">
+        <v>38.108882521489903</v>
+      </c>
+      <c r="P78" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q78" s="3">
+        <v>14</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78">
+        <v>8.5243553008596002</v>
+      </c>
+      <c r="T78" t="s">
+        <v>57</v>
+      </c>
+      <c r="U78" t="s">
+        <v>58</v>
+      </c>
+      <c r="V78" s="2">
+        <v>1</v>
+      </c>
+      <c r="W78" s="2">
+        <v>1</v>
+      </c>
+      <c r="X78" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC78" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE78">
+        <v>89.300848068352806</v>
+      </c>
+    </row>
+    <row r="79" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>13</v>
+      </c>
+      <c r="B79" t="s">
+        <v>50</v>
+      </c>
+      <c r="C79" t="s">
+        <v>62</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>28</v>
+      </c>
+      <c r="I79">
+        <v>28</v>
+      </c>
+      <c r="J79">
+        <v>28</v>
+      </c>
+      <c r="M79" t="s">
+        <v>54</v>
+      </c>
+      <c r="N79" t="s">
+        <v>55</v>
+      </c>
+      <c r="O79">
+        <v>6.0171919770773403</v>
+      </c>
+      <c r="P79" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q79" s="3">
+        <v>14</v>
+      </c>
+      <c r="R79">
+        <v>0</v>
+      </c>
+      <c r="T79" t="s">
+        <v>57</v>
+      </c>
+      <c r="U79" t="s">
+        <v>58</v>
+      </c>
+      <c r="V79" s="2">
+        <v>1</v>
+      </c>
+      <c r="W79" s="2">
+        <v>1</v>
+      </c>
+      <c r="X79" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB79" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC79" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>14</v>
+      </c>
+      <c r="B80" t="s">
+        <v>50</v>
+      </c>
+      <c r="C80" t="s">
+        <v>62</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="H80">
+        <v>28</v>
+      </c>
+      <c r="I80">
+        <v>25</v>
+      </c>
+      <c r="J80">
+        <v>31</v>
+      </c>
+      <c r="K80">
+        <v>24</v>
+      </c>
+      <c r="M80" t="s">
+        <v>54</v>
+      </c>
+      <c r="N80" t="s">
+        <v>55</v>
+      </c>
+      <c r="O80">
+        <v>108.30945558739199</v>
+      </c>
+      <c r="P80" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q80" s="3">
+        <v>9</v>
+      </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80">
+        <v>23.567335243552897</v>
+      </c>
+      <c r="T80" t="s">
+        <v>57</v>
+      </c>
+      <c r="U80" t="s">
+        <v>58</v>
+      </c>
+      <c r="V80" s="2">
+        <v>1</v>
+      </c>
+      <c r="W80" s="2">
+        <v>1</v>
+      </c>
+      <c r="X80" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB80" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC80" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE80">
+        <v>457.30831983303801</v>
+      </c>
+    </row>
+    <row r="81" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>14</v>
+      </c>
+      <c r="B81" t="s">
+        <v>50</v>
+      </c>
+      <c r="C81" t="s">
+        <v>62</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>28</v>
+      </c>
+      <c r="I81">
+        <v>25</v>
+      </c>
+      <c r="J81">
+        <v>31</v>
+      </c>
+      <c r="K81">
+        <v>24</v>
+      </c>
+      <c r="M81" t="s">
+        <v>54</v>
+      </c>
+      <c r="N81" t="s">
+        <v>55</v>
+      </c>
+      <c r="O81">
+        <v>97.277936962750601</v>
+      </c>
+      <c r="P81" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="3">
+        <v>9</v>
+      </c>
+      <c r="R81">
+        <v>0</v>
+      </c>
+      <c r="S81">
+        <v>22.564469914039947</v>
+      </c>
+      <c r="T81" t="s">
+        <v>57</v>
+      </c>
+      <c r="U81" t="s">
+        <v>58</v>
+      </c>
+      <c r="V81" s="2">
+        <v>1</v>
+      </c>
+      <c r="W81" s="2">
+        <v>1</v>
+      </c>
+      <c r="X81" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB81" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC81" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE81">
+        <v>389.93560215159101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>14</v>
+      </c>
+      <c r="B82" t="s">
+        <v>50</v>
+      </c>
+      <c r="C82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>28</v>
+      </c>
+      <c r="I82">
+        <v>25</v>
+      </c>
+      <c r="J82">
+        <v>31</v>
+      </c>
+      <c r="K82">
+        <v>24</v>
+      </c>
+      <c r="M82" t="s">
+        <v>54</v>
+      </c>
+      <c r="N82" t="s">
+        <v>55</v>
+      </c>
+      <c r="O82">
+        <v>95.272206303724801</v>
+      </c>
+      <c r="P82" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q82" s="3">
+        <v>9</v>
+      </c>
+      <c r="R82">
+        <v>0</v>
+      </c>
+      <c r="S82">
+        <v>12.034383954154549</v>
+      </c>
+      <c r="T82" t="s">
+        <v>57</v>
+      </c>
+      <c r="U82" t="s">
+        <v>58</v>
+      </c>
+      <c r="V82" s="2">
+        <v>1</v>
+      </c>
+      <c r="W82" s="2">
+        <v>1</v>
+      </c>
+      <c r="X82" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC82" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE82">
+        <v>269.21702132566099</v>
+      </c>
+    </row>
+    <row r="83" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>14</v>
+      </c>
+      <c r="B83" t="s">
+        <v>50</v>
+      </c>
+      <c r="C83" t="s">
+        <v>62</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <v>28</v>
+      </c>
+      <c r="I83">
+        <v>25</v>
+      </c>
+      <c r="J83">
+        <v>31</v>
+      </c>
+      <c r="K83">
+        <v>24</v>
+      </c>
+      <c r="M83" t="s">
+        <v>54</v>
+      </c>
+      <c r="N83" t="s">
+        <v>55</v>
+      </c>
+      <c r="O83">
+        <v>60.171919770773599</v>
+      </c>
+      <c r="P83" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q83" s="3">
+        <v>9</v>
+      </c>
+      <c r="R83">
+        <v>0</v>
+      </c>
+      <c r="S83">
+        <v>6.5186246418337497</v>
+      </c>
+      <c r="T83" t="s">
+        <v>57</v>
+      </c>
+      <c r="U83" t="s">
+        <v>58</v>
+      </c>
+      <c r="V83" s="2">
+        <v>1</v>
+      </c>
+      <c r="W83" s="2">
+        <v>1</v>
+      </c>
+      <c r="X83" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC83" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE83">
+        <v>178.77465365257399</v>
+      </c>
+    </row>
+    <row r="84" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>14</v>
+      </c>
+      <c r="B84" t="s">
+        <v>50</v>
+      </c>
+      <c r="C84" t="s">
+        <v>62</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+      <c r="F84">
+        <v>1</v>
+      </c>
+      <c r="H84">
+        <v>28</v>
+      </c>
+      <c r="I84">
+        <v>25</v>
+      </c>
+      <c r="J84">
+        <v>31</v>
+      </c>
+      <c r="K84">
+        <v>24</v>
+      </c>
+      <c r="M84" t="s">
+        <v>54</v>
+      </c>
+      <c r="N84" t="s">
+        <v>55</v>
+      </c>
+      <c r="O84">
+        <v>29.083094555873799</v>
+      </c>
+      <c r="P84" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q84" s="3">
+        <v>9</v>
+      </c>
+      <c r="R84">
+        <v>0</v>
+      </c>
+      <c r="S84">
+        <v>4.5128939828080004</v>
+      </c>
+      <c r="T84" t="s">
+        <v>57</v>
+      </c>
+      <c r="U84" t="s">
+        <v>58</v>
+      </c>
+      <c r="V84" s="2">
+        <v>1</v>
+      </c>
+      <c r="W84" s="2">
+        <v>1</v>
+      </c>
+      <c r="X84" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC84" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE84">
+        <v>89.326791695733107</v>
+      </c>
+    </row>
+    <row r="85" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>14</v>
+      </c>
+      <c r="B85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85" t="s">
+        <v>62</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="H85">
+        <v>28</v>
+      </c>
+      <c r="I85">
+        <v>25</v>
+      </c>
+      <c r="J85">
+        <v>31</v>
+      </c>
+      <c r="K85">
+        <v>24</v>
+      </c>
+      <c r="M85" t="s">
+        <v>54</v>
+      </c>
+      <c r="N85" t="s">
+        <v>55</v>
+      </c>
+      <c r="O85">
+        <v>6.0171919770773403</v>
+      </c>
+      <c r="P85" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q85" s="3">
+        <v>9</v>
+      </c>
+      <c r="R85">
+        <v>0</v>
+      </c>
+      <c r="T85" t="s">
+        <v>57</v>
+      </c>
+      <c r="U85" t="s">
+        <v>58</v>
+      </c>
+      <c r="V85" s="2">
+        <v>1</v>
+      </c>
+      <c r="W85" s="2">
+        <v>1</v>
+      </c>
+      <c r="X85" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC85" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>15</v>
+      </c>
+      <c r="B86" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" t="s">
+        <v>62</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>28</v>
+      </c>
+      <c r="I86">
+        <v>22</v>
+      </c>
+      <c r="J86">
+        <v>34</v>
+      </c>
+      <c r="K86">
+        <v>24</v>
+      </c>
+      <c r="M86" t="s">
+        <v>54</v>
+      </c>
+      <c r="N86" t="s">
+        <v>55</v>
+      </c>
+      <c r="O86">
+        <v>108.30945558739199</v>
+      </c>
+      <c r="P86" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q86" s="3">
+        <v>3</v>
+      </c>
+      <c r="R86">
+        <v>0</v>
+      </c>
+      <c r="S86">
+        <v>24.570200573065897</v>
+      </c>
+      <c r="T86" t="s">
+        <v>57</v>
+      </c>
+      <c r="U86" t="s">
+        <v>58</v>
+      </c>
+      <c r="V86" s="2">
+        <v>1</v>
+      </c>
+      <c r="W86" s="2">
+        <v>1</v>
+      </c>
+      <c r="X86" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC86" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE86">
+        <v>457.30831983303801</v>
+      </c>
+    </row>
+    <row r="87" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>15</v>
+      </c>
+      <c r="B87" t="s">
+        <v>50</v>
+      </c>
+      <c r="C87" t="s">
+        <v>62</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>28</v>
+      </c>
+      <c r="I87">
+        <v>22</v>
+      </c>
+      <c r="J87">
+        <v>34</v>
+      </c>
+      <c r="K87">
+        <v>24</v>
+      </c>
+      <c r="M87" t="s">
+        <v>54</v>
+      </c>
+      <c r="N87" t="s">
+        <v>55</v>
+      </c>
+      <c r="O87">
+        <v>112.32091690544399</v>
+      </c>
+      <c r="P87" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q87" s="3">
+        <v>3</v>
+      </c>
+      <c r="R87">
+        <v>0</v>
+      </c>
+      <c r="S87">
+        <v>17.800859598853748</v>
+      </c>
+      <c r="T87" t="s">
+        <v>57</v>
+      </c>
+      <c r="U87" t="s">
+        <v>58</v>
+      </c>
+      <c r="V87" s="2">
+        <v>1</v>
+      </c>
+      <c r="W87" s="2">
+        <v>1</v>
+      </c>
+      <c r="X87" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB87" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC87" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE87">
+        <v>389.89236277262398</v>
+      </c>
+    </row>
+    <row r="88" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>15</v>
+      </c>
+      <c r="B88" t="s">
+        <v>50</v>
+      </c>
+      <c r="C88" t="s">
+        <v>62</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>28</v>
+      </c>
+      <c r="I88">
+        <v>22</v>
+      </c>
+      <c r="J88">
+        <v>34</v>
+      </c>
+      <c r="K88">
+        <v>24</v>
+      </c>
+      <c r="M88" t="s">
+        <v>54</v>
+      </c>
+      <c r="N88" t="s">
+        <v>55</v>
+      </c>
+      <c r="O88">
+        <v>103.295128939828</v>
+      </c>
+      <c r="P88" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q88" s="3">
+        <v>3</v>
+      </c>
+      <c r="R88">
+        <v>0</v>
+      </c>
+      <c r="S88">
+        <v>18.553008595988551</v>
+      </c>
+      <c r="T88" t="s">
+        <v>57</v>
+      </c>
+      <c r="U88" t="s">
+        <v>58</v>
+      </c>
+      <c r="V88" s="2">
+        <v>1</v>
+      </c>
+      <c r="W88" s="2">
+        <v>1</v>
+      </c>
+      <c r="X88" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB88" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC88" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE88">
+        <v>269.19396032354501</v>
+      </c>
+    </row>
+    <row r="89" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>15</v>
+      </c>
+      <c r="B89" t="s">
+        <v>50</v>
+      </c>
+      <c r="C89" t="s">
+        <v>62</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>1</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <v>28</v>
+      </c>
+      <c r="I89">
+        <v>22</v>
+      </c>
+      <c r="J89">
+        <v>34</v>
+      </c>
+      <c r="K89">
+        <v>24</v>
+      </c>
+      <c r="M89" t="s">
+        <v>54</v>
+      </c>
+      <c r="N89" t="s">
+        <v>55</v>
+      </c>
+      <c r="O89">
+        <v>61.174785100286499</v>
+      </c>
+      <c r="P89" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q89" s="3">
+        <v>3</v>
+      </c>
+      <c r="R89">
+        <v>0</v>
+      </c>
+      <c r="S89">
+        <v>10.028653295128951</v>
+      </c>
+      <c r="T89" t="s">
+        <v>57</v>
+      </c>
+      <c r="U89" t="s">
+        <v>58</v>
+      </c>
+      <c r="V89" s="2">
+        <v>1</v>
+      </c>
+      <c r="W89" s="2">
+        <v>1</v>
+      </c>
+      <c r="X89" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB89" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC89" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE89">
+        <v>180.783843461917</v>
+      </c>
+    </row>
+    <row r="90" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>15</v>
+      </c>
+      <c r="B90" t="s">
+        <v>50</v>
+      </c>
+      <c r="C90" t="s">
+        <v>62</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>1</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="H90">
+        <v>28</v>
+      </c>
+      <c r="I90">
+        <v>22</v>
+      </c>
+      <c r="J90">
+        <v>34</v>
+      </c>
+      <c r="K90">
+        <v>24</v>
+      </c>
+      <c r="M90" t="s">
+        <v>54</v>
+      </c>
+      <c r="N90" t="s">
+        <v>55</v>
+      </c>
+      <c r="O90">
+        <v>39.111747851002796</v>
+      </c>
+      <c r="P90" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q90" s="3">
+        <v>3</v>
+      </c>
+      <c r="R90">
+        <v>0</v>
+      </c>
+      <c r="S90">
+        <v>11.03151862464185</v>
+      </c>
+      <c r="T90" t="s">
+        <v>57</v>
+      </c>
+      <c r="U90" t="s">
+        <v>58</v>
+      </c>
+      <c r="V90" s="2">
+        <v>1</v>
+      </c>
+      <c r="W90" s="2">
+        <v>1</v>
+      </c>
+      <c r="X90" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB90" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC90" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE90">
+        <v>89.297965443088302</v>
+      </c>
+    </row>
+    <row r="91" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>15</v>
+      </c>
+      <c r="B91" t="s">
+        <v>50</v>
+      </c>
+      <c r="C91" t="s">
+        <v>62</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>28</v>
+      </c>
+      <c r="I91">
+        <v>22</v>
+      </c>
+      <c r="J91">
+        <v>34</v>
+      </c>
+      <c r="K91">
+        <v>24</v>
+      </c>
+      <c r="M91" t="s">
+        <v>54</v>
+      </c>
+      <c r="N91" t="s">
+        <v>55</v>
+      </c>
+      <c r="O91">
+        <v>6.0171919770773403</v>
+      </c>
+      <c r="P91" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q91" s="3">
+        <v>3</v>
+      </c>
+      <c r="R91">
+        <v>0</v>
+      </c>
+      <c r="T91" t="s">
+        <v>57</v>
+      </c>
+      <c r="U91" t="s">
+        <v>58</v>
+      </c>
+      <c r="V91" s="2">
+        <v>1</v>
+      </c>
+      <c r="W91" s="2">
+        <v>1</v>
+      </c>
+      <c r="X91" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB91" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC91" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE91">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
kern et al 2015 physio extraction
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EF2C25-70AB-BC4A-AB87-12B438C1D548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC228BDB-9828-2D48-8D95-645420FB026F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="600" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="440" yWindow="600" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="75">
   <si>
     <t>study_id</t>
   </si>
@@ -220,6 +220,36 @@
   </si>
   <si>
     <t>figure 2b</t>
+  </si>
+  <si>
+    <t>kern_2015phys</t>
+  </si>
+  <si>
+    <t>development to stages 35-37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g </t>
+  </si>
+  <si>
+    <t>body length</t>
+  </si>
+  <si>
+    <t>tail length</t>
+  </si>
+  <si>
+    <t>Limnodynastes</t>
+  </si>
+  <si>
+    <t>peronii</t>
+  </si>
+  <si>
+    <t>tasmaniensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platyplectrum </t>
+  </si>
+  <si>
+    <t>ornatum</t>
   </si>
 </sst>
 </file>
@@ -586,11 +616,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AF89"/>
+  <dimension ref="A1:AF117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H90" sqref="H90"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A117" sqref="A107:A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4699,9 +4729,6 @@
       <c r="J56">
         <v>15</v>
       </c>
-      <c r="K56">
-        <v>24</v>
-      </c>
       <c r="L56" t="s">
         <v>45</v>
       </c>
@@ -4767,9 +4794,6 @@
       <c r="J57">
         <v>18</v>
       </c>
-      <c r="K57">
-        <v>24</v>
-      </c>
       <c r="L57" t="s">
         <v>45</v>
       </c>
@@ -4835,9 +4859,6 @@
       <c r="J58">
         <v>21</v>
       </c>
-      <c r="K58">
-        <v>24</v>
-      </c>
       <c r="L58" t="s">
         <v>45</v>
       </c>
@@ -4903,9 +4924,6 @@
       <c r="J59">
         <v>24</v>
       </c>
-      <c r="K59">
-        <v>24</v>
-      </c>
       <c r="L59" t="s">
         <v>45</v>
       </c>
@@ -4971,9 +4989,6 @@
       <c r="J60">
         <v>27</v>
       </c>
-      <c r="K60">
-        <v>24</v>
-      </c>
       <c r="L60" t="s">
         <v>45</v>
       </c>
@@ -5039,9 +5054,6 @@
       <c r="J61">
         <v>30</v>
       </c>
-      <c r="K61">
-        <v>24</v>
-      </c>
       <c r="L61" t="s">
         <v>45</v>
       </c>
@@ -5107,9 +5119,6 @@
       <c r="J62">
         <v>32</v>
       </c>
-      <c r="K62">
-        <v>24</v>
-      </c>
       <c r="L62" t="s">
         <v>45</v>
       </c>
@@ -5175,9 +5184,6 @@
       <c r="J63">
         <v>34</v>
       </c>
-      <c r="K63">
-        <v>24</v>
-      </c>
       <c r="L63" t="s">
         <v>45</v>
       </c>
@@ -6098,9 +6104,6 @@
       <c r="J76">
         <v>28</v>
       </c>
-      <c r="K76">
-        <v>28</v>
-      </c>
       <c r="L76" t="s">
         <v>50</v>
       </c>
@@ -6172,9 +6175,6 @@
       <c r="J77">
         <v>28</v>
       </c>
-      <c r="K77">
-        <v>28</v>
-      </c>
       <c r="L77" t="s">
         <v>50</v>
       </c>
@@ -6400,9 +6400,6 @@
       <c r="J80">
         <v>28</v>
       </c>
-      <c r="K80">
-        <v>28</v>
-      </c>
       <c r="L80" t="s">
         <v>50</v>
       </c>
@@ -6474,9 +6471,6 @@
       <c r="J81">
         <v>28</v>
       </c>
-      <c r="K81">
-        <v>28</v>
-      </c>
       <c r="L81" t="s">
         <v>50</v>
       </c>
@@ -6702,9 +6696,6 @@
       <c r="J84">
         <v>28</v>
       </c>
-      <c r="K84">
-        <v>28</v>
-      </c>
       <c r="L84" t="s">
         <v>52</v>
       </c>
@@ -6776,9 +6767,6 @@
       <c r="J85">
         <v>28</v>
       </c>
-      <c r="K85">
-        <v>28</v>
-      </c>
       <c r="L85" t="s">
         <v>52</v>
       </c>
@@ -7004,9 +6992,6 @@
       <c r="J88">
         <v>28</v>
       </c>
-      <c r="K88">
-        <v>28</v>
-      </c>
       <c r="L88" t="s">
         <v>52</v>
       </c>
@@ -7078,9 +7063,6 @@
       <c r="J89">
         <v>28</v>
       </c>
-      <c r="K89">
-        <v>28</v>
-      </c>
       <c r="L89" t="s">
         <v>52</v>
       </c>
@@ -7125,6 +7107,1754 @@
       </c>
       <c r="AD89" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>16</v>
+      </c>
+      <c r="B90" t="s">
+        <v>65</v>
+      </c>
+      <c r="C90" t="s">
+        <v>44</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>24</v>
+      </c>
+      <c r="I90">
+        <v>24</v>
+      </c>
+      <c r="J90">
+        <v>24</v>
+      </c>
+      <c r="L90" t="s">
+        <v>66</v>
+      </c>
+      <c r="M90" t="s">
+        <v>46</v>
+      </c>
+      <c r="N90">
+        <v>90.79</v>
+      </c>
+      <c r="O90">
+        <v>0</v>
+      </c>
+      <c r="Q90">
+        <v>0</v>
+      </c>
+      <c r="R90">
+        <v>0.72</v>
+      </c>
+      <c r="S90" t="s">
+        <v>70</v>
+      </c>
+      <c r="T90" t="s">
+        <v>71</v>
+      </c>
+      <c r="U90" s="1">
+        <v>1</v>
+      </c>
+      <c r="V90" s="1">
+        <v>1</v>
+      </c>
+      <c r="W90" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>16</v>
+      </c>
+      <c r="B91" t="s">
+        <v>65</v>
+      </c>
+      <c r="C91" t="s">
+        <v>44</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>25</v>
+      </c>
+      <c r="I91">
+        <v>20</v>
+      </c>
+      <c r="J91">
+        <v>30</v>
+      </c>
+      <c r="K91">
+        <v>24</v>
+      </c>
+      <c r="L91" t="s">
+        <v>66</v>
+      </c>
+      <c r="M91" t="s">
+        <v>46</v>
+      </c>
+      <c r="N91">
+        <v>115.55</v>
+      </c>
+      <c r="O91">
+        <v>0</v>
+      </c>
+      <c r="Q91">
+        <v>0</v>
+      </c>
+      <c r="R91">
+        <v>0.86</v>
+      </c>
+      <c r="S91" t="s">
+        <v>70</v>
+      </c>
+      <c r="T91" t="s">
+        <v>71</v>
+      </c>
+      <c r="U91" s="1">
+        <v>1</v>
+      </c>
+      <c r="V91" s="1">
+        <v>1</v>
+      </c>
+      <c r="W91" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>16</v>
+      </c>
+      <c r="B92" t="s">
+        <v>65</v>
+      </c>
+      <c r="C92" t="s">
+        <v>44</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>24</v>
+      </c>
+      <c r="I92">
+        <v>24</v>
+      </c>
+      <c r="J92">
+        <v>24</v>
+      </c>
+      <c r="L92" t="s">
+        <v>34</v>
+      </c>
+      <c r="M92" t="s">
+        <v>67</v>
+      </c>
+      <c r="N92">
+        <v>338.24</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+      <c r="Q92">
+        <v>0</v>
+      </c>
+      <c r="R92">
+        <v>7.41</v>
+      </c>
+      <c r="S92" t="s">
+        <v>70</v>
+      </c>
+      <c r="T92" t="s">
+        <v>71</v>
+      </c>
+      <c r="U92" s="1">
+        <v>1</v>
+      </c>
+      <c r="V92" s="1">
+        <v>1</v>
+      </c>
+      <c r="W92" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>16</v>
+      </c>
+      <c r="B93" t="s">
+        <v>65</v>
+      </c>
+      <c r="C93" t="s">
+        <v>44</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <v>1</v>
+      </c>
+      <c r="H93">
+        <v>25</v>
+      </c>
+      <c r="I93">
+        <v>20</v>
+      </c>
+      <c r="J93">
+        <v>30</v>
+      </c>
+      <c r="K93">
+        <v>24</v>
+      </c>
+      <c r="L93" t="s">
+        <v>34</v>
+      </c>
+      <c r="M93" t="s">
+        <v>67</v>
+      </c>
+      <c r="N93">
+        <v>320.95</v>
+      </c>
+      <c r="O93">
+        <v>0</v>
+      </c>
+      <c r="Q93">
+        <v>0</v>
+      </c>
+      <c r="R93">
+        <v>5.4</v>
+      </c>
+      <c r="S93" t="s">
+        <v>70</v>
+      </c>
+      <c r="T93" t="s">
+        <v>71</v>
+      </c>
+      <c r="U93" s="1">
+        <v>1</v>
+      </c>
+      <c r="V93" s="1">
+        <v>1</v>
+      </c>
+      <c r="W93" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>16</v>
+      </c>
+      <c r="B94" t="s">
+        <v>65</v>
+      </c>
+      <c r="C94" t="s">
+        <v>44</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>24</v>
+      </c>
+      <c r="I94">
+        <v>24</v>
+      </c>
+      <c r="J94">
+        <v>24</v>
+      </c>
+      <c r="L94" t="s">
+        <v>68</v>
+      </c>
+      <c r="M94" t="s">
+        <v>33</v>
+      </c>
+      <c r="N94">
+        <v>12.44</v>
+      </c>
+      <c r="O94">
+        <v>0</v>
+      </c>
+      <c r="Q94">
+        <v>0</v>
+      </c>
+      <c r="R94">
+        <v>0.1</v>
+      </c>
+      <c r="S94" t="s">
+        <v>70</v>
+      </c>
+      <c r="T94" t="s">
+        <v>71</v>
+      </c>
+      <c r="U94" s="1">
+        <v>1</v>
+      </c>
+      <c r="V94" s="1">
+        <v>1</v>
+      </c>
+      <c r="W94" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>16</v>
+      </c>
+      <c r="B95" t="s">
+        <v>65</v>
+      </c>
+      <c r="C95" t="s">
+        <v>44</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95">
+        <v>1</v>
+      </c>
+      <c r="H95">
+        <v>25</v>
+      </c>
+      <c r="I95">
+        <v>20</v>
+      </c>
+      <c r="J95">
+        <v>30</v>
+      </c>
+      <c r="K95">
+        <v>24</v>
+      </c>
+      <c r="L95" t="s">
+        <v>68</v>
+      </c>
+      <c r="M95" t="s">
+        <v>33</v>
+      </c>
+      <c r="N95">
+        <v>12.46</v>
+      </c>
+      <c r="O95">
+        <v>0</v>
+      </c>
+      <c r="Q95">
+        <v>0</v>
+      </c>
+      <c r="R95">
+        <v>0.1</v>
+      </c>
+      <c r="S95" t="s">
+        <v>70</v>
+      </c>
+      <c r="T95" t="s">
+        <v>71</v>
+      </c>
+      <c r="U95" s="1">
+        <v>1</v>
+      </c>
+      <c r="V95" s="1">
+        <v>1</v>
+      </c>
+      <c r="W95" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>16</v>
+      </c>
+      <c r="B96" t="s">
+        <v>65</v>
+      </c>
+      <c r="C96" t="s">
+        <v>44</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>24</v>
+      </c>
+      <c r="I96">
+        <v>24</v>
+      </c>
+      <c r="J96">
+        <v>24</v>
+      </c>
+      <c r="L96" t="s">
+        <v>69</v>
+      </c>
+      <c r="M96" t="s">
+        <v>33</v>
+      </c>
+      <c r="N96">
+        <v>26.2</v>
+      </c>
+      <c r="O96">
+        <v>0</v>
+      </c>
+      <c r="Q96">
+        <v>0</v>
+      </c>
+      <c r="R96">
+        <v>0.3</v>
+      </c>
+      <c r="S96" t="s">
+        <v>70</v>
+      </c>
+      <c r="T96" t="s">
+        <v>71</v>
+      </c>
+      <c r="U96" s="1">
+        <v>1</v>
+      </c>
+      <c r="V96" s="1">
+        <v>1</v>
+      </c>
+      <c r="W96" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>16</v>
+      </c>
+      <c r="B97" t="s">
+        <v>65</v>
+      </c>
+      <c r="C97" t="s">
+        <v>44</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="H97">
+        <v>25</v>
+      </c>
+      <c r="I97">
+        <v>20</v>
+      </c>
+      <c r="J97">
+        <v>30</v>
+      </c>
+      <c r="K97">
+        <v>24</v>
+      </c>
+      <c r="L97" t="s">
+        <v>69</v>
+      </c>
+      <c r="M97" t="s">
+        <v>33</v>
+      </c>
+      <c r="N97">
+        <v>25.12</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="Q97">
+        <v>0</v>
+      </c>
+      <c r="R97">
+        <v>0.25</v>
+      </c>
+      <c r="S97" t="s">
+        <v>70</v>
+      </c>
+      <c r="T97" t="s">
+        <v>71</v>
+      </c>
+      <c r="U97" s="1">
+        <v>1</v>
+      </c>
+      <c r="V97" s="1">
+        <v>1</v>
+      </c>
+      <c r="W97" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>17</v>
+      </c>
+      <c r="B98" t="s">
+        <v>65</v>
+      </c>
+      <c r="C98" t="s">
+        <v>44</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>24</v>
+      </c>
+      <c r="I98">
+        <v>24</v>
+      </c>
+      <c r="J98">
+        <v>24</v>
+      </c>
+      <c r="L98" t="s">
+        <v>66</v>
+      </c>
+      <c r="M98" t="s">
+        <v>46</v>
+      </c>
+      <c r="N98">
+        <v>156.43</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+      <c r="Q98">
+        <v>0</v>
+      </c>
+      <c r="R98">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S98" t="s">
+        <v>70</v>
+      </c>
+      <c r="T98" t="s">
+        <v>72</v>
+      </c>
+      <c r="U98" s="1">
+        <v>1</v>
+      </c>
+      <c r="V98" s="1">
+        <v>1</v>
+      </c>
+      <c r="W98" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>17</v>
+      </c>
+      <c r="B99" t="s">
+        <v>65</v>
+      </c>
+      <c r="C99" t="s">
+        <v>44</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>25</v>
+      </c>
+      <c r="I99">
+        <v>20</v>
+      </c>
+      <c r="J99">
+        <v>30</v>
+      </c>
+      <c r="K99">
+        <v>24</v>
+      </c>
+      <c r="L99" t="s">
+        <v>66</v>
+      </c>
+      <c r="M99" t="s">
+        <v>46</v>
+      </c>
+      <c r="N99">
+        <v>200.93</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="Q99">
+        <v>0</v>
+      </c>
+      <c r="R99">
+        <v>0.65</v>
+      </c>
+      <c r="S99" t="s">
+        <v>70</v>
+      </c>
+      <c r="T99" t="s">
+        <v>72</v>
+      </c>
+      <c r="U99" s="1">
+        <v>1</v>
+      </c>
+      <c r="V99" s="1">
+        <v>1</v>
+      </c>
+      <c r="W99" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>17</v>
+      </c>
+      <c r="B100" t="s">
+        <v>65</v>
+      </c>
+      <c r="C100" t="s">
+        <v>44</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>24</v>
+      </c>
+      <c r="I100">
+        <v>24</v>
+      </c>
+      <c r="J100">
+        <v>24</v>
+      </c>
+      <c r="L100" t="s">
+        <v>34</v>
+      </c>
+      <c r="M100" t="s">
+        <v>67</v>
+      </c>
+      <c r="N100">
+        <v>463.13</v>
+      </c>
+      <c r="O100">
+        <v>0</v>
+      </c>
+      <c r="Q100">
+        <v>0</v>
+      </c>
+      <c r="R100">
+        <v>8.92</v>
+      </c>
+      <c r="S100" t="s">
+        <v>70</v>
+      </c>
+      <c r="T100" t="s">
+        <v>72</v>
+      </c>
+      <c r="U100" s="1">
+        <v>1</v>
+      </c>
+      <c r="V100" s="1">
+        <v>1</v>
+      </c>
+      <c r="W100" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>17</v>
+      </c>
+      <c r="B101" t="s">
+        <v>65</v>
+      </c>
+      <c r="C101" t="s">
+        <v>44</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+      <c r="H101">
+        <v>25</v>
+      </c>
+      <c r="I101">
+        <v>20</v>
+      </c>
+      <c r="J101">
+        <v>30</v>
+      </c>
+      <c r="K101">
+        <v>24</v>
+      </c>
+      <c r="L101" t="s">
+        <v>34</v>
+      </c>
+      <c r="M101" t="s">
+        <v>67</v>
+      </c>
+      <c r="N101">
+        <v>370.12</v>
+      </c>
+      <c r="O101">
+        <v>0</v>
+      </c>
+      <c r="Q101">
+        <v>0</v>
+      </c>
+      <c r="R101">
+        <v>9.24</v>
+      </c>
+      <c r="S101" t="s">
+        <v>70</v>
+      </c>
+      <c r="T101" t="s">
+        <v>72</v>
+      </c>
+      <c r="U101" s="1">
+        <v>1</v>
+      </c>
+      <c r="V101" s="1">
+        <v>1</v>
+      </c>
+      <c r="W101" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>17</v>
+      </c>
+      <c r="B102" t="s">
+        <v>65</v>
+      </c>
+      <c r="C102" t="s">
+        <v>44</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>24</v>
+      </c>
+      <c r="I102">
+        <v>24</v>
+      </c>
+      <c r="J102">
+        <v>24</v>
+      </c>
+      <c r="L102" t="s">
+        <v>68</v>
+      </c>
+      <c r="M102" t="s">
+        <v>33</v>
+      </c>
+      <c r="N102">
+        <v>14.16</v>
+      </c>
+      <c r="O102">
+        <v>0</v>
+      </c>
+      <c r="Q102">
+        <v>0</v>
+      </c>
+      <c r="R102">
+        <v>0.12</v>
+      </c>
+      <c r="S102" t="s">
+        <v>70</v>
+      </c>
+      <c r="T102" t="s">
+        <v>72</v>
+      </c>
+      <c r="U102" s="1">
+        <v>1</v>
+      </c>
+      <c r="V102" s="1">
+        <v>1</v>
+      </c>
+      <c r="W102" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>17</v>
+      </c>
+      <c r="B103" t="s">
+        <v>65</v>
+      </c>
+      <c r="C103" t="s">
+        <v>44</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>1</v>
+      </c>
+      <c r="H103">
+        <v>25</v>
+      </c>
+      <c r="I103">
+        <v>20</v>
+      </c>
+      <c r="J103">
+        <v>30</v>
+      </c>
+      <c r="K103">
+        <v>24</v>
+      </c>
+      <c r="L103" t="s">
+        <v>68</v>
+      </c>
+      <c r="M103" t="s">
+        <v>33</v>
+      </c>
+      <c r="N103">
+        <v>13.46</v>
+      </c>
+      <c r="O103">
+        <v>0</v>
+      </c>
+      <c r="Q103">
+        <v>0</v>
+      </c>
+      <c r="R103">
+        <v>0.13</v>
+      </c>
+      <c r="S103" t="s">
+        <v>70</v>
+      </c>
+      <c r="T103" t="s">
+        <v>72</v>
+      </c>
+      <c r="U103" s="1">
+        <v>1</v>
+      </c>
+      <c r="V103" s="1">
+        <v>1</v>
+      </c>
+      <c r="W103" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>17</v>
+      </c>
+      <c r="B104" t="s">
+        <v>65</v>
+      </c>
+      <c r="C104" t="s">
+        <v>44</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>24</v>
+      </c>
+      <c r="I104">
+        <v>24</v>
+      </c>
+      <c r="J104">
+        <v>24</v>
+      </c>
+      <c r="L104" t="s">
+        <v>69</v>
+      </c>
+      <c r="M104" t="s">
+        <v>33</v>
+      </c>
+      <c r="N104">
+        <v>28.03</v>
+      </c>
+      <c r="O104">
+        <v>0</v>
+      </c>
+      <c r="Q104">
+        <v>0</v>
+      </c>
+      <c r="R104">
+        <v>0.24</v>
+      </c>
+      <c r="S104" t="s">
+        <v>70</v>
+      </c>
+      <c r="T104" t="s">
+        <v>72</v>
+      </c>
+      <c r="U104" s="1">
+        <v>1</v>
+      </c>
+      <c r="V104" s="1">
+        <v>1</v>
+      </c>
+      <c r="W104" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>17</v>
+      </c>
+      <c r="B105" t="s">
+        <v>65</v>
+      </c>
+      <c r="C105" t="s">
+        <v>44</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="H105">
+        <v>25</v>
+      </c>
+      <c r="I105">
+        <v>20</v>
+      </c>
+      <c r="J105">
+        <v>30</v>
+      </c>
+      <c r="K105">
+        <v>24</v>
+      </c>
+      <c r="L105" t="s">
+        <v>69</v>
+      </c>
+      <c r="M105" t="s">
+        <v>33</v>
+      </c>
+      <c r="N105">
+        <v>24.1</v>
+      </c>
+      <c r="O105">
+        <v>0</v>
+      </c>
+      <c r="Q105">
+        <v>0</v>
+      </c>
+      <c r="R105">
+        <v>0.25</v>
+      </c>
+      <c r="S105" t="s">
+        <v>70</v>
+      </c>
+      <c r="T105" t="s">
+        <v>72</v>
+      </c>
+      <c r="U105" s="1">
+        <v>1</v>
+      </c>
+      <c r="V105" s="1">
+        <v>1</v>
+      </c>
+      <c r="W105" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>18</v>
+      </c>
+      <c r="B106" t="s">
+        <v>65</v>
+      </c>
+      <c r="C106" t="s">
+        <v>44</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>24</v>
+      </c>
+      <c r="I106">
+        <v>24</v>
+      </c>
+      <c r="J106">
+        <v>24</v>
+      </c>
+      <c r="L106" t="s">
+        <v>66</v>
+      </c>
+      <c r="M106" t="s">
+        <v>46</v>
+      </c>
+      <c r="N106">
+        <v>29.75</v>
+      </c>
+      <c r="O106">
+        <v>0</v>
+      </c>
+      <c r="Q106">
+        <v>0</v>
+      </c>
+      <c r="R106">
+        <v>0.38</v>
+      </c>
+      <c r="S106" t="s">
+        <v>73</v>
+      </c>
+      <c r="T106" t="s">
+        <v>74</v>
+      </c>
+      <c r="U106" s="1">
+        <v>1</v>
+      </c>
+      <c r="V106" s="1">
+        <v>1</v>
+      </c>
+      <c r="W106" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>18</v>
+      </c>
+      <c r="B107" t="s">
+        <v>65</v>
+      </c>
+      <c r="C107" t="s">
+        <v>44</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+      <c r="H107">
+        <v>25</v>
+      </c>
+      <c r="I107">
+        <v>20</v>
+      </c>
+      <c r="J107">
+        <v>30</v>
+      </c>
+      <c r="K107">
+        <v>24</v>
+      </c>
+      <c r="L107" t="s">
+        <v>66</v>
+      </c>
+      <c r="M107" t="s">
+        <v>46</v>
+      </c>
+      <c r="N107">
+        <v>25.6</v>
+      </c>
+      <c r="O107">
+        <v>0</v>
+      </c>
+      <c r="Q107">
+        <v>0</v>
+      </c>
+      <c r="R107">
+        <v>0.33</v>
+      </c>
+      <c r="S107" t="s">
+        <v>73</v>
+      </c>
+      <c r="T107" t="s">
+        <v>74</v>
+      </c>
+      <c r="U107" s="1">
+        <v>1</v>
+      </c>
+      <c r="V107" s="1">
+        <v>1</v>
+      </c>
+      <c r="W107" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>18</v>
+      </c>
+      <c r="B108" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108" t="s">
+        <v>44</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <v>1</v>
+      </c>
+      <c r="H108">
+        <v>28</v>
+      </c>
+      <c r="I108">
+        <v>18</v>
+      </c>
+      <c r="J108">
+        <v>38</v>
+      </c>
+      <c r="K108">
+        <v>24</v>
+      </c>
+      <c r="L108" t="s">
+        <v>66</v>
+      </c>
+      <c r="M108" t="s">
+        <v>46</v>
+      </c>
+      <c r="N108">
+        <v>25.74</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
+      </c>
+      <c r="Q108">
+        <v>0</v>
+      </c>
+      <c r="R108">
+        <v>0.46</v>
+      </c>
+      <c r="S108" t="s">
+        <v>73</v>
+      </c>
+      <c r="T108" t="s">
+        <v>74</v>
+      </c>
+      <c r="U108" s="1">
+        <v>1</v>
+      </c>
+      <c r="V108" s="1">
+        <v>1</v>
+      </c>
+      <c r="W108" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>18</v>
+      </c>
+      <c r="B109" t="s">
+        <v>65</v>
+      </c>
+      <c r="C109" t="s">
+        <v>44</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>24</v>
+      </c>
+      <c r="I109">
+        <v>24</v>
+      </c>
+      <c r="J109">
+        <v>24</v>
+      </c>
+      <c r="L109" t="s">
+        <v>34</v>
+      </c>
+      <c r="M109" t="s">
+        <v>67</v>
+      </c>
+      <c r="N109">
+        <v>243.26</v>
+      </c>
+      <c r="O109">
+        <v>0</v>
+      </c>
+      <c r="Q109">
+        <v>0</v>
+      </c>
+      <c r="R109">
+        <v>6.16</v>
+      </c>
+      <c r="S109" t="s">
+        <v>73</v>
+      </c>
+      <c r="T109" t="s">
+        <v>74</v>
+      </c>
+      <c r="U109" s="1">
+        <v>1</v>
+      </c>
+      <c r="V109" s="1">
+        <v>1</v>
+      </c>
+      <c r="W109" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>18</v>
+      </c>
+      <c r="B110" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110" t="s">
+        <v>44</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>1</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="H110">
+        <v>25</v>
+      </c>
+      <c r="I110">
+        <v>20</v>
+      </c>
+      <c r="J110">
+        <v>30</v>
+      </c>
+      <c r="K110">
+        <v>24</v>
+      </c>
+      <c r="L110" t="s">
+        <v>34</v>
+      </c>
+      <c r="M110" t="s">
+        <v>67</v>
+      </c>
+      <c r="N110">
+        <v>182.66</v>
+      </c>
+      <c r="O110">
+        <v>0</v>
+      </c>
+      <c r="Q110">
+        <v>0</v>
+      </c>
+      <c r="R110">
+        <v>4.62</v>
+      </c>
+      <c r="S110" t="s">
+        <v>73</v>
+      </c>
+      <c r="T110" t="s">
+        <v>74</v>
+      </c>
+      <c r="U110" s="1">
+        <v>1</v>
+      </c>
+      <c r="V110" s="1">
+        <v>1</v>
+      </c>
+      <c r="W110" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>18</v>
+      </c>
+      <c r="B111" t="s">
+        <v>65</v>
+      </c>
+      <c r="C111" t="s">
+        <v>44</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>1</v>
+      </c>
+      <c r="H111">
+        <v>28</v>
+      </c>
+      <c r="I111">
+        <v>18</v>
+      </c>
+      <c r="J111">
+        <v>38</v>
+      </c>
+      <c r="K111">
+        <v>24</v>
+      </c>
+      <c r="L111" t="s">
+        <v>34</v>
+      </c>
+      <c r="M111" t="s">
+        <v>67</v>
+      </c>
+      <c r="N111">
+        <v>140.44999999999999</v>
+      </c>
+      <c r="O111">
+        <v>0</v>
+      </c>
+      <c r="Q111">
+        <v>0</v>
+      </c>
+      <c r="R111">
+        <v>3.6</v>
+      </c>
+      <c r="S111" t="s">
+        <v>73</v>
+      </c>
+      <c r="T111" t="s">
+        <v>74</v>
+      </c>
+      <c r="U111" s="1">
+        <v>1</v>
+      </c>
+      <c r="V111" s="1">
+        <v>1</v>
+      </c>
+      <c r="W111" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>18</v>
+      </c>
+      <c r="B112" t="s">
+        <v>65</v>
+      </c>
+      <c r="C112" t="s">
+        <v>44</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>24</v>
+      </c>
+      <c r="I112">
+        <v>24</v>
+      </c>
+      <c r="J112">
+        <v>24</v>
+      </c>
+      <c r="L112" t="s">
+        <v>68</v>
+      </c>
+      <c r="M112" t="s">
+        <v>33</v>
+      </c>
+      <c r="N112">
+        <v>11.48</v>
+      </c>
+      <c r="O112">
+        <v>0</v>
+      </c>
+      <c r="Q112">
+        <v>0</v>
+      </c>
+      <c r="R112">
+        <v>0.12</v>
+      </c>
+      <c r="S112" t="s">
+        <v>73</v>
+      </c>
+      <c r="T112" t="s">
+        <v>74</v>
+      </c>
+      <c r="U112" s="1">
+        <v>1</v>
+      </c>
+      <c r="V112" s="1">
+        <v>1</v>
+      </c>
+      <c r="W112" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>18</v>
+      </c>
+      <c r="B113" t="s">
+        <v>65</v>
+      </c>
+      <c r="C113" t="s">
+        <v>44</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <v>1</v>
+      </c>
+      <c r="H113">
+        <v>25</v>
+      </c>
+      <c r="I113">
+        <v>20</v>
+      </c>
+      <c r="J113">
+        <v>30</v>
+      </c>
+      <c r="K113">
+        <v>24</v>
+      </c>
+      <c r="L113" t="s">
+        <v>68</v>
+      </c>
+      <c r="M113" t="s">
+        <v>33</v>
+      </c>
+      <c r="N113">
+        <v>10.46</v>
+      </c>
+      <c r="O113">
+        <v>0</v>
+      </c>
+      <c r="Q113">
+        <v>0</v>
+      </c>
+      <c r="R113">
+        <v>0.11</v>
+      </c>
+      <c r="S113" t="s">
+        <v>73</v>
+      </c>
+      <c r="T113" t="s">
+        <v>74</v>
+      </c>
+      <c r="U113" s="1">
+        <v>1</v>
+      </c>
+      <c r="V113" s="1">
+        <v>1</v>
+      </c>
+      <c r="W113" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>18</v>
+      </c>
+      <c r="B114" t="s">
+        <v>65</v>
+      </c>
+      <c r="C114" t="s">
+        <v>44</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
+      </c>
+      <c r="H114">
+        <v>28</v>
+      </c>
+      <c r="I114">
+        <v>18</v>
+      </c>
+      <c r="J114">
+        <v>38</v>
+      </c>
+      <c r="K114">
+        <v>24</v>
+      </c>
+      <c r="L114" t="s">
+        <v>68</v>
+      </c>
+      <c r="M114" t="s">
+        <v>33</v>
+      </c>
+      <c r="N114">
+        <v>9.67</v>
+      </c>
+      <c r="O114">
+        <v>0</v>
+      </c>
+      <c r="Q114">
+        <v>0</v>
+      </c>
+      <c r="R114">
+        <v>0.09</v>
+      </c>
+      <c r="S114" t="s">
+        <v>73</v>
+      </c>
+      <c r="T114" t="s">
+        <v>74</v>
+      </c>
+      <c r="U114" s="1">
+        <v>1</v>
+      </c>
+      <c r="V114" s="1">
+        <v>1</v>
+      </c>
+      <c r="W114" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>18</v>
+      </c>
+      <c r="B115" t="s">
+        <v>65</v>
+      </c>
+      <c r="C115" t="s">
+        <v>44</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>24</v>
+      </c>
+      <c r="I115">
+        <v>24</v>
+      </c>
+      <c r="J115">
+        <v>24</v>
+      </c>
+      <c r="L115" t="s">
+        <v>69</v>
+      </c>
+      <c r="M115" t="s">
+        <v>33</v>
+      </c>
+      <c r="N115">
+        <v>19.77</v>
+      </c>
+      <c r="O115">
+        <v>0</v>
+      </c>
+      <c r="Q115">
+        <v>0</v>
+      </c>
+      <c r="R115">
+        <v>0.21</v>
+      </c>
+      <c r="S115" t="s">
+        <v>73</v>
+      </c>
+      <c r="T115" t="s">
+        <v>74</v>
+      </c>
+      <c r="U115" s="1">
+        <v>1</v>
+      </c>
+      <c r="V115" s="1">
+        <v>1</v>
+      </c>
+      <c r="W115" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>18</v>
+      </c>
+      <c r="B116" t="s">
+        <v>65</v>
+      </c>
+      <c r="C116" t="s">
+        <v>44</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>1</v>
+      </c>
+      <c r="H116">
+        <v>25</v>
+      </c>
+      <c r="I116">
+        <v>20</v>
+      </c>
+      <c r="J116">
+        <v>30</v>
+      </c>
+      <c r="K116">
+        <v>24</v>
+      </c>
+      <c r="L116" t="s">
+        <v>69</v>
+      </c>
+      <c r="M116" t="s">
+        <v>33</v>
+      </c>
+      <c r="N116">
+        <v>17.78</v>
+      </c>
+      <c r="O116">
+        <v>0</v>
+      </c>
+      <c r="Q116">
+        <v>0</v>
+      </c>
+      <c r="R116">
+        <v>0.22</v>
+      </c>
+      <c r="S116" t="s">
+        <v>73</v>
+      </c>
+      <c r="T116" t="s">
+        <v>74</v>
+      </c>
+      <c r="U116" s="1">
+        <v>1</v>
+      </c>
+      <c r="V116" s="1">
+        <v>1</v>
+      </c>
+      <c r="W116" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>18</v>
+      </c>
+      <c r="B117" t="s">
+        <v>65</v>
+      </c>
+      <c r="C117" t="s">
+        <v>44</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>1</v>
+      </c>
+      <c r="H117">
+        <v>28</v>
+      </c>
+      <c r="I117">
+        <v>18</v>
+      </c>
+      <c r="J117">
+        <v>38</v>
+      </c>
+      <c r="K117">
+        <v>24</v>
+      </c>
+      <c r="L117" t="s">
+        <v>69</v>
+      </c>
+      <c r="M117" t="s">
+        <v>33</v>
+      </c>
+      <c r="N117">
+        <v>17.02</v>
+      </c>
+      <c r="O117">
+        <v>0</v>
+      </c>
+      <c r="Q117">
+        <v>0</v>
+      </c>
+      <c r="R117">
+        <v>0.2</v>
+      </c>
+      <c r="S117" t="s">
+        <v>73</v>
+      </c>
+      <c r="T117" t="s">
+        <v>74</v>
+      </c>
+      <c r="U117" s="1">
+        <v>1</v>
+      </c>
+      <c r="V117" s="1">
+        <v>1</v>
+      </c>
+      <c r="W117" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maneti et al 2014 extraction and corresponding files
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D1E85C-DFAC-D649-A3A3-E65714189BA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7839CC7-8502-CA4E-A20F-B872231CC0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="600" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="101">
   <si>
     <t>study_id</t>
   </si>
@@ -280,6 +280,54 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>maneti2014</t>
+  </si>
+  <si>
+    <t>figure 2c</t>
+  </si>
+  <si>
+    <t>figure 2e</t>
+  </si>
+  <si>
+    <t>figure 2f</t>
+  </si>
+  <si>
+    <t>figure 2g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">figure 2h </t>
+  </si>
+  <si>
+    <t>offspring/female</t>
+  </si>
+  <si>
+    <t>productivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">egg to adult viability </t>
+  </si>
+  <si>
+    <t>body (centroid) size</t>
+  </si>
+  <si>
+    <t>pixels</t>
+  </si>
+  <si>
+    <t>time to  death (hour)</t>
+  </si>
+  <si>
+    <t>dessication tolerance</t>
+  </si>
+  <si>
+    <t>startvation tolerance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drosophila </t>
+  </si>
+  <si>
+    <t>simulans</t>
   </si>
 </sst>
 </file>
@@ -646,11 +694,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AF129"/>
+  <dimension ref="A1:AF147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B125" sqref="B125:C129"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G131" sqref="G131:G147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9727,6 +9775,1248 @@
         <v>82</v>
       </c>
     </row>
+    <row r="130" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>25</v>
+      </c>
+      <c r="B130" t="s">
+        <v>85</v>
+      </c>
+      <c r="C130" t="s">
+        <v>65</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="G130">
+        <v>23</v>
+      </c>
+      <c r="H130">
+        <v>23</v>
+      </c>
+      <c r="I130">
+        <v>23</v>
+      </c>
+      <c r="J130">
+        <v>23</v>
+      </c>
+      <c r="L130" t="s">
+        <v>92</v>
+      </c>
+      <c r="M130" t="s">
+        <v>91</v>
+      </c>
+      <c r="N130">
+        <v>78.12</v>
+      </c>
+      <c r="O130">
+        <v>0</v>
+      </c>
+      <c r="P130">
+        <v>20</v>
+      </c>
+      <c r="Q130">
+        <v>0</v>
+      </c>
+      <c r="R130">
+        <v>2.1600000000000037</v>
+      </c>
+      <c r="S130" t="s">
+        <v>99</v>
+      </c>
+      <c r="T130" t="s">
+        <v>100</v>
+      </c>
+      <c r="U130" s="1">
+        <v>1</v>
+      </c>
+      <c r="V130" s="1">
+        <v>1</v>
+      </c>
+      <c r="W130" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>25</v>
+      </c>
+      <c r="B131" t="s">
+        <v>85</v>
+      </c>
+      <c r="C131" t="s">
+        <v>65</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>2</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
+      <c r="G131">
+        <v>23</v>
+      </c>
+      <c r="H131">
+        <v>23</v>
+      </c>
+      <c r="I131">
+        <v>13</v>
+      </c>
+      <c r="J131">
+        <v>28</v>
+      </c>
+      <c r="K131">
+        <v>24</v>
+      </c>
+      <c r="L131" t="s">
+        <v>92</v>
+      </c>
+      <c r="M131" t="s">
+        <v>91</v>
+      </c>
+      <c r="N131">
+        <v>70.56</v>
+      </c>
+      <c r="O131">
+        <v>0</v>
+      </c>
+      <c r="P131">
+        <v>20</v>
+      </c>
+      <c r="Q131">
+        <v>0</v>
+      </c>
+      <c r="R131">
+        <v>2.7000000000000028</v>
+      </c>
+      <c r="S131" t="s">
+        <v>99</v>
+      </c>
+      <c r="T131" t="s">
+        <v>100</v>
+      </c>
+      <c r="U131" s="1">
+        <v>1</v>
+      </c>
+      <c r="V131" s="1">
+        <v>1</v>
+      </c>
+      <c r="W131" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>25</v>
+      </c>
+      <c r="B132" t="s">
+        <v>85</v>
+      </c>
+      <c r="C132" t="s">
+        <v>65</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>3</v>
+      </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
+      <c r="G132">
+        <v>23</v>
+      </c>
+      <c r="H132">
+        <v>23</v>
+      </c>
+      <c r="I132">
+        <v>13</v>
+      </c>
+      <c r="J132">
+        <v>28</v>
+      </c>
+      <c r="K132">
+        <v>24</v>
+      </c>
+      <c r="L132" t="s">
+        <v>92</v>
+      </c>
+      <c r="M132" t="s">
+        <v>91</v>
+      </c>
+      <c r="N132">
+        <v>72.84</v>
+      </c>
+      <c r="O132">
+        <v>0</v>
+      </c>
+      <c r="P132">
+        <v>20</v>
+      </c>
+      <c r="Q132">
+        <v>0</v>
+      </c>
+      <c r="R132">
+        <v>2.3999999999999986</v>
+      </c>
+      <c r="S132" t="s">
+        <v>99</v>
+      </c>
+      <c r="T132" t="s">
+        <v>100</v>
+      </c>
+      <c r="U132" s="1">
+        <v>1</v>
+      </c>
+      <c r="V132" s="1">
+        <v>1</v>
+      </c>
+      <c r="W132" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>26</v>
+      </c>
+      <c r="B133" t="s">
+        <v>85</v>
+      </c>
+      <c r="C133" t="s">
+        <v>86</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="G133">
+        <v>23</v>
+      </c>
+      <c r="H133">
+        <v>23</v>
+      </c>
+      <c r="I133">
+        <v>23</v>
+      </c>
+      <c r="J133">
+        <v>23</v>
+      </c>
+      <c r="L133" t="s">
+        <v>93</v>
+      </c>
+      <c r="M133" t="s">
+        <v>79</v>
+      </c>
+      <c r="N133">
+        <v>70.906874731397906</v>
+      </c>
+      <c r="O133">
+        <v>0</v>
+      </c>
+      <c r="P133">
+        <v>20</v>
+      </c>
+      <c r="Q133">
+        <v>0</v>
+      </c>
+      <c r="R133">
+        <v>2.3895582329317477</v>
+      </c>
+      <c r="S133" t="s">
+        <v>99</v>
+      </c>
+      <c r="T133" t="s">
+        <v>100</v>
+      </c>
+      <c r="U133" s="1">
+        <v>1</v>
+      </c>
+      <c r="V133" s="1">
+        <v>1</v>
+      </c>
+      <c r="W133" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>26</v>
+      </c>
+      <c r="B134" t="s">
+        <v>85</v>
+      </c>
+      <c r="C134" t="s">
+        <v>86</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>2</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
+      <c r="G134">
+        <v>23</v>
+      </c>
+      <c r="H134">
+        <v>23</v>
+      </c>
+      <c r="I134">
+        <v>13</v>
+      </c>
+      <c r="J134">
+        <v>28</v>
+      </c>
+      <c r="K134">
+        <v>24</v>
+      </c>
+      <c r="L134" t="s">
+        <v>93</v>
+      </c>
+      <c r="M134" t="s">
+        <v>79</v>
+      </c>
+      <c r="N134">
+        <v>71.961350938810497</v>
+      </c>
+      <c r="O134">
+        <v>0</v>
+      </c>
+      <c r="P134">
+        <v>20</v>
+      </c>
+      <c r="Q134">
+        <v>0</v>
+      </c>
+      <c r="R134">
+        <v>3.092369477911646</v>
+      </c>
+      <c r="S134" t="s">
+        <v>99</v>
+      </c>
+      <c r="T134" t="s">
+        <v>100</v>
+      </c>
+      <c r="U134" s="1">
+        <v>1</v>
+      </c>
+      <c r="V134" s="1">
+        <v>1</v>
+      </c>
+      <c r="W134" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>26</v>
+      </c>
+      <c r="B135" t="s">
+        <v>85</v>
+      </c>
+      <c r="C135" t="s">
+        <v>86</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>3</v>
+      </c>
+      <c r="F135">
+        <v>1</v>
+      </c>
+      <c r="G135">
+        <v>23</v>
+      </c>
+      <c r="H135">
+        <v>23</v>
+      </c>
+      <c r="I135">
+        <v>13</v>
+      </c>
+      <c r="J135">
+        <v>28</v>
+      </c>
+      <c r="K135">
+        <v>24</v>
+      </c>
+      <c r="L135" t="s">
+        <v>93</v>
+      </c>
+      <c r="M135" t="s">
+        <v>79</v>
+      </c>
+      <c r="N135">
+        <v>82.011811081966201</v>
+      </c>
+      <c r="O135">
+        <v>0</v>
+      </c>
+      <c r="P135">
+        <v>20</v>
+      </c>
+      <c r="Q135">
+        <v>0</v>
+      </c>
+      <c r="R135">
+        <v>3.0923694779116531</v>
+      </c>
+      <c r="S135" t="s">
+        <v>99</v>
+      </c>
+      <c r="T135" t="s">
+        <v>100</v>
+      </c>
+      <c r="U135" s="1">
+        <v>1</v>
+      </c>
+      <c r="V135" s="1">
+        <v>1</v>
+      </c>
+      <c r="W135" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>27</v>
+      </c>
+      <c r="B136" t="s">
+        <v>85</v>
+      </c>
+      <c r="C136" t="s">
+        <v>87</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="G136">
+        <v>23</v>
+      </c>
+      <c r="H136">
+        <v>23</v>
+      </c>
+      <c r="I136">
+        <v>23</v>
+      </c>
+      <c r="J136">
+        <v>23</v>
+      </c>
+      <c r="L136" t="s">
+        <v>46</v>
+      </c>
+      <c r="M136" t="s">
+        <v>47</v>
+      </c>
+      <c r="N136">
+        <v>10.2313253012048</v>
+      </c>
+      <c r="O136">
+        <v>0</v>
+      </c>
+      <c r="P136">
+        <v>20</v>
+      </c>
+      <c r="Q136">
+        <v>0</v>
+      </c>
+      <c r="R136">
+        <v>1.4457831325300319E-2</v>
+      </c>
+      <c r="S136" t="s">
+        <v>99</v>
+      </c>
+      <c r="T136" t="s">
+        <v>100</v>
+      </c>
+      <c r="U136" s="1">
+        <v>1</v>
+      </c>
+      <c r="V136" s="1">
+        <v>1</v>
+      </c>
+      <c r="W136" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>27</v>
+      </c>
+      <c r="B137" t="s">
+        <v>85</v>
+      </c>
+      <c r="C137" t="s">
+        <v>87</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>2</v>
+      </c>
+      <c r="F137">
+        <v>1</v>
+      </c>
+      <c r="G137">
+        <v>23</v>
+      </c>
+      <c r="H137">
+        <v>23</v>
+      </c>
+      <c r="I137">
+        <v>13</v>
+      </c>
+      <c r="J137">
+        <v>28</v>
+      </c>
+      <c r="K137">
+        <v>24</v>
+      </c>
+      <c r="L137" t="s">
+        <v>46</v>
+      </c>
+      <c r="M137" t="s">
+        <v>47</v>
+      </c>
+      <c r="N137">
+        <v>11.0939759036144</v>
+      </c>
+      <c r="O137">
+        <v>0</v>
+      </c>
+      <c r="P137">
+        <v>20</v>
+      </c>
+      <c r="Q137">
+        <v>0</v>
+      </c>
+      <c r="R137">
+        <v>1.6867469879500163E-2</v>
+      </c>
+      <c r="S137" t="s">
+        <v>99</v>
+      </c>
+      <c r="T137" t="s">
+        <v>100</v>
+      </c>
+      <c r="U137" s="1">
+        <v>1</v>
+      </c>
+      <c r="V137" s="1">
+        <v>1</v>
+      </c>
+      <c r="W137" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>27</v>
+      </c>
+      <c r="B138" t="s">
+        <v>85</v>
+      </c>
+      <c r="C138" t="s">
+        <v>87</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>3</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
+      <c r="G138">
+        <v>23</v>
+      </c>
+      <c r="H138">
+        <v>23</v>
+      </c>
+      <c r="I138">
+        <v>13</v>
+      </c>
+      <c r="J138">
+        <v>28</v>
+      </c>
+      <c r="K138">
+        <v>24</v>
+      </c>
+      <c r="L138" t="s">
+        <v>46</v>
+      </c>
+      <c r="M138" t="s">
+        <v>47</v>
+      </c>
+      <c r="N138">
+        <v>10.048192771084301</v>
+      </c>
+      <c r="O138">
+        <v>0</v>
+      </c>
+      <c r="P138">
+        <v>20</v>
+      </c>
+      <c r="Q138">
+        <v>0</v>
+      </c>
+      <c r="R138">
+        <v>1.9277108433749746E-2</v>
+      </c>
+      <c r="S138" t="s">
+        <v>99</v>
+      </c>
+      <c r="T138" t="s">
+        <v>100</v>
+      </c>
+      <c r="U138" s="1">
+        <v>1</v>
+      </c>
+      <c r="V138" s="1">
+        <v>1</v>
+      </c>
+      <c r="W138" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>28</v>
+      </c>
+      <c r="B139" t="s">
+        <v>85</v>
+      </c>
+      <c r="C139" t="s">
+        <v>88</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="G139">
+        <v>23</v>
+      </c>
+      <c r="H139">
+        <v>23</v>
+      </c>
+      <c r="I139">
+        <v>23</v>
+      </c>
+      <c r="J139">
+        <v>23</v>
+      </c>
+      <c r="L139" t="s">
+        <v>97</v>
+      </c>
+      <c r="M139" t="s">
+        <v>96</v>
+      </c>
+      <c r="N139">
+        <v>15.530718915646601</v>
+      </c>
+      <c r="O139">
+        <v>0</v>
+      </c>
+      <c r="P139">
+        <v>20</v>
+      </c>
+      <c r="Q139">
+        <v>0</v>
+      </c>
+      <c r="R139">
+        <v>0.35141081105024963</v>
+      </c>
+      <c r="S139" t="s">
+        <v>99</v>
+      </c>
+      <c r="T139" t="s">
+        <v>100</v>
+      </c>
+      <c r="U139" s="1">
+        <v>1</v>
+      </c>
+      <c r="V139" s="1">
+        <v>1</v>
+      </c>
+      <c r="W139" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>28</v>
+      </c>
+      <c r="B140" t="s">
+        <v>85</v>
+      </c>
+      <c r="C140" t="s">
+        <v>88</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>2</v>
+      </c>
+      <c r="F140">
+        <v>1</v>
+      </c>
+      <c r="G140">
+        <v>23</v>
+      </c>
+      <c r="H140">
+        <v>23</v>
+      </c>
+      <c r="I140">
+        <v>13</v>
+      </c>
+      <c r="J140">
+        <v>28</v>
+      </c>
+      <c r="K140">
+        <v>24</v>
+      </c>
+      <c r="L140" t="s">
+        <v>97</v>
+      </c>
+      <c r="M140" t="s">
+        <v>96</v>
+      </c>
+      <c r="N140">
+        <v>14.576963397168001</v>
+      </c>
+      <c r="O140">
+        <v>0</v>
+      </c>
+      <c r="P140">
+        <v>20</v>
+      </c>
+      <c r="Q140">
+        <v>0</v>
+      </c>
+      <c r="R140">
+        <v>0.32128988438879968</v>
+      </c>
+      <c r="S140" t="s">
+        <v>99</v>
+      </c>
+      <c r="T140" t="s">
+        <v>100</v>
+      </c>
+      <c r="U140" s="1">
+        <v>1</v>
+      </c>
+      <c r="V140" s="1">
+        <v>1</v>
+      </c>
+      <c r="W140" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>28</v>
+      </c>
+      <c r="B141" t="s">
+        <v>85</v>
+      </c>
+      <c r="C141" t="s">
+        <v>88</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>3</v>
+      </c>
+      <c r="F141">
+        <v>1</v>
+      </c>
+      <c r="G141">
+        <v>23</v>
+      </c>
+      <c r="H141">
+        <v>23</v>
+      </c>
+      <c r="I141">
+        <v>13</v>
+      </c>
+      <c r="J141">
+        <v>28</v>
+      </c>
+      <c r="K141">
+        <v>24</v>
+      </c>
+      <c r="L141" t="s">
+        <v>97</v>
+      </c>
+      <c r="M141" t="s">
+        <v>96</v>
+      </c>
+      <c r="N141">
+        <v>13.844020848406</v>
+      </c>
+      <c r="O141">
+        <v>0</v>
+      </c>
+      <c r="P141">
+        <v>20</v>
+      </c>
+      <c r="Q141">
+        <v>0</v>
+      </c>
+      <c r="R141">
+        <v>0.30120926661444969</v>
+      </c>
+      <c r="S141" t="s">
+        <v>99</v>
+      </c>
+      <c r="T141" t="s">
+        <v>100</v>
+      </c>
+      <c r="U141" s="1">
+        <v>1</v>
+      </c>
+      <c r="V141" s="1">
+        <v>1</v>
+      </c>
+      <c r="W141" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>29</v>
+      </c>
+      <c r="B142" t="s">
+        <v>85</v>
+      </c>
+      <c r="C142" t="s">
+        <v>89</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <v>23</v>
+      </c>
+      <c r="H142">
+        <v>23</v>
+      </c>
+      <c r="I142">
+        <v>23</v>
+      </c>
+      <c r="J142">
+        <v>23</v>
+      </c>
+      <c r="L142" t="s">
+        <v>94</v>
+      </c>
+      <c r="M142" t="s">
+        <v>95</v>
+      </c>
+      <c r="N142">
+        <v>1460.33382352941</v>
+      </c>
+      <c r="O142">
+        <v>0</v>
+      </c>
+      <c r="P142">
+        <v>20</v>
+      </c>
+      <c r="Q142">
+        <v>0</v>
+      </c>
+      <c r="R142">
+        <v>4.6000000000000227</v>
+      </c>
+      <c r="S142" t="s">
+        <v>99</v>
+      </c>
+      <c r="T142" t="s">
+        <v>100</v>
+      </c>
+      <c r="U142" s="1">
+        <v>1</v>
+      </c>
+      <c r="V142" s="1">
+        <v>1</v>
+      </c>
+      <c r="W142" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>29</v>
+      </c>
+      <c r="B143" t="s">
+        <v>85</v>
+      </c>
+      <c r="C143" t="s">
+        <v>89</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>2</v>
+      </c>
+      <c r="F143">
+        <v>1</v>
+      </c>
+      <c r="G143">
+        <v>23</v>
+      </c>
+      <c r="H143">
+        <v>23</v>
+      </c>
+      <c r="I143">
+        <v>13</v>
+      </c>
+      <c r="J143">
+        <v>28</v>
+      </c>
+      <c r="K143">
+        <v>24</v>
+      </c>
+      <c r="L143" t="s">
+        <v>94</v>
+      </c>
+      <c r="M143" t="s">
+        <v>95</v>
+      </c>
+      <c r="N143">
+        <v>1416.9338235294099</v>
+      </c>
+      <c r="O143">
+        <v>0</v>
+      </c>
+      <c r="P143">
+        <v>20</v>
+      </c>
+      <c r="Q143">
+        <v>0</v>
+      </c>
+      <c r="R143">
+        <v>5.3999999999999773</v>
+      </c>
+      <c r="S143" t="s">
+        <v>99</v>
+      </c>
+      <c r="T143" t="s">
+        <v>100</v>
+      </c>
+      <c r="U143" s="1">
+        <v>1</v>
+      </c>
+      <c r="V143" s="1">
+        <v>1</v>
+      </c>
+      <c r="W143" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>29</v>
+      </c>
+      <c r="B144" t="s">
+        <v>85</v>
+      </c>
+      <c r="C144" t="s">
+        <v>89</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>3</v>
+      </c>
+      <c r="F144">
+        <v>1</v>
+      </c>
+      <c r="G144">
+        <v>23</v>
+      </c>
+      <c r="H144">
+        <v>23</v>
+      </c>
+      <c r="I144">
+        <v>13</v>
+      </c>
+      <c r="J144">
+        <v>28</v>
+      </c>
+      <c r="K144">
+        <v>24</v>
+      </c>
+      <c r="L144" t="s">
+        <v>94</v>
+      </c>
+      <c r="M144" t="s">
+        <v>95</v>
+      </c>
+      <c r="N144">
+        <v>1437.9338235294099</v>
+      </c>
+      <c r="O144">
+        <v>0</v>
+      </c>
+      <c r="P144">
+        <v>20</v>
+      </c>
+      <c r="Q144">
+        <v>0</v>
+      </c>
+      <c r="R144">
+        <v>4.6000000000000227</v>
+      </c>
+      <c r="S144" t="s">
+        <v>99</v>
+      </c>
+      <c r="T144" t="s">
+        <v>100</v>
+      </c>
+      <c r="U144" s="1">
+        <v>1</v>
+      </c>
+      <c r="V144" s="1">
+        <v>1</v>
+      </c>
+      <c r="W144" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>30</v>
+      </c>
+      <c r="B145" t="s">
+        <v>85</v>
+      </c>
+      <c r="C145" t="s">
+        <v>90</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>23</v>
+      </c>
+      <c r="H145">
+        <v>23</v>
+      </c>
+      <c r="I145">
+        <v>23</v>
+      </c>
+      <c r="J145">
+        <v>23</v>
+      </c>
+      <c r="L145" t="s">
+        <v>98</v>
+      </c>
+      <c r="M145" t="s">
+        <v>96</v>
+      </c>
+      <c r="N145">
+        <v>4.00120561738209</v>
+      </c>
+      <c r="O145">
+        <v>0</v>
+      </c>
+      <c r="P145">
+        <v>20</v>
+      </c>
+      <c r="Q145">
+        <v>0</v>
+      </c>
+      <c r="R145">
+        <v>5.9459459459459962E-2</v>
+      </c>
+      <c r="S145" t="s">
+        <v>99</v>
+      </c>
+      <c r="T145" t="s">
+        <v>100</v>
+      </c>
+      <c r="U145" s="1">
+        <v>1</v>
+      </c>
+      <c r="V145" s="1">
+        <v>1</v>
+      </c>
+      <c r="W145" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>30</v>
+      </c>
+      <c r="B146" t="s">
+        <v>85</v>
+      </c>
+      <c r="C146" t="s">
+        <v>90</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>2</v>
+      </c>
+      <c r="F146">
+        <v>1</v>
+      </c>
+      <c r="G146">
+        <v>23</v>
+      </c>
+      <c r="H146">
+        <v>23</v>
+      </c>
+      <c r="I146">
+        <v>13</v>
+      </c>
+      <c r="J146">
+        <v>28</v>
+      </c>
+      <c r="K146">
+        <v>24</v>
+      </c>
+      <c r="L146" t="s">
+        <v>98</v>
+      </c>
+      <c r="M146" t="s">
+        <v>96</v>
+      </c>
+      <c r="N146">
+        <v>4.0174218335983003</v>
+      </c>
+      <c r="O146">
+        <v>0</v>
+      </c>
+      <c r="P146">
+        <v>20</v>
+      </c>
+      <c r="Q146">
+        <v>0</v>
+      </c>
+      <c r="R146">
+        <v>5.7657657657659955E-2</v>
+      </c>
+      <c r="S146" t="s">
+        <v>99</v>
+      </c>
+      <c r="T146" t="s">
+        <v>100</v>
+      </c>
+      <c r="U146" s="1">
+        <v>1</v>
+      </c>
+      <c r="V146" s="1">
+        <v>1</v>
+      </c>
+      <c r="W146" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>30</v>
+      </c>
+      <c r="B147" t="s">
+        <v>85</v>
+      </c>
+      <c r="C147" t="s">
+        <v>90</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147">
+        <v>3</v>
+      </c>
+      <c r="F147">
+        <v>1</v>
+      </c>
+      <c r="G147">
+        <v>23</v>
+      </c>
+      <c r="H147">
+        <v>23</v>
+      </c>
+      <c r="I147">
+        <v>13</v>
+      </c>
+      <c r="J147">
+        <v>28</v>
+      </c>
+      <c r="K147">
+        <v>24</v>
+      </c>
+      <c r="L147" t="s">
+        <v>98</v>
+      </c>
+      <c r="M147" t="s">
+        <v>96</v>
+      </c>
+      <c r="N147">
+        <v>3.8102278749337501</v>
+      </c>
+      <c r="O147">
+        <v>0</v>
+      </c>
+      <c r="P147">
+        <v>20</v>
+      </c>
+      <c r="Q147">
+        <v>0</v>
+      </c>
+      <c r="R147">
+        <v>5.5862480127184977E-2</v>
+      </c>
+      <c r="S147" t="s">
+        <v>99</v>
+      </c>
+      <c r="T147" t="s">
+        <v>100</v>
+      </c>
+      <c r="U147" s="1">
+        <v>1</v>
+      </c>
+      <c r="V147" s="1">
+        <v>1</v>
+      </c>
+      <c r="W147" s="1">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
arranging and updating full dataset files
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E813B6-33CB-2049-9CE8-8E702D7DB675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CD30784-6674-FD4E-9465-47052F0DB325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="metanaly_fulldataset" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="124">
   <si>
     <t>study_id</t>
   </si>
@@ -361,6 +361,42 @@
   </si>
   <si>
     <t>average cumulative number of eggs laid per female</t>
+  </si>
+  <si>
+    <t>simonici</t>
+  </si>
+  <si>
+    <t>incubation period</t>
+  </si>
+  <si>
+    <t>percent females</t>
+  </si>
+  <si>
+    <t>hatching success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total length </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mass </t>
+  </si>
+  <si>
+    <t>Caiman</t>
+  </si>
+  <si>
+    <t>latirostris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year of experiment </t>
+  </si>
+  <si>
+    <t>first year</t>
+  </si>
+  <si>
+    <t>second year</t>
   </si>
 </sst>
 </file>
@@ -727,11 +763,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AG259"/>
+  <dimension ref="A1:AG289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A247" sqref="A247:A259"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K265" sqref="K265:K284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19086,6 +19122,2091 @@
         <v>107</v>
       </c>
     </row>
+    <row r="260" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>39</v>
+      </c>
+      <c r="B260" t="s">
+        <v>112</v>
+      </c>
+      <c r="C260" t="s">
+        <v>45</v>
+      </c>
+      <c r="D260">
+        <v>0</v>
+      </c>
+      <c r="H260">
+        <v>31</v>
+      </c>
+      <c r="I260">
+        <v>31</v>
+      </c>
+      <c r="J260">
+        <v>31</v>
+      </c>
+      <c r="L260" t="s">
+        <v>114</v>
+      </c>
+      <c r="M260" t="s">
+        <v>79</v>
+      </c>
+      <c r="N260">
+        <v>100</v>
+      </c>
+      <c r="O260">
+        <v>0</v>
+      </c>
+      <c r="P260">
+        <v>18</v>
+      </c>
+      <c r="Q260">
+        <v>0</v>
+      </c>
+      <c r="R260">
+        <v>0</v>
+      </c>
+      <c r="S260" t="s">
+        <v>119</v>
+      </c>
+      <c r="T260" t="s">
+        <v>120</v>
+      </c>
+      <c r="U260" s="1">
+        <v>1</v>
+      </c>
+      <c r="V260" s="1">
+        <v>1</v>
+      </c>
+      <c r="W260" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA260" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB260" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="261" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>39</v>
+      </c>
+      <c r="B261" t="s">
+        <v>112</v>
+      </c>
+      <c r="C261" t="s">
+        <v>45</v>
+      </c>
+      <c r="D261">
+        <v>0</v>
+      </c>
+      <c r="H261">
+        <v>31</v>
+      </c>
+      <c r="I261">
+        <v>31</v>
+      </c>
+      <c r="J261">
+        <v>31</v>
+      </c>
+      <c r="L261" t="s">
+        <v>113</v>
+      </c>
+      <c r="M261" t="s">
+        <v>47</v>
+      </c>
+      <c r="N261">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="O261">
+        <v>0</v>
+      </c>
+      <c r="P261">
+        <v>18</v>
+      </c>
+      <c r="Q261">
+        <v>0</v>
+      </c>
+      <c r="R261">
+        <v>0.3</v>
+      </c>
+      <c r="S261" t="s">
+        <v>119</v>
+      </c>
+      <c r="T261" t="s">
+        <v>120</v>
+      </c>
+      <c r="U261" s="1">
+        <v>1</v>
+      </c>
+      <c r="V261" s="1">
+        <v>1</v>
+      </c>
+      <c r="W261" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA261" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB261" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="262" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>39</v>
+      </c>
+      <c r="B262" t="s">
+        <v>112</v>
+      </c>
+      <c r="C262" t="s">
+        <v>45</v>
+      </c>
+      <c r="D262">
+        <v>0</v>
+      </c>
+      <c r="H262">
+        <v>31</v>
+      </c>
+      <c r="I262">
+        <v>31</v>
+      </c>
+      <c r="J262">
+        <v>31</v>
+      </c>
+      <c r="L262" t="s">
+        <v>115</v>
+      </c>
+      <c r="M262" t="s">
+        <v>79</v>
+      </c>
+      <c r="N262">
+        <v>71</v>
+      </c>
+      <c r="O262">
+        <v>0</v>
+      </c>
+      <c r="P262">
+        <v>18</v>
+      </c>
+      <c r="Q262">
+        <v>0</v>
+      </c>
+      <c r="R262">
+        <v>5</v>
+      </c>
+      <c r="S262" t="s">
+        <v>119</v>
+      </c>
+      <c r="T262" t="s">
+        <v>120</v>
+      </c>
+      <c r="U262" s="1">
+        <v>1</v>
+      </c>
+      <c r="V262" s="1">
+        <v>1</v>
+      </c>
+      <c r="W262" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA262" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB262" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="263" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>39</v>
+      </c>
+      <c r="B263" t="s">
+        <v>112</v>
+      </c>
+      <c r="C263" t="s">
+        <v>45</v>
+      </c>
+      <c r="D263">
+        <v>0</v>
+      </c>
+      <c r="H263">
+        <v>31</v>
+      </c>
+      <c r="I263">
+        <v>31</v>
+      </c>
+      <c r="J263">
+        <v>31</v>
+      </c>
+      <c r="L263" t="s">
+        <v>116</v>
+      </c>
+      <c r="M263" t="s">
+        <v>117</v>
+      </c>
+      <c r="N263">
+        <v>24.2</v>
+      </c>
+      <c r="O263">
+        <v>0</v>
+      </c>
+      <c r="P263">
+        <v>18</v>
+      </c>
+      <c r="Q263">
+        <v>0</v>
+      </c>
+      <c r="R263">
+        <v>0.2</v>
+      </c>
+      <c r="S263" t="s">
+        <v>119</v>
+      </c>
+      <c r="T263" t="s">
+        <v>120</v>
+      </c>
+      <c r="U263" s="1">
+        <v>1</v>
+      </c>
+      <c r="V263" s="1">
+        <v>1</v>
+      </c>
+      <c r="W263" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA263" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB263" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="264" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>39</v>
+      </c>
+      <c r="B264" t="s">
+        <v>112</v>
+      </c>
+      <c r="C264" t="s">
+        <v>45</v>
+      </c>
+      <c r="D264">
+        <v>0</v>
+      </c>
+      <c r="H264">
+        <v>31</v>
+      </c>
+      <c r="I264">
+        <v>31</v>
+      </c>
+      <c r="J264">
+        <v>31</v>
+      </c>
+      <c r="L264" t="s">
+        <v>118</v>
+      </c>
+      <c r="M264" t="s">
+        <v>69</v>
+      </c>
+      <c r="N264">
+        <v>51.6</v>
+      </c>
+      <c r="O264">
+        <v>0</v>
+      </c>
+      <c r="P264">
+        <v>18</v>
+      </c>
+      <c r="Q264">
+        <v>0</v>
+      </c>
+      <c r="R264">
+        <v>1</v>
+      </c>
+      <c r="S264" t="s">
+        <v>119</v>
+      </c>
+      <c r="T264" t="s">
+        <v>120</v>
+      </c>
+      <c r="U264" s="1">
+        <v>1</v>
+      </c>
+      <c r="V264" s="1">
+        <v>1</v>
+      </c>
+      <c r="W264" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA264" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB264" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="265" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>40</v>
+      </c>
+      <c r="B265" t="s">
+        <v>112</v>
+      </c>
+      <c r="C265" t="s">
+        <v>45</v>
+      </c>
+      <c r="D265">
+        <v>1</v>
+      </c>
+      <c r="E265">
+        <v>1</v>
+      </c>
+      <c r="F265">
+        <v>1</v>
+      </c>
+      <c r="H265">
+        <v>31</v>
+      </c>
+      <c r="I265">
+        <v>29</v>
+      </c>
+      <c r="J265">
+        <v>33</v>
+      </c>
+      <c r="K265">
+        <v>24</v>
+      </c>
+      <c r="L265" t="s">
+        <v>114</v>
+      </c>
+      <c r="M265" t="s">
+        <v>79</v>
+      </c>
+      <c r="N265">
+        <v>89.4</v>
+      </c>
+      <c r="O265">
+        <v>0</v>
+      </c>
+      <c r="P265">
+        <v>27</v>
+      </c>
+      <c r="Q265">
+        <v>0</v>
+      </c>
+      <c r="R265">
+        <v>6</v>
+      </c>
+      <c r="S265" t="s">
+        <v>119</v>
+      </c>
+      <c r="T265" t="s">
+        <v>120</v>
+      </c>
+      <c r="U265" s="1">
+        <v>1</v>
+      </c>
+      <c r="V265" s="1">
+        <v>1</v>
+      </c>
+      <c r="W265" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA265" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB265" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="266" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>40</v>
+      </c>
+      <c r="B266" t="s">
+        <v>112</v>
+      </c>
+      <c r="C266" t="s">
+        <v>45</v>
+      </c>
+      <c r="D266">
+        <v>1</v>
+      </c>
+      <c r="E266">
+        <v>1</v>
+      </c>
+      <c r="F266">
+        <v>1</v>
+      </c>
+      <c r="H266">
+        <v>31</v>
+      </c>
+      <c r="I266">
+        <v>29</v>
+      </c>
+      <c r="J266">
+        <v>33</v>
+      </c>
+      <c r="K266">
+        <v>24</v>
+      </c>
+      <c r="L266" t="s">
+        <v>113</v>
+      </c>
+      <c r="M266" t="s">
+        <v>47</v>
+      </c>
+      <c r="N266">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="O266">
+        <v>0</v>
+      </c>
+      <c r="P266">
+        <v>27</v>
+      </c>
+      <c r="Q266">
+        <v>0</v>
+      </c>
+      <c r="R266">
+        <v>0.3</v>
+      </c>
+      <c r="S266" t="s">
+        <v>119</v>
+      </c>
+      <c r="T266" t="s">
+        <v>120</v>
+      </c>
+      <c r="U266" s="1">
+        <v>1</v>
+      </c>
+      <c r="V266" s="1">
+        <v>1</v>
+      </c>
+      <c r="W266" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA266" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB266" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="267" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>40</v>
+      </c>
+      <c r="B267" t="s">
+        <v>112</v>
+      </c>
+      <c r="C267" t="s">
+        <v>45</v>
+      </c>
+      <c r="D267">
+        <v>1</v>
+      </c>
+      <c r="E267">
+        <v>1</v>
+      </c>
+      <c r="F267">
+        <v>1</v>
+      </c>
+      <c r="H267">
+        <v>31</v>
+      </c>
+      <c r="I267">
+        <v>29</v>
+      </c>
+      <c r="J267">
+        <v>33</v>
+      </c>
+      <c r="K267">
+        <v>24</v>
+      </c>
+      <c r="L267" t="s">
+        <v>115</v>
+      </c>
+      <c r="M267" t="s">
+        <v>79</v>
+      </c>
+      <c r="N267">
+        <v>83</v>
+      </c>
+      <c r="O267">
+        <v>0</v>
+      </c>
+      <c r="P267">
+        <v>27</v>
+      </c>
+      <c r="Q267">
+        <v>0</v>
+      </c>
+      <c r="R267">
+        <v>4</v>
+      </c>
+      <c r="S267" t="s">
+        <v>119</v>
+      </c>
+      <c r="T267" t="s">
+        <v>120</v>
+      </c>
+      <c r="U267" s="1">
+        <v>1</v>
+      </c>
+      <c r="V267" s="1">
+        <v>1</v>
+      </c>
+      <c r="W267" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA267" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB267" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="268" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>40</v>
+      </c>
+      <c r="B268" t="s">
+        <v>112</v>
+      </c>
+      <c r="C268" t="s">
+        <v>45</v>
+      </c>
+      <c r="D268">
+        <v>1</v>
+      </c>
+      <c r="E268">
+        <v>1</v>
+      </c>
+      <c r="F268">
+        <v>1</v>
+      </c>
+      <c r="H268">
+        <v>31</v>
+      </c>
+      <c r="I268">
+        <v>29</v>
+      </c>
+      <c r="J268">
+        <v>33</v>
+      </c>
+      <c r="K268">
+        <v>24</v>
+      </c>
+      <c r="L268" t="s">
+        <v>116</v>
+      </c>
+      <c r="M268" t="s">
+        <v>117</v>
+      </c>
+      <c r="N268">
+        <v>24.9</v>
+      </c>
+      <c r="O268">
+        <v>0</v>
+      </c>
+      <c r="P268">
+        <v>27</v>
+      </c>
+      <c r="Q268">
+        <v>0</v>
+      </c>
+      <c r="R268">
+        <v>0.5</v>
+      </c>
+      <c r="S268" t="s">
+        <v>119</v>
+      </c>
+      <c r="T268" t="s">
+        <v>120</v>
+      </c>
+      <c r="U268" s="1">
+        <v>1</v>
+      </c>
+      <c r="V268" s="1">
+        <v>1</v>
+      </c>
+      <c r="W268" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA268" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB268" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="269" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>40</v>
+      </c>
+      <c r="B269" t="s">
+        <v>112</v>
+      </c>
+      <c r="C269" t="s">
+        <v>45</v>
+      </c>
+      <c r="D269">
+        <v>1</v>
+      </c>
+      <c r="E269">
+        <v>1</v>
+      </c>
+      <c r="F269">
+        <v>1</v>
+      </c>
+      <c r="H269">
+        <v>31</v>
+      </c>
+      <c r="I269">
+        <v>29</v>
+      </c>
+      <c r="J269">
+        <v>33</v>
+      </c>
+      <c r="K269">
+        <v>24</v>
+      </c>
+      <c r="L269" t="s">
+        <v>118</v>
+      </c>
+      <c r="M269" t="s">
+        <v>69</v>
+      </c>
+      <c r="N269">
+        <v>51.4</v>
+      </c>
+      <c r="O269">
+        <v>0</v>
+      </c>
+      <c r="P269">
+        <v>27</v>
+      </c>
+      <c r="Q269">
+        <v>0</v>
+      </c>
+      <c r="R269">
+        <v>1</v>
+      </c>
+      <c r="S269" t="s">
+        <v>119</v>
+      </c>
+      <c r="T269" t="s">
+        <v>120</v>
+      </c>
+      <c r="U269" s="1">
+        <v>1</v>
+      </c>
+      <c r="V269" s="1">
+        <v>1</v>
+      </c>
+      <c r="W269" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA269" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB269" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="270" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>41</v>
+      </c>
+      <c r="B270" t="s">
+        <v>112</v>
+      </c>
+      <c r="C270" t="s">
+        <v>45</v>
+      </c>
+      <c r="D270">
+        <v>0</v>
+      </c>
+      <c r="H270">
+        <v>32</v>
+      </c>
+      <c r="I270">
+        <v>32</v>
+      </c>
+      <c r="J270">
+        <v>32</v>
+      </c>
+      <c r="L270" t="s">
+        <v>114</v>
+      </c>
+      <c r="M270" t="s">
+        <v>79</v>
+      </c>
+      <c r="N270">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="O270">
+        <v>0</v>
+      </c>
+      <c r="P270">
+        <v>25</v>
+      </c>
+      <c r="Q270">
+        <v>0</v>
+      </c>
+      <c r="R270">
+        <v>10</v>
+      </c>
+      <c r="S270" t="s">
+        <v>119</v>
+      </c>
+      <c r="T270" t="s">
+        <v>120</v>
+      </c>
+      <c r="U270" s="1">
+        <v>1</v>
+      </c>
+      <c r="V270" s="1">
+        <v>1</v>
+      </c>
+      <c r="W270" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA270" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB270" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="271" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>41</v>
+      </c>
+      <c r="B271" t="s">
+        <v>112</v>
+      </c>
+      <c r="C271" t="s">
+        <v>45</v>
+      </c>
+      <c r="D271">
+        <v>0</v>
+      </c>
+      <c r="H271">
+        <v>32</v>
+      </c>
+      <c r="I271">
+        <v>32</v>
+      </c>
+      <c r="J271">
+        <v>32</v>
+      </c>
+      <c r="L271" t="s">
+        <v>113</v>
+      </c>
+      <c r="M271" t="s">
+        <v>47</v>
+      </c>
+      <c r="N271">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="O271">
+        <v>0</v>
+      </c>
+      <c r="P271">
+        <v>25</v>
+      </c>
+      <c r="Q271">
+        <v>0</v>
+      </c>
+      <c r="R271">
+        <v>0.4</v>
+      </c>
+      <c r="S271" t="s">
+        <v>119</v>
+      </c>
+      <c r="T271" t="s">
+        <v>120</v>
+      </c>
+      <c r="U271" s="1">
+        <v>1</v>
+      </c>
+      <c r="V271" s="1">
+        <v>1</v>
+      </c>
+      <c r="W271" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA271" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB271" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="272" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>41</v>
+      </c>
+      <c r="B272" t="s">
+        <v>112</v>
+      </c>
+      <c r="C272" t="s">
+        <v>45</v>
+      </c>
+      <c r="D272">
+        <v>0</v>
+      </c>
+      <c r="H272">
+        <v>32</v>
+      </c>
+      <c r="I272">
+        <v>32</v>
+      </c>
+      <c r="J272">
+        <v>32</v>
+      </c>
+      <c r="L272" t="s">
+        <v>115</v>
+      </c>
+      <c r="M272" t="s">
+        <v>79</v>
+      </c>
+      <c r="N272">
+        <v>85</v>
+      </c>
+      <c r="O272">
+        <v>0</v>
+      </c>
+      <c r="P272">
+        <v>25</v>
+      </c>
+      <c r="Q272">
+        <v>0</v>
+      </c>
+      <c r="R272">
+        <v>6</v>
+      </c>
+      <c r="S272" t="s">
+        <v>119</v>
+      </c>
+      <c r="T272" t="s">
+        <v>120</v>
+      </c>
+      <c r="U272" s="1">
+        <v>1</v>
+      </c>
+      <c r="V272" s="1">
+        <v>1</v>
+      </c>
+      <c r="W272" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA272" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB272" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="273" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>41</v>
+      </c>
+      <c r="B273" t="s">
+        <v>112</v>
+      </c>
+      <c r="C273" t="s">
+        <v>45</v>
+      </c>
+      <c r="D273">
+        <v>0</v>
+      </c>
+      <c r="H273">
+        <v>32</v>
+      </c>
+      <c r="I273">
+        <v>32</v>
+      </c>
+      <c r="J273">
+        <v>32</v>
+      </c>
+      <c r="L273" t="s">
+        <v>116</v>
+      </c>
+      <c r="M273" t="s">
+        <v>117</v>
+      </c>
+      <c r="N273">
+        <v>22.2</v>
+      </c>
+      <c r="O273">
+        <v>0</v>
+      </c>
+      <c r="P273">
+        <v>25</v>
+      </c>
+      <c r="Q273">
+        <v>0</v>
+      </c>
+      <c r="R273">
+        <v>0.3</v>
+      </c>
+      <c r="S273" t="s">
+        <v>119</v>
+      </c>
+      <c r="T273" t="s">
+        <v>120</v>
+      </c>
+      <c r="U273" s="1">
+        <v>1</v>
+      </c>
+      <c r="V273" s="1">
+        <v>1</v>
+      </c>
+      <c r="W273" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA273" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB273" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="274" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>41</v>
+      </c>
+      <c r="B274" t="s">
+        <v>112</v>
+      </c>
+      <c r="C274" t="s">
+        <v>45</v>
+      </c>
+      <c r="D274">
+        <v>0</v>
+      </c>
+      <c r="H274">
+        <v>32</v>
+      </c>
+      <c r="I274">
+        <v>32</v>
+      </c>
+      <c r="J274">
+        <v>32</v>
+      </c>
+      <c r="L274" t="s">
+        <v>118</v>
+      </c>
+      <c r="M274" t="s">
+        <v>69</v>
+      </c>
+      <c r="N274">
+        <v>44.3</v>
+      </c>
+      <c r="O274">
+        <v>0</v>
+      </c>
+      <c r="P274">
+        <v>25</v>
+      </c>
+      <c r="Q274">
+        <v>0</v>
+      </c>
+      <c r="R274">
+        <v>0.7</v>
+      </c>
+      <c r="S274" t="s">
+        <v>119</v>
+      </c>
+      <c r="T274" t="s">
+        <v>120</v>
+      </c>
+      <c r="U274" s="1">
+        <v>1</v>
+      </c>
+      <c r="V274" s="1">
+        <v>1</v>
+      </c>
+      <c r="W274" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA274" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB274" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="275" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>42</v>
+      </c>
+      <c r="B275" t="s">
+        <v>112</v>
+      </c>
+      <c r="C275" t="s">
+        <v>45</v>
+      </c>
+      <c r="D275">
+        <v>1</v>
+      </c>
+      <c r="E275">
+        <v>1</v>
+      </c>
+      <c r="F275">
+        <v>1</v>
+      </c>
+      <c r="H275">
+        <v>32</v>
+      </c>
+      <c r="I275">
+        <v>31</v>
+      </c>
+      <c r="J275">
+        <v>33</v>
+      </c>
+      <c r="K275">
+        <v>24</v>
+      </c>
+      <c r="L275" t="s">
+        <v>114</v>
+      </c>
+      <c r="M275" t="s">
+        <v>79</v>
+      </c>
+      <c r="N275">
+        <v>65</v>
+      </c>
+      <c r="O275">
+        <v>0</v>
+      </c>
+      <c r="P275">
+        <v>21</v>
+      </c>
+      <c r="Q275">
+        <v>0</v>
+      </c>
+      <c r="R275">
+        <v>11</v>
+      </c>
+      <c r="S275" t="s">
+        <v>119</v>
+      </c>
+      <c r="T275" t="s">
+        <v>120</v>
+      </c>
+      <c r="U275" s="1">
+        <v>1</v>
+      </c>
+      <c r="V275" s="1">
+        <v>1</v>
+      </c>
+      <c r="W275" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA275" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB275" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="276" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>42</v>
+      </c>
+      <c r="B276" t="s">
+        <v>112</v>
+      </c>
+      <c r="C276" t="s">
+        <v>45</v>
+      </c>
+      <c r="D276">
+        <v>1</v>
+      </c>
+      <c r="E276">
+        <v>1</v>
+      </c>
+      <c r="F276">
+        <v>1</v>
+      </c>
+      <c r="H276">
+        <v>32</v>
+      </c>
+      <c r="I276">
+        <v>31</v>
+      </c>
+      <c r="J276">
+        <v>33</v>
+      </c>
+      <c r="K276">
+        <v>24</v>
+      </c>
+      <c r="L276" t="s">
+        <v>113</v>
+      </c>
+      <c r="M276" t="s">
+        <v>47</v>
+      </c>
+      <c r="N276">
+        <v>71.8</v>
+      </c>
+      <c r="O276">
+        <v>0</v>
+      </c>
+      <c r="P276">
+        <v>21</v>
+      </c>
+      <c r="Q276">
+        <v>0</v>
+      </c>
+      <c r="R276">
+        <v>0.4</v>
+      </c>
+      <c r="S276" t="s">
+        <v>119</v>
+      </c>
+      <c r="T276" t="s">
+        <v>120</v>
+      </c>
+      <c r="U276" s="1">
+        <v>1</v>
+      </c>
+      <c r="V276" s="1">
+        <v>1</v>
+      </c>
+      <c r="W276" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA276" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB276" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="277" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>42</v>
+      </c>
+      <c r="B277" t="s">
+        <v>112</v>
+      </c>
+      <c r="C277" t="s">
+        <v>45</v>
+      </c>
+      <c r="D277">
+        <v>1</v>
+      </c>
+      <c r="E277">
+        <v>1</v>
+      </c>
+      <c r="F277">
+        <v>1</v>
+      </c>
+      <c r="H277">
+        <v>32</v>
+      </c>
+      <c r="I277">
+        <v>31</v>
+      </c>
+      <c r="J277">
+        <v>33</v>
+      </c>
+      <c r="K277">
+        <v>24</v>
+      </c>
+      <c r="L277" t="s">
+        <v>115</v>
+      </c>
+      <c r="M277" t="s">
+        <v>79</v>
+      </c>
+      <c r="N277">
+        <v>52.5</v>
+      </c>
+      <c r="O277">
+        <v>0</v>
+      </c>
+      <c r="P277">
+        <v>21</v>
+      </c>
+      <c r="Q277">
+        <v>0</v>
+      </c>
+      <c r="R277">
+        <v>8</v>
+      </c>
+      <c r="S277" t="s">
+        <v>119</v>
+      </c>
+      <c r="T277" t="s">
+        <v>120</v>
+      </c>
+      <c r="U277" s="1">
+        <v>1</v>
+      </c>
+      <c r="V277" s="1">
+        <v>1</v>
+      </c>
+      <c r="W277" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA277" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB277" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="278" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>42</v>
+      </c>
+      <c r="B278" t="s">
+        <v>112</v>
+      </c>
+      <c r="C278" t="s">
+        <v>45</v>
+      </c>
+      <c r="D278">
+        <v>1</v>
+      </c>
+      <c r="E278">
+        <v>1</v>
+      </c>
+      <c r="F278">
+        <v>1</v>
+      </c>
+      <c r="H278">
+        <v>32</v>
+      </c>
+      <c r="I278">
+        <v>31</v>
+      </c>
+      <c r="J278">
+        <v>33</v>
+      </c>
+      <c r="K278">
+        <v>24</v>
+      </c>
+      <c r="L278" t="s">
+        <v>116</v>
+      </c>
+      <c r="M278" t="s">
+        <v>117</v>
+      </c>
+      <c r="N278">
+        <v>20.3</v>
+      </c>
+      <c r="O278">
+        <v>0</v>
+      </c>
+      <c r="P278">
+        <v>21</v>
+      </c>
+      <c r="Q278">
+        <v>0</v>
+      </c>
+      <c r="R278">
+        <v>0.3</v>
+      </c>
+      <c r="S278" t="s">
+        <v>119</v>
+      </c>
+      <c r="T278" t="s">
+        <v>120</v>
+      </c>
+      <c r="U278" s="1">
+        <v>1</v>
+      </c>
+      <c r="V278" s="1">
+        <v>1</v>
+      </c>
+      <c r="W278" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA278" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB278" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="279" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>42</v>
+      </c>
+      <c r="B279" t="s">
+        <v>112</v>
+      </c>
+      <c r="C279" t="s">
+        <v>45</v>
+      </c>
+      <c r="D279">
+        <v>1</v>
+      </c>
+      <c r="E279">
+        <v>1</v>
+      </c>
+      <c r="F279">
+        <v>1</v>
+      </c>
+      <c r="H279">
+        <v>32</v>
+      </c>
+      <c r="I279">
+        <v>31</v>
+      </c>
+      <c r="J279">
+        <v>33</v>
+      </c>
+      <c r="K279">
+        <v>24</v>
+      </c>
+      <c r="L279" t="s">
+        <v>118</v>
+      </c>
+      <c r="M279" t="s">
+        <v>69</v>
+      </c>
+      <c r="N279">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="O279">
+        <v>0</v>
+      </c>
+      <c r="P279">
+        <v>21</v>
+      </c>
+      <c r="Q279">
+        <v>0</v>
+      </c>
+      <c r="R279">
+        <v>0.7</v>
+      </c>
+      <c r="S279" t="s">
+        <v>119</v>
+      </c>
+      <c r="T279" t="s">
+        <v>120</v>
+      </c>
+      <c r="U279" s="1">
+        <v>1</v>
+      </c>
+      <c r="V279" s="1">
+        <v>1</v>
+      </c>
+      <c r="W279" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA279" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB279" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="280" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>43</v>
+      </c>
+      <c r="B280" t="s">
+        <v>112</v>
+      </c>
+      <c r="C280" t="s">
+        <v>45</v>
+      </c>
+      <c r="D280">
+        <v>1</v>
+      </c>
+      <c r="E280">
+        <v>1</v>
+      </c>
+      <c r="F280">
+        <v>1</v>
+      </c>
+      <c r="H280">
+        <v>32</v>
+      </c>
+      <c r="I280">
+        <v>30</v>
+      </c>
+      <c r="J280">
+        <v>34</v>
+      </c>
+      <c r="K280">
+        <v>24</v>
+      </c>
+      <c r="L280" t="s">
+        <v>114</v>
+      </c>
+      <c r="M280" t="s">
+        <v>79</v>
+      </c>
+      <c r="N280">
+        <v>84</v>
+      </c>
+      <c r="O280">
+        <v>0</v>
+      </c>
+      <c r="P280">
+        <v>26</v>
+      </c>
+      <c r="Q280">
+        <v>0</v>
+      </c>
+      <c r="R280">
+        <v>7</v>
+      </c>
+      <c r="S280" t="s">
+        <v>119</v>
+      </c>
+      <c r="T280" t="s">
+        <v>120</v>
+      </c>
+      <c r="U280" s="1">
+        <v>1</v>
+      </c>
+      <c r="V280" s="1">
+        <v>1</v>
+      </c>
+      <c r="W280" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA280" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB280" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="281" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>43</v>
+      </c>
+      <c r="B281" t="s">
+        <v>112</v>
+      </c>
+      <c r="C281" t="s">
+        <v>45</v>
+      </c>
+      <c r="D281">
+        <v>1</v>
+      </c>
+      <c r="E281">
+        <v>1</v>
+      </c>
+      <c r="F281">
+        <v>1</v>
+      </c>
+      <c r="H281">
+        <v>32</v>
+      </c>
+      <c r="I281">
+        <v>30</v>
+      </c>
+      <c r="J281">
+        <v>34</v>
+      </c>
+      <c r="K281">
+        <v>24</v>
+      </c>
+      <c r="L281" t="s">
+        <v>113</v>
+      </c>
+      <c r="M281" t="s">
+        <v>47</v>
+      </c>
+      <c r="N281">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="O281">
+        <v>0</v>
+      </c>
+      <c r="P281">
+        <v>26</v>
+      </c>
+      <c r="Q281">
+        <v>0</v>
+      </c>
+      <c r="R281">
+        <v>0.6</v>
+      </c>
+      <c r="S281" t="s">
+        <v>119</v>
+      </c>
+      <c r="T281" t="s">
+        <v>120</v>
+      </c>
+      <c r="U281" s="1">
+        <v>1</v>
+      </c>
+      <c r="V281" s="1">
+        <v>1</v>
+      </c>
+      <c r="W281" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA281" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB281" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="282" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>43</v>
+      </c>
+      <c r="B282" t="s">
+        <v>112</v>
+      </c>
+      <c r="C282" t="s">
+        <v>45</v>
+      </c>
+      <c r="D282">
+        <v>1</v>
+      </c>
+      <c r="E282">
+        <v>1</v>
+      </c>
+      <c r="F282">
+        <v>1</v>
+      </c>
+      <c r="H282">
+        <v>32</v>
+      </c>
+      <c r="I282">
+        <v>30</v>
+      </c>
+      <c r="J282">
+        <v>34</v>
+      </c>
+      <c r="K282">
+        <v>24</v>
+      </c>
+      <c r="L282" t="s">
+        <v>115</v>
+      </c>
+      <c r="M282" t="s">
+        <v>79</v>
+      </c>
+      <c r="N282">
+        <v>62</v>
+      </c>
+      <c r="O282">
+        <v>0</v>
+      </c>
+      <c r="P282">
+        <v>26</v>
+      </c>
+      <c r="Q282">
+        <v>0</v>
+      </c>
+      <c r="R282">
+        <v>8</v>
+      </c>
+      <c r="S282" t="s">
+        <v>119</v>
+      </c>
+      <c r="T282" t="s">
+        <v>120</v>
+      </c>
+      <c r="U282" s="1">
+        <v>1</v>
+      </c>
+      <c r="V282" s="1">
+        <v>1</v>
+      </c>
+      <c r="W282" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA282" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB282" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="283" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>43</v>
+      </c>
+      <c r="B283" t="s">
+        <v>112</v>
+      </c>
+      <c r="C283" t="s">
+        <v>45</v>
+      </c>
+      <c r="D283">
+        <v>1</v>
+      </c>
+      <c r="E283">
+        <v>1</v>
+      </c>
+      <c r="F283">
+        <v>1</v>
+      </c>
+      <c r="H283">
+        <v>32</v>
+      </c>
+      <c r="I283">
+        <v>30</v>
+      </c>
+      <c r="J283">
+        <v>34</v>
+      </c>
+      <c r="K283">
+        <v>24</v>
+      </c>
+      <c r="L283" t="s">
+        <v>116</v>
+      </c>
+      <c r="M283" t="s">
+        <v>117</v>
+      </c>
+      <c r="N283">
+        <v>20.3</v>
+      </c>
+      <c r="O283">
+        <v>0</v>
+      </c>
+      <c r="P283">
+        <v>26</v>
+      </c>
+      <c r="Q283">
+        <v>0</v>
+      </c>
+      <c r="R283">
+        <v>0.3</v>
+      </c>
+      <c r="S283" t="s">
+        <v>119</v>
+      </c>
+      <c r="T283" t="s">
+        <v>120</v>
+      </c>
+      <c r="U283" s="1">
+        <v>1</v>
+      </c>
+      <c r="V283" s="1">
+        <v>1</v>
+      </c>
+      <c r="W283" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA283" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB283" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="284" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>43</v>
+      </c>
+      <c r="B284" t="s">
+        <v>112</v>
+      </c>
+      <c r="C284" t="s">
+        <v>45</v>
+      </c>
+      <c r="D284">
+        <v>1</v>
+      </c>
+      <c r="E284">
+        <v>1</v>
+      </c>
+      <c r="F284">
+        <v>1</v>
+      </c>
+      <c r="H284">
+        <v>32</v>
+      </c>
+      <c r="I284">
+        <v>30</v>
+      </c>
+      <c r="J284">
+        <v>34</v>
+      </c>
+      <c r="K284">
+        <v>24</v>
+      </c>
+      <c r="L284" t="s">
+        <v>118</v>
+      </c>
+      <c r="M284" t="s">
+        <v>69</v>
+      </c>
+      <c r="N284">
+        <v>37.9</v>
+      </c>
+      <c r="O284">
+        <v>0</v>
+      </c>
+      <c r="P284">
+        <v>26</v>
+      </c>
+      <c r="Q284">
+        <v>0</v>
+      </c>
+      <c r="R284">
+        <v>0.8</v>
+      </c>
+      <c r="S284" t="s">
+        <v>119</v>
+      </c>
+      <c r="T284" t="s">
+        <v>120</v>
+      </c>
+      <c r="U284" s="1">
+        <v>1</v>
+      </c>
+      <c r="V284" s="1">
+        <v>1</v>
+      </c>
+      <c r="W284" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA284" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB284" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="285" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A285">
+        <v>44</v>
+      </c>
+      <c r="B285" t="s">
+        <v>112</v>
+      </c>
+      <c r="C285" t="s">
+        <v>45</v>
+      </c>
+      <c r="D285">
+        <v>0</v>
+      </c>
+      <c r="H285">
+        <v>33</v>
+      </c>
+      <c r="I285">
+        <v>33</v>
+      </c>
+      <c r="J285">
+        <v>33</v>
+      </c>
+      <c r="L285" t="s">
+        <v>114</v>
+      </c>
+      <c r="M285" t="s">
+        <v>79</v>
+      </c>
+      <c r="N285">
+        <v>0</v>
+      </c>
+      <c r="O285">
+        <v>0</v>
+      </c>
+      <c r="P285">
+        <v>34</v>
+      </c>
+      <c r="Q285">
+        <v>0</v>
+      </c>
+      <c r="R285">
+        <v>0</v>
+      </c>
+      <c r="S285" t="s">
+        <v>119</v>
+      </c>
+      <c r="T285" t="s">
+        <v>120</v>
+      </c>
+      <c r="U285" s="1">
+        <v>1</v>
+      </c>
+      <c r="V285" s="1">
+        <v>1</v>
+      </c>
+      <c r="W285" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA285" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB285" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="286" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A286">
+        <v>44</v>
+      </c>
+      <c r="B286" t="s">
+        <v>112</v>
+      </c>
+      <c r="C286" t="s">
+        <v>45</v>
+      </c>
+      <c r="D286">
+        <v>0</v>
+      </c>
+      <c r="H286">
+        <v>33</v>
+      </c>
+      <c r="I286">
+        <v>33</v>
+      </c>
+      <c r="J286">
+        <v>33</v>
+      </c>
+      <c r="L286" t="s">
+        <v>113</v>
+      </c>
+      <c r="M286" t="s">
+        <v>47</v>
+      </c>
+      <c r="N286">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="O286">
+        <v>0</v>
+      </c>
+      <c r="P286">
+        <v>34</v>
+      </c>
+      <c r="Q286">
+        <v>0</v>
+      </c>
+      <c r="R286">
+        <v>0.3</v>
+      </c>
+      <c r="S286" t="s">
+        <v>119</v>
+      </c>
+      <c r="T286" t="s">
+        <v>120</v>
+      </c>
+      <c r="U286" s="1">
+        <v>1</v>
+      </c>
+      <c r="V286" s="1">
+        <v>1</v>
+      </c>
+      <c r="W286" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA286" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB286" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="287" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A287">
+        <v>44</v>
+      </c>
+      <c r="B287" t="s">
+        <v>112</v>
+      </c>
+      <c r="C287" t="s">
+        <v>45</v>
+      </c>
+      <c r="D287">
+        <v>0</v>
+      </c>
+      <c r="H287">
+        <v>33</v>
+      </c>
+      <c r="I287">
+        <v>33</v>
+      </c>
+      <c r="J287">
+        <v>33</v>
+      </c>
+      <c r="L287" t="s">
+        <v>115</v>
+      </c>
+      <c r="M287" t="s">
+        <v>79</v>
+      </c>
+      <c r="N287">
+        <v>85.6</v>
+      </c>
+      <c r="O287">
+        <v>0</v>
+      </c>
+      <c r="P287">
+        <v>34</v>
+      </c>
+      <c r="Q287">
+        <v>0</v>
+      </c>
+      <c r="R287">
+        <v>6</v>
+      </c>
+      <c r="S287" t="s">
+        <v>119</v>
+      </c>
+      <c r="T287" t="s">
+        <v>120</v>
+      </c>
+      <c r="U287" s="1">
+        <v>1</v>
+      </c>
+      <c r="V287" s="1">
+        <v>1</v>
+      </c>
+      <c r="W287" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA287" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB287" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="288" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A288">
+        <v>44</v>
+      </c>
+      <c r="B288" t="s">
+        <v>112</v>
+      </c>
+      <c r="C288" t="s">
+        <v>45</v>
+      </c>
+      <c r="D288">
+        <v>0</v>
+      </c>
+      <c r="H288">
+        <v>33</v>
+      </c>
+      <c r="I288">
+        <v>33</v>
+      </c>
+      <c r="J288">
+        <v>33</v>
+      </c>
+      <c r="L288" t="s">
+        <v>116</v>
+      </c>
+      <c r="M288" t="s">
+        <v>117</v>
+      </c>
+      <c r="N288">
+        <v>22</v>
+      </c>
+      <c r="O288">
+        <v>0</v>
+      </c>
+      <c r="P288">
+        <v>34</v>
+      </c>
+      <c r="Q288">
+        <v>0</v>
+      </c>
+      <c r="R288">
+        <v>0.2</v>
+      </c>
+      <c r="S288" t="s">
+        <v>119</v>
+      </c>
+      <c r="T288" t="s">
+        <v>120</v>
+      </c>
+      <c r="U288" s="1">
+        <v>1</v>
+      </c>
+      <c r="V288" s="1">
+        <v>1</v>
+      </c>
+      <c r="W288" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA288" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB288" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="289" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A289">
+        <v>44</v>
+      </c>
+      <c r="B289" t="s">
+        <v>112</v>
+      </c>
+      <c r="C289" t="s">
+        <v>45</v>
+      </c>
+      <c r="D289">
+        <v>0</v>
+      </c>
+      <c r="H289">
+        <v>33</v>
+      </c>
+      <c r="I289">
+        <v>33</v>
+      </c>
+      <c r="J289">
+        <v>33</v>
+      </c>
+      <c r="L289" t="s">
+        <v>118</v>
+      </c>
+      <c r="M289" t="s">
+        <v>69</v>
+      </c>
+      <c r="N289">
+        <v>42.2</v>
+      </c>
+      <c r="O289">
+        <v>0</v>
+      </c>
+      <c r="P289">
+        <v>34</v>
+      </c>
+      <c r="Q289">
+        <v>0</v>
+      </c>
+      <c r="R289">
+        <v>1</v>
+      </c>
+      <c r="S289" t="s">
+        <v>119</v>
+      </c>
+      <c r="T289" t="s">
+        <v>120</v>
+      </c>
+      <c r="U289" s="1">
+        <v>1</v>
+      </c>
+      <c r="V289" s="1">
+        <v>1</v>
+      </c>
+      <c r="W289" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA289" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB289" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wang et al 2015 extraction
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CD30784-6674-FD4E-9465-47052F0DB325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F117B680-0350-F441-870B-8A8CFA3A89D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="460" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="metanaly_fulldataset" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="128">
   <si>
     <t>study_id</t>
   </si>
@@ -363,9 +363,6 @@
     <t>average cumulative number of eggs laid per female</t>
   </si>
   <si>
-    <t>simonici</t>
-  </si>
-  <si>
     <t>incubation period</t>
   </si>
   <si>
@@ -397,6 +394,21 @@
   </si>
   <si>
     <t>second year</t>
+  </si>
+  <si>
+    <t>wang2015</t>
+  </si>
+  <si>
+    <t>simonici2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dry weight of mycelium per petri dish </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esteya </t>
+  </si>
+  <si>
+    <t>vermicola</t>
   </si>
 </sst>
 </file>
@@ -763,11 +775,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AG289"/>
+  <dimension ref="A1:AG294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K265" sqref="K265:K284"/>
+      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W300" sqref="W300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19127,7 +19139,7 @@
         <v>39</v>
       </c>
       <c r="B260" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C260" t="s">
         <v>45</v>
@@ -19145,7 +19157,7 @@
         <v>31</v>
       </c>
       <c r="L260" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M260" t="s">
         <v>79</v>
@@ -19166,10 +19178,10 @@
         <v>0</v>
       </c>
       <c r="S260" t="s">
+        <v>118</v>
+      </c>
+      <c r="T260" t="s">
         <v>119</v>
-      </c>
-      <c r="T260" t="s">
-        <v>120</v>
       </c>
       <c r="U260" s="1">
         <v>1</v>
@@ -19181,10 +19193,10 @@
         <v>3</v>
       </c>
       <c r="AA260" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB260" t="s">
         <v>121</v>
-      </c>
-      <c r="AB260" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="261" spans="1:33" x14ac:dyDescent="0.2">
@@ -19192,7 +19204,7 @@
         <v>39</v>
       </c>
       <c r="B261" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C261" t="s">
         <v>45</v>
@@ -19210,7 +19222,7 @@
         <v>31</v>
       </c>
       <c r="L261" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M261" t="s">
         <v>47</v>
@@ -19231,10 +19243,10 @@
         <v>0.3</v>
       </c>
       <c r="S261" t="s">
+        <v>118</v>
+      </c>
+      <c r="T261" t="s">
         <v>119</v>
-      </c>
-      <c r="T261" t="s">
-        <v>120</v>
       </c>
       <c r="U261" s="1">
         <v>1</v>
@@ -19246,10 +19258,10 @@
         <v>3</v>
       </c>
       <c r="AA261" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB261" t="s">
         <v>121</v>
-      </c>
-      <c r="AB261" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="262" spans="1:33" x14ac:dyDescent="0.2">
@@ -19257,7 +19269,7 @@
         <v>39</v>
       </c>
       <c r="B262" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C262" t="s">
         <v>45</v>
@@ -19275,7 +19287,7 @@
         <v>31</v>
       </c>
       <c r="L262" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M262" t="s">
         <v>79</v>
@@ -19296,10 +19308,10 @@
         <v>5</v>
       </c>
       <c r="S262" t="s">
+        <v>118</v>
+      </c>
+      <c r="T262" t="s">
         <v>119</v>
-      </c>
-      <c r="T262" t="s">
-        <v>120</v>
       </c>
       <c r="U262" s="1">
         <v>1</v>
@@ -19311,10 +19323,10 @@
         <v>3</v>
       </c>
       <c r="AA262" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB262" t="s">
         <v>121</v>
-      </c>
-      <c r="AB262" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="263" spans="1:33" x14ac:dyDescent="0.2">
@@ -19322,7 +19334,7 @@
         <v>39</v>
       </c>
       <c r="B263" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C263" t="s">
         <v>45</v>
@@ -19340,10 +19352,10 @@
         <v>31</v>
       </c>
       <c r="L263" t="s">
+        <v>115</v>
+      </c>
+      <c r="M263" t="s">
         <v>116</v>
-      </c>
-      <c r="M263" t="s">
-        <v>117</v>
       </c>
       <c r="N263">
         <v>24.2</v>
@@ -19361,10 +19373,10 @@
         <v>0.2</v>
       </c>
       <c r="S263" t="s">
+        <v>118</v>
+      </c>
+      <c r="T263" t="s">
         <v>119</v>
-      </c>
-      <c r="T263" t="s">
-        <v>120</v>
       </c>
       <c r="U263" s="1">
         <v>1</v>
@@ -19376,10 +19388,10 @@
         <v>3</v>
       </c>
       <c r="AA263" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB263" t="s">
         <v>121</v>
-      </c>
-      <c r="AB263" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="264" spans="1:33" x14ac:dyDescent="0.2">
@@ -19387,7 +19399,7 @@
         <v>39</v>
       </c>
       <c r="B264" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C264" t="s">
         <v>45</v>
@@ -19405,7 +19417,7 @@
         <v>31</v>
       </c>
       <c r="L264" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M264" t="s">
         <v>69</v>
@@ -19426,10 +19438,10 @@
         <v>1</v>
       </c>
       <c r="S264" t="s">
+        <v>118</v>
+      </c>
+      <c r="T264" t="s">
         <v>119</v>
-      </c>
-      <c r="T264" t="s">
-        <v>120</v>
       </c>
       <c r="U264" s="1">
         <v>1</v>
@@ -19441,10 +19453,10 @@
         <v>3</v>
       </c>
       <c r="AA264" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB264" t="s">
         <v>121</v>
-      </c>
-      <c r="AB264" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="265" spans="1:33" x14ac:dyDescent="0.2">
@@ -19452,7 +19464,7 @@
         <v>40</v>
       </c>
       <c r="B265" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C265" t="s">
         <v>45</v>
@@ -19479,7 +19491,7 @@
         <v>24</v>
       </c>
       <c r="L265" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M265" t="s">
         <v>79</v>
@@ -19500,10 +19512,10 @@
         <v>6</v>
       </c>
       <c r="S265" t="s">
+        <v>118</v>
+      </c>
+      <c r="T265" t="s">
         <v>119</v>
-      </c>
-      <c r="T265" t="s">
-        <v>120</v>
       </c>
       <c r="U265" s="1">
         <v>1</v>
@@ -19515,10 +19527,10 @@
         <v>3</v>
       </c>
       <c r="AA265" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB265" t="s">
         <v>121</v>
-      </c>
-      <c r="AB265" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="266" spans="1:33" x14ac:dyDescent="0.2">
@@ -19526,7 +19538,7 @@
         <v>40</v>
       </c>
       <c r="B266" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C266" t="s">
         <v>45</v>
@@ -19553,7 +19565,7 @@
         <v>24</v>
       </c>
       <c r="L266" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M266" t="s">
         <v>47</v>
@@ -19574,10 +19586,10 @@
         <v>0.3</v>
       </c>
       <c r="S266" t="s">
+        <v>118</v>
+      </c>
+      <c r="T266" t="s">
         <v>119</v>
-      </c>
-      <c r="T266" t="s">
-        <v>120</v>
       </c>
       <c r="U266" s="1">
         <v>1</v>
@@ -19589,10 +19601,10 @@
         <v>3</v>
       </c>
       <c r="AA266" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB266" t="s">
         <v>121</v>
-      </c>
-      <c r="AB266" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="267" spans="1:33" x14ac:dyDescent="0.2">
@@ -19600,7 +19612,7 @@
         <v>40</v>
       </c>
       <c r="B267" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C267" t="s">
         <v>45</v>
@@ -19627,7 +19639,7 @@
         <v>24</v>
       </c>
       <c r="L267" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M267" t="s">
         <v>79</v>
@@ -19648,10 +19660,10 @@
         <v>4</v>
       </c>
       <c r="S267" t="s">
+        <v>118</v>
+      </c>
+      <c r="T267" t="s">
         <v>119</v>
-      </c>
-      <c r="T267" t="s">
-        <v>120</v>
       </c>
       <c r="U267" s="1">
         <v>1</v>
@@ -19663,10 +19675,10 @@
         <v>3</v>
       </c>
       <c r="AA267" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB267" t="s">
         <v>121</v>
-      </c>
-      <c r="AB267" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="268" spans="1:33" x14ac:dyDescent="0.2">
@@ -19674,7 +19686,7 @@
         <v>40</v>
       </c>
       <c r="B268" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C268" t="s">
         <v>45</v>
@@ -19701,10 +19713,10 @@
         <v>24</v>
       </c>
       <c r="L268" t="s">
+        <v>115</v>
+      </c>
+      <c r="M268" t="s">
         <v>116</v>
-      </c>
-      <c r="M268" t="s">
-        <v>117</v>
       </c>
       <c r="N268">
         <v>24.9</v>
@@ -19722,10 +19734,10 @@
         <v>0.5</v>
       </c>
       <c r="S268" t="s">
+        <v>118</v>
+      </c>
+      <c r="T268" t="s">
         <v>119</v>
-      </c>
-      <c r="T268" t="s">
-        <v>120</v>
       </c>
       <c r="U268" s="1">
         <v>1</v>
@@ -19737,10 +19749,10 @@
         <v>3</v>
       </c>
       <c r="AA268" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB268" t="s">
         <v>121</v>
-      </c>
-      <c r="AB268" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="269" spans="1:33" x14ac:dyDescent="0.2">
@@ -19748,7 +19760,7 @@
         <v>40</v>
       </c>
       <c r="B269" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C269" t="s">
         <v>45</v>
@@ -19775,7 +19787,7 @@
         <v>24</v>
       </c>
       <c r="L269" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M269" t="s">
         <v>69</v>
@@ -19796,10 +19808,10 @@
         <v>1</v>
       </c>
       <c r="S269" t="s">
+        <v>118</v>
+      </c>
+      <c r="T269" t="s">
         <v>119</v>
-      </c>
-      <c r="T269" t="s">
-        <v>120</v>
       </c>
       <c r="U269" s="1">
         <v>1</v>
@@ -19811,10 +19823,10 @@
         <v>3</v>
       </c>
       <c r="AA269" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB269" t="s">
         <v>121</v>
-      </c>
-      <c r="AB269" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="270" spans="1:33" x14ac:dyDescent="0.2">
@@ -19822,7 +19834,7 @@
         <v>41</v>
       </c>
       <c r="B270" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C270" t="s">
         <v>45</v>
@@ -19840,7 +19852,7 @@
         <v>32</v>
       </c>
       <c r="L270" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M270" t="s">
         <v>79</v>
@@ -19861,10 +19873,10 @@
         <v>10</v>
       </c>
       <c r="S270" t="s">
+        <v>118</v>
+      </c>
+      <c r="T270" t="s">
         <v>119</v>
-      </c>
-      <c r="T270" t="s">
-        <v>120</v>
       </c>
       <c r="U270" s="1">
         <v>1</v>
@@ -19876,10 +19888,10 @@
         <v>3</v>
       </c>
       <c r="AA270" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB270" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="271" spans="1:33" x14ac:dyDescent="0.2">
@@ -19887,7 +19899,7 @@
         <v>41</v>
       </c>
       <c r="B271" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C271" t="s">
         <v>45</v>
@@ -19905,7 +19917,7 @@
         <v>32</v>
       </c>
       <c r="L271" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M271" t="s">
         <v>47</v>
@@ -19926,10 +19938,10 @@
         <v>0.4</v>
       </c>
       <c r="S271" t="s">
+        <v>118</v>
+      </c>
+      <c r="T271" t="s">
         <v>119</v>
-      </c>
-      <c r="T271" t="s">
-        <v>120</v>
       </c>
       <c r="U271" s="1">
         <v>1</v>
@@ -19941,10 +19953,10 @@
         <v>3</v>
       </c>
       <c r="AA271" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB271" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="272" spans="1:33" x14ac:dyDescent="0.2">
@@ -19952,7 +19964,7 @@
         <v>41</v>
       </c>
       <c r="B272" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C272" t="s">
         <v>45</v>
@@ -19970,7 +19982,7 @@
         <v>32</v>
       </c>
       <c r="L272" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M272" t="s">
         <v>79</v>
@@ -19991,10 +20003,10 @@
         <v>6</v>
       </c>
       <c r="S272" t="s">
+        <v>118</v>
+      </c>
+      <c r="T272" t="s">
         <v>119</v>
-      </c>
-      <c r="T272" t="s">
-        <v>120</v>
       </c>
       <c r="U272" s="1">
         <v>1</v>
@@ -20006,10 +20018,10 @@
         <v>3</v>
       </c>
       <c r="AA272" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB272" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="273" spans="1:28" x14ac:dyDescent="0.2">
@@ -20017,7 +20029,7 @@
         <v>41</v>
       </c>
       <c r="B273" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C273" t="s">
         <v>45</v>
@@ -20035,10 +20047,10 @@
         <v>32</v>
       </c>
       <c r="L273" t="s">
+        <v>115</v>
+      </c>
+      <c r="M273" t="s">
         <v>116</v>
-      </c>
-      <c r="M273" t="s">
-        <v>117</v>
       </c>
       <c r="N273">
         <v>22.2</v>
@@ -20056,10 +20068,10 @@
         <v>0.3</v>
       </c>
       <c r="S273" t="s">
+        <v>118</v>
+      </c>
+      <c r="T273" t="s">
         <v>119</v>
-      </c>
-      <c r="T273" t="s">
-        <v>120</v>
       </c>
       <c r="U273" s="1">
         <v>1</v>
@@ -20071,10 +20083,10 @@
         <v>3</v>
       </c>
       <c r="AA273" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB273" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="274" spans="1:28" x14ac:dyDescent="0.2">
@@ -20082,7 +20094,7 @@
         <v>41</v>
       </c>
       <c r="B274" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C274" t="s">
         <v>45</v>
@@ -20100,7 +20112,7 @@
         <v>32</v>
       </c>
       <c r="L274" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M274" t="s">
         <v>69</v>
@@ -20121,10 +20133,10 @@
         <v>0.7</v>
       </c>
       <c r="S274" t="s">
+        <v>118</v>
+      </c>
+      <c r="T274" t="s">
         <v>119</v>
-      </c>
-      <c r="T274" t="s">
-        <v>120</v>
       </c>
       <c r="U274" s="1">
         <v>1</v>
@@ -20136,10 +20148,10 @@
         <v>3</v>
       </c>
       <c r="AA274" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB274" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="275" spans="1:28" x14ac:dyDescent="0.2">
@@ -20147,7 +20159,7 @@
         <v>42</v>
       </c>
       <c r="B275" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C275" t="s">
         <v>45</v>
@@ -20174,7 +20186,7 @@
         <v>24</v>
       </c>
       <c r="L275" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M275" t="s">
         <v>79</v>
@@ -20195,10 +20207,10 @@
         <v>11</v>
       </c>
       <c r="S275" t="s">
+        <v>118</v>
+      </c>
+      <c r="T275" t="s">
         <v>119</v>
-      </c>
-      <c r="T275" t="s">
-        <v>120</v>
       </c>
       <c r="U275" s="1">
         <v>1</v>
@@ -20210,10 +20222,10 @@
         <v>3</v>
       </c>
       <c r="AA275" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB275" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="276" spans="1:28" x14ac:dyDescent="0.2">
@@ -20221,7 +20233,7 @@
         <v>42</v>
       </c>
       <c r="B276" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C276" t="s">
         <v>45</v>
@@ -20248,7 +20260,7 @@
         <v>24</v>
       </c>
       <c r="L276" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M276" t="s">
         <v>47</v>
@@ -20269,10 +20281,10 @@
         <v>0.4</v>
       </c>
       <c r="S276" t="s">
+        <v>118</v>
+      </c>
+      <c r="T276" t="s">
         <v>119</v>
-      </c>
-      <c r="T276" t="s">
-        <v>120</v>
       </c>
       <c r="U276" s="1">
         <v>1</v>
@@ -20284,10 +20296,10 @@
         <v>3</v>
       </c>
       <c r="AA276" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB276" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="277" spans="1:28" x14ac:dyDescent="0.2">
@@ -20295,7 +20307,7 @@
         <v>42</v>
       </c>
       <c r="B277" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C277" t="s">
         <v>45</v>
@@ -20322,7 +20334,7 @@
         <v>24</v>
       </c>
       <c r="L277" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M277" t="s">
         <v>79</v>
@@ -20343,10 +20355,10 @@
         <v>8</v>
       </c>
       <c r="S277" t="s">
+        <v>118</v>
+      </c>
+      <c r="T277" t="s">
         <v>119</v>
-      </c>
-      <c r="T277" t="s">
-        <v>120</v>
       </c>
       <c r="U277" s="1">
         <v>1</v>
@@ -20358,10 +20370,10 @@
         <v>3</v>
       </c>
       <c r="AA277" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB277" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="278" spans="1:28" x14ac:dyDescent="0.2">
@@ -20369,7 +20381,7 @@
         <v>42</v>
       </c>
       <c r="B278" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C278" t="s">
         <v>45</v>
@@ -20396,10 +20408,10 @@
         <v>24</v>
       </c>
       <c r="L278" t="s">
+        <v>115</v>
+      </c>
+      <c r="M278" t="s">
         <v>116</v>
-      </c>
-      <c r="M278" t="s">
-        <v>117</v>
       </c>
       <c r="N278">
         <v>20.3</v>
@@ -20417,10 +20429,10 @@
         <v>0.3</v>
       </c>
       <c r="S278" t="s">
+        <v>118</v>
+      </c>
+      <c r="T278" t="s">
         <v>119</v>
-      </c>
-      <c r="T278" t="s">
-        <v>120</v>
       </c>
       <c r="U278" s="1">
         <v>1</v>
@@ -20432,10 +20444,10 @@
         <v>3</v>
       </c>
       <c r="AA278" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB278" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="279" spans="1:28" x14ac:dyDescent="0.2">
@@ -20443,7 +20455,7 @@
         <v>42</v>
       </c>
       <c r="B279" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C279" t="s">
         <v>45</v>
@@ -20470,7 +20482,7 @@
         <v>24</v>
       </c>
       <c r="L279" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M279" t="s">
         <v>69</v>
@@ -20491,10 +20503,10 @@
         <v>0.7</v>
       </c>
       <c r="S279" t="s">
+        <v>118</v>
+      </c>
+      <c r="T279" t="s">
         <v>119</v>
-      </c>
-      <c r="T279" t="s">
-        <v>120</v>
       </c>
       <c r="U279" s="1">
         <v>1</v>
@@ -20506,10 +20518,10 @@
         <v>3</v>
       </c>
       <c r="AA279" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB279" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="280" spans="1:28" x14ac:dyDescent="0.2">
@@ -20517,7 +20529,7 @@
         <v>43</v>
       </c>
       <c r="B280" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C280" t="s">
         <v>45</v>
@@ -20544,7 +20556,7 @@
         <v>24</v>
       </c>
       <c r="L280" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M280" t="s">
         <v>79</v>
@@ -20565,10 +20577,10 @@
         <v>7</v>
       </c>
       <c r="S280" t="s">
+        <v>118</v>
+      </c>
+      <c r="T280" t="s">
         <v>119</v>
-      </c>
-      <c r="T280" t="s">
-        <v>120</v>
       </c>
       <c r="U280" s="1">
         <v>1</v>
@@ -20580,10 +20592,10 @@
         <v>3</v>
       </c>
       <c r="AA280" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB280" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="281" spans="1:28" x14ac:dyDescent="0.2">
@@ -20591,7 +20603,7 @@
         <v>43</v>
       </c>
       <c r="B281" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C281" t="s">
         <v>45</v>
@@ -20618,7 +20630,7 @@
         <v>24</v>
       </c>
       <c r="L281" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M281" t="s">
         <v>47</v>
@@ -20639,10 +20651,10 @@
         <v>0.6</v>
       </c>
       <c r="S281" t="s">
+        <v>118</v>
+      </c>
+      <c r="T281" t="s">
         <v>119</v>
-      </c>
-      <c r="T281" t="s">
-        <v>120</v>
       </c>
       <c r="U281" s="1">
         <v>1</v>
@@ -20654,10 +20666,10 @@
         <v>3</v>
       </c>
       <c r="AA281" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB281" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="282" spans="1:28" x14ac:dyDescent="0.2">
@@ -20665,7 +20677,7 @@
         <v>43</v>
       </c>
       <c r="B282" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C282" t="s">
         <v>45</v>
@@ -20692,7 +20704,7 @@
         <v>24</v>
       </c>
       <c r="L282" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M282" t="s">
         <v>79</v>
@@ -20713,10 +20725,10 @@
         <v>8</v>
       </c>
       <c r="S282" t="s">
+        <v>118</v>
+      </c>
+      <c r="T282" t="s">
         <v>119</v>
-      </c>
-      <c r="T282" t="s">
-        <v>120</v>
       </c>
       <c r="U282" s="1">
         <v>1</v>
@@ -20728,10 +20740,10 @@
         <v>3</v>
       </c>
       <c r="AA282" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB282" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="283" spans="1:28" x14ac:dyDescent="0.2">
@@ -20739,7 +20751,7 @@
         <v>43</v>
       </c>
       <c r="B283" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C283" t="s">
         <v>45</v>
@@ -20766,10 +20778,10 @@
         <v>24</v>
       </c>
       <c r="L283" t="s">
+        <v>115</v>
+      </c>
+      <c r="M283" t="s">
         <v>116</v>
-      </c>
-      <c r="M283" t="s">
-        <v>117</v>
       </c>
       <c r="N283">
         <v>20.3</v>
@@ -20787,10 +20799,10 @@
         <v>0.3</v>
       </c>
       <c r="S283" t="s">
+        <v>118</v>
+      </c>
+      <c r="T283" t="s">
         <v>119</v>
-      </c>
-      <c r="T283" t="s">
-        <v>120</v>
       </c>
       <c r="U283" s="1">
         <v>1</v>
@@ -20802,10 +20814,10 @@
         <v>3</v>
       </c>
       <c r="AA283" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB283" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="284" spans="1:28" x14ac:dyDescent="0.2">
@@ -20813,7 +20825,7 @@
         <v>43</v>
       </c>
       <c r="B284" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C284" t="s">
         <v>45</v>
@@ -20840,7 +20852,7 @@
         <v>24</v>
       </c>
       <c r="L284" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M284" t="s">
         <v>69</v>
@@ -20861,10 +20873,10 @@
         <v>0.8</v>
       </c>
       <c r="S284" t="s">
+        <v>118</v>
+      </c>
+      <c r="T284" t="s">
         <v>119</v>
-      </c>
-      <c r="T284" t="s">
-        <v>120</v>
       </c>
       <c r="U284" s="1">
         <v>1</v>
@@ -20876,10 +20888,10 @@
         <v>3</v>
       </c>
       <c r="AA284" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB284" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="285" spans="1:28" x14ac:dyDescent="0.2">
@@ -20887,7 +20899,7 @@
         <v>44</v>
       </c>
       <c r="B285" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C285" t="s">
         <v>45</v>
@@ -20905,7 +20917,7 @@
         <v>33</v>
       </c>
       <c r="L285" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M285" t="s">
         <v>79</v>
@@ -20926,10 +20938,10 @@
         <v>0</v>
       </c>
       <c r="S285" t="s">
+        <v>118</v>
+      </c>
+      <c r="T285" t="s">
         <v>119</v>
-      </c>
-      <c r="T285" t="s">
-        <v>120</v>
       </c>
       <c r="U285" s="1">
         <v>1</v>
@@ -20941,10 +20953,10 @@
         <v>3</v>
       </c>
       <c r="AA285" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB285" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="286" spans="1:28" x14ac:dyDescent="0.2">
@@ -20952,7 +20964,7 @@
         <v>44</v>
       </c>
       <c r="B286" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C286" t="s">
         <v>45</v>
@@ -20970,7 +20982,7 @@
         <v>33</v>
       </c>
       <c r="L286" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M286" t="s">
         <v>47</v>
@@ -20991,10 +21003,10 @@
         <v>0.3</v>
       </c>
       <c r="S286" t="s">
+        <v>118</v>
+      </c>
+      <c r="T286" t="s">
         <v>119</v>
-      </c>
-      <c r="T286" t="s">
-        <v>120</v>
       </c>
       <c r="U286" s="1">
         <v>1</v>
@@ -21006,10 +21018,10 @@
         <v>3</v>
       </c>
       <c r="AA286" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB286" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="287" spans="1:28" x14ac:dyDescent="0.2">
@@ -21017,7 +21029,7 @@
         <v>44</v>
       </c>
       <c r="B287" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C287" t="s">
         <v>45</v>
@@ -21035,7 +21047,7 @@
         <v>33</v>
       </c>
       <c r="L287" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M287" t="s">
         <v>79</v>
@@ -21056,10 +21068,10 @@
         <v>6</v>
       </c>
       <c r="S287" t="s">
+        <v>118</v>
+      </c>
+      <c r="T287" t="s">
         <v>119</v>
-      </c>
-      <c r="T287" t="s">
-        <v>120</v>
       </c>
       <c r="U287" s="1">
         <v>1</v>
@@ -21071,10 +21083,10 @@
         <v>3</v>
       </c>
       <c r="AA287" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB287" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="288" spans="1:28" x14ac:dyDescent="0.2">
@@ -21082,7 +21094,7 @@
         <v>44</v>
       </c>
       <c r="B288" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C288" t="s">
         <v>45</v>
@@ -21100,10 +21112,10 @@
         <v>33</v>
       </c>
       <c r="L288" t="s">
+        <v>115</v>
+      </c>
+      <c r="M288" t="s">
         <v>116</v>
-      </c>
-      <c r="M288" t="s">
-        <v>117</v>
       </c>
       <c r="N288">
         <v>22</v>
@@ -21121,10 +21133,10 @@
         <v>0.2</v>
       </c>
       <c r="S288" t="s">
+        <v>118</v>
+      </c>
+      <c r="T288" t="s">
         <v>119</v>
-      </c>
-      <c r="T288" t="s">
-        <v>120</v>
       </c>
       <c r="U288" s="1">
         <v>1</v>
@@ -21136,10 +21148,10 @@
         <v>3</v>
       </c>
       <c r="AA288" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB288" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="289" spans="1:28" x14ac:dyDescent="0.2">
@@ -21147,7 +21159,7 @@
         <v>44</v>
       </c>
       <c r="B289" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C289" t="s">
         <v>45</v>
@@ -21165,7 +21177,7 @@
         <v>33</v>
       </c>
       <c r="L289" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M289" t="s">
         <v>69</v>
@@ -21186,10 +21198,10 @@
         <v>1</v>
       </c>
       <c r="S289" t="s">
+        <v>118</v>
+      </c>
+      <c r="T289" t="s">
         <v>119</v>
-      </c>
-      <c r="T289" t="s">
-        <v>120</v>
       </c>
       <c r="U289" s="1">
         <v>1</v>
@@ -21201,10 +21213,320 @@
         <v>3</v>
       </c>
       <c r="AA289" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB289" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="290" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A290">
+        <v>45</v>
+      </c>
+      <c r="B290" t="s">
         <v>123</v>
+      </c>
+      <c r="C290" t="s">
+        <v>29</v>
+      </c>
+      <c r="D290">
+        <v>0</v>
+      </c>
+      <c r="H290">
+        <v>26</v>
+      </c>
+      <c r="I290">
+        <v>26</v>
+      </c>
+      <c r="J290">
+        <v>26</v>
+      </c>
+      <c r="L290" t="s">
+        <v>125</v>
+      </c>
+      <c r="M290" t="s">
+        <v>69</v>
+      </c>
+      <c r="N290">
+        <v>9.5596072931276296E-2</v>
+      </c>
+      <c r="O290">
+        <v>1</v>
+      </c>
+      <c r="Q290">
+        <v>1</v>
+      </c>
+      <c r="R290">
+        <v>1.1949509116408699E-2</v>
+      </c>
+      <c r="S290" t="s">
+        <v>126</v>
+      </c>
+      <c r="T290" t="s">
+        <v>127</v>
+      </c>
+      <c r="U290" s="1">
+        <v>3</v>
+      </c>
+      <c r="V290" s="1">
+        <v>0</v>
+      </c>
+      <c r="W290" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A291">
+        <v>45</v>
+      </c>
+      <c r="B291" t="s">
+        <v>123</v>
+      </c>
+      <c r="C291" t="s">
+        <v>29</v>
+      </c>
+      <c r="D291">
+        <v>1</v>
+      </c>
+      <c r="E291">
+        <v>1</v>
+      </c>
+      <c r="F291">
+        <v>0</v>
+      </c>
+      <c r="H291">
+        <v>20.5</v>
+      </c>
+      <c r="I291">
+        <v>15</v>
+      </c>
+      <c r="J291">
+        <v>26</v>
+      </c>
+      <c r="K291">
+        <v>24</v>
+      </c>
+      <c r="L291" t="s">
+        <v>125</v>
+      </c>
+      <c r="M291" t="s">
+        <v>69</v>
+      </c>
+      <c r="N291">
+        <v>9.0042075736325305E-2</v>
+      </c>
+      <c r="O291">
+        <v>1</v>
+      </c>
+      <c r="Q291">
+        <v>1</v>
+      </c>
+      <c r="R291">
+        <v>4.544179523141692E-3</v>
+      </c>
+      <c r="S291" t="s">
+        <v>126</v>
+      </c>
+      <c r="T291" t="s">
+        <v>127</v>
+      </c>
+      <c r="U291" s="1">
+        <v>3</v>
+      </c>
+      <c r="V291" s="1">
+        <v>0</v>
+      </c>
+      <c r="W291" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A292">
+        <v>45</v>
+      </c>
+      <c r="B292" t="s">
+        <v>123</v>
+      </c>
+      <c r="C292" t="s">
+        <v>29</v>
+      </c>
+      <c r="D292">
+        <v>1</v>
+      </c>
+      <c r="E292">
+        <v>1</v>
+      </c>
+      <c r="F292">
+        <v>0</v>
+      </c>
+      <c r="H292">
+        <v>30.5</v>
+      </c>
+      <c r="I292">
+        <v>26</v>
+      </c>
+      <c r="J292">
+        <v>35</v>
+      </c>
+      <c r="K292">
+        <v>24</v>
+      </c>
+      <c r="L292" t="s">
+        <v>125</v>
+      </c>
+      <c r="N292">
+        <v>7.8934081346423504E-2</v>
+      </c>
+      <c r="O292">
+        <v>1</v>
+      </c>
+      <c r="Q292">
+        <v>1</v>
+      </c>
+      <c r="R292">
+        <v>2.0701262272089793E-2</v>
+      </c>
+      <c r="S292" t="s">
+        <v>126</v>
+      </c>
+      <c r="T292" t="s">
+        <v>127</v>
+      </c>
+      <c r="U292" s="1">
+        <v>3</v>
+      </c>
+      <c r="V292" s="1">
+        <v>0</v>
+      </c>
+      <c r="W292" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A293">
+        <v>45</v>
+      </c>
+      <c r="B293" t="s">
+        <v>123</v>
+      </c>
+      <c r="C293" t="s">
+        <v>29</v>
+      </c>
+      <c r="D293">
+        <v>1</v>
+      </c>
+      <c r="E293">
+        <v>1</v>
+      </c>
+      <c r="F293">
+        <v>0</v>
+      </c>
+      <c r="H293">
+        <v>25</v>
+      </c>
+      <c r="I293">
+        <v>20</v>
+      </c>
+      <c r="J293">
+        <v>30</v>
+      </c>
+      <c r="K293">
+        <v>24</v>
+      </c>
+      <c r="L293" t="s">
+        <v>125</v>
+      </c>
+      <c r="M293" t="s">
+        <v>69</v>
+      </c>
+      <c r="N293">
+        <v>0.104347826086956</v>
+      </c>
+      <c r="O293">
+        <v>1</v>
+      </c>
+      <c r="Q293">
+        <v>1</v>
+      </c>
+      <c r="R293">
+        <v>7.4053295932679924E-3</v>
+      </c>
+      <c r="S293" t="s">
+        <v>126</v>
+      </c>
+      <c r="T293" t="s">
+        <v>127</v>
+      </c>
+      <c r="U293" s="1">
+        <v>3</v>
+      </c>
+      <c r="V293" s="1">
+        <v>0</v>
+      </c>
+      <c r="W293" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A294">
+        <v>45</v>
+      </c>
+      <c r="B294" t="s">
+        <v>123</v>
+      </c>
+      <c r="C294" t="s">
+        <v>29</v>
+      </c>
+      <c r="D294">
+        <v>1</v>
+      </c>
+      <c r="E294">
+        <v>1</v>
+      </c>
+      <c r="F294">
+        <v>0</v>
+      </c>
+      <c r="H294">
+        <v>25</v>
+      </c>
+      <c r="I294">
+        <v>15</v>
+      </c>
+      <c r="J294">
+        <v>35</v>
+      </c>
+      <c r="K294">
+        <v>24</v>
+      </c>
+      <c r="M294" t="s">
+        <v>69</v>
+      </c>
+      <c r="N294">
+        <v>4.7629733520336601E-2</v>
+      </c>
+      <c r="O294">
+        <v>1</v>
+      </c>
+      <c r="Q294">
+        <v>1</v>
+      </c>
+      <c r="R294">
+        <v>1.2622720897615701E-2</v>
+      </c>
+      <c r="S294" t="s">
+        <v>126</v>
+      </c>
+      <c r="T294" t="s">
+        <v>127</v>
+      </c>
+      <c r="U294" s="1">
+        <v>3</v>
+      </c>
+      <c r="V294" s="1">
+        <v>0</v>
+      </c>
+      <c r="W294" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delava et al and lowenborg et al data extraction + files
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{01081FF6-279F-E045-855C-54093BA74858}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8C518245-1126-A44D-B2F8-3E3A693AB18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27640" windowHeight="15080" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="2100" yWindow="460" windowWidth="24460" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="metanaly_fulldataset" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2417" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2599" uniqueCount="149">
   <si>
     <t>study_id</t>
   </si>
@@ -435,6 +435,45 @@
   <si>
     <t>melanogaster</t>
   </si>
+  <si>
+    <t>lowenborg2012</t>
+  </si>
+  <si>
+    <t>figure 4a</t>
+  </si>
+  <si>
+    <t>figure 4b</t>
+  </si>
+  <si>
+    <t>figure 4c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incubation time </t>
+  </si>
+  <si>
+    <t>days to first slough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aquatic speed </t>
+  </si>
+  <si>
+    <t>m * s^-1</t>
+  </si>
+  <si>
+    <t>terrestrial speed</t>
+  </si>
+  <si>
+    <t>distance covered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natrix </t>
+  </si>
+  <si>
+    <t>natrix</t>
+  </si>
 </sst>
 </file>
 
@@ -800,11 +839,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AG294"/>
+  <dimension ref="A1:AG322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D300" sqref="D300"/>
+      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D325" sqref="D325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11139,6 +11178,9 @@
       <c r="D148">
         <v>0</v>
       </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
       <c r="H148">
         <v>24</v>
       </c>
@@ -11204,6 +11246,9 @@
       <c r="D149">
         <v>0</v>
       </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
       <c r="H149">
         <v>24</v>
       </c>
@@ -11272,6 +11317,9 @@
       <c r="D150">
         <v>0</v>
       </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
       <c r="H150">
         <v>24</v>
       </c>
@@ -11340,6 +11388,9 @@
       <c r="D151">
         <v>0</v>
       </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
       <c r="H151">
         <v>24</v>
       </c>
@@ -11408,6 +11459,9 @@
       <c r="D152">
         <v>0</v>
       </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
       <c r="H152">
         <v>24</v>
       </c>
@@ -11476,6 +11530,9 @@
       <c r="D153">
         <v>0</v>
       </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
       <c r="H153">
         <v>24</v>
       </c>
@@ -11544,6 +11601,9 @@
       <c r="D154">
         <v>0</v>
       </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
       <c r="H154">
         <v>24</v>
       </c>
@@ -11612,6 +11672,9 @@
       <c r="D155">
         <v>0</v>
       </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
       <c r="H155">
         <v>24</v>
       </c>
@@ -11680,6 +11743,9 @@
       <c r="D156">
         <v>0</v>
       </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
       <c r="H156">
         <v>24</v>
       </c>
@@ -11748,6 +11814,9 @@
       <c r="D157">
         <v>0</v>
       </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
       <c r="H157">
         <v>24</v>
       </c>
@@ -11816,6 +11885,9 @@
       <c r="D158">
         <v>0</v>
       </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
       <c r="H158">
         <v>24</v>
       </c>
@@ -11884,6 +11956,9 @@
       <c r="D159">
         <v>0</v>
       </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
       <c r="H159">
         <v>24</v>
       </c>
@@ -11952,6 +12027,9 @@
       <c r="D160">
         <v>0</v>
       </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
       <c r="H160">
         <v>24</v>
       </c>
@@ -12017,6 +12095,9 @@
       <c r="D161">
         <v>0</v>
       </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
       <c r="H161">
         <v>24</v>
       </c>
@@ -12080,7 +12161,7 @@
         <v>66</v>
       </c>
       <c r="D162">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E162">
         <v>1</v>
@@ -12157,7 +12238,7 @@
         <v>66</v>
       </c>
       <c r="D163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E163">
         <v>1</v>
@@ -12234,7 +12315,7 @@
         <v>66</v>
       </c>
       <c r="D164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E164">
         <v>1</v>
@@ -12311,7 +12392,7 @@
         <v>66</v>
       </c>
       <c r="D165">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E165">
         <v>1</v>
@@ -12388,7 +12469,7 @@
         <v>66</v>
       </c>
       <c r="D166">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E166">
         <v>1</v>
@@ -12465,7 +12546,7 @@
         <v>66</v>
       </c>
       <c r="D167">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E167">
         <v>1</v>
@@ -12542,7 +12623,7 @@
         <v>66</v>
       </c>
       <c r="D168">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -12619,7 +12700,7 @@
         <v>66</v>
       </c>
       <c r="D169">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E169">
         <v>1</v>
@@ -12696,7 +12777,7 @@
         <v>66</v>
       </c>
       <c r="D170">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E170">
         <v>1</v>
@@ -12773,7 +12854,7 @@
         <v>66</v>
       </c>
       <c r="D171">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E171">
         <v>1</v>
@@ -12850,7 +12931,7 @@
         <v>66</v>
       </c>
       <c r="D172">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E172">
         <v>1</v>
@@ -12927,7 +13008,7 @@
         <v>66</v>
       </c>
       <c r="D173">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E173">
         <v>1</v>
@@ -13004,7 +13085,7 @@
         <v>66</v>
       </c>
       <c r="D174">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E174">
         <v>1</v>
@@ -13081,7 +13162,7 @@
         <v>66</v>
       </c>
       <c r="D175">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -13160,6 +13241,9 @@
       <c r="D176">
         <v>0</v>
       </c>
+      <c r="E176">
+        <v>0</v>
+      </c>
       <c r="H176">
         <v>24</v>
       </c>
@@ -13225,6 +13309,9 @@
       <c r="D177">
         <v>0</v>
       </c>
+      <c r="E177">
+        <v>0</v>
+      </c>
       <c r="H177">
         <v>24</v>
       </c>
@@ -13290,6 +13377,9 @@
       <c r="D178">
         <v>0</v>
       </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
       <c r="H178">
         <v>24</v>
       </c>
@@ -13355,6 +13445,9 @@
       <c r="D179">
         <v>0</v>
       </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
       <c r="H179">
         <v>24</v>
       </c>
@@ -13420,6 +13513,9 @@
       <c r="D180">
         <v>0</v>
       </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
       <c r="H180">
         <v>24</v>
       </c>
@@ -13488,6 +13584,9 @@
       <c r="D181">
         <v>0</v>
       </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
       <c r="H181">
         <v>24</v>
       </c>
@@ -13556,6 +13655,9 @@
       <c r="D182">
         <v>0</v>
       </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
       <c r="H182">
         <v>24</v>
       </c>
@@ -13624,6 +13726,9 @@
       <c r="D183">
         <v>0</v>
       </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
       <c r="H183">
         <v>24</v>
       </c>
@@ -13692,6 +13797,9 @@
       <c r="D184">
         <v>0</v>
       </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
       <c r="H184">
         <v>24</v>
       </c>
@@ -13760,6 +13868,9 @@
       <c r="D185">
         <v>0</v>
       </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
       <c r="H185">
         <v>24</v>
       </c>
@@ -13828,6 +13939,9 @@
       <c r="D186">
         <v>0</v>
       </c>
+      <c r="E186">
+        <v>0</v>
+      </c>
       <c r="H186">
         <v>24</v>
       </c>
@@ -13896,6 +14010,9 @@
       <c r="D187">
         <v>0</v>
       </c>
+      <c r="E187">
+        <v>0</v>
+      </c>
       <c r="H187">
         <v>24</v>
       </c>
@@ -13964,6 +14081,9 @@
       <c r="D188">
         <v>0</v>
       </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
       <c r="H188">
         <v>24</v>
       </c>
@@ -14032,6 +14152,9 @@
       <c r="D189">
         <v>0</v>
       </c>
+      <c r="E189">
+        <v>0</v>
+      </c>
       <c r="H189">
         <v>24</v>
       </c>
@@ -14098,7 +14221,7 @@
         <v>66</v>
       </c>
       <c r="D190">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -14172,7 +14295,7 @@
         <v>66</v>
       </c>
       <c r="D191">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -14246,7 +14369,7 @@
         <v>66</v>
       </c>
       <c r="D192">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -14320,7 +14443,7 @@
         <v>66</v>
       </c>
       <c r="D193">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E193">
         <v>1</v>
@@ -14394,7 +14517,7 @@
         <v>66</v>
       </c>
       <c r="D194">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E194">
         <v>1</v>
@@ -14468,7 +14591,7 @@
         <v>66</v>
       </c>
       <c r="D195">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E195">
         <v>1</v>
@@ -14545,7 +14668,7 @@
         <v>66</v>
       </c>
       <c r="D196">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -14622,7 +14745,7 @@
         <v>66</v>
       </c>
       <c r="D197">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E197">
         <v>1</v>
@@ -14699,7 +14822,7 @@
         <v>66</v>
       </c>
       <c r="D198">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -14776,7 +14899,7 @@
         <v>66</v>
       </c>
       <c r="D199">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E199">
         <v>1</v>
@@ -14853,7 +14976,7 @@
         <v>66</v>
       </c>
       <c r="D200">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -14930,7 +15053,7 @@
         <v>66</v>
       </c>
       <c r="D201">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E201">
         <v>1</v>
@@ -15007,7 +15130,7 @@
         <v>66</v>
       </c>
       <c r="D202">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E202">
         <v>1</v>
@@ -15084,7 +15207,7 @@
         <v>66</v>
       </c>
       <c r="D203">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E203">
         <v>1</v>
@@ -15160,6 +15283,9 @@
       <c r="D204">
         <v>0</v>
       </c>
+      <c r="E204">
+        <v>0</v>
+      </c>
       <c r="H204">
         <v>24</v>
       </c>
@@ -15225,6 +15351,9 @@
       <c r="D205">
         <v>0</v>
       </c>
+      <c r="E205">
+        <v>0</v>
+      </c>
       <c r="H205">
         <v>24</v>
       </c>
@@ -15290,6 +15419,9 @@
       <c r="D206">
         <v>0</v>
       </c>
+      <c r="E206">
+        <v>0</v>
+      </c>
       <c r="H206">
         <v>24</v>
       </c>
@@ -15358,6 +15490,9 @@
       <c r="D207">
         <v>0</v>
       </c>
+      <c r="E207">
+        <v>0</v>
+      </c>
       <c r="H207">
         <v>24</v>
       </c>
@@ -15426,6 +15561,9 @@
       <c r="D208">
         <v>0</v>
       </c>
+      <c r="E208">
+        <v>0</v>
+      </c>
       <c r="H208">
         <v>24</v>
       </c>
@@ -15494,6 +15632,9 @@
       <c r="D209">
         <v>0</v>
       </c>
+      <c r="E209">
+        <v>0</v>
+      </c>
       <c r="H209">
         <v>24</v>
       </c>
@@ -15562,6 +15703,9 @@
       <c r="D210">
         <v>0</v>
       </c>
+      <c r="E210">
+        <v>0</v>
+      </c>
       <c r="H210">
         <v>24</v>
       </c>
@@ -15630,6 +15774,9 @@
       <c r="D211">
         <v>0</v>
       </c>
+      <c r="E211">
+        <v>0</v>
+      </c>
       <c r="H211">
         <v>24</v>
       </c>
@@ -15698,6 +15845,9 @@
       <c r="D212">
         <v>0</v>
       </c>
+      <c r="E212">
+        <v>0</v>
+      </c>
       <c r="H212">
         <v>24</v>
       </c>
@@ -15766,6 +15916,9 @@
       <c r="D213">
         <v>0</v>
       </c>
+      <c r="E213">
+        <v>0</v>
+      </c>
       <c r="H213">
         <v>24</v>
       </c>
@@ -15834,6 +15987,9 @@
       <c r="D214">
         <v>0</v>
       </c>
+      <c r="E214">
+        <v>0</v>
+      </c>
       <c r="H214">
         <v>24</v>
       </c>
@@ -15902,6 +16058,9 @@
       <c r="D215">
         <v>0</v>
       </c>
+      <c r="E215">
+        <v>0</v>
+      </c>
       <c r="H215">
         <v>24</v>
       </c>
@@ -15970,6 +16129,9 @@
       <c r="D216">
         <v>0</v>
       </c>
+      <c r="E216">
+        <v>0</v>
+      </c>
       <c r="H216">
         <v>24</v>
       </c>
@@ -16038,6 +16200,9 @@
       <c r="D217">
         <v>0</v>
       </c>
+      <c r="E217">
+        <v>0</v>
+      </c>
       <c r="H217">
         <v>24</v>
       </c>
@@ -16104,7 +16269,7 @@
         <v>67</v>
       </c>
       <c r="D218">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E218">
         <v>1</v>
@@ -16178,7 +16343,7 @@
         <v>67</v>
       </c>
       <c r="D219">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E219">
         <v>1</v>
@@ -16252,7 +16417,7 @@
         <v>67</v>
       </c>
       <c r="D220">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E220">
         <v>1</v>
@@ -16326,7 +16491,7 @@
         <v>67</v>
       </c>
       <c r="D221">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E221">
         <v>1</v>
@@ -16403,7 +16568,7 @@
         <v>67</v>
       </c>
       <c r="D222">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E222">
         <v>1</v>
@@ -16480,7 +16645,7 @@
         <v>67</v>
       </c>
       <c r="D223">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E223">
         <v>1</v>
@@ -16557,7 +16722,7 @@
         <v>67</v>
       </c>
       <c r="D224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E224">
         <v>1</v>
@@ -16634,7 +16799,7 @@
         <v>67</v>
       </c>
       <c r="D225">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E225">
         <v>1</v>
@@ -16711,7 +16876,7 @@
         <v>67</v>
       </c>
       <c r="D226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E226">
         <v>1</v>
@@ -16788,7 +16953,7 @@
         <v>67</v>
       </c>
       <c r="D227">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E227">
         <v>1</v>
@@ -16865,7 +17030,7 @@
         <v>67</v>
       </c>
       <c r="D228">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E228">
         <v>1</v>
@@ -16942,7 +17107,7 @@
         <v>67</v>
       </c>
       <c r="D229">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E229">
         <v>1</v>
@@ -17019,7 +17184,7 @@
         <v>67</v>
       </c>
       <c r="D230">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E230">
         <v>1</v>
@@ -17096,7 +17261,7 @@
         <v>67</v>
       </c>
       <c r="D231">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E231">
         <v>1</v>
@@ -17175,6 +17340,9 @@
       <c r="D232">
         <v>0</v>
       </c>
+      <c r="E232">
+        <v>0</v>
+      </c>
       <c r="H232">
         <v>24</v>
       </c>
@@ -17240,6 +17408,9 @@
       <c r="D233">
         <v>0</v>
       </c>
+      <c r="E233">
+        <v>0</v>
+      </c>
       <c r="H233">
         <v>24</v>
       </c>
@@ -17305,6 +17476,9 @@
       <c r="D234">
         <v>0</v>
       </c>
+      <c r="E234">
+        <v>0</v>
+      </c>
       <c r="H234">
         <v>24</v>
       </c>
@@ -17370,6 +17544,9 @@
       <c r="D235">
         <v>0</v>
       </c>
+      <c r="E235">
+        <v>0</v>
+      </c>
       <c r="H235">
         <v>24</v>
       </c>
@@ -17435,6 +17612,9 @@
       <c r="D236">
         <v>0</v>
       </c>
+      <c r="E236">
+        <v>0</v>
+      </c>
       <c r="H236">
         <v>24</v>
       </c>
@@ -17500,6 +17680,9 @@
       <c r="D237">
         <v>0</v>
       </c>
+      <c r="E237">
+        <v>0</v>
+      </c>
       <c r="H237">
         <v>24</v>
       </c>
@@ -17568,6 +17751,9 @@
       <c r="D238">
         <v>0</v>
       </c>
+      <c r="E238">
+        <v>0</v>
+      </c>
       <c r="H238">
         <v>24</v>
       </c>
@@ -17636,6 +17822,9 @@
       <c r="D239">
         <v>0</v>
       </c>
+      <c r="E239">
+        <v>0</v>
+      </c>
       <c r="H239">
         <v>24</v>
       </c>
@@ -17704,6 +17893,9 @@
       <c r="D240">
         <v>0</v>
       </c>
+      <c r="E240">
+        <v>0</v>
+      </c>
       <c r="H240">
         <v>24</v>
       </c>
@@ -17772,6 +17964,9 @@
       <c r="D241">
         <v>0</v>
       </c>
+      <c r="E241">
+        <v>0</v>
+      </c>
       <c r="H241">
         <v>24</v>
       </c>
@@ -17840,6 +18035,9 @@
       <c r="D242">
         <v>0</v>
       </c>
+      <c r="E242">
+        <v>0</v>
+      </c>
       <c r="H242">
         <v>24</v>
       </c>
@@ -17908,6 +18106,9 @@
       <c r="D243">
         <v>0</v>
       </c>
+      <c r="E243">
+        <v>0</v>
+      </c>
       <c r="H243">
         <v>24</v>
       </c>
@@ -17976,6 +18177,9 @@
       <c r="D244">
         <v>0</v>
       </c>
+      <c r="E244">
+        <v>0</v>
+      </c>
       <c r="H244">
         <v>24</v>
       </c>
@@ -18044,6 +18248,9 @@
       <c r="D245">
         <v>0</v>
       </c>
+      <c r="E245">
+        <v>0</v>
+      </c>
       <c r="H245">
         <v>24</v>
       </c>
@@ -18110,7 +18317,7 @@
         <v>67</v>
       </c>
       <c r="D246">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E246">
         <v>1</v>
@@ -18184,7 +18391,7 @@
         <v>67</v>
       </c>
       <c r="D247">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E247">
         <v>1</v>
@@ -18258,7 +18465,7 @@
         <v>67</v>
       </c>
       <c r="D248">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E248">
         <v>1</v>
@@ -18332,7 +18539,7 @@
         <v>67</v>
       </c>
       <c r="D249">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E249">
         <v>1</v>
@@ -18406,7 +18613,7 @@
         <v>67</v>
       </c>
       <c r="D250">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E250">
         <v>1</v>
@@ -18480,7 +18687,7 @@
         <v>67</v>
       </c>
       <c r="D251">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E251">
         <v>1</v>
@@ -18554,7 +18761,7 @@
         <v>67</v>
       </c>
       <c r="D252">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E252">
         <v>1</v>
@@ -18631,7 +18838,7 @@
         <v>67</v>
       </c>
       <c r="D253">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E253">
         <v>1</v>
@@ -18708,7 +18915,7 @@
         <v>67</v>
       </c>
       <c r="D254">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E254">
         <v>1</v>
@@ -18785,7 +18992,7 @@
         <v>67</v>
       </c>
       <c r="D255">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E255">
         <v>1</v>
@@ -18862,7 +19069,7 @@
         <v>67</v>
       </c>
       <c r="D256">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E256">
         <v>1</v>
@@ -18939,7 +19146,7 @@
         <v>67</v>
       </c>
       <c r="D257">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E257">
         <v>1</v>
@@ -19016,7 +19223,7 @@
         <v>67</v>
       </c>
       <c r="D258">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E258">
         <v>1</v>
@@ -19093,7 +19300,7 @@
         <v>67</v>
       </c>
       <c r="D259">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E259">
         <v>1</v>
@@ -19172,6 +19379,9 @@
       <c r="D260">
         <v>0</v>
       </c>
+      <c r="E260">
+        <v>0</v>
+      </c>
       <c r="H260">
         <v>31</v>
       </c>
@@ -19237,6 +19447,9 @@
       <c r="D261">
         <v>0</v>
       </c>
+      <c r="E261">
+        <v>0</v>
+      </c>
       <c r="H261">
         <v>31</v>
       </c>
@@ -19302,6 +19515,9 @@
       <c r="D262">
         <v>0</v>
       </c>
+      <c r="E262">
+        <v>0</v>
+      </c>
       <c r="H262">
         <v>31</v>
       </c>
@@ -19367,6 +19583,9 @@
       <c r="D263">
         <v>0</v>
       </c>
+      <c r="E263">
+        <v>0</v>
+      </c>
       <c r="H263">
         <v>31</v>
       </c>
@@ -19432,6 +19651,9 @@
       <c r="D264">
         <v>0</v>
       </c>
+      <c r="E264">
+        <v>0</v>
+      </c>
       <c r="H264">
         <v>31</v>
       </c>
@@ -19495,7 +19717,7 @@
         <v>46</v>
       </c>
       <c r="D265">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E265">
         <v>1</v>
@@ -19569,7 +19791,7 @@
         <v>46</v>
       </c>
       <c r="D266">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E266">
         <v>1</v>
@@ -19643,7 +19865,7 @@
         <v>46</v>
       </c>
       <c r="D267">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E267">
         <v>1</v>
@@ -19717,7 +19939,7 @@
         <v>46</v>
       </c>
       <c r="D268">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E268">
         <v>1</v>
@@ -19791,7 +20013,7 @@
         <v>46</v>
       </c>
       <c r="D269">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E269">
         <v>1</v>
@@ -19867,6 +20089,9 @@
       <c r="D270">
         <v>0</v>
       </c>
+      <c r="E270">
+        <v>0</v>
+      </c>
       <c r="H270">
         <v>32</v>
       </c>
@@ -19932,6 +20157,9 @@
       <c r="D271">
         <v>0</v>
       </c>
+      <c r="E271">
+        <v>0</v>
+      </c>
       <c r="H271">
         <v>32</v>
       </c>
@@ -19997,6 +20225,9 @@
       <c r="D272">
         <v>0</v>
       </c>
+      <c r="E272">
+        <v>0</v>
+      </c>
       <c r="H272">
         <v>32</v>
       </c>
@@ -20062,6 +20293,9 @@
       <c r="D273">
         <v>0</v>
       </c>
+      <c r="E273">
+        <v>0</v>
+      </c>
       <c r="H273">
         <v>32</v>
       </c>
@@ -20127,6 +20361,9 @@
       <c r="D274">
         <v>0</v>
       </c>
+      <c r="E274">
+        <v>0</v>
+      </c>
       <c r="H274">
         <v>32</v>
       </c>
@@ -20190,7 +20427,7 @@
         <v>46</v>
       </c>
       <c r="D275">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E275">
         <v>1</v>
@@ -20264,7 +20501,7 @@
         <v>46</v>
       </c>
       <c r="D276">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E276">
         <v>1</v>
@@ -20338,7 +20575,7 @@
         <v>46</v>
       </c>
       <c r="D277">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E277">
         <v>1</v>
@@ -20412,7 +20649,7 @@
         <v>46</v>
       </c>
       <c r="D278">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E278">
         <v>1</v>
@@ -20486,7 +20723,7 @@
         <v>46</v>
       </c>
       <c r="D279">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E279">
         <v>1</v>
@@ -20560,7 +20797,7 @@
         <v>46</v>
       </c>
       <c r="D280">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E280">
         <v>1</v>
@@ -20634,7 +20871,7 @@
         <v>46</v>
       </c>
       <c r="D281">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E281">
         <v>1</v>
@@ -20708,7 +20945,7 @@
         <v>46</v>
       </c>
       <c r="D282">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E282">
         <v>1</v>
@@ -20782,7 +21019,7 @@
         <v>46</v>
       </c>
       <c r="D283">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E283">
         <v>1</v>
@@ -20856,7 +21093,7 @@
         <v>46</v>
       </c>
       <c r="D284">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E284">
         <v>1</v>
@@ -20932,6 +21169,9 @@
       <c r="D285">
         <v>0</v>
       </c>
+      <c r="E285">
+        <v>0</v>
+      </c>
       <c r="H285">
         <v>33</v>
       </c>
@@ -20997,6 +21237,9 @@
       <c r="D286">
         <v>0</v>
       </c>
+      <c r="E286">
+        <v>0</v>
+      </c>
       <c r="H286">
         <v>33</v>
       </c>
@@ -21062,6 +21305,9 @@
       <c r="D287">
         <v>0</v>
       </c>
+      <c r="E287">
+        <v>0</v>
+      </c>
       <c r="H287">
         <v>33</v>
       </c>
@@ -21127,6 +21373,9 @@
       <c r="D288">
         <v>0</v>
       </c>
+      <c r="E288">
+        <v>0</v>
+      </c>
       <c r="H288">
         <v>33</v>
       </c>
@@ -21192,6 +21441,9 @@
       <c r="D289">
         <v>0</v>
       </c>
+      <c r="E289">
+        <v>0</v>
+      </c>
       <c r="H289">
         <v>33</v>
       </c>
@@ -21257,6 +21509,9 @@
       <c r="D290">
         <v>0</v>
       </c>
+      <c r="E290">
+        <v>0</v>
+      </c>
       <c r="H290">
         <v>26</v>
       </c>
@@ -21291,7 +21546,7 @@
         <v>128</v>
       </c>
       <c r="U290" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V290" s="1">
         <v>0</v>
@@ -21311,7 +21566,7 @@
         <v>29</v>
       </c>
       <c r="D291">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E291">
         <v>1</v>
@@ -21356,7 +21611,7 @@
         <v>128</v>
       </c>
       <c r="U291" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V291" s="1">
         <v>0</v>
@@ -21376,7 +21631,7 @@
         <v>29</v>
       </c>
       <c r="D292">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E292">
         <v>1</v>
@@ -21399,6 +21654,9 @@
       <c r="L292" t="s">
         <v>126</v>
       </c>
+      <c r="M292" t="s">
+        <v>70</v>
+      </c>
       <c r="N292">
         <v>7.8934081346423504E-2</v>
       </c>
@@ -21418,7 +21676,7 @@
         <v>128</v>
       </c>
       <c r="U292" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V292" s="1">
         <v>0</v>
@@ -21438,7 +21696,7 @@
         <v>29</v>
       </c>
       <c r="D293">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E293">
         <v>1</v>
@@ -21483,7 +21741,7 @@
         <v>128</v>
       </c>
       <c r="U293" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V293" s="1">
         <v>0</v>
@@ -21503,7 +21761,7 @@
         <v>29</v>
       </c>
       <c r="D294">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E294">
         <v>1</v>
@@ -21523,6 +21781,9 @@
       <c r="K294">
         <v>24</v>
       </c>
+      <c r="L294" t="s">
+        <v>126</v>
+      </c>
       <c r="M294" t="s">
         <v>70</v>
       </c>
@@ -21545,13 +21806,1818 @@
         <v>128</v>
       </c>
       <c r="U294" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V294" s="1">
         <v>0</v>
       </c>
       <c r="W294" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A295">
+        <v>46</v>
+      </c>
+      <c r="B295" t="s">
+        <v>129</v>
+      </c>
+      <c r="C295" t="s">
+        <v>46</v>
+      </c>
+      <c r="D295">
+        <v>0</v>
+      </c>
+      <c r="E295">
+        <v>0</v>
+      </c>
+      <c r="G295">
+        <v>25</v>
+      </c>
+      <c r="H295">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I295">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J295">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L295" t="s">
+        <v>79</v>
+      </c>
+      <c r="M295" t="s">
+        <v>31</v>
+      </c>
+      <c r="N295">
+        <v>67</v>
+      </c>
+      <c r="O295">
+        <v>0</v>
+      </c>
+      <c r="P295">
+        <v>84</v>
+      </c>
+      <c r="Q295">
+        <v>0</v>
+      </c>
+      <c r="R295">
+        <v>11.4</v>
+      </c>
+      <c r="S295" t="s">
+        <v>100</v>
+      </c>
+      <c r="T295" t="s">
+        <v>135</v>
+      </c>
+      <c r="U295" s="1">
+        <v>1</v>
+      </c>
+      <c r="V295" s="1">
+        <v>1</v>
+      </c>
+      <c r="W295" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A296">
+        <v>46</v>
+      </c>
+      <c r="B296" t="s">
+        <v>129</v>
+      </c>
+      <c r="C296" t="s">
+        <v>46</v>
+      </c>
+      <c r="D296">
+        <v>0</v>
+      </c>
+      <c r="E296">
+        <v>0</v>
+      </c>
+      <c r="G296">
+        <v>25</v>
+      </c>
+      <c r="H296">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I296">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J296">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L296" t="s">
+        <v>132</v>
+      </c>
+      <c r="M296" t="s">
+        <v>48</v>
+      </c>
+      <c r="N296">
+        <v>36.270000000000003</v>
+      </c>
+      <c r="O296">
+        <v>0</v>
+      </c>
+      <c r="P296">
+        <v>84</v>
+      </c>
+      <c r="Q296">
+        <v>0</v>
+      </c>
+      <c r="R296">
+        <v>4.82</v>
+      </c>
+      <c r="S296" t="s">
+        <v>134</v>
+      </c>
+      <c r="T296" t="s">
+        <v>133</v>
+      </c>
+      <c r="U296" s="1">
+        <v>1</v>
+      </c>
+      <c r="V296" s="1">
+        <v>1</v>
+      </c>
+      <c r="W296" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A297">
+        <v>46</v>
+      </c>
+      <c r="B297" t="s">
+        <v>129</v>
+      </c>
+      <c r="C297" t="s">
+        <v>46</v>
+      </c>
+      <c r="D297">
+        <v>0</v>
+      </c>
+      <c r="E297">
+        <v>0</v>
+      </c>
+      <c r="G297">
+        <v>25</v>
+      </c>
+      <c r="H297">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I297">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J297">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L297" t="s">
+        <v>131</v>
+      </c>
+      <c r="M297" t="s">
+        <v>31</v>
+      </c>
+      <c r="N297">
+        <v>70</v>
+      </c>
+      <c r="O297">
+        <v>0</v>
+      </c>
+      <c r="P297">
+        <v>84</v>
+      </c>
+      <c r="Q297">
+        <v>0</v>
+      </c>
+      <c r="R297">
+        <v>14.4</v>
+      </c>
+      <c r="S297" t="s">
+        <v>100</v>
+      </c>
+      <c r="T297" t="s">
+        <v>135</v>
+      </c>
+      <c r="U297" s="1">
+        <v>1</v>
+      </c>
+      <c r="V297" s="1">
+        <v>1</v>
+      </c>
+      <c r="W297" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A298">
+        <v>46</v>
+      </c>
+      <c r="B298" t="s">
+        <v>129</v>
+      </c>
+      <c r="C298" t="s">
+        <v>46</v>
+      </c>
+      <c r="D298">
+        <v>0</v>
+      </c>
+      <c r="E298">
+        <v>0</v>
+      </c>
+      <c r="G298">
+        <v>25</v>
+      </c>
+      <c r="H298">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I298">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J298">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L298" t="s">
+        <v>130</v>
+      </c>
+      <c r="M298" t="s">
+        <v>80</v>
+      </c>
+      <c r="N298">
+        <v>39.840000000000003</v>
+      </c>
+      <c r="O298">
+        <v>0</v>
+      </c>
+      <c r="P298">
+        <v>84</v>
+      </c>
+      <c r="Q298">
+        <v>0</v>
+      </c>
+      <c r="R298">
+        <v>13.3</v>
+      </c>
+      <c r="S298" t="s">
+        <v>134</v>
+      </c>
+      <c r="T298" t="s">
+        <v>133</v>
+      </c>
+      <c r="U298" s="1">
+        <v>1</v>
+      </c>
+      <c r="V298" s="1">
+        <v>1</v>
+      </c>
+      <c r="W298" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A299">
+        <v>47</v>
+      </c>
+      <c r="B299" t="s">
+        <v>129</v>
+      </c>
+      <c r="C299" t="s">
+        <v>46</v>
+      </c>
+      <c r="D299">
+        <v>0</v>
+      </c>
+      <c r="E299">
+        <v>1</v>
+      </c>
+      <c r="F299">
+        <v>1</v>
+      </c>
+      <c r="G299">
+        <v>25</v>
+      </c>
+      <c r="H299">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I299">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J299">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="K299">
+        <v>24</v>
+      </c>
+      <c r="L299" t="s">
+        <v>79</v>
+      </c>
+      <c r="M299" t="s">
+        <v>31</v>
+      </c>
+      <c r="N299">
+        <v>65.2</v>
+      </c>
+      <c r="O299">
+        <v>0</v>
+      </c>
+      <c r="P299">
+        <v>84</v>
+      </c>
+      <c r="Q299">
+        <v>0</v>
+      </c>
+      <c r="R299">
+        <v>13.18</v>
+      </c>
+      <c r="S299" t="s">
+        <v>100</v>
+      </c>
+      <c r="T299" t="s">
+        <v>135</v>
+      </c>
+      <c r="U299" s="1">
+        <v>1</v>
+      </c>
+      <c r="V299" s="1">
+        <v>1</v>
+      </c>
+      <c r="W299" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A300">
+        <v>47</v>
+      </c>
+      <c r="B300" t="s">
+        <v>129</v>
+      </c>
+      <c r="C300" t="s">
+        <v>46</v>
+      </c>
+      <c r="D300">
+        <v>0</v>
+      </c>
+      <c r="E300">
+        <v>1</v>
+      </c>
+      <c r="F300">
+        <v>1</v>
+      </c>
+      <c r="G300">
+        <v>25</v>
+      </c>
+      <c r="H300">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I300">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J300">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="K300">
+        <v>24</v>
+      </c>
+      <c r="L300" t="s">
+        <v>132</v>
+      </c>
+      <c r="M300" t="s">
+        <v>48</v>
+      </c>
+      <c r="N300">
+        <v>30.51</v>
+      </c>
+      <c r="O300">
+        <v>0</v>
+      </c>
+      <c r="P300">
+        <v>84</v>
+      </c>
+      <c r="Q300">
+        <v>0</v>
+      </c>
+      <c r="R300">
+        <v>0.89</v>
+      </c>
+      <c r="S300" t="s">
+        <v>134</v>
+      </c>
+      <c r="T300" t="s">
+        <v>133</v>
+      </c>
+      <c r="U300" s="1">
+        <v>1</v>
+      </c>
+      <c r="V300" s="1">
+        <v>1</v>
+      </c>
+      <c r="W300" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A301">
+        <v>47</v>
+      </c>
+      <c r="B301" t="s">
+        <v>129</v>
+      </c>
+      <c r="C301" t="s">
+        <v>46</v>
+      </c>
+      <c r="D301">
+        <v>0</v>
+      </c>
+      <c r="E301">
+        <v>1</v>
+      </c>
+      <c r="F301">
+        <v>1</v>
+      </c>
+      <c r="G301">
+        <v>25</v>
+      </c>
+      <c r="H301">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I301">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J301">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="K301">
+        <v>24</v>
+      </c>
+      <c r="L301" t="s">
+        <v>131</v>
+      </c>
+      <c r="M301" t="s">
+        <v>31</v>
+      </c>
+      <c r="N301">
+        <v>61.25</v>
+      </c>
+      <c r="O301">
+        <v>0</v>
+      </c>
+      <c r="P301">
+        <v>84</v>
+      </c>
+      <c r="Q301">
+        <v>0</v>
+      </c>
+      <c r="R301">
+        <v>10.84</v>
+      </c>
+      <c r="S301" t="s">
+        <v>100</v>
+      </c>
+      <c r="T301" t="s">
+        <v>135</v>
+      </c>
+      <c r="U301" s="1">
+        <v>1</v>
+      </c>
+      <c r="V301" s="1">
+        <v>1</v>
+      </c>
+      <c r="W301" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A302">
+        <v>47</v>
+      </c>
+      <c r="B302" t="s">
+        <v>129</v>
+      </c>
+      <c r="C302" t="s">
+        <v>46</v>
+      </c>
+      <c r="D302">
+        <v>0</v>
+      </c>
+      <c r="E302">
+        <v>1</v>
+      </c>
+      <c r="F302">
+        <v>1</v>
+      </c>
+      <c r="G302">
+        <v>25</v>
+      </c>
+      <c r="H302">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I302">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J302">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="K302">
+        <v>24</v>
+      </c>
+      <c r="L302" t="s">
+        <v>130</v>
+      </c>
+      <c r="M302" t="s">
+        <v>80</v>
+      </c>
+      <c r="N302">
+        <v>60.19</v>
+      </c>
+      <c r="O302">
+        <v>0</v>
+      </c>
+      <c r="P302">
+        <v>84</v>
+      </c>
+      <c r="Q302">
+        <v>0</v>
+      </c>
+      <c r="R302">
+        <v>15.35</v>
+      </c>
+      <c r="S302" t="s">
+        <v>134</v>
+      </c>
+      <c r="T302" t="s">
+        <v>133</v>
+      </c>
+      <c r="U302" s="1">
+        <v>1</v>
+      </c>
+      <c r="V302" s="1">
+        <v>1</v>
+      </c>
+      <c r="W302" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A303">
+        <v>48</v>
+      </c>
+      <c r="B303" t="s">
+        <v>136</v>
+      </c>
+      <c r="C303" t="s">
+        <v>66</v>
+      </c>
+      <c r="D303">
+        <v>0</v>
+      </c>
+      <c r="E303">
+        <v>0</v>
+      </c>
+      <c r="H303">
+        <v>19</v>
+      </c>
+      <c r="I303">
+        <v>19</v>
+      </c>
+      <c r="J303">
+        <v>19</v>
+      </c>
+      <c r="L303" t="s">
+        <v>140</v>
+      </c>
+      <c r="M303" t="s">
+        <v>48</v>
+      </c>
+      <c r="N303">
+        <v>76.055996307661601</v>
+      </c>
+      <c r="O303">
+        <v>1</v>
+      </c>
+      <c r="P303">
+        <v>28</v>
+      </c>
+      <c r="Q303">
+        <v>0</v>
+      </c>
+      <c r="S303" t="s">
+        <v>147</v>
+      </c>
+      <c r="T303" t="s">
+        <v>148</v>
+      </c>
+      <c r="U303" s="1">
+        <v>1</v>
+      </c>
+      <c r="V303" s="1">
+        <v>1</v>
+      </c>
+      <c r="W303" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A304">
+        <v>48</v>
+      </c>
+      <c r="B304" t="s">
+        <v>136</v>
+      </c>
+      <c r="C304" t="s">
+        <v>66</v>
+      </c>
+      <c r="D304">
+        <v>0</v>
+      </c>
+      <c r="E304">
+        <v>0</v>
+      </c>
+      <c r="H304">
+        <v>25</v>
+      </c>
+      <c r="I304">
+        <v>25</v>
+      </c>
+      <c r="J304">
+        <v>25</v>
+      </c>
+      <c r="L304" t="s">
+        <v>140</v>
+      </c>
+      <c r="M304" t="s">
+        <v>48</v>
+      </c>
+      <c r="N304">
+        <v>39.944677294613598</v>
+      </c>
+      <c r="O304">
+        <v>1</v>
+      </c>
+      <c r="P304">
+        <v>25</v>
+      </c>
+      <c r="Q304">
+        <v>0</v>
+      </c>
+      <c r="R304">
+        <v>2.0161290322580996</v>
+      </c>
+      <c r="S304" t="s">
+        <v>147</v>
+      </c>
+      <c r="T304" t="s">
+        <v>148</v>
+      </c>
+      <c r="U304" s="1">
+        <v>1</v>
+      </c>
+      <c r="V304" s="1">
+        <v>1</v>
+      </c>
+      <c r="W304" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="305" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A305">
+        <v>48</v>
+      </c>
+      <c r="B305" t="s">
+        <v>136</v>
+      </c>
+      <c r="C305" t="s">
+        <v>66</v>
+      </c>
+      <c r="D305">
+        <v>0</v>
+      </c>
+      <c r="E305">
+        <v>1</v>
+      </c>
+      <c r="F305">
+        <v>1</v>
+      </c>
+      <c r="H305">
+        <v>25</v>
+      </c>
+      <c r="I305">
+        <v>19</v>
+      </c>
+      <c r="J305">
+        <v>31</v>
+      </c>
+      <c r="K305">
+        <v>24</v>
+      </c>
+      <c r="L305" t="s">
+        <v>140</v>
+      </c>
+      <c r="M305" t="s">
+        <v>48</v>
+      </c>
+      <c r="N305">
+        <v>41.199573385225598</v>
+      </c>
+      <c r="O305">
+        <v>1</v>
+      </c>
+      <c r="P305">
+        <v>29</v>
+      </c>
+      <c r="Q305">
+        <v>0</v>
+      </c>
+      <c r="R305">
+        <v>2.4865591397849514</v>
+      </c>
+      <c r="S305" t="s">
+        <v>147</v>
+      </c>
+      <c r="T305" t="s">
+        <v>148</v>
+      </c>
+      <c r="U305" s="1">
+        <v>1</v>
+      </c>
+      <c r="V305" s="1">
+        <v>1</v>
+      </c>
+      <c r="W305" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="306" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A306">
+        <v>48</v>
+      </c>
+      <c r="B306" t="s">
+        <v>136</v>
+      </c>
+      <c r="C306" t="s">
+        <v>66</v>
+      </c>
+      <c r="D306">
+        <v>0</v>
+      </c>
+      <c r="E306">
+        <v>0</v>
+      </c>
+      <c r="H306">
+        <v>31</v>
+      </c>
+      <c r="I306">
+        <v>31</v>
+      </c>
+      <c r="J306">
+        <v>31</v>
+      </c>
+      <c r="L306" t="s">
+        <v>140</v>
+      </c>
+      <c r="M306" t="s">
+        <v>48</v>
+      </c>
+      <c r="N306">
+        <v>31.969974802285201</v>
+      </c>
+      <c r="O306">
+        <v>1</v>
+      </c>
+      <c r="P306">
+        <v>25</v>
+      </c>
+      <c r="Q306">
+        <v>0</v>
+      </c>
+      <c r="R306">
+        <v>1.9492365840880002</v>
+      </c>
+      <c r="S306" t="s">
+        <v>147</v>
+      </c>
+      <c r="T306" t="s">
+        <v>148</v>
+      </c>
+      <c r="U306" s="1">
+        <v>1</v>
+      </c>
+      <c r="V306" s="1">
+        <v>1</v>
+      </c>
+      <c r="W306" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A307">
+        <v>49</v>
+      </c>
+      <c r="B307" t="s">
+        <v>136</v>
+      </c>
+      <c r="C307" t="s">
+        <v>67</v>
+      </c>
+      <c r="D307">
+        <v>0</v>
+      </c>
+      <c r="E307">
+        <v>0</v>
+      </c>
+      <c r="H307">
+        <v>19</v>
+      </c>
+      <c r="I307">
+        <v>19</v>
+      </c>
+      <c r="J307">
+        <v>19</v>
+      </c>
+      <c r="L307" t="s">
+        <v>141</v>
+      </c>
+      <c r="M307" t="s">
+        <v>48</v>
+      </c>
+      <c r="N307">
+        <v>13.494950000312601</v>
+      </c>
+      <c r="O307">
+        <v>1</v>
+      </c>
+      <c r="P307">
+        <v>28</v>
+      </c>
+      <c r="Q307">
+        <v>0</v>
+      </c>
+      <c r="S307" t="s">
+        <v>147</v>
+      </c>
+      <c r="T307" t="s">
+        <v>148</v>
+      </c>
+      <c r="U307" s="1">
+        <v>1</v>
+      </c>
+      <c r="V307" s="1">
+        <v>1</v>
+      </c>
+      <c r="W307" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="308" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A308">
+        <v>49</v>
+      </c>
+      <c r="B308" t="s">
+        <v>136</v>
+      </c>
+      <c r="C308" t="s">
+        <v>67</v>
+      </c>
+      <c r="D308">
+        <v>0</v>
+      </c>
+      <c r="E308">
+        <v>0</v>
+      </c>
+      <c r="H308">
+        <v>25</v>
+      </c>
+      <c r="I308">
+        <v>25</v>
+      </c>
+      <c r="J308">
+        <v>25</v>
+      </c>
+      <c r="L308" t="s">
+        <v>141</v>
+      </c>
+      <c r="M308" t="s">
+        <v>48</v>
+      </c>
+      <c r="N308">
+        <v>9.0026203713547801</v>
+      </c>
+      <c r="O308">
+        <v>1</v>
+      </c>
+      <c r="P308">
+        <v>25</v>
+      </c>
+      <c r="Q308">
+        <v>0</v>
+      </c>
+      <c r="R308">
+        <v>0.87334037935972963</v>
+      </c>
+      <c r="S308" t="s">
+        <v>147</v>
+      </c>
+      <c r="T308" t="s">
+        <v>148</v>
+      </c>
+      <c r="U308" s="1">
+        <v>1</v>
+      </c>
+      <c r="V308" s="1">
+        <v>1</v>
+      </c>
+      <c r="W308" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A309">
+        <v>49</v>
+      </c>
+      <c r="B309" t="s">
+        <v>136</v>
+      </c>
+      <c r="C309" t="s">
+        <v>67</v>
+      </c>
+      <c r="D309">
+        <v>0</v>
+      </c>
+      <c r="E309">
+        <v>1</v>
+      </c>
+      <c r="F309">
+        <v>1</v>
+      </c>
+      <c r="H309">
+        <v>25</v>
+      </c>
+      <c r="I309">
+        <v>19</v>
+      </c>
+      <c r="J309">
+        <v>31</v>
+      </c>
+      <c r="K309">
+        <v>24</v>
+      </c>
+      <c r="L309" t="s">
+        <v>141</v>
+      </c>
+      <c r="M309" t="s">
+        <v>48</v>
+      </c>
+      <c r="N309">
+        <v>10.246039737087299</v>
+      </c>
+      <c r="O309">
+        <v>1</v>
+      </c>
+      <c r="P309">
+        <v>29</v>
+      </c>
+      <c r="Q309">
+        <v>0</v>
+      </c>
+      <c r="R309">
+        <v>1.1644455006535095</v>
+      </c>
+      <c r="S309" t="s">
+        <v>147</v>
+      </c>
+      <c r="T309" t="s">
+        <v>148</v>
+      </c>
+      <c r="U309" s="1">
+        <v>1</v>
+      </c>
+      <c r="V309" s="1">
+        <v>1</v>
+      </c>
+      <c r="W309" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="310" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A310">
+        <v>49</v>
+      </c>
+      <c r="B310" t="s">
+        <v>136</v>
+      </c>
+      <c r="C310" t="s">
+        <v>67</v>
+      </c>
+      <c r="D310">
+        <v>0</v>
+      </c>
+      <c r="E310">
+        <v>0</v>
+      </c>
+      <c r="H310">
+        <v>31</v>
+      </c>
+      <c r="I310">
+        <v>31</v>
+      </c>
+      <c r="J310">
+        <v>31</v>
+      </c>
+      <c r="L310" t="s">
+        <v>141</v>
+      </c>
+      <c r="M310" t="s">
+        <v>48</v>
+      </c>
+      <c r="N310">
+        <v>13.343956573129599</v>
+      </c>
+      <c r="O310">
+        <v>1</v>
+      </c>
+      <c r="P310">
+        <v>25</v>
+      </c>
+      <c r="Q310">
+        <v>0</v>
+      </c>
+      <c r="R310">
+        <v>1.3800539083558014</v>
+      </c>
+      <c r="S310" t="s">
+        <v>147</v>
+      </c>
+      <c r="T310" t="s">
+        <v>148</v>
+      </c>
+      <c r="U310" s="1">
+        <v>1</v>
+      </c>
+      <c r="V310" s="1">
+        <v>1</v>
+      </c>
+      <c r="W310" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="311" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A311">
+        <v>50</v>
+      </c>
+      <c r="B311" t="s">
+        <v>136</v>
+      </c>
+      <c r="C311" t="s">
+        <v>137</v>
+      </c>
+      <c r="D311">
+        <v>0</v>
+      </c>
+      <c r="E311">
+        <v>0</v>
+      </c>
+      <c r="H311">
+        <v>19</v>
+      </c>
+      <c r="I311">
+        <v>19</v>
+      </c>
+      <c r="J311">
+        <v>19</v>
+      </c>
+      <c r="L311" t="s">
+        <v>142</v>
+      </c>
+      <c r="M311" t="s">
+        <v>143</v>
+      </c>
+      <c r="N311">
+        <v>0.20204081632653001</v>
+      </c>
+      <c r="O311">
+        <v>1</v>
+      </c>
+      <c r="P311">
+        <v>28</v>
+      </c>
+      <c r="Q311">
+        <v>0</v>
+      </c>
+      <c r="S311" t="s">
+        <v>147</v>
+      </c>
+      <c r="T311" t="s">
+        <v>148</v>
+      </c>
+      <c r="U311" s="1">
+        <v>1</v>
+      </c>
+      <c r="V311" s="1">
+        <v>1</v>
+      </c>
+      <c r="W311" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A312">
+        <v>50</v>
+      </c>
+      <c r="B312" t="s">
+        <v>136</v>
+      </c>
+      <c r="C312" t="s">
+        <v>137</v>
+      </c>
+      <c r="D312">
+        <v>0</v>
+      </c>
+      <c r="E312">
+        <v>0</v>
+      </c>
+      <c r="H312">
+        <v>25</v>
+      </c>
+      <c r="I312">
+        <v>25</v>
+      </c>
+      <c r="J312">
+        <v>25</v>
+      </c>
+      <c r="L312" t="s">
+        <v>142</v>
+      </c>
+      <c r="M312" t="s">
+        <v>143</v>
+      </c>
+      <c r="N312">
+        <v>0.24693877551020399</v>
+      </c>
+      <c r="O312">
+        <v>1</v>
+      </c>
+      <c r="P312">
+        <v>25</v>
+      </c>
+      <c r="Q312">
+        <v>0</v>
+      </c>
+      <c r="R312">
+        <v>5.2380952380952486E-2</v>
+      </c>
+      <c r="S312" t="s">
+        <v>147</v>
+      </c>
+      <c r="T312" t="s">
+        <v>148</v>
+      </c>
+      <c r="U312" s="1">
+        <v>1</v>
+      </c>
+      <c r="V312" s="1">
+        <v>1</v>
+      </c>
+      <c r="W312" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="313" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A313">
+        <v>50</v>
+      </c>
+      <c r="B313" t="s">
+        <v>136</v>
+      </c>
+      <c r="C313" t="s">
+        <v>137</v>
+      </c>
+      <c r="D313">
+        <v>0</v>
+      </c>
+      <c r="E313">
+        <v>1</v>
+      </c>
+      <c r="F313">
+        <v>1</v>
+      </c>
+      <c r="H313">
+        <v>25</v>
+      </c>
+      <c r="I313">
+        <v>19</v>
+      </c>
+      <c r="J313">
+        <v>31</v>
+      </c>
+      <c r="K313">
+        <v>24</v>
+      </c>
+      <c r="L313" t="s">
+        <v>142</v>
+      </c>
+      <c r="M313" t="s">
+        <v>143</v>
+      </c>
+      <c r="N313">
+        <v>0.27278911564625802</v>
+      </c>
+      <c r="O313">
+        <v>1</v>
+      </c>
+      <c r="P313">
+        <v>29</v>
+      </c>
+      <c r="Q313">
+        <v>0</v>
+      </c>
+      <c r="R313">
+        <v>4.7619047619047492E-2</v>
+      </c>
+      <c r="S313" t="s">
+        <v>147</v>
+      </c>
+      <c r="T313" t="s">
+        <v>148</v>
+      </c>
+      <c r="U313" s="1">
+        <v>1</v>
+      </c>
+      <c r="V313" s="1">
+        <v>1</v>
+      </c>
+      <c r="W313" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A314">
+        <v>50</v>
+      </c>
+      <c r="B314" t="s">
+        <v>136</v>
+      </c>
+      <c r="C314" t="s">
+        <v>137</v>
+      </c>
+      <c r="D314">
+        <v>0</v>
+      </c>
+      <c r="E314">
+        <v>0</v>
+      </c>
+      <c r="H314">
+        <v>31</v>
+      </c>
+      <c r="I314">
+        <v>31</v>
+      </c>
+      <c r="J314">
+        <v>31</v>
+      </c>
+      <c r="L314" t="s">
+        <v>142</v>
+      </c>
+      <c r="M314" t="s">
+        <v>143</v>
+      </c>
+      <c r="N314">
+        <v>0.25714285714285701</v>
+      </c>
+      <c r="O314">
+        <v>1</v>
+      </c>
+      <c r="P314">
+        <v>25</v>
+      </c>
+      <c r="Q314">
+        <v>0</v>
+      </c>
+      <c r="R314">
+        <v>5.7142857142857009E-2</v>
+      </c>
+      <c r="S314" t="s">
+        <v>147</v>
+      </c>
+      <c r="T314" t="s">
+        <v>148</v>
+      </c>
+      <c r="U314" s="1">
+        <v>1</v>
+      </c>
+      <c r="V314" s="1">
+        <v>1</v>
+      </c>
+      <c r="W314" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="315" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A315">
+        <v>51</v>
+      </c>
+      <c r="B315" t="s">
+        <v>136</v>
+      </c>
+      <c r="C315" t="s">
+        <v>138</v>
+      </c>
+      <c r="D315">
+        <v>0</v>
+      </c>
+      <c r="E315">
+        <v>0</v>
+      </c>
+      <c r="H315">
+        <v>19</v>
+      </c>
+      <c r="I315">
+        <v>19</v>
+      </c>
+      <c r="J315">
+        <v>19</v>
+      </c>
+      <c r="L315" t="s">
+        <v>144</v>
+      </c>
+      <c r="M315" t="s">
+        <v>143</v>
+      </c>
+      <c r="N315">
+        <v>6.8296257078838601E-2</v>
+      </c>
+      <c r="O315">
+        <v>1</v>
+      </c>
+      <c r="P315">
+        <v>28</v>
+      </c>
+      <c r="Q315">
+        <v>0</v>
+      </c>
+      <c r="R315">
+        <v>4.7866894197951398E-2</v>
+      </c>
+      <c r="S315" t="s">
+        <v>147</v>
+      </c>
+      <c r="T315" t="s">
+        <v>148</v>
+      </c>
+      <c r="U315" s="1">
+        <v>1</v>
+      </c>
+      <c r="V315" s="1">
+        <v>1</v>
+      </c>
+      <c r="W315" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="316" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A316">
+        <v>51</v>
+      </c>
+      <c r="B316" t="s">
+        <v>136</v>
+      </c>
+      <c r="C316" t="s">
+        <v>138</v>
+      </c>
+      <c r="D316">
+        <v>0</v>
+      </c>
+      <c r="E316">
+        <v>0</v>
+      </c>
+      <c r="H316">
+        <v>25</v>
+      </c>
+      <c r="I316">
+        <v>25</v>
+      </c>
+      <c r="J316">
+        <v>25</v>
+      </c>
+      <c r="L316" t="s">
+        <v>144</v>
+      </c>
+      <c r="M316" t="s">
+        <v>143</v>
+      </c>
+      <c r="N316">
+        <v>0.15308183562913</v>
+      </c>
+      <c r="O316">
+        <v>1</v>
+      </c>
+      <c r="P316">
+        <v>25</v>
+      </c>
+      <c r="Q316">
+        <v>0</v>
+      </c>
+      <c r="R316">
+        <v>4.0827645051195009E-2</v>
+      </c>
+      <c r="S316" t="s">
+        <v>147</v>
+      </c>
+      <c r="T316" t="s">
+        <v>148</v>
+      </c>
+      <c r="U316" s="1">
+        <v>1</v>
+      </c>
+      <c r="V316" s="1">
+        <v>1</v>
+      </c>
+      <c r="W316" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A317">
+        <v>51</v>
+      </c>
+      <c r="B317" t="s">
+        <v>136</v>
+      </c>
+      <c r="C317" t="s">
+        <v>138</v>
+      </c>
+      <c r="D317">
+        <v>0</v>
+      </c>
+      <c r="E317">
+        <v>1</v>
+      </c>
+      <c r="F317">
+        <v>1</v>
+      </c>
+      <c r="H317">
+        <v>25</v>
+      </c>
+      <c r="I317">
+        <v>19</v>
+      </c>
+      <c r="J317">
+        <v>31</v>
+      </c>
+      <c r="K317">
+        <v>24</v>
+      </c>
+      <c r="L317" t="s">
+        <v>144</v>
+      </c>
+      <c r="M317" t="s">
+        <v>143</v>
+      </c>
+      <c r="N317">
+        <v>0.149642158206725</v>
+      </c>
+      <c r="O317">
+        <v>1</v>
+      </c>
+      <c r="P317">
+        <v>29</v>
+      </c>
+      <c r="Q317">
+        <v>0</v>
+      </c>
+      <c r="R317">
+        <v>4.9274744027303308E-2</v>
+      </c>
+      <c r="S317" t="s">
+        <v>147</v>
+      </c>
+      <c r="T317" t="s">
+        <v>148</v>
+      </c>
+      <c r="U317" s="1">
+        <v>1</v>
+      </c>
+      <c r="V317" s="1">
+        <v>1</v>
+      </c>
+      <c r="W317" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="318" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A318">
+        <v>51</v>
+      </c>
+      <c r="B318" t="s">
+        <v>136</v>
+      </c>
+      <c r="C318" t="s">
+        <v>138</v>
+      </c>
+      <c r="D318">
+        <v>0</v>
+      </c>
+      <c r="E318">
+        <v>0</v>
+      </c>
+      <c r="H318">
+        <v>31</v>
+      </c>
+      <c r="I318">
+        <v>31</v>
+      </c>
+      <c r="J318">
+        <v>31</v>
+      </c>
+      <c r="L318" t="s">
+        <v>144</v>
+      </c>
+      <c r="M318" t="s">
+        <v>143</v>
+      </c>
+      <c r="N318">
+        <v>0.153711013207529</v>
+      </c>
+      <c r="O318">
+        <v>1</v>
+      </c>
+      <c r="P318">
+        <v>25</v>
+      </c>
+      <c r="Q318">
+        <v>0</v>
+      </c>
+      <c r="R318">
+        <v>5.2090443686006654E-2</v>
+      </c>
+      <c r="S318" t="s">
+        <v>147</v>
+      </c>
+      <c r="T318" t="s">
+        <v>148</v>
+      </c>
+      <c r="U318" s="1">
+        <v>1</v>
+      </c>
+      <c r="V318" s="1">
+        <v>1</v>
+      </c>
+      <c r="W318" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="319" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A319">
+        <v>52</v>
+      </c>
+      <c r="B319" t="s">
+        <v>136</v>
+      </c>
+      <c r="C319" t="s">
+        <v>139</v>
+      </c>
+      <c r="D319">
+        <v>0</v>
+      </c>
+      <c r="E319">
+        <v>0</v>
+      </c>
+      <c r="H319">
+        <v>19</v>
+      </c>
+      <c r="I319">
+        <v>19</v>
+      </c>
+      <c r="J319">
+        <v>19</v>
+      </c>
+      <c r="L319" t="s">
+        <v>145</v>
+      </c>
+      <c r="M319" t="s">
+        <v>146</v>
+      </c>
+      <c r="N319">
+        <v>1.7421602787456401</v>
+      </c>
+      <c r="O319">
+        <v>1</v>
+      </c>
+      <c r="P319">
+        <v>28</v>
+      </c>
+      <c r="Q319">
+        <v>0</v>
+      </c>
+      <c r="R319">
+        <v>0.8710801393728298</v>
+      </c>
+      <c r="S319" t="s">
+        <v>147</v>
+      </c>
+      <c r="T319" t="s">
+        <v>148</v>
+      </c>
+      <c r="U319" s="1">
+        <v>1</v>
+      </c>
+      <c r="V319" s="1">
+        <v>1</v>
+      </c>
+      <c r="W319" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="320" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A320">
+        <v>52</v>
+      </c>
+      <c r="B320" t="s">
+        <v>136</v>
+      </c>
+      <c r="C320" t="s">
+        <v>139</v>
+      </c>
+      <c r="D320">
+        <v>0</v>
+      </c>
+      <c r="E320">
+        <v>0</v>
+      </c>
+      <c r="H320">
+        <v>25</v>
+      </c>
+      <c r="I320">
+        <v>25</v>
+      </c>
+      <c r="J320">
+        <v>25</v>
+      </c>
+      <c r="L320" t="s">
+        <v>145</v>
+      </c>
+      <c r="M320" t="s">
+        <v>146</v>
+      </c>
+      <c r="N320">
+        <v>2.8222996515679499</v>
+      </c>
+      <c r="O320">
+        <v>1</v>
+      </c>
+      <c r="P320">
+        <v>25</v>
+      </c>
+      <c r="Q320">
+        <v>0</v>
+      </c>
+      <c r="R320">
+        <v>2.5958188153310111</v>
+      </c>
+      <c r="S320" t="s">
+        <v>147</v>
+      </c>
+      <c r="T320" t="s">
+        <v>148</v>
+      </c>
+      <c r="U320" s="1">
+        <v>1</v>
+      </c>
+      <c r="V320" s="1">
+        <v>1</v>
+      </c>
+      <c r="W320" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="321" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A321">
+        <v>52</v>
+      </c>
+      <c r="B321" t="s">
+        <v>136</v>
+      </c>
+      <c r="C321" t="s">
+        <v>139</v>
+      </c>
+      <c r="D321">
+        <v>0</v>
+      </c>
+      <c r="E321">
+        <v>1</v>
+      </c>
+      <c r="F321">
+        <v>1</v>
+      </c>
+      <c r="H321">
+        <v>25</v>
+      </c>
+      <c r="I321">
+        <v>19</v>
+      </c>
+      <c r="J321">
+        <v>31</v>
+      </c>
+      <c r="K321">
+        <v>24</v>
+      </c>
+      <c r="L321" t="s">
+        <v>145</v>
+      </c>
+      <c r="M321" t="s">
+        <v>146</v>
+      </c>
+      <c r="N321">
+        <v>3.1358885017421598</v>
+      </c>
+      <c r="O321">
+        <v>1</v>
+      </c>
+      <c r="P321">
+        <v>29</v>
+      </c>
+      <c r="Q321">
+        <v>0</v>
+      </c>
+      <c r="R321">
+        <v>2.822299651567941</v>
+      </c>
+      <c r="S321" t="s">
+        <v>147</v>
+      </c>
+      <c r="T321" t="s">
+        <v>148</v>
+      </c>
+      <c r="U321" s="1">
+        <v>1</v>
+      </c>
+      <c r="V321" s="1">
+        <v>1</v>
+      </c>
+      <c r="W321" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="322" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A322">
+        <v>52</v>
+      </c>
+      <c r="B322" t="s">
+        <v>136</v>
+      </c>
+      <c r="C322" t="s">
+        <v>139</v>
+      </c>
+      <c r="D322">
+        <v>0</v>
+      </c>
+      <c r="E322">
+        <v>0</v>
+      </c>
+      <c r="H322">
+        <v>31</v>
+      </c>
+      <c r="I322">
+        <v>31</v>
+      </c>
+      <c r="J322">
+        <v>31</v>
+      </c>
+      <c r="L322" t="s">
+        <v>145</v>
+      </c>
+      <c r="M322" t="s">
+        <v>146</v>
+      </c>
+      <c r="N322">
+        <v>5.6445993031358901</v>
+      </c>
+      <c r="O322">
+        <v>1</v>
+      </c>
+      <c r="P322">
+        <v>25</v>
+      </c>
+      <c r="Q322">
+        <v>0</v>
+      </c>
+      <c r="R322">
+        <v>4.5470383275261259</v>
+      </c>
+      <c r="S322" t="s">
+        <v>147</v>
+      </c>
+      <c r="T322" t="s">
+        <v>148</v>
+      </c>
+      <c r="U322" s="1">
+        <v>1</v>
+      </c>
+      <c r="V322" s="1">
+        <v>1</v>
+      </c>
+      <c r="W322" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -21561,10 +23627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C63C9F3-EFBE-D44D-B609-615DB2D2DDEC}">
-  <dimension ref="B1:T6"/>
+  <dimension ref="B1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B1" sqref="B1:T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21589,10 +23655,10 @@
         <v>20.100000000000001</v>
       </c>
       <c r="L1" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="M1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="O1">
         <v>0</v>
@@ -21604,10 +23670,10 @@
         <v>0</v>
       </c>
       <c r="S1" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="T1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.2">
@@ -21630,10 +23696,10 @@
         <v>20.100000000000001</v>
       </c>
       <c r="L2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="O2">
         <v>0</v>
@@ -21645,10 +23711,10 @@
         <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="T2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
@@ -21671,10 +23737,10 @@
         <v>20.100000000000001</v>
       </c>
       <c r="L3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="M3" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -21700,31 +23766,22 @@
         <v>46</v>
       </c>
       <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
         <v>0</v>
       </c>
       <c r="H4">
         <v>20.100000000000001</v>
       </c>
       <c r="I4">
-        <v>16</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="J4">
-        <v>23</v>
-      </c>
-      <c r="K4">
-        <v>24</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="L4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -21752,26 +23809,17 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
       <c r="H5">
         <v>20.100000000000001</v>
       </c>
       <c r="I5">
-        <v>16</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="J5">
-        <v>23</v>
-      </c>
-      <c r="K5">
-        <v>24</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="L5" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="M5" t="s">
         <v>31</v>
@@ -21802,29 +23850,20 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
       <c r="H6">
         <v>20.100000000000001</v>
       </c>
       <c r="I6">
-        <v>16</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="J6">
-        <v>23</v>
-      </c>
-      <c r="K6">
-        <v>24</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="L6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="M6" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -21839,6 +23878,88 @@
         <v>134</v>
       </c>
       <c r="T6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I7">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J7">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L7" t="s">
+        <v>131</v>
+      </c>
+      <c r="M7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>84</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="S7" t="s">
+        <v>134</v>
+      </c>
+      <c r="T7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I8">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J8">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L8" t="s">
+        <v>130</v>
+      </c>
+      <c r="M8" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>84</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="S8" t="s">
+        <v>134</v>
+      </c>
+      <c r="T8" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
kern et al 2014 extraction
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8C518245-1126-A44D-B2F8-3E3A693AB18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{422FD1BC-AAA0-614B-A97B-1FB874C823B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="460" windowWidth="24460" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="2080" yWindow="460" windowWidth="24460" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="metanaly_fulldataset" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2599" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="165">
   <si>
     <t>study_id</t>
   </si>
@@ -474,6 +474,54 @@
   <si>
     <t>natrix</t>
   </si>
+  <si>
+    <t>qu2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">table 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">body mass </t>
+  </si>
+  <si>
+    <t>snout-vent length</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>abdomen length</t>
+  </si>
+  <si>
+    <t>head length</t>
+  </si>
+  <si>
+    <t>fore-limb length</t>
+  </si>
+  <si>
+    <t>hind-limb length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximal length </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprint speed </t>
+  </si>
+  <si>
+    <t>head width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plestiodon </t>
+  </si>
+  <si>
+    <t>chinensis</t>
+  </si>
+  <si>
+    <t>kern2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C </t>
+  </si>
 </sst>
 </file>
 
@@ -839,11 +887,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AG322"/>
+  <dimension ref="A1:AG380"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D325" sqref="D325"/>
+      <pane ySplit="1" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G387" sqref="G387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23617,6 +23665,3770 @@
         <v>1</v>
       </c>
       <c r="W322" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="323" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A323">
+        <v>53</v>
+      </c>
+      <c r="B323" t="s">
+        <v>149</v>
+      </c>
+      <c r="C323" t="s">
+        <v>150</v>
+      </c>
+      <c r="D323">
+        <v>0</v>
+      </c>
+      <c r="E323">
+        <v>0</v>
+      </c>
+      <c r="H323">
+        <v>27</v>
+      </c>
+      <c r="I323">
+        <v>27</v>
+      </c>
+      <c r="J323">
+        <v>27</v>
+      </c>
+      <c r="L323" t="s">
+        <v>151</v>
+      </c>
+      <c r="M323" t="s">
+        <v>70</v>
+      </c>
+      <c r="N323">
+        <v>0.71</v>
+      </c>
+      <c r="O323">
+        <v>0</v>
+      </c>
+      <c r="P323">
+        <v>20</v>
+      </c>
+      <c r="Q323">
+        <v>0</v>
+      </c>
+      <c r="R323">
+        <v>0.02</v>
+      </c>
+      <c r="S323" t="s">
+        <v>161</v>
+      </c>
+      <c r="T323" t="s">
+        <v>162</v>
+      </c>
+      <c r="U323" s="1">
+        <v>1</v>
+      </c>
+      <c r="V323" s="1">
+        <v>1</v>
+      </c>
+      <c r="W323" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="324" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A324">
+        <v>53</v>
+      </c>
+      <c r="B324" t="s">
+        <v>149</v>
+      </c>
+      <c r="C324" t="s">
+        <v>150</v>
+      </c>
+      <c r="D324">
+        <v>0</v>
+      </c>
+      <c r="E324">
+        <v>0</v>
+      </c>
+      <c r="H324">
+        <v>27</v>
+      </c>
+      <c r="I324">
+        <v>27</v>
+      </c>
+      <c r="J324">
+        <v>27</v>
+      </c>
+      <c r="L324" t="s">
+        <v>152</v>
+      </c>
+      <c r="M324" t="s">
+        <v>35</v>
+      </c>
+      <c r="N324">
+        <v>31.3</v>
+      </c>
+      <c r="O324">
+        <v>0</v>
+      </c>
+      <c r="P324">
+        <v>20</v>
+      </c>
+      <c r="Q324">
+        <v>0</v>
+      </c>
+      <c r="R324">
+        <v>0.2</v>
+      </c>
+      <c r="S324" t="s">
+        <v>161</v>
+      </c>
+      <c r="T324" t="s">
+        <v>162</v>
+      </c>
+      <c r="U324" s="1">
+        <v>1</v>
+      </c>
+      <c r="V324" s="1">
+        <v>1</v>
+      </c>
+      <c r="W324" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="325" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A325">
+        <v>53</v>
+      </c>
+      <c r="B325" t="s">
+        <v>149</v>
+      </c>
+      <c r="C325" t="s">
+        <v>150</v>
+      </c>
+      <c r="D325">
+        <v>0</v>
+      </c>
+      <c r="E325">
+        <v>0</v>
+      </c>
+      <c r="H325">
+        <v>27</v>
+      </c>
+      <c r="I325">
+        <v>27</v>
+      </c>
+      <c r="J325">
+        <v>27</v>
+      </c>
+      <c r="L325" t="s">
+        <v>154</v>
+      </c>
+      <c r="M325" t="s">
+        <v>35</v>
+      </c>
+      <c r="N325">
+        <v>14</v>
+      </c>
+      <c r="O325">
+        <v>0</v>
+      </c>
+      <c r="P325">
+        <v>20</v>
+      </c>
+      <c r="Q325">
+        <v>0</v>
+      </c>
+      <c r="R325">
+        <v>0.2</v>
+      </c>
+      <c r="S325" t="s">
+        <v>161</v>
+      </c>
+      <c r="T325" t="s">
+        <v>162</v>
+      </c>
+      <c r="U325" s="1">
+        <v>1</v>
+      </c>
+      <c r="V325" s="1">
+        <v>1</v>
+      </c>
+      <c r="W325" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="326" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A326">
+        <v>53</v>
+      </c>
+      <c r="B326" t="s">
+        <v>149</v>
+      </c>
+      <c r="C326" t="s">
+        <v>150</v>
+      </c>
+      <c r="D326">
+        <v>0</v>
+      </c>
+      <c r="E326">
+        <v>0</v>
+      </c>
+      <c r="H326">
+        <v>27</v>
+      </c>
+      <c r="I326">
+        <v>27</v>
+      </c>
+      <c r="J326">
+        <v>27</v>
+      </c>
+      <c r="L326" t="s">
+        <v>72</v>
+      </c>
+      <c r="M326" t="s">
+        <v>35</v>
+      </c>
+      <c r="N326">
+        <v>37.6</v>
+      </c>
+      <c r="O326">
+        <v>0</v>
+      </c>
+      <c r="P326">
+        <v>20</v>
+      </c>
+      <c r="Q326">
+        <v>0</v>
+      </c>
+      <c r="R326">
+        <v>0.5</v>
+      </c>
+      <c r="S326" t="s">
+        <v>161</v>
+      </c>
+      <c r="T326" t="s">
+        <v>162</v>
+      </c>
+      <c r="U326" s="1">
+        <v>1</v>
+      </c>
+      <c r="V326" s="1">
+        <v>1</v>
+      </c>
+      <c r="W326" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="327" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A327">
+        <v>53</v>
+      </c>
+      <c r="B327" t="s">
+        <v>149</v>
+      </c>
+      <c r="C327" t="s">
+        <v>150</v>
+      </c>
+      <c r="D327">
+        <v>0</v>
+      </c>
+      <c r="E327">
+        <v>0</v>
+      </c>
+      <c r="H327">
+        <v>27</v>
+      </c>
+      <c r="I327">
+        <v>27</v>
+      </c>
+      <c r="J327">
+        <v>27</v>
+      </c>
+      <c r="L327" t="s">
+        <v>155</v>
+      </c>
+      <c r="M327" t="s">
+        <v>35</v>
+      </c>
+      <c r="N327">
+        <v>7.2</v>
+      </c>
+      <c r="O327">
+        <v>0</v>
+      </c>
+      <c r="P327">
+        <v>20</v>
+      </c>
+      <c r="Q327">
+        <v>0</v>
+      </c>
+      <c r="R327">
+        <v>0.03</v>
+      </c>
+      <c r="S327" t="s">
+        <v>161</v>
+      </c>
+      <c r="T327" t="s">
+        <v>162</v>
+      </c>
+      <c r="U327" s="1">
+        <v>1</v>
+      </c>
+      <c r="V327" s="1">
+        <v>1</v>
+      </c>
+      <c r="W327" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A328">
+        <v>53</v>
+      </c>
+      <c r="B328" t="s">
+        <v>149</v>
+      </c>
+      <c r="C328" t="s">
+        <v>150</v>
+      </c>
+      <c r="D328">
+        <v>0</v>
+      </c>
+      <c r="E328">
+        <v>0</v>
+      </c>
+      <c r="H328">
+        <v>27</v>
+      </c>
+      <c r="I328">
+        <v>27</v>
+      </c>
+      <c r="J328">
+        <v>27</v>
+      </c>
+      <c r="L328" t="s">
+        <v>160</v>
+      </c>
+      <c r="M328" t="s">
+        <v>35</v>
+      </c>
+      <c r="N328">
+        <v>5.2</v>
+      </c>
+      <c r="O328">
+        <v>0</v>
+      </c>
+      <c r="P328">
+        <v>20</v>
+      </c>
+      <c r="Q328">
+        <v>0</v>
+      </c>
+      <c r="R328">
+        <v>0.04</v>
+      </c>
+      <c r="S328" t="s">
+        <v>161</v>
+      </c>
+      <c r="T328" t="s">
+        <v>162</v>
+      </c>
+      <c r="U328" s="1">
+        <v>1</v>
+      </c>
+      <c r="V328" s="1">
+        <v>1</v>
+      </c>
+      <c r="W328" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="329" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A329">
+        <v>53</v>
+      </c>
+      <c r="B329" t="s">
+        <v>149</v>
+      </c>
+      <c r="C329" t="s">
+        <v>150</v>
+      </c>
+      <c r="D329">
+        <v>0</v>
+      </c>
+      <c r="E329">
+        <v>0</v>
+      </c>
+      <c r="H329">
+        <v>27</v>
+      </c>
+      <c r="I329">
+        <v>27</v>
+      </c>
+      <c r="J329">
+        <v>27</v>
+      </c>
+      <c r="L329" t="s">
+        <v>156</v>
+      </c>
+      <c r="M329" t="s">
+        <v>35</v>
+      </c>
+      <c r="N329">
+        <v>6.2</v>
+      </c>
+      <c r="O329">
+        <v>0</v>
+      </c>
+      <c r="P329">
+        <v>20</v>
+      </c>
+      <c r="Q329">
+        <v>0</v>
+      </c>
+      <c r="R329">
+        <v>0.04</v>
+      </c>
+      <c r="S329" t="s">
+        <v>161</v>
+      </c>
+      <c r="T329" t="s">
+        <v>162</v>
+      </c>
+      <c r="U329" s="1">
+        <v>1</v>
+      </c>
+      <c r="V329" s="1">
+        <v>1</v>
+      </c>
+      <c r="W329" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A330">
+        <v>53</v>
+      </c>
+      <c r="B330" t="s">
+        <v>149</v>
+      </c>
+      <c r="C330" t="s">
+        <v>150</v>
+      </c>
+      <c r="D330">
+        <v>0</v>
+      </c>
+      <c r="E330">
+        <v>0</v>
+      </c>
+      <c r="H330">
+        <v>27</v>
+      </c>
+      <c r="I330">
+        <v>27</v>
+      </c>
+      <c r="J330">
+        <v>27</v>
+      </c>
+      <c r="L330" t="s">
+        <v>157</v>
+      </c>
+      <c r="M330" t="s">
+        <v>35</v>
+      </c>
+      <c r="N330">
+        <v>7.2</v>
+      </c>
+      <c r="O330">
+        <v>0</v>
+      </c>
+      <c r="P330">
+        <v>20</v>
+      </c>
+      <c r="Q330">
+        <v>0</v>
+      </c>
+      <c r="R330">
+        <v>0.05</v>
+      </c>
+      <c r="S330" t="s">
+        <v>161</v>
+      </c>
+      <c r="T330" t="s">
+        <v>162</v>
+      </c>
+      <c r="U330" s="1">
+        <v>1</v>
+      </c>
+      <c r="V330" s="1">
+        <v>1</v>
+      </c>
+      <c r="W330" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="331" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A331">
+        <v>53</v>
+      </c>
+      <c r="B331" t="s">
+        <v>149</v>
+      </c>
+      <c r="C331" t="s">
+        <v>150</v>
+      </c>
+      <c r="D331">
+        <v>0</v>
+      </c>
+      <c r="E331">
+        <v>0</v>
+      </c>
+      <c r="H331">
+        <v>27</v>
+      </c>
+      <c r="I331">
+        <v>27</v>
+      </c>
+      <c r="J331">
+        <v>27</v>
+      </c>
+      <c r="L331" t="s">
+        <v>158</v>
+      </c>
+      <c r="M331" t="s">
+        <v>153</v>
+      </c>
+      <c r="N331">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O331">
+        <v>0</v>
+      </c>
+      <c r="P331">
+        <v>20</v>
+      </c>
+      <c r="Q331">
+        <v>0</v>
+      </c>
+      <c r="R331">
+        <v>0.03</v>
+      </c>
+      <c r="S331" t="s">
+        <v>161</v>
+      </c>
+      <c r="T331" t="s">
+        <v>162</v>
+      </c>
+      <c r="U331" s="1">
+        <v>1</v>
+      </c>
+      <c r="V331" s="1">
+        <v>1</v>
+      </c>
+      <c r="W331" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A332">
+        <v>53</v>
+      </c>
+      <c r="B332" t="s">
+        <v>149</v>
+      </c>
+      <c r="C332" t="s">
+        <v>150</v>
+      </c>
+      <c r="D332">
+        <v>0</v>
+      </c>
+      <c r="E332">
+        <v>0</v>
+      </c>
+      <c r="H332">
+        <v>27</v>
+      </c>
+      <c r="I332">
+        <v>27</v>
+      </c>
+      <c r="J332">
+        <v>27</v>
+      </c>
+      <c r="L332" t="s">
+        <v>159</v>
+      </c>
+      <c r="M332" t="s">
+        <v>143</v>
+      </c>
+      <c r="N332">
+        <v>0.43</v>
+      </c>
+      <c r="O332">
+        <v>0</v>
+      </c>
+      <c r="P332">
+        <v>20</v>
+      </c>
+      <c r="Q332">
+        <v>0</v>
+      </c>
+      <c r="R332">
+        <v>0.01</v>
+      </c>
+      <c r="S332" t="s">
+        <v>161</v>
+      </c>
+      <c r="T332" t="s">
+        <v>162</v>
+      </c>
+      <c r="U332" s="1">
+        <v>1</v>
+      </c>
+      <c r="V332" s="1">
+        <v>1</v>
+      </c>
+      <c r="W332" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="333" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A333">
+        <v>54</v>
+      </c>
+      <c r="B333" t="s">
+        <v>149</v>
+      </c>
+      <c r="C333" t="s">
+        <v>150</v>
+      </c>
+      <c r="D333">
+        <v>0</v>
+      </c>
+      <c r="E333">
+        <v>1</v>
+      </c>
+      <c r="F333">
+        <v>1</v>
+      </c>
+      <c r="H333">
+        <v>27</v>
+      </c>
+      <c r="I333">
+        <v>24</v>
+      </c>
+      <c r="J333">
+        <v>30</v>
+      </c>
+      <c r="K333">
+        <v>24</v>
+      </c>
+      <c r="L333" t="s">
+        <v>151</v>
+      </c>
+      <c r="M333" t="s">
+        <v>70</v>
+      </c>
+      <c r="N333">
+        <v>0.7</v>
+      </c>
+      <c r="O333">
+        <v>0</v>
+      </c>
+      <c r="P333">
+        <v>20</v>
+      </c>
+      <c r="Q333">
+        <v>0</v>
+      </c>
+      <c r="R333">
+        <v>0.01</v>
+      </c>
+      <c r="S333" t="s">
+        <v>161</v>
+      </c>
+      <c r="T333" t="s">
+        <v>162</v>
+      </c>
+      <c r="U333" s="1">
+        <v>1</v>
+      </c>
+      <c r="V333" s="1">
+        <v>1</v>
+      </c>
+      <c r="W333" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="334" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A334">
+        <v>54</v>
+      </c>
+      <c r="B334" t="s">
+        <v>149</v>
+      </c>
+      <c r="C334" t="s">
+        <v>150</v>
+      </c>
+      <c r="D334">
+        <v>0</v>
+      </c>
+      <c r="E334">
+        <v>1</v>
+      </c>
+      <c r="F334">
+        <v>1</v>
+      </c>
+      <c r="H334">
+        <v>27</v>
+      </c>
+      <c r="I334">
+        <v>24</v>
+      </c>
+      <c r="J334">
+        <v>30</v>
+      </c>
+      <c r="K334">
+        <v>24</v>
+      </c>
+      <c r="L334" t="s">
+        <v>152</v>
+      </c>
+      <c r="M334" t="s">
+        <v>35</v>
+      </c>
+      <c r="N334">
+        <v>30.7</v>
+      </c>
+      <c r="O334">
+        <v>0</v>
+      </c>
+      <c r="P334">
+        <v>20</v>
+      </c>
+      <c r="Q334">
+        <v>0</v>
+      </c>
+      <c r="R334">
+        <v>0.3</v>
+      </c>
+      <c r="S334" t="s">
+        <v>161</v>
+      </c>
+      <c r="T334" t="s">
+        <v>162</v>
+      </c>
+      <c r="U334" s="1">
+        <v>1</v>
+      </c>
+      <c r="V334" s="1">
+        <v>1</v>
+      </c>
+      <c r="W334" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="335" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A335">
+        <v>54</v>
+      </c>
+      <c r="B335" t="s">
+        <v>149</v>
+      </c>
+      <c r="C335" t="s">
+        <v>150</v>
+      </c>
+      <c r="D335">
+        <v>0</v>
+      </c>
+      <c r="E335">
+        <v>1</v>
+      </c>
+      <c r="F335">
+        <v>1</v>
+      </c>
+      <c r="H335">
+        <v>27</v>
+      </c>
+      <c r="I335">
+        <v>24</v>
+      </c>
+      <c r="J335">
+        <v>30</v>
+      </c>
+      <c r="K335">
+        <v>24</v>
+      </c>
+      <c r="L335" t="s">
+        <v>154</v>
+      </c>
+      <c r="M335" t="s">
+        <v>35</v>
+      </c>
+      <c r="N335">
+        <v>13.9</v>
+      </c>
+      <c r="O335">
+        <v>0</v>
+      </c>
+      <c r="P335">
+        <v>20</v>
+      </c>
+      <c r="Q335">
+        <v>0</v>
+      </c>
+      <c r="R335">
+        <v>0.2</v>
+      </c>
+      <c r="S335" t="s">
+        <v>161</v>
+      </c>
+      <c r="T335" t="s">
+        <v>162</v>
+      </c>
+      <c r="U335" s="1">
+        <v>1</v>
+      </c>
+      <c r="V335" s="1">
+        <v>1</v>
+      </c>
+      <c r="W335" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="336" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A336">
+        <v>54</v>
+      </c>
+      <c r="B336" t="s">
+        <v>149</v>
+      </c>
+      <c r="C336" t="s">
+        <v>150</v>
+      </c>
+      <c r="D336">
+        <v>0</v>
+      </c>
+      <c r="E336">
+        <v>1</v>
+      </c>
+      <c r="F336">
+        <v>1</v>
+      </c>
+      <c r="H336">
+        <v>27</v>
+      </c>
+      <c r="I336">
+        <v>24</v>
+      </c>
+      <c r="J336">
+        <v>30</v>
+      </c>
+      <c r="K336">
+        <v>24</v>
+      </c>
+      <c r="L336" t="s">
+        <v>72</v>
+      </c>
+      <c r="M336" t="s">
+        <v>35</v>
+      </c>
+      <c r="N336">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="O336">
+        <v>0</v>
+      </c>
+      <c r="P336">
+        <v>20</v>
+      </c>
+      <c r="Q336">
+        <v>0</v>
+      </c>
+      <c r="R336">
+        <v>0.5</v>
+      </c>
+      <c r="S336" t="s">
+        <v>161</v>
+      </c>
+      <c r="T336" t="s">
+        <v>162</v>
+      </c>
+      <c r="U336" s="1">
+        <v>1</v>
+      </c>
+      <c r="V336" s="1">
+        <v>1</v>
+      </c>
+      <c r="W336" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="337" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A337">
+        <v>54</v>
+      </c>
+      <c r="B337" t="s">
+        <v>149</v>
+      </c>
+      <c r="C337" t="s">
+        <v>150</v>
+      </c>
+      <c r="D337">
+        <v>0</v>
+      </c>
+      <c r="E337">
+        <v>1</v>
+      </c>
+      <c r="F337">
+        <v>1</v>
+      </c>
+      <c r="H337">
+        <v>27</v>
+      </c>
+      <c r="I337">
+        <v>24</v>
+      </c>
+      <c r="J337">
+        <v>30</v>
+      </c>
+      <c r="K337">
+        <v>24</v>
+      </c>
+      <c r="L337" t="s">
+        <v>155</v>
+      </c>
+      <c r="M337" t="s">
+        <v>35</v>
+      </c>
+      <c r="N337">
+        <v>7.2</v>
+      </c>
+      <c r="O337">
+        <v>0</v>
+      </c>
+      <c r="P337">
+        <v>20</v>
+      </c>
+      <c r="Q337">
+        <v>0</v>
+      </c>
+      <c r="R337">
+        <v>0.05</v>
+      </c>
+      <c r="S337" t="s">
+        <v>161</v>
+      </c>
+      <c r="T337" t="s">
+        <v>162</v>
+      </c>
+      <c r="U337" s="1">
+        <v>1</v>
+      </c>
+      <c r="V337" s="1">
+        <v>1</v>
+      </c>
+      <c r="W337" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A338">
+        <v>54</v>
+      </c>
+      <c r="B338" t="s">
+        <v>149</v>
+      </c>
+      <c r="C338" t="s">
+        <v>150</v>
+      </c>
+      <c r="D338">
+        <v>0</v>
+      </c>
+      <c r="E338">
+        <v>1</v>
+      </c>
+      <c r="F338">
+        <v>1</v>
+      </c>
+      <c r="H338">
+        <v>27</v>
+      </c>
+      <c r="I338">
+        <v>24</v>
+      </c>
+      <c r="J338">
+        <v>30</v>
+      </c>
+      <c r="K338">
+        <v>24</v>
+      </c>
+      <c r="L338" t="s">
+        <v>160</v>
+      </c>
+      <c r="M338" t="s">
+        <v>35</v>
+      </c>
+      <c r="N338">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="O338">
+        <v>0</v>
+      </c>
+      <c r="P338">
+        <v>20</v>
+      </c>
+      <c r="Q338">
+        <v>0</v>
+      </c>
+      <c r="R338">
+        <v>0.03</v>
+      </c>
+      <c r="S338" t="s">
+        <v>161</v>
+      </c>
+      <c r="T338" t="s">
+        <v>162</v>
+      </c>
+      <c r="U338" s="1">
+        <v>1</v>
+      </c>
+      <c r="V338" s="1">
+        <v>1</v>
+      </c>
+      <c r="W338" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="339" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A339">
+        <v>54</v>
+      </c>
+      <c r="B339" t="s">
+        <v>149</v>
+      </c>
+      <c r="C339" t="s">
+        <v>150</v>
+      </c>
+      <c r="D339">
+        <v>0</v>
+      </c>
+      <c r="E339">
+        <v>1</v>
+      </c>
+      <c r="F339">
+        <v>1</v>
+      </c>
+      <c r="H339">
+        <v>27</v>
+      </c>
+      <c r="I339">
+        <v>24</v>
+      </c>
+      <c r="J339">
+        <v>30</v>
+      </c>
+      <c r="K339">
+        <v>24</v>
+      </c>
+      <c r="L339" t="s">
+        <v>156</v>
+      </c>
+      <c r="M339" t="s">
+        <v>35</v>
+      </c>
+      <c r="N339">
+        <v>6.1</v>
+      </c>
+      <c r="O339">
+        <v>0</v>
+      </c>
+      <c r="P339">
+        <v>20</v>
+      </c>
+      <c r="Q339">
+        <v>0</v>
+      </c>
+      <c r="R339">
+        <v>0.06</v>
+      </c>
+      <c r="S339" t="s">
+        <v>161</v>
+      </c>
+      <c r="T339" t="s">
+        <v>162</v>
+      </c>
+      <c r="U339" s="1">
+        <v>1</v>
+      </c>
+      <c r="V339" s="1">
+        <v>1</v>
+      </c>
+      <c r="W339" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="340" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A340">
+        <v>54</v>
+      </c>
+      <c r="B340" t="s">
+        <v>149</v>
+      </c>
+      <c r="C340" t="s">
+        <v>150</v>
+      </c>
+      <c r="D340">
+        <v>0</v>
+      </c>
+      <c r="E340">
+        <v>1</v>
+      </c>
+      <c r="F340">
+        <v>1</v>
+      </c>
+      <c r="H340">
+        <v>27</v>
+      </c>
+      <c r="I340">
+        <v>24</v>
+      </c>
+      <c r="J340">
+        <v>30</v>
+      </c>
+      <c r="K340">
+        <v>24</v>
+      </c>
+      <c r="L340" t="s">
+        <v>157</v>
+      </c>
+      <c r="M340" t="s">
+        <v>35</v>
+      </c>
+      <c r="N340">
+        <v>7.1</v>
+      </c>
+      <c r="O340">
+        <v>0</v>
+      </c>
+      <c r="P340">
+        <v>20</v>
+      </c>
+      <c r="Q340">
+        <v>0</v>
+      </c>
+      <c r="R340">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S340" t="s">
+        <v>161</v>
+      </c>
+      <c r="T340" t="s">
+        <v>162</v>
+      </c>
+      <c r="U340" s="1">
+        <v>1</v>
+      </c>
+      <c r="V340" s="1">
+        <v>1</v>
+      </c>
+      <c r="W340" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A341">
+        <v>54</v>
+      </c>
+      <c r="B341" t="s">
+        <v>149</v>
+      </c>
+      <c r="C341" t="s">
+        <v>150</v>
+      </c>
+      <c r="D341">
+        <v>0</v>
+      </c>
+      <c r="E341">
+        <v>1</v>
+      </c>
+      <c r="F341">
+        <v>1</v>
+      </c>
+      <c r="H341">
+        <v>27</v>
+      </c>
+      <c r="I341">
+        <v>24</v>
+      </c>
+      <c r="J341">
+        <v>30</v>
+      </c>
+      <c r="K341">
+        <v>24</v>
+      </c>
+      <c r="L341" t="s">
+        <v>158</v>
+      </c>
+      <c r="M341" t="s">
+        <v>153</v>
+      </c>
+      <c r="N341">
+        <v>0.67</v>
+      </c>
+      <c r="O341">
+        <v>0</v>
+      </c>
+      <c r="P341">
+        <v>20</v>
+      </c>
+      <c r="Q341">
+        <v>0</v>
+      </c>
+      <c r="R341">
+        <v>0.08</v>
+      </c>
+      <c r="S341" t="s">
+        <v>161</v>
+      </c>
+      <c r="T341" t="s">
+        <v>162</v>
+      </c>
+      <c r="U341" s="1">
+        <v>1</v>
+      </c>
+      <c r="V341" s="1">
+        <v>1</v>
+      </c>
+      <c r="W341" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="342" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A342">
+        <v>54</v>
+      </c>
+      <c r="B342" t="s">
+        <v>149</v>
+      </c>
+      <c r="C342" t="s">
+        <v>150</v>
+      </c>
+      <c r="D342">
+        <v>0</v>
+      </c>
+      <c r="E342">
+        <v>1</v>
+      </c>
+      <c r="F342">
+        <v>1</v>
+      </c>
+      <c r="H342">
+        <v>27</v>
+      </c>
+      <c r="I342">
+        <v>24</v>
+      </c>
+      <c r="J342">
+        <v>30</v>
+      </c>
+      <c r="K342">
+        <v>24</v>
+      </c>
+      <c r="L342" t="s">
+        <v>159</v>
+      </c>
+      <c r="M342" t="s">
+        <v>143</v>
+      </c>
+      <c r="N342">
+        <v>0.43</v>
+      </c>
+      <c r="O342">
+        <v>0</v>
+      </c>
+      <c r="P342">
+        <v>20</v>
+      </c>
+      <c r="Q342">
+        <v>0</v>
+      </c>
+      <c r="R342">
+        <v>0.02</v>
+      </c>
+      <c r="S342" t="s">
+        <v>161</v>
+      </c>
+      <c r="T342" t="s">
+        <v>162</v>
+      </c>
+      <c r="U342" s="1">
+        <v>1</v>
+      </c>
+      <c r="V342" s="1">
+        <v>1</v>
+      </c>
+      <c r="W342" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="343" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A343">
+        <v>55</v>
+      </c>
+      <c r="B343" t="s">
+        <v>149</v>
+      </c>
+      <c r="C343" t="s">
+        <v>150</v>
+      </c>
+      <c r="D343">
+        <v>0</v>
+      </c>
+      <c r="E343">
+        <v>1</v>
+      </c>
+      <c r="F343">
+        <v>1</v>
+      </c>
+      <c r="H343">
+        <v>27</v>
+      </c>
+      <c r="I343">
+        <v>22</v>
+      </c>
+      <c r="J343">
+        <v>32</v>
+      </c>
+      <c r="K343">
+        <v>24</v>
+      </c>
+      <c r="L343" t="s">
+        <v>151</v>
+      </c>
+      <c r="M343" t="s">
+        <v>70</v>
+      </c>
+      <c r="N343">
+        <v>0.67</v>
+      </c>
+      <c r="O343">
+        <v>0</v>
+      </c>
+      <c r="P343">
+        <v>20</v>
+      </c>
+      <c r="Q343">
+        <v>0</v>
+      </c>
+      <c r="R343">
+        <v>0.01</v>
+      </c>
+      <c r="S343" t="s">
+        <v>161</v>
+      </c>
+      <c r="T343" t="s">
+        <v>162</v>
+      </c>
+      <c r="U343" s="1">
+        <v>1</v>
+      </c>
+      <c r="V343" s="1">
+        <v>1</v>
+      </c>
+      <c r="W343" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="344" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A344">
+        <v>55</v>
+      </c>
+      <c r="B344" t="s">
+        <v>149</v>
+      </c>
+      <c r="C344" t="s">
+        <v>150</v>
+      </c>
+      <c r="D344">
+        <v>0</v>
+      </c>
+      <c r="E344">
+        <v>1</v>
+      </c>
+      <c r="F344">
+        <v>1</v>
+      </c>
+      <c r="H344">
+        <v>27</v>
+      </c>
+      <c r="I344">
+        <v>22</v>
+      </c>
+      <c r="J344">
+        <v>32</v>
+      </c>
+      <c r="K344">
+        <v>24</v>
+      </c>
+      <c r="L344" t="s">
+        <v>152</v>
+      </c>
+      <c r="M344" t="s">
+        <v>35</v>
+      </c>
+      <c r="N344">
+        <v>30.8</v>
+      </c>
+      <c r="O344">
+        <v>0</v>
+      </c>
+      <c r="P344">
+        <v>20</v>
+      </c>
+      <c r="Q344">
+        <v>0</v>
+      </c>
+      <c r="R344">
+        <v>0.3</v>
+      </c>
+      <c r="S344" t="s">
+        <v>161</v>
+      </c>
+      <c r="T344" t="s">
+        <v>162</v>
+      </c>
+      <c r="U344" s="1">
+        <v>1</v>
+      </c>
+      <c r="V344" s="1">
+        <v>1</v>
+      </c>
+      <c r="W344" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A345">
+        <v>55</v>
+      </c>
+      <c r="B345" t="s">
+        <v>149</v>
+      </c>
+      <c r="C345" t="s">
+        <v>150</v>
+      </c>
+      <c r="D345">
+        <v>0</v>
+      </c>
+      <c r="E345">
+        <v>1</v>
+      </c>
+      <c r="F345">
+        <v>1</v>
+      </c>
+      <c r="H345">
+        <v>27</v>
+      </c>
+      <c r="I345">
+        <v>22</v>
+      </c>
+      <c r="J345">
+        <v>32</v>
+      </c>
+      <c r="K345">
+        <v>24</v>
+      </c>
+      <c r="L345" t="s">
+        <v>154</v>
+      </c>
+      <c r="M345" t="s">
+        <v>35</v>
+      </c>
+      <c r="N345">
+        <v>13.8</v>
+      </c>
+      <c r="O345">
+        <v>0</v>
+      </c>
+      <c r="P345">
+        <v>20</v>
+      </c>
+      <c r="Q345">
+        <v>0</v>
+      </c>
+      <c r="R345">
+        <v>0.2</v>
+      </c>
+      <c r="S345" t="s">
+        <v>161</v>
+      </c>
+      <c r="T345" t="s">
+        <v>162</v>
+      </c>
+      <c r="U345" s="1">
+        <v>1</v>
+      </c>
+      <c r="V345" s="1">
+        <v>1</v>
+      </c>
+      <c r="W345" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="346" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A346">
+        <v>55</v>
+      </c>
+      <c r="B346" t="s">
+        <v>149</v>
+      </c>
+      <c r="C346" t="s">
+        <v>150</v>
+      </c>
+      <c r="D346">
+        <v>0</v>
+      </c>
+      <c r="E346">
+        <v>1</v>
+      </c>
+      <c r="F346">
+        <v>1</v>
+      </c>
+      <c r="H346">
+        <v>27</v>
+      </c>
+      <c r="I346">
+        <v>22</v>
+      </c>
+      <c r="J346">
+        <v>32</v>
+      </c>
+      <c r="K346">
+        <v>24</v>
+      </c>
+      <c r="L346" t="s">
+        <v>72</v>
+      </c>
+      <c r="M346" t="s">
+        <v>35</v>
+      </c>
+      <c r="N346">
+        <v>36.9</v>
+      </c>
+      <c r="O346">
+        <v>0</v>
+      </c>
+      <c r="P346">
+        <v>20</v>
+      </c>
+      <c r="Q346">
+        <v>0</v>
+      </c>
+      <c r="R346">
+        <v>0.6</v>
+      </c>
+      <c r="S346" t="s">
+        <v>161</v>
+      </c>
+      <c r="T346" t="s">
+        <v>162</v>
+      </c>
+      <c r="U346" s="1">
+        <v>1</v>
+      </c>
+      <c r="V346" s="1">
+        <v>1</v>
+      </c>
+      <c r="W346" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="347" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A347">
+        <v>55</v>
+      </c>
+      <c r="B347" t="s">
+        <v>149</v>
+      </c>
+      <c r="C347" t="s">
+        <v>150</v>
+      </c>
+      <c r="D347">
+        <v>0</v>
+      </c>
+      <c r="E347">
+        <v>1</v>
+      </c>
+      <c r="F347">
+        <v>1</v>
+      </c>
+      <c r="H347">
+        <v>27</v>
+      </c>
+      <c r="I347">
+        <v>22</v>
+      </c>
+      <c r="J347">
+        <v>32</v>
+      </c>
+      <c r="K347">
+        <v>24</v>
+      </c>
+      <c r="L347" t="s">
+        <v>155</v>
+      </c>
+      <c r="M347" t="s">
+        <v>35</v>
+      </c>
+      <c r="N347">
+        <v>7.1</v>
+      </c>
+      <c r="O347">
+        <v>0</v>
+      </c>
+      <c r="P347">
+        <v>20</v>
+      </c>
+      <c r="Q347">
+        <v>0</v>
+      </c>
+      <c r="R347">
+        <v>0.05</v>
+      </c>
+      <c r="S347" t="s">
+        <v>161</v>
+      </c>
+      <c r="T347" t="s">
+        <v>162</v>
+      </c>
+      <c r="U347" s="1">
+        <v>1</v>
+      </c>
+      <c r="V347" s="1">
+        <v>1</v>
+      </c>
+      <c r="W347" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="348" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A348">
+        <v>55</v>
+      </c>
+      <c r="B348" t="s">
+        <v>149</v>
+      </c>
+      <c r="C348" t="s">
+        <v>150</v>
+      </c>
+      <c r="D348">
+        <v>0</v>
+      </c>
+      <c r="E348">
+        <v>1</v>
+      </c>
+      <c r="F348">
+        <v>1</v>
+      </c>
+      <c r="H348">
+        <v>27</v>
+      </c>
+      <c r="I348">
+        <v>22</v>
+      </c>
+      <c r="J348">
+        <v>32</v>
+      </c>
+      <c r="K348">
+        <v>24</v>
+      </c>
+      <c r="L348" t="s">
+        <v>160</v>
+      </c>
+      <c r="M348" t="s">
+        <v>35</v>
+      </c>
+      <c r="N348">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="O348">
+        <v>0</v>
+      </c>
+      <c r="P348">
+        <v>20</v>
+      </c>
+      <c r="Q348">
+        <v>0</v>
+      </c>
+      <c r="R348">
+        <v>0.04</v>
+      </c>
+      <c r="S348" t="s">
+        <v>161</v>
+      </c>
+      <c r="T348" t="s">
+        <v>162</v>
+      </c>
+      <c r="U348" s="1">
+        <v>1</v>
+      </c>
+      <c r="V348" s="1">
+        <v>1</v>
+      </c>
+      <c r="W348" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="349" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A349">
+        <v>55</v>
+      </c>
+      <c r="B349" t="s">
+        <v>149</v>
+      </c>
+      <c r="C349" t="s">
+        <v>150</v>
+      </c>
+      <c r="D349">
+        <v>0</v>
+      </c>
+      <c r="E349">
+        <v>1</v>
+      </c>
+      <c r="F349">
+        <v>1</v>
+      </c>
+      <c r="H349">
+        <v>27</v>
+      </c>
+      <c r="I349">
+        <v>22</v>
+      </c>
+      <c r="J349">
+        <v>32</v>
+      </c>
+      <c r="K349">
+        <v>24</v>
+      </c>
+      <c r="L349" t="s">
+        <v>156</v>
+      </c>
+      <c r="M349" t="s">
+        <v>35</v>
+      </c>
+      <c r="N349">
+        <v>6</v>
+      </c>
+      <c r="O349">
+        <v>0</v>
+      </c>
+      <c r="P349">
+        <v>20</v>
+      </c>
+      <c r="Q349">
+        <v>0</v>
+      </c>
+      <c r="R349">
+        <v>0.06</v>
+      </c>
+      <c r="S349" t="s">
+        <v>161</v>
+      </c>
+      <c r="T349" t="s">
+        <v>162</v>
+      </c>
+      <c r="U349" s="1">
+        <v>1</v>
+      </c>
+      <c r="V349" s="1">
+        <v>1</v>
+      </c>
+      <c r="W349" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="350" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A350">
+        <v>55</v>
+      </c>
+      <c r="B350" t="s">
+        <v>149</v>
+      </c>
+      <c r="C350" t="s">
+        <v>150</v>
+      </c>
+      <c r="D350">
+        <v>0</v>
+      </c>
+      <c r="E350">
+        <v>1</v>
+      </c>
+      <c r="F350">
+        <v>1</v>
+      </c>
+      <c r="H350">
+        <v>27</v>
+      </c>
+      <c r="I350">
+        <v>22</v>
+      </c>
+      <c r="J350">
+        <v>32</v>
+      </c>
+      <c r="K350">
+        <v>24</v>
+      </c>
+      <c r="L350" t="s">
+        <v>157</v>
+      </c>
+      <c r="M350" t="s">
+        <v>35</v>
+      </c>
+      <c r="N350">
+        <v>7.1</v>
+      </c>
+      <c r="O350">
+        <v>0</v>
+      </c>
+      <c r="P350">
+        <v>20</v>
+      </c>
+      <c r="Q350">
+        <v>0</v>
+      </c>
+      <c r="R350">
+        <v>0.06</v>
+      </c>
+      <c r="S350" t="s">
+        <v>161</v>
+      </c>
+      <c r="T350" t="s">
+        <v>162</v>
+      </c>
+      <c r="U350" s="1">
+        <v>1</v>
+      </c>
+      <c r="V350" s="1">
+        <v>1</v>
+      </c>
+      <c r="W350" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A351">
+        <v>55</v>
+      </c>
+      <c r="B351" t="s">
+        <v>149</v>
+      </c>
+      <c r="C351" t="s">
+        <v>150</v>
+      </c>
+      <c r="D351">
+        <v>0</v>
+      </c>
+      <c r="E351">
+        <v>1</v>
+      </c>
+      <c r="F351">
+        <v>1</v>
+      </c>
+      <c r="H351">
+        <v>27</v>
+      </c>
+      <c r="I351">
+        <v>22</v>
+      </c>
+      <c r="J351">
+        <v>32</v>
+      </c>
+      <c r="K351">
+        <v>24</v>
+      </c>
+      <c r="L351" t="s">
+        <v>158</v>
+      </c>
+      <c r="M351" t="s">
+        <v>153</v>
+      </c>
+      <c r="N351">
+        <v>0.67</v>
+      </c>
+      <c r="O351">
+        <v>0</v>
+      </c>
+      <c r="P351">
+        <v>20</v>
+      </c>
+      <c r="Q351">
+        <v>0</v>
+      </c>
+      <c r="R351">
+        <v>0.06</v>
+      </c>
+      <c r="S351" t="s">
+        <v>161</v>
+      </c>
+      <c r="T351" t="s">
+        <v>162</v>
+      </c>
+      <c r="U351" s="1">
+        <v>1</v>
+      </c>
+      <c r="V351" s="1">
+        <v>1</v>
+      </c>
+      <c r="W351" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="352" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A352">
+        <v>55</v>
+      </c>
+      <c r="B352" t="s">
+        <v>149</v>
+      </c>
+      <c r="C352" t="s">
+        <v>150</v>
+      </c>
+      <c r="D352">
+        <v>0</v>
+      </c>
+      <c r="E352">
+        <v>1</v>
+      </c>
+      <c r="F352">
+        <v>1</v>
+      </c>
+      <c r="H352">
+        <v>27</v>
+      </c>
+      <c r="I352">
+        <v>22</v>
+      </c>
+      <c r="J352">
+        <v>32</v>
+      </c>
+      <c r="K352">
+        <v>24</v>
+      </c>
+      <c r="L352" t="s">
+        <v>159</v>
+      </c>
+      <c r="M352" t="s">
+        <v>143</v>
+      </c>
+      <c r="N352">
+        <v>0.46</v>
+      </c>
+      <c r="O352">
+        <v>0</v>
+      </c>
+      <c r="P352">
+        <v>20</v>
+      </c>
+      <c r="Q352">
+        <v>0</v>
+      </c>
+      <c r="R352">
+        <v>0.03</v>
+      </c>
+      <c r="S352" t="s">
+        <v>161</v>
+      </c>
+      <c r="T352" t="s">
+        <v>162</v>
+      </c>
+      <c r="U352" s="1">
+        <v>1</v>
+      </c>
+      <c r="V352" s="1">
+        <v>1</v>
+      </c>
+      <c r="W352" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="353" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A353">
+        <v>56</v>
+      </c>
+      <c r="B353" t="s">
+        <v>149</v>
+      </c>
+      <c r="C353" t="s">
+        <v>150</v>
+      </c>
+      <c r="D353">
+        <v>0</v>
+      </c>
+      <c r="E353">
+        <v>2</v>
+      </c>
+      <c r="H353">
+        <v>27</v>
+      </c>
+      <c r="I353">
+        <v>26.2</v>
+      </c>
+      <c r="J353">
+        <v>28.3</v>
+      </c>
+      <c r="L353" t="s">
+        <v>151</v>
+      </c>
+      <c r="M353" t="s">
+        <v>70</v>
+      </c>
+      <c r="N353">
+        <v>0.67</v>
+      </c>
+      <c r="O353">
+        <v>0</v>
+      </c>
+      <c r="P353">
+        <v>20</v>
+      </c>
+      <c r="Q353">
+        <v>0</v>
+      </c>
+      <c r="R353">
+        <v>0.01</v>
+      </c>
+      <c r="S353" t="s">
+        <v>161</v>
+      </c>
+      <c r="T353" t="s">
+        <v>162</v>
+      </c>
+      <c r="U353" s="1">
+        <v>1</v>
+      </c>
+      <c r="V353" s="1">
+        <v>1</v>
+      </c>
+      <c r="W353" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="354" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A354">
+        <v>56</v>
+      </c>
+      <c r="B354" t="s">
+        <v>149</v>
+      </c>
+      <c r="C354" t="s">
+        <v>150</v>
+      </c>
+      <c r="D354">
+        <v>0</v>
+      </c>
+      <c r="E354">
+        <v>2</v>
+      </c>
+      <c r="H354">
+        <v>27</v>
+      </c>
+      <c r="I354">
+        <v>26.2</v>
+      </c>
+      <c r="J354">
+        <v>28.3</v>
+      </c>
+      <c r="L354" t="s">
+        <v>152</v>
+      </c>
+      <c r="M354" t="s">
+        <v>35</v>
+      </c>
+      <c r="N354">
+        <v>30.8</v>
+      </c>
+      <c r="O354">
+        <v>0</v>
+      </c>
+      <c r="P354">
+        <v>20</v>
+      </c>
+      <c r="Q354">
+        <v>0</v>
+      </c>
+      <c r="R354">
+        <v>0.2</v>
+      </c>
+      <c r="S354" t="s">
+        <v>161</v>
+      </c>
+      <c r="T354" t="s">
+        <v>162</v>
+      </c>
+      <c r="U354" s="1">
+        <v>1</v>
+      </c>
+      <c r="V354" s="1">
+        <v>1</v>
+      </c>
+      <c r="W354" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="355" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A355">
+        <v>56</v>
+      </c>
+      <c r="B355" t="s">
+        <v>149</v>
+      </c>
+      <c r="C355" t="s">
+        <v>150</v>
+      </c>
+      <c r="D355">
+        <v>0</v>
+      </c>
+      <c r="E355">
+        <v>2</v>
+      </c>
+      <c r="H355">
+        <v>27</v>
+      </c>
+      <c r="I355">
+        <v>26.2</v>
+      </c>
+      <c r="J355">
+        <v>28.3</v>
+      </c>
+      <c r="L355" t="s">
+        <v>154</v>
+      </c>
+      <c r="M355" t="s">
+        <v>35</v>
+      </c>
+      <c r="N355">
+        <v>14.1</v>
+      </c>
+      <c r="O355">
+        <v>0</v>
+      </c>
+      <c r="P355">
+        <v>20</v>
+      </c>
+      <c r="Q355">
+        <v>0</v>
+      </c>
+      <c r="R355">
+        <v>0.1</v>
+      </c>
+      <c r="S355" t="s">
+        <v>161</v>
+      </c>
+      <c r="T355" t="s">
+        <v>162</v>
+      </c>
+      <c r="U355" s="1">
+        <v>1</v>
+      </c>
+      <c r="V355" s="1">
+        <v>1</v>
+      </c>
+      <c r="W355" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="356" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A356">
+        <v>56</v>
+      </c>
+      <c r="B356" t="s">
+        <v>149</v>
+      </c>
+      <c r="C356" t="s">
+        <v>150</v>
+      </c>
+      <c r="D356">
+        <v>0</v>
+      </c>
+      <c r="E356">
+        <v>2</v>
+      </c>
+      <c r="H356">
+        <v>27</v>
+      </c>
+      <c r="I356">
+        <v>26.2</v>
+      </c>
+      <c r="J356">
+        <v>28.3</v>
+      </c>
+      <c r="L356" t="s">
+        <v>72</v>
+      </c>
+      <c r="M356" t="s">
+        <v>35</v>
+      </c>
+      <c r="N356">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="O356">
+        <v>0</v>
+      </c>
+      <c r="P356">
+        <v>20</v>
+      </c>
+      <c r="Q356">
+        <v>0</v>
+      </c>
+      <c r="R356">
+        <v>0.5</v>
+      </c>
+      <c r="S356" t="s">
+        <v>161</v>
+      </c>
+      <c r="T356" t="s">
+        <v>162</v>
+      </c>
+      <c r="U356" s="1">
+        <v>1</v>
+      </c>
+      <c r="V356" s="1">
+        <v>1</v>
+      </c>
+      <c r="W356" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="357" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A357">
+        <v>56</v>
+      </c>
+      <c r="B357" t="s">
+        <v>149</v>
+      </c>
+      <c r="C357" t="s">
+        <v>150</v>
+      </c>
+      <c r="D357">
+        <v>0</v>
+      </c>
+      <c r="E357">
+        <v>2</v>
+      </c>
+      <c r="H357">
+        <v>27</v>
+      </c>
+      <c r="I357">
+        <v>26.2</v>
+      </c>
+      <c r="J357">
+        <v>28.3</v>
+      </c>
+      <c r="L357" t="s">
+        <v>155</v>
+      </c>
+      <c r="M357" t="s">
+        <v>35</v>
+      </c>
+      <c r="N357">
+        <v>7.1</v>
+      </c>
+      <c r="O357">
+        <v>0</v>
+      </c>
+      <c r="P357">
+        <v>20</v>
+      </c>
+      <c r="Q357">
+        <v>0</v>
+      </c>
+      <c r="R357">
+        <v>0.03</v>
+      </c>
+      <c r="S357" t="s">
+        <v>161</v>
+      </c>
+      <c r="T357" t="s">
+        <v>162</v>
+      </c>
+      <c r="U357" s="1">
+        <v>1</v>
+      </c>
+      <c r="V357" s="1">
+        <v>1</v>
+      </c>
+      <c r="W357" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="358" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A358">
+        <v>56</v>
+      </c>
+      <c r="B358" t="s">
+        <v>149</v>
+      </c>
+      <c r="C358" t="s">
+        <v>150</v>
+      </c>
+      <c r="D358">
+        <v>0</v>
+      </c>
+      <c r="E358">
+        <v>2</v>
+      </c>
+      <c r="H358">
+        <v>27</v>
+      </c>
+      <c r="I358">
+        <v>26.2</v>
+      </c>
+      <c r="J358">
+        <v>28.3</v>
+      </c>
+      <c r="L358" t="s">
+        <v>160</v>
+      </c>
+      <c r="M358" t="s">
+        <v>35</v>
+      </c>
+      <c r="N358">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="O358">
+        <v>0</v>
+      </c>
+      <c r="P358">
+        <v>20</v>
+      </c>
+      <c r="Q358">
+        <v>0</v>
+      </c>
+      <c r="R358">
+        <v>0.03</v>
+      </c>
+      <c r="S358" t="s">
+        <v>161</v>
+      </c>
+      <c r="T358" t="s">
+        <v>162</v>
+      </c>
+      <c r="U358" s="1">
+        <v>1</v>
+      </c>
+      <c r="V358" s="1">
+        <v>1</v>
+      </c>
+      <c r="W358" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="359" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A359">
+        <v>56</v>
+      </c>
+      <c r="B359" t="s">
+        <v>149</v>
+      </c>
+      <c r="C359" t="s">
+        <v>150</v>
+      </c>
+      <c r="D359">
+        <v>0</v>
+      </c>
+      <c r="E359">
+        <v>2</v>
+      </c>
+      <c r="H359">
+        <v>27</v>
+      </c>
+      <c r="I359">
+        <v>26.2</v>
+      </c>
+      <c r="J359">
+        <v>28.3</v>
+      </c>
+      <c r="L359" t="s">
+        <v>156</v>
+      </c>
+      <c r="M359" t="s">
+        <v>35</v>
+      </c>
+      <c r="N359">
+        <v>6.1</v>
+      </c>
+      <c r="O359">
+        <v>0</v>
+      </c>
+      <c r="P359">
+        <v>20</v>
+      </c>
+      <c r="Q359">
+        <v>0</v>
+      </c>
+      <c r="R359">
+        <v>0.05</v>
+      </c>
+      <c r="S359" t="s">
+        <v>161</v>
+      </c>
+      <c r="T359" t="s">
+        <v>162</v>
+      </c>
+      <c r="U359" s="1">
+        <v>1</v>
+      </c>
+      <c r="V359" s="1">
+        <v>1</v>
+      </c>
+      <c r="W359" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="360" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A360">
+        <v>56</v>
+      </c>
+      <c r="B360" t="s">
+        <v>149</v>
+      </c>
+      <c r="C360" t="s">
+        <v>150</v>
+      </c>
+      <c r="D360">
+        <v>0</v>
+      </c>
+      <c r="E360">
+        <v>2</v>
+      </c>
+      <c r="H360">
+        <v>27</v>
+      </c>
+      <c r="I360">
+        <v>26.2</v>
+      </c>
+      <c r="J360">
+        <v>28.3</v>
+      </c>
+      <c r="L360" t="s">
+        <v>157</v>
+      </c>
+      <c r="M360" t="s">
+        <v>35</v>
+      </c>
+      <c r="N360">
+        <v>7.2</v>
+      </c>
+      <c r="O360">
+        <v>0</v>
+      </c>
+      <c r="P360">
+        <v>20</v>
+      </c>
+      <c r="Q360">
+        <v>0</v>
+      </c>
+      <c r="R360">
+        <v>0.05</v>
+      </c>
+      <c r="S360" t="s">
+        <v>161</v>
+      </c>
+      <c r="T360" t="s">
+        <v>162</v>
+      </c>
+      <c r="U360" s="1">
+        <v>1</v>
+      </c>
+      <c r="V360" s="1">
+        <v>1</v>
+      </c>
+      <c r="W360" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="361" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A361">
+        <v>56</v>
+      </c>
+      <c r="B361" t="s">
+        <v>149</v>
+      </c>
+      <c r="C361" t="s">
+        <v>150</v>
+      </c>
+      <c r="D361">
+        <v>0</v>
+      </c>
+      <c r="E361">
+        <v>2</v>
+      </c>
+      <c r="H361">
+        <v>27</v>
+      </c>
+      <c r="I361">
+        <v>26.2</v>
+      </c>
+      <c r="J361">
+        <v>28.3</v>
+      </c>
+      <c r="L361" t="s">
+        <v>158</v>
+      </c>
+      <c r="M361" t="s">
+        <v>153</v>
+      </c>
+      <c r="N361">
+        <v>0.67</v>
+      </c>
+      <c r="O361">
+        <v>0</v>
+      </c>
+      <c r="P361">
+        <v>20</v>
+      </c>
+      <c r="Q361">
+        <v>0</v>
+      </c>
+      <c r="R361">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S361" t="s">
+        <v>161</v>
+      </c>
+      <c r="T361" t="s">
+        <v>162</v>
+      </c>
+      <c r="U361" s="1">
+        <v>1</v>
+      </c>
+      <c r="V361" s="1">
+        <v>1</v>
+      </c>
+      <c r="W361" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="362" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A362">
+        <v>56</v>
+      </c>
+      <c r="B362" t="s">
+        <v>149</v>
+      </c>
+      <c r="C362" t="s">
+        <v>150</v>
+      </c>
+      <c r="D362">
+        <v>0</v>
+      </c>
+      <c r="E362">
+        <v>2</v>
+      </c>
+      <c r="H362">
+        <v>27</v>
+      </c>
+      <c r="I362">
+        <v>26.2</v>
+      </c>
+      <c r="J362">
+        <v>28.3</v>
+      </c>
+      <c r="L362" t="s">
+        <v>159</v>
+      </c>
+      <c r="M362" t="s">
+        <v>143</v>
+      </c>
+      <c r="N362">
+        <v>0.44</v>
+      </c>
+      <c r="O362">
+        <v>0</v>
+      </c>
+      <c r="P362">
+        <v>20</v>
+      </c>
+      <c r="Q362">
+        <v>0</v>
+      </c>
+      <c r="R362">
+        <v>0.02</v>
+      </c>
+      <c r="S362" t="s">
+        <v>161</v>
+      </c>
+      <c r="T362" t="s">
+        <v>162</v>
+      </c>
+      <c r="U362" s="1">
+        <v>1</v>
+      </c>
+      <c r="V362" s="1">
+        <v>1</v>
+      </c>
+      <c r="W362" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="363" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A363">
+        <v>57</v>
+      </c>
+      <c r="B363" t="s">
+        <v>149</v>
+      </c>
+      <c r="C363" t="s">
+        <v>150</v>
+      </c>
+      <c r="D363">
+        <v>0</v>
+      </c>
+      <c r="E363">
+        <v>2</v>
+      </c>
+      <c r="H363">
+        <v>26.1</v>
+      </c>
+      <c r="I363">
+        <v>24.7</v>
+      </c>
+      <c r="J363">
+        <v>28.2</v>
+      </c>
+      <c r="L363" t="s">
+        <v>151</v>
+      </c>
+      <c r="M363" t="s">
+        <v>70</v>
+      </c>
+      <c r="N363">
+        <v>0.69</v>
+      </c>
+      <c r="O363">
+        <v>0</v>
+      </c>
+      <c r="P363">
+        <v>20</v>
+      </c>
+      <c r="Q363">
+        <v>0</v>
+      </c>
+      <c r="R363">
+        <v>0.01</v>
+      </c>
+      <c r="S363" t="s">
+        <v>161</v>
+      </c>
+      <c r="T363" t="s">
+        <v>162</v>
+      </c>
+      <c r="U363" s="1">
+        <v>1</v>
+      </c>
+      <c r="V363" s="1">
+        <v>1</v>
+      </c>
+      <c r="W363" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="364" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A364">
+        <v>57</v>
+      </c>
+      <c r="B364" t="s">
+        <v>149</v>
+      </c>
+      <c r="C364" t="s">
+        <v>150</v>
+      </c>
+      <c r="D364">
+        <v>0</v>
+      </c>
+      <c r="E364">
+        <v>2</v>
+      </c>
+      <c r="H364">
+        <v>26.1</v>
+      </c>
+      <c r="I364">
+        <v>24.7</v>
+      </c>
+      <c r="J364">
+        <v>28.2</v>
+      </c>
+      <c r="L364" t="s">
+        <v>152</v>
+      </c>
+      <c r="M364" t="s">
+        <v>35</v>
+      </c>
+      <c r="N364">
+        <v>30.9</v>
+      </c>
+      <c r="O364">
+        <v>0</v>
+      </c>
+      <c r="P364">
+        <v>20</v>
+      </c>
+      <c r="Q364">
+        <v>0</v>
+      </c>
+      <c r="R364">
+        <v>0.2</v>
+      </c>
+      <c r="S364" t="s">
+        <v>161</v>
+      </c>
+      <c r="T364" t="s">
+        <v>162</v>
+      </c>
+      <c r="U364" s="1">
+        <v>1</v>
+      </c>
+      <c r="V364" s="1">
+        <v>1</v>
+      </c>
+      <c r="W364" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="365" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A365">
+        <v>57</v>
+      </c>
+      <c r="B365" t="s">
+        <v>149</v>
+      </c>
+      <c r="C365" t="s">
+        <v>150</v>
+      </c>
+      <c r="D365">
+        <v>0</v>
+      </c>
+      <c r="E365">
+        <v>2</v>
+      </c>
+      <c r="H365">
+        <v>26.1</v>
+      </c>
+      <c r="I365">
+        <v>24.7</v>
+      </c>
+      <c r="J365">
+        <v>28.2</v>
+      </c>
+      <c r="L365" t="s">
+        <v>154</v>
+      </c>
+      <c r="M365" t="s">
+        <v>35</v>
+      </c>
+      <c r="N365">
+        <v>13.9</v>
+      </c>
+      <c r="O365">
+        <v>0</v>
+      </c>
+      <c r="P365">
+        <v>20</v>
+      </c>
+      <c r="Q365">
+        <v>0</v>
+      </c>
+      <c r="R365">
+        <v>0.1</v>
+      </c>
+      <c r="S365" t="s">
+        <v>161</v>
+      </c>
+      <c r="T365" t="s">
+        <v>162</v>
+      </c>
+      <c r="U365" s="1">
+        <v>1</v>
+      </c>
+      <c r="V365" s="1">
+        <v>1</v>
+      </c>
+      <c r="W365" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="366" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A366">
+        <v>57</v>
+      </c>
+      <c r="B366" t="s">
+        <v>149</v>
+      </c>
+      <c r="C366" t="s">
+        <v>150</v>
+      </c>
+      <c r="D366">
+        <v>0</v>
+      </c>
+      <c r="E366">
+        <v>2</v>
+      </c>
+      <c r="H366">
+        <v>26.1</v>
+      </c>
+      <c r="I366">
+        <v>24.7</v>
+      </c>
+      <c r="J366">
+        <v>28.2</v>
+      </c>
+      <c r="L366" t="s">
+        <v>72</v>
+      </c>
+      <c r="M366" t="s">
+        <v>35</v>
+      </c>
+      <c r="N366">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="O366">
+        <v>0</v>
+      </c>
+      <c r="P366">
+        <v>20</v>
+      </c>
+      <c r="Q366">
+        <v>0</v>
+      </c>
+      <c r="R366">
+        <v>0.5</v>
+      </c>
+      <c r="S366" t="s">
+        <v>161</v>
+      </c>
+      <c r="T366" t="s">
+        <v>162</v>
+      </c>
+      <c r="U366" s="1">
+        <v>1</v>
+      </c>
+      <c r="V366" s="1">
+        <v>1</v>
+      </c>
+      <c r="W366" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="367" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A367">
+        <v>57</v>
+      </c>
+      <c r="B367" t="s">
+        <v>149</v>
+      </c>
+      <c r="C367" t="s">
+        <v>150</v>
+      </c>
+      <c r="D367">
+        <v>0</v>
+      </c>
+      <c r="E367">
+        <v>2</v>
+      </c>
+      <c r="H367">
+        <v>26.1</v>
+      </c>
+      <c r="I367">
+        <v>24.7</v>
+      </c>
+      <c r="J367">
+        <v>28.2</v>
+      </c>
+      <c r="L367" t="s">
+        <v>155</v>
+      </c>
+      <c r="M367" t="s">
+        <v>35</v>
+      </c>
+      <c r="N367">
+        <v>7.2</v>
+      </c>
+      <c r="O367">
+        <v>0</v>
+      </c>
+      <c r="P367">
+        <v>20</v>
+      </c>
+      <c r="Q367">
+        <v>0</v>
+      </c>
+      <c r="R367">
+        <v>0.02</v>
+      </c>
+      <c r="S367" t="s">
+        <v>161</v>
+      </c>
+      <c r="T367" t="s">
+        <v>162</v>
+      </c>
+      <c r="U367" s="1">
+        <v>1</v>
+      </c>
+      <c r="V367" s="1">
+        <v>1</v>
+      </c>
+      <c r="W367" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="368" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A368">
+        <v>57</v>
+      </c>
+      <c r="B368" t="s">
+        <v>149</v>
+      </c>
+      <c r="C368" t="s">
+        <v>150</v>
+      </c>
+      <c r="D368">
+        <v>0</v>
+      </c>
+      <c r="E368">
+        <v>2</v>
+      </c>
+      <c r="H368">
+        <v>26.1</v>
+      </c>
+      <c r="I368">
+        <v>24.7</v>
+      </c>
+      <c r="J368">
+        <v>28.2</v>
+      </c>
+      <c r="L368" t="s">
+        <v>160</v>
+      </c>
+      <c r="M368" t="s">
+        <v>35</v>
+      </c>
+      <c r="N368">
+        <v>5.2</v>
+      </c>
+      <c r="O368">
+        <v>0</v>
+      </c>
+      <c r="P368">
+        <v>20</v>
+      </c>
+      <c r="Q368">
+        <v>0</v>
+      </c>
+      <c r="R368">
+        <v>0.02</v>
+      </c>
+      <c r="S368" t="s">
+        <v>161</v>
+      </c>
+      <c r="T368" t="s">
+        <v>162</v>
+      </c>
+      <c r="U368" s="1">
+        <v>1</v>
+      </c>
+      <c r="V368" s="1">
+        <v>1</v>
+      </c>
+      <c r="W368" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="369" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A369">
+        <v>57</v>
+      </c>
+      <c r="B369" t="s">
+        <v>149</v>
+      </c>
+      <c r="C369" t="s">
+        <v>150</v>
+      </c>
+      <c r="D369">
+        <v>0</v>
+      </c>
+      <c r="E369">
+        <v>2</v>
+      </c>
+      <c r="H369">
+        <v>26.1</v>
+      </c>
+      <c r="I369">
+        <v>24.7</v>
+      </c>
+      <c r="J369">
+        <v>28.2</v>
+      </c>
+      <c r="L369" t="s">
+        <v>156</v>
+      </c>
+      <c r="M369" t="s">
+        <v>35</v>
+      </c>
+      <c r="N369">
+        <v>6.1</v>
+      </c>
+      <c r="O369">
+        <v>0</v>
+      </c>
+      <c r="P369">
+        <v>20</v>
+      </c>
+      <c r="Q369">
+        <v>0</v>
+      </c>
+      <c r="R369">
+        <v>0.04</v>
+      </c>
+      <c r="S369" t="s">
+        <v>161</v>
+      </c>
+      <c r="T369" t="s">
+        <v>162</v>
+      </c>
+      <c r="U369" s="1">
+        <v>1</v>
+      </c>
+      <c r="V369" s="1">
+        <v>1</v>
+      </c>
+      <c r="W369" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="370" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A370">
+        <v>57</v>
+      </c>
+      <c r="B370" t="s">
+        <v>149</v>
+      </c>
+      <c r="C370" t="s">
+        <v>150</v>
+      </c>
+      <c r="D370">
+        <v>0</v>
+      </c>
+      <c r="E370">
+        <v>2</v>
+      </c>
+      <c r="H370">
+        <v>26.1</v>
+      </c>
+      <c r="I370">
+        <v>24.7</v>
+      </c>
+      <c r="J370">
+        <v>28.2</v>
+      </c>
+      <c r="L370" t="s">
+        <v>157</v>
+      </c>
+      <c r="M370" t="s">
+        <v>35</v>
+      </c>
+      <c r="N370">
+        <v>7.2</v>
+      </c>
+      <c r="O370">
+        <v>0</v>
+      </c>
+      <c r="P370">
+        <v>20</v>
+      </c>
+      <c r="Q370">
+        <v>0</v>
+      </c>
+      <c r="R370">
+        <v>0.04</v>
+      </c>
+      <c r="S370" t="s">
+        <v>161</v>
+      </c>
+      <c r="T370" t="s">
+        <v>162</v>
+      </c>
+      <c r="U370" s="1">
+        <v>1</v>
+      </c>
+      <c r="V370" s="1">
+        <v>1</v>
+      </c>
+      <c r="W370" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="371" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A371">
+        <v>57</v>
+      </c>
+      <c r="B371" t="s">
+        <v>149</v>
+      </c>
+      <c r="C371" t="s">
+        <v>150</v>
+      </c>
+      <c r="D371">
+        <v>0</v>
+      </c>
+      <c r="E371">
+        <v>2</v>
+      </c>
+      <c r="H371">
+        <v>26.1</v>
+      </c>
+      <c r="I371">
+        <v>24.7</v>
+      </c>
+      <c r="J371">
+        <v>28.2</v>
+      </c>
+      <c r="L371" t="s">
+        <v>158</v>
+      </c>
+      <c r="M371" t="s">
+        <v>153</v>
+      </c>
+      <c r="N371">
+        <v>0.64</v>
+      </c>
+      <c r="O371">
+        <v>0</v>
+      </c>
+      <c r="P371">
+        <v>20</v>
+      </c>
+      <c r="Q371">
+        <v>0</v>
+      </c>
+      <c r="R371">
+        <v>0.04</v>
+      </c>
+      <c r="S371" t="s">
+        <v>161</v>
+      </c>
+      <c r="T371" t="s">
+        <v>162</v>
+      </c>
+      <c r="U371" s="1">
+        <v>1</v>
+      </c>
+      <c r="V371" s="1">
+        <v>1</v>
+      </c>
+      <c r="W371" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="372" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A372">
+        <v>57</v>
+      </c>
+      <c r="B372" t="s">
+        <v>149</v>
+      </c>
+      <c r="C372" t="s">
+        <v>150</v>
+      </c>
+      <c r="D372">
+        <v>0</v>
+      </c>
+      <c r="E372">
+        <v>2</v>
+      </c>
+      <c r="H372">
+        <v>26.1</v>
+      </c>
+      <c r="I372">
+        <v>24.7</v>
+      </c>
+      <c r="J372">
+        <v>28.2</v>
+      </c>
+      <c r="L372" t="s">
+        <v>159</v>
+      </c>
+      <c r="M372" t="s">
+        <v>143</v>
+      </c>
+      <c r="N372">
+        <v>0.45</v>
+      </c>
+      <c r="O372">
+        <v>0</v>
+      </c>
+      <c r="P372">
+        <v>20</v>
+      </c>
+      <c r="Q372">
+        <v>0</v>
+      </c>
+      <c r="R372">
+        <v>0.02</v>
+      </c>
+      <c r="S372" t="s">
+        <v>161</v>
+      </c>
+      <c r="T372" t="s">
+        <v>162</v>
+      </c>
+      <c r="U372" s="1">
+        <v>1</v>
+      </c>
+      <c r="V372" s="1">
+        <v>1</v>
+      </c>
+      <c r="W372" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="373" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A373">
+        <v>58</v>
+      </c>
+      <c r="B373" t="s">
+        <v>163</v>
+      </c>
+      <c r="C373" t="s">
+        <v>52</v>
+      </c>
+      <c r="D373">
+        <v>0</v>
+      </c>
+      <c r="E373">
+        <v>0</v>
+      </c>
+      <c r="G373">
+        <v>24</v>
+      </c>
+      <c r="H373">
+        <v>24</v>
+      </c>
+      <c r="I373">
+        <v>24</v>
+      </c>
+      <c r="J373">
+        <v>24</v>
+      </c>
+      <c r="L373" t="s">
+        <v>151</v>
+      </c>
+      <c r="M373" t="s">
+        <v>70</v>
+      </c>
+      <c r="N373">
+        <v>0.28354430379746798</v>
+      </c>
+      <c r="O373">
+        <v>1</v>
+      </c>
+      <c r="P373">
+        <v>91</v>
+      </c>
+      <c r="Q373">
+        <v>0</v>
+      </c>
+      <c r="R373">
+        <v>5.9071729957805019E-3</v>
+      </c>
+      <c r="S373" t="s">
+        <v>76</v>
+      </c>
+      <c r="T373" t="s">
+        <v>77</v>
+      </c>
+      <c r="U373" s="1">
+        <v>1</v>
+      </c>
+      <c r="V373" s="1">
+        <v>1</v>
+      </c>
+      <c r="W373" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="374" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A374">
+        <v>58</v>
+      </c>
+      <c r="B374" t="s">
+        <v>163</v>
+      </c>
+      <c r="C374" t="s">
+        <v>52</v>
+      </c>
+      <c r="D374">
+        <v>0</v>
+      </c>
+      <c r="E374">
+        <v>0</v>
+      </c>
+      <c r="G374">
+        <v>24</v>
+      </c>
+      <c r="H374">
+        <v>24</v>
+      </c>
+      <c r="I374">
+        <v>24</v>
+      </c>
+      <c r="J374">
+        <v>24</v>
+      </c>
+      <c r="L374" t="s">
+        <v>151</v>
+      </c>
+      <c r="M374" t="s">
+        <v>70</v>
+      </c>
+      <c r="N374">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="O374">
+        <v>1</v>
+      </c>
+      <c r="P374">
+        <v>94</v>
+      </c>
+      <c r="Q374">
+        <v>0</v>
+      </c>
+      <c r="R374">
+        <v>6.4697609001405088E-3</v>
+      </c>
+      <c r="S374" t="s">
+        <v>76</v>
+      </c>
+      <c r="T374" t="s">
+        <v>77</v>
+      </c>
+      <c r="U374" s="1">
+        <v>1</v>
+      </c>
+      <c r="V374" s="1">
+        <v>1</v>
+      </c>
+      <c r="W374" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="375" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A375">
+        <v>58</v>
+      </c>
+      <c r="B375" t="s">
+        <v>163</v>
+      </c>
+      <c r="C375" t="s">
+        <v>52</v>
+      </c>
+      <c r="D375">
+        <v>0</v>
+      </c>
+      <c r="E375">
+        <v>1</v>
+      </c>
+      <c r="F375">
+        <v>1</v>
+      </c>
+      <c r="G375">
+        <v>24</v>
+      </c>
+      <c r="H375">
+        <v>24</v>
+      </c>
+      <c r="I375">
+        <v>18</v>
+      </c>
+      <c r="J375">
+        <v>32</v>
+      </c>
+      <c r="K375">
+        <v>24</v>
+      </c>
+      <c r="L375" t="s">
+        <v>151</v>
+      </c>
+      <c r="M375" t="s">
+        <v>70</v>
+      </c>
+      <c r="N375">
+        <v>0.25147679324894501</v>
+      </c>
+      <c r="O375">
+        <v>1</v>
+      </c>
+      <c r="P375">
+        <v>107</v>
+      </c>
+      <c r="Q375">
+        <v>0</v>
+      </c>
+      <c r="R375">
+        <v>5.9071729957805158E-3</v>
+      </c>
+      <c r="S375" t="s">
+        <v>76</v>
+      </c>
+      <c r="T375" t="s">
+        <v>77</v>
+      </c>
+      <c r="U375" s="1">
+        <v>1</v>
+      </c>
+      <c r="V375" s="1">
+        <v>1</v>
+      </c>
+      <c r="W375" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="376" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A376">
+        <v>58</v>
+      </c>
+      <c r="B376" t="s">
+        <v>163</v>
+      </c>
+      <c r="C376" t="s">
+        <v>52</v>
+      </c>
+      <c r="D376">
+        <v>0</v>
+      </c>
+      <c r="E376">
+        <v>1</v>
+      </c>
+      <c r="F376">
+        <v>1</v>
+      </c>
+      <c r="G376">
+        <v>24</v>
+      </c>
+      <c r="H376">
+        <v>24</v>
+      </c>
+      <c r="I376">
+        <v>18</v>
+      </c>
+      <c r="J376">
+        <v>32</v>
+      </c>
+      <c r="K376">
+        <v>24</v>
+      </c>
+      <c r="L376" t="s">
+        <v>151</v>
+      </c>
+      <c r="M376" t="s">
+        <v>70</v>
+      </c>
+      <c r="N376">
+        <v>0.241912798874824</v>
+      </c>
+      <c r="O376">
+        <v>1</v>
+      </c>
+      <c r="P376">
+        <v>84</v>
+      </c>
+      <c r="Q376">
+        <v>0</v>
+      </c>
+      <c r="R376">
+        <v>6.1884669479604915E-3</v>
+      </c>
+      <c r="S376" t="s">
+        <v>76</v>
+      </c>
+      <c r="T376" t="s">
+        <v>77</v>
+      </c>
+      <c r="U376" s="1">
+        <v>1</v>
+      </c>
+      <c r="V376" s="1">
+        <v>1</v>
+      </c>
+      <c r="W376" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="377" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A377">
+        <v>59</v>
+      </c>
+      <c r="B377" t="s">
+        <v>163</v>
+      </c>
+      <c r="C377" t="s">
+        <v>33</v>
+      </c>
+      <c r="D377">
+        <v>0</v>
+      </c>
+      <c r="E377">
+        <v>0</v>
+      </c>
+      <c r="G377">
+        <v>24</v>
+      </c>
+      <c r="H377">
+        <v>24</v>
+      </c>
+      <c r="I377">
+        <v>24</v>
+      </c>
+      <c r="J377">
+        <v>24</v>
+      </c>
+      <c r="L377" t="s">
+        <v>84</v>
+      </c>
+      <c r="M377" t="s">
+        <v>164</v>
+      </c>
+      <c r="N377">
+        <v>42.153846153846096</v>
+      </c>
+      <c r="O377">
+        <v>1</v>
+      </c>
+      <c r="P377">
+        <v>8</v>
+      </c>
+      <c r="Q377">
+        <v>0</v>
+      </c>
+      <c r="R377">
+        <v>0.12587412587410185</v>
+      </c>
+      <c r="S377" t="s">
+        <v>76</v>
+      </c>
+      <c r="T377" t="s">
+        <v>77</v>
+      </c>
+      <c r="U377" s="1">
+        <v>1</v>
+      </c>
+      <c r="V377" s="1">
+        <v>1</v>
+      </c>
+      <c r="W377" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="378" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A378">
+        <v>59</v>
+      </c>
+      <c r="B378" t="s">
+        <v>163</v>
+      </c>
+      <c r="C378" t="s">
+        <v>33</v>
+      </c>
+      <c r="D378">
+        <v>0</v>
+      </c>
+      <c r="E378">
+        <v>0</v>
+      </c>
+      <c r="G378">
+        <v>24</v>
+      </c>
+      <c r="H378">
+        <v>24</v>
+      </c>
+      <c r="I378">
+        <v>24</v>
+      </c>
+      <c r="J378">
+        <v>24</v>
+      </c>
+      <c r="L378" t="s">
+        <v>84</v>
+      </c>
+      <c r="M378" t="s">
+        <v>164</v>
+      </c>
+      <c r="N378">
+        <v>41.398601398601301</v>
+      </c>
+      <c r="O378">
+        <v>1</v>
+      </c>
+      <c r="P378">
+        <v>8</v>
+      </c>
+      <c r="Q378">
+        <v>0</v>
+      </c>
+      <c r="R378">
+        <v>0.12237762237764827</v>
+      </c>
+      <c r="S378" t="s">
+        <v>76</v>
+      </c>
+      <c r="T378" t="s">
+        <v>77</v>
+      </c>
+      <c r="U378" s="1">
+        <v>1</v>
+      </c>
+      <c r="V378" s="1">
+        <v>1</v>
+      </c>
+      <c r="W378" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="379" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A379">
+        <v>59</v>
+      </c>
+      <c r="B379" t="s">
+        <v>163</v>
+      </c>
+      <c r="C379" t="s">
+        <v>33</v>
+      </c>
+      <c r="D379">
+        <v>0</v>
+      </c>
+      <c r="E379">
+        <v>1</v>
+      </c>
+      <c r="F379">
+        <v>1</v>
+      </c>
+      <c r="G379">
+        <v>24</v>
+      </c>
+      <c r="H379">
+        <v>24</v>
+      </c>
+      <c r="I379">
+        <v>18</v>
+      </c>
+      <c r="J379">
+        <v>32</v>
+      </c>
+      <c r="K379">
+        <v>24</v>
+      </c>
+      <c r="L379" t="s">
+        <v>84</v>
+      </c>
+      <c r="M379" t="s">
+        <v>164</v>
+      </c>
+      <c r="N379">
+        <v>42.335664335664298</v>
+      </c>
+      <c r="O379">
+        <v>1</v>
+      </c>
+      <c r="P379">
+        <v>8</v>
+      </c>
+      <c r="Q379">
+        <v>0</v>
+      </c>
+      <c r="R379">
+        <v>0.12937062937060162</v>
+      </c>
+      <c r="S379" t="s">
+        <v>76</v>
+      </c>
+      <c r="T379" t="s">
+        <v>77</v>
+      </c>
+      <c r="U379" s="1">
+        <v>1</v>
+      </c>
+      <c r="V379" s="1">
+        <v>1</v>
+      </c>
+      <c r="W379" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="380" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A380">
+        <v>59</v>
+      </c>
+      <c r="B380" t="s">
+        <v>163</v>
+      </c>
+      <c r="C380" t="s">
+        <v>33</v>
+      </c>
+      <c r="D380">
+        <v>0</v>
+      </c>
+      <c r="E380">
+        <v>1</v>
+      </c>
+      <c r="F380">
+        <v>1</v>
+      </c>
+      <c r="G380">
+        <v>24</v>
+      </c>
+      <c r="H380">
+        <v>24</v>
+      </c>
+      <c r="I380">
+        <v>18</v>
+      </c>
+      <c r="J380">
+        <v>32</v>
+      </c>
+      <c r="K380">
+        <v>24</v>
+      </c>
+      <c r="L380" t="s">
+        <v>84</v>
+      </c>
+      <c r="M380" t="s">
+        <v>164</v>
+      </c>
+      <c r="N380">
+        <v>43.006993006993</v>
+      </c>
+      <c r="O380">
+        <v>1</v>
+      </c>
+      <c r="P380">
+        <v>8</v>
+      </c>
+      <c r="Q380">
+        <v>0</v>
+      </c>
+      <c r="R380">
+        <v>0.19580419580420028</v>
+      </c>
+      <c r="S380" t="s">
+        <v>76</v>
+      </c>
+      <c r="T380" t="s">
+        <v>77</v>
+      </c>
+      <c r="U380" s="1">
+        <v>1</v>
+      </c>
+      <c r="V380" s="1">
+        <v>1</v>
+      </c>
+      <c r="W380" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
piccau et al extraction and recalculating SD for lowenborg et al 2012
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9ABEB69D-C6EA-4D4D-8726-D50E4D851676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06CAEDC-440B-0249-ADE6-A9E1DB8E534D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2080" yWindow="460" windowWidth="24460" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2899" uniqueCount="183">
   <si>
     <t>study_id</t>
   </si>
@@ -555,6 +555,27 @@
   <si>
     <t>high food</t>
   </si>
+  <si>
+    <t>piccau2017</t>
+  </si>
+  <si>
+    <t>germination</t>
+  </si>
+  <si>
+    <t>Clematis</t>
+  </si>
+  <si>
+    <t>vitalba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 hours </t>
+  </si>
+  <si>
+    <t xml:space="preserve">irradiance per day </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 hours </t>
+  </si>
 </sst>
 </file>
 
@@ -920,11 +941,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AG372"/>
+  <dimension ref="A1:AG375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A343" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L89" sqref="L89"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A300" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R303" sqref="R303:R322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22472,7 +22493,7 @@
         <v>48</v>
       </c>
       <c r="N303">
-        <v>76.055996307661601</v>
+        <v>75.8333333333333</v>
       </c>
       <c r="O303">
         <v>1</v>
@@ -22481,7 +22502,10 @@
         <v>28</v>
       </c>
       <c r="Q303">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="R303">
+        <v>13.341298287534817</v>
       </c>
       <c r="S303" t="s">
         <v>148</v>
@@ -22531,7 +22555,7 @@
         <v>48</v>
       </c>
       <c r="N304">
-        <v>39.944677294613598</v>
+        <v>40.080645161290299</v>
       </c>
       <c r="O304">
         <v>1</v>
@@ -22540,10 +22564,10 @@
         <v>25</v>
       </c>
       <c r="Q304">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R304">
-        <v>2.0161290322580996</v>
+        <v>0.39824771007562587</v>
       </c>
       <c r="S304" t="s">
         <v>148</v>
@@ -22599,7 +22623,7 @@
         <v>48</v>
       </c>
       <c r="N305">
-        <v>41.199573385225598</v>
+        <v>41.693548387096698</v>
       </c>
       <c r="O305">
         <v>1</v>
@@ -22608,10 +22632,10 @@
         <v>29</v>
       </c>
       <c r="Q305">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R305">
-        <v>2.4865591397849514</v>
+        <v>1.3938669852648142</v>
       </c>
       <c r="S305" t="s">
         <v>148</v>
@@ -22661,7 +22685,7 @@
         <v>48</v>
       </c>
       <c r="N306">
-        <v>31.969974802285201</v>
+        <v>32.016129032258</v>
       </c>
       <c r="O306">
         <v>1</v>
@@ -22670,10 +22694,10 @@
         <v>25</v>
       </c>
       <c r="Q306">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R306">
-        <v>1.9492365840880002</v>
+        <v>1.3938669852648142</v>
       </c>
       <c r="S306" t="s">
         <v>148</v>
@@ -22723,7 +22747,7 @@
         <v>48</v>
       </c>
       <c r="N307">
-        <v>13.494950000312601</v>
+        <v>13.505376344086001</v>
       </c>
       <c r="O307">
         <v>1</v>
@@ -22732,7 +22756,10 @@
         <v>28</v>
       </c>
       <c r="Q307">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="R307">
+        <v>14.723217841497405</v>
       </c>
       <c r="S307" t="s">
         <v>148</v>
@@ -22782,7 +22809,7 @@
         <v>48</v>
       </c>
       <c r="N308">
-        <v>9.0026203713547801</v>
+        <v>9.0752688172043001</v>
       </c>
       <c r="O308">
         <v>1</v>
@@ -22791,10 +22818,10 @@
         <v>25</v>
       </c>
       <c r="Q308">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R308">
-        <v>0.87334037935972963</v>
+        <v>0.4938271604938293</v>
       </c>
       <c r="S308" t="s">
         <v>148</v>
@@ -22850,7 +22877,7 @@
         <v>48</v>
       </c>
       <c r="N309">
-        <v>10.246039737087299</v>
+        <v>10.2795698924731</v>
       </c>
       <c r="O309">
         <v>1</v>
@@ -22859,10 +22886,10 @@
         <v>29</v>
       </c>
       <c r="Q309">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R309">
-        <v>1.1644455006535095</v>
+        <v>0.54161688570287381</v>
       </c>
       <c r="S309" t="s">
         <v>148</v>
@@ -22912,7 +22939,7 @@
         <v>48</v>
       </c>
       <c r="N310">
-        <v>13.343956573129599</v>
+        <v>13.3978494623655</v>
       </c>
       <c r="O310">
         <v>1</v>
@@ -22921,10 +22948,10 @@
         <v>25</v>
       </c>
       <c r="Q310">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R310">
-        <v>1.3800539083558014</v>
+        <v>0.86021505376348084</v>
       </c>
       <c r="S310" t="s">
         <v>148</v>
@@ -22974,7 +23001,7 @@
         <v>144</v>
       </c>
       <c r="N311">
-        <v>0.20204081632653001</v>
+        <v>0.20170648464163801</v>
       </c>
       <c r="O311">
         <v>1</v>
@@ -22983,7 +23010,10 @@
         <v>28</v>
       </c>
       <c r="Q311">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="R311">
+        <v>1.8202502844140753E-2</v>
       </c>
       <c r="S311" t="s">
         <v>148</v>
@@ -23033,7 +23063,7 @@
         <v>144</v>
       </c>
       <c r="N312">
-        <v>0.24693877551020399</v>
+        <v>0.24675767918088701</v>
       </c>
       <c r="O312">
         <v>1</v>
@@ -23042,10 +23072,10 @@
         <v>25</v>
       </c>
       <c r="Q312">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R312">
-        <v>5.2380952380952486E-2</v>
+        <v>2.5281253950196304E-2</v>
       </c>
       <c r="S312" t="s">
         <v>148</v>
@@ -23101,7 +23131,7 @@
         <v>144</v>
       </c>
       <c r="N313">
-        <v>0.27278911564625802</v>
+        <v>0.27269624573378798</v>
       </c>
       <c r="O313">
         <v>1</v>
@@ -23110,10 +23140,10 @@
         <v>29</v>
       </c>
       <c r="Q313">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R313">
-        <v>4.7619047619047492E-2</v>
+        <v>2.2247503476172575E-2</v>
       </c>
       <c r="S313" t="s">
         <v>148</v>
@@ -23163,7 +23193,7 @@
         <v>144</v>
       </c>
       <c r="N314">
-        <v>0.25714285714285701</v>
+        <v>0.25631399317406101</v>
       </c>
       <c r="O314">
         <v>1</v>
@@ -23172,10 +23202,10 @@
         <v>25</v>
       </c>
       <c r="Q314">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R314">
-        <v>5.7142857142857009E-2</v>
+        <v>3.1348754898242959E-2</v>
       </c>
       <c r="S314" t="s">
         <v>148</v>
@@ -23225,7 +23255,7 @@
         <v>144</v>
       </c>
       <c r="N315">
-        <v>6.8296257078838601E-2</v>
+        <v>6.7091836734693905E-2</v>
       </c>
       <c r="O315">
         <v>1</v>
@@ -23234,10 +23264,10 @@
         <v>28</v>
       </c>
       <c r="Q315">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R315">
-        <v>4.7866894197951398E-2</v>
+        <v>7.136558327034459E-2</v>
       </c>
       <c r="S315" t="s">
         <v>148</v>
@@ -23287,7 +23317,7 @@
         <v>144</v>
       </c>
       <c r="N316">
-        <v>0.15308183562913</v>
+        <v>0.152210884353741</v>
       </c>
       <c r="O316">
         <v>1</v>
@@ -23296,10 +23326,10 @@
         <v>25</v>
       </c>
       <c r="Q316">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R316">
-        <v>4.0827645051195009E-2</v>
+        <v>2.9100529100528891E-2</v>
       </c>
       <c r="S316" t="s">
         <v>148</v>
@@ -23355,7 +23385,7 @@
         <v>144</v>
       </c>
       <c r="N317">
-        <v>0.149642158206725</v>
+        <v>0.14940476190476101</v>
       </c>
       <c r="O317">
         <v>1</v>
@@ -23364,10 +23394,10 @@
         <v>29</v>
       </c>
       <c r="Q317">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R317">
-        <v>4.9274744027303308E-2</v>
+        <v>4.2957923910304431E-2</v>
       </c>
       <c r="S317" t="s">
         <v>148</v>
@@ -23417,7 +23447,7 @@
         <v>144</v>
       </c>
       <c r="N318">
-        <v>0.153711013207529</v>
+        <v>0.15314625850340099</v>
       </c>
       <c r="O318">
         <v>1</v>
@@ -23426,10 +23456,10 @@
         <v>25</v>
       </c>
       <c r="Q318">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R318">
-        <v>5.2090443686006654E-2</v>
+        <v>3.1872008062484455E-2</v>
       </c>
       <c r="S318" t="s">
         <v>148</v>
@@ -23479,7 +23509,7 @@
         <v>147</v>
       </c>
       <c r="N319">
-        <v>1.7421602787456401</v>
+        <v>1.70138888888888</v>
       </c>
       <c r="O319">
         <v>1</v>
@@ -23488,10 +23518,10 @@
         <v>28</v>
       </c>
       <c r="Q319">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R319">
-        <v>0.8710801393728298</v>
+        <v>1.2860082304526761</v>
       </c>
       <c r="S319" t="s">
         <v>148</v>
@@ -23541,7 +23571,7 @@
         <v>147</v>
       </c>
       <c r="N320">
-        <v>2.8222996515679499</v>
+        <v>2.8125</v>
       </c>
       <c r="O320">
         <v>1</v>
@@ -23550,10 +23580,10 @@
         <v>25</v>
       </c>
       <c r="Q320">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R320">
-        <v>2.5958188153310111</v>
+        <v>1.7746913580246884</v>
       </c>
       <c r="S320" t="s">
         <v>148</v>
@@ -23609,7 +23639,7 @@
         <v>147</v>
       </c>
       <c r="N321">
-        <v>3.1358885017421598</v>
+        <v>3.125</v>
       </c>
       <c r="O321">
         <v>1</v>
@@ -23618,10 +23648,10 @@
         <v>29</v>
       </c>
       <c r="Q321">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R321">
-        <v>2.822299651567941</v>
+        <v>1.8004115226337407</v>
       </c>
       <c r="S321" t="s">
         <v>148</v>
@@ -23671,7 +23701,7 @@
         <v>147</v>
       </c>
       <c r="N322">
-        <v>5.6445993031358901</v>
+        <v>5.625</v>
       </c>
       <c r="O322">
         <v>1</v>
@@ -23680,10 +23710,10 @@
         <v>25</v>
       </c>
       <c r="Q322">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R322">
-        <v>4.5470383275261259</v>
+        <v>3.8580246913580223</v>
       </c>
       <c r="S322" t="s">
         <v>148</v>
@@ -27123,6 +27153,222 @@
       </c>
       <c r="AB372" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="373" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A373">
+        <v>60</v>
+      </c>
+      <c r="B373" t="s">
+        <v>176</v>
+      </c>
+      <c r="C373" t="s">
+        <v>29</v>
+      </c>
+      <c r="D373">
+        <v>1</v>
+      </c>
+      <c r="E373">
+        <v>1</v>
+      </c>
+      <c r="F373">
+        <v>1</v>
+      </c>
+      <c r="H373">
+        <v>17.5</v>
+      </c>
+      <c r="I373">
+        <v>10</v>
+      </c>
+      <c r="J373">
+        <v>25</v>
+      </c>
+      <c r="K373">
+        <v>24</v>
+      </c>
+      <c r="L373" t="s">
+        <v>177</v>
+      </c>
+      <c r="M373" t="s">
+        <v>81</v>
+      </c>
+      <c r="N373" s="2">
+        <v>86.871961099999993</v>
+      </c>
+      <c r="O373">
+        <v>1</v>
+      </c>
+      <c r="P373">
+        <v>120</v>
+      </c>
+      <c r="Q373">
+        <v>1</v>
+      </c>
+      <c r="R373">
+        <v>6.8881685600000004</v>
+      </c>
+      <c r="S373" t="s">
+        <v>178</v>
+      </c>
+      <c r="T373" t="s">
+        <v>179</v>
+      </c>
+      <c r="U373" s="1">
+        <v>0</v>
+      </c>
+      <c r="V373" s="1">
+        <v>0</v>
+      </c>
+      <c r="W373" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA373" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB373" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="374" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A374">
+        <v>60</v>
+      </c>
+      <c r="B374" t="s">
+        <v>176</v>
+      </c>
+      <c r="C374" t="s">
+        <v>29</v>
+      </c>
+      <c r="D374">
+        <v>1</v>
+      </c>
+      <c r="E374">
+        <v>0</v>
+      </c>
+      <c r="H374">
+        <v>10</v>
+      </c>
+      <c r="I374">
+        <v>10</v>
+      </c>
+      <c r="J374">
+        <v>10</v>
+      </c>
+      <c r="L374" t="s">
+        <v>177</v>
+      </c>
+      <c r="M374" t="s">
+        <v>81</v>
+      </c>
+      <c r="N374" s="2">
+        <v>0.81037276999999996</v>
+      </c>
+      <c r="O374">
+        <v>1</v>
+      </c>
+      <c r="P374">
+        <v>120</v>
+      </c>
+      <c r="Q374">
+        <v>1</v>
+      </c>
+      <c r="R374">
+        <v>1.6207455399999999</v>
+      </c>
+      <c r="S374" t="s">
+        <v>178</v>
+      </c>
+      <c r="T374" t="s">
+        <v>179</v>
+      </c>
+      <c r="U374" s="1">
+        <v>0</v>
+      </c>
+      <c r="V374" s="1">
+        <v>0</v>
+      </c>
+      <c r="W374" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA374" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB374" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="375" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A375">
+        <v>60</v>
+      </c>
+      <c r="B375" t="s">
+        <v>176</v>
+      </c>
+      <c r="C375" t="s">
+        <v>29</v>
+      </c>
+      <c r="D375">
+        <v>1</v>
+      </c>
+      <c r="E375">
+        <v>1</v>
+      </c>
+      <c r="F375">
+        <v>1</v>
+      </c>
+      <c r="H375">
+        <v>17.5</v>
+      </c>
+      <c r="I375">
+        <v>10</v>
+      </c>
+      <c r="J375">
+        <v>25</v>
+      </c>
+      <c r="K375">
+        <v>24</v>
+      </c>
+      <c r="L375" t="s">
+        <v>177</v>
+      </c>
+      <c r="M375" t="s">
+        <v>81</v>
+      </c>
+      <c r="N375" s="2">
+        <v>87.520259300000006</v>
+      </c>
+      <c r="O375">
+        <v>1</v>
+      </c>
+      <c r="P375">
+        <v>120</v>
+      </c>
+      <c r="Q375">
+        <v>1</v>
+      </c>
+      <c r="R375">
+        <v>7.3743922199999998</v>
+      </c>
+      <c r="S375" t="s">
+        <v>178</v>
+      </c>
+      <c r="T375" t="s">
+        <v>179</v>
+      </c>
+      <c r="U375" s="1">
+        <v>0</v>
+      </c>
+      <c r="V375" s="1">
+        <v>0</v>
+      </c>
+      <c r="W375" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA375" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB375" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -27132,343 +27378,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C63C9F3-EFBE-D44D-B609-615DB2D2DDEC}">
-  <dimension ref="B1:T8"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:T8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I1">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J1">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L1" t="s">
-        <v>80</v>
-      </c>
-      <c r="M1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1">
-        <v>0</v>
-      </c>
-      <c r="P1">
-        <v>84</v>
-      </c>
-      <c r="Q1">
-        <v>0</v>
-      </c>
-      <c r="S1" t="s">
-        <v>101</v>
-      </c>
-      <c r="T1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I2">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J2">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M2" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>84</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="S2" t="s">
-        <v>135</v>
-      </c>
-      <c r="T2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I3">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J3">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L3" t="s">
-        <v>132</v>
-      </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>84</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="S3" t="s">
-        <v>135</v>
-      </c>
-      <c r="T3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L4" t="s">
-        <v>131</v>
-      </c>
-      <c r="M4" t="s">
-        <v>81</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>84</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="S4" t="s">
-        <v>135</v>
-      </c>
-      <c r="T4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I5">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J5">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L5" t="s">
-        <v>80</v>
-      </c>
-      <c r="M5" t="s">
-        <v>31</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>84</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="S5" t="s">
-        <v>101</v>
-      </c>
-      <c r="T5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I6">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J6">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L6" t="s">
-        <v>133</v>
-      </c>
-      <c r="M6" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>84</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="S6" t="s">
-        <v>135</v>
-      </c>
-      <c r="T6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I7">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J7">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L7" t="s">
-        <v>132</v>
-      </c>
-      <c r="M7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>84</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="S7" t="s">
-        <v>135</v>
-      </c>
-      <c r="T7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I8">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="J8">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L8" t="s">
-        <v>131</v>
-      </c>
-      <c r="M8" t="s">
-        <v>81</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>84</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="S8" t="s">
-        <v>135</v>
-      </c>
-      <c r="T8" t="s">
-        <v>134</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commiting to save work so far
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06CAEDC-440B-0249-ADE6-A9E1DB8E534D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440C264F-DC98-0F4C-94B5-859FE8D0C8E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="460" windowWidth="24460" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="28820" yWindow="-8760" windowWidth="24460" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="metanaly_fulldataset" sheetId="1" r:id="rId1"/>
@@ -944,8 +944,8 @@
   <dimension ref="A1:AG375"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A300" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R303" sqref="R303:R322"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S305" sqref="S305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21958,7 +21958,7 @@
         <v>0</v>
       </c>
       <c r="P295">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="Q295">
         <v>0</v>
@@ -22023,7 +22023,7 @@
         <v>0</v>
       </c>
       <c r="P296">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="Q296">
         <v>0</v>
@@ -22058,7 +22058,7 @@
         <v>46</v>
       </c>
       <c r="D297">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E297">
         <v>0</v>
@@ -22088,7 +22088,7 @@
         <v>0</v>
       </c>
       <c r="P297">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="Q297">
         <v>0</v>
@@ -22097,10 +22097,10 @@
         <v>14.4</v>
       </c>
       <c r="S297" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="T297" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="U297" s="1">
         <v>1</v>
@@ -22123,7 +22123,7 @@
         <v>46</v>
       </c>
       <c r="D298">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E298">
         <v>0</v>
@@ -22153,7 +22153,7 @@
         <v>0</v>
       </c>
       <c r="P298">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="Q298">
         <v>0</v>
@@ -22224,7 +22224,7 @@
         <v>0</v>
       </c>
       <c r="P299">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="Q299">
         <v>0</v>
@@ -22295,7 +22295,7 @@
         <v>0</v>
       </c>
       <c r="P300">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="Q300">
         <v>0</v>
@@ -22330,7 +22330,7 @@
         <v>46</v>
       </c>
       <c r="D301">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E301">
         <v>1</v>
@@ -22366,7 +22366,7 @@
         <v>0</v>
       </c>
       <c r="P301">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="Q301">
         <v>0</v>
@@ -22375,10 +22375,10 @@
         <v>10.84</v>
       </c>
       <c r="S301" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="T301" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="U301" s="1">
         <v>1</v>
@@ -22401,7 +22401,7 @@
         <v>46</v>
       </c>
       <c r="D302">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E302">
         <v>1</v>
@@ -22437,7 +22437,7 @@
         <v>0</v>
       </c>
       <c r="P302">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="Q302">
         <v>0</v>

</xml_diff>

<commit_message>
updated full extraction and metadata files
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440C264F-DC98-0F4C-94B5-859FE8D0C8E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F35053-0F4E-0C4A-AE2F-106495CBDEBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="-8760" windowWidth="24460" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="28820" yWindow="-16820" windowWidth="24460" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="metanaly_fulldataset" sheetId="1" r:id="rId1"/>
-    <sheet name="holding " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -944,8 +943,8 @@
   <dimension ref="A1:AG375"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S305" sqref="S305"/>
+      <pane ySplit="1" topLeftCell="A361" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27374,18 +27373,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C63C9F3-EFBE-D44D-B609-615DB2D2DDEC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updating metadata files for acclimation and pulse press
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF933726-06AA-F142-A12D-FDB5B4C7E2C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C5A3AE-CFC9-F749-BD10-DF40830A0374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="27500" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
@@ -991,9 +991,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
   <dimension ref="A1:AG493"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A452" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A487" sqref="A487:A493"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
saxon et al extraction, including raw data for semenov and treidel
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73951C34-8200-A442-8740-EEB27F5E27A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588EF591-C0B7-244A-8132-C6763BABB014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28860" yWindow="-9540" windowWidth="23540" windowHeight="11100" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="28840" yWindow="-7060" windowWidth="23540" windowHeight="11100" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="metanaly_fulldataset" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3957" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4048" uniqueCount="211">
   <si>
     <t>study_id</t>
   </si>
@@ -644,6 +644,21 @@
   <si>
     <t>scripta</t>
   </si>
+  <si>
+    <t>saxon2017</t>
+  </si>
+  <si>
+    <t>total offspring</t>
+  </si>
+  <si>
+    <t>offspring per mating</t>
+  </si>
+  <si>
+    <t>wing centroid</t>
+  </si>
+  <si>
+    <t>birchii</t>
+  </si>
 </sst>
 </file>
 
@@ -691,12 +706,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1011,11 +1027,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AG501"/>
+  <dimension ref="A1:AG517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A482" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q497" sqref="Q497"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A511" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D520" sqref="D520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36951,6 +36967,1028 @@
         <v>2</v>
       </c>
     </row>
+    <row r="502" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A502">
+        <v>78</v>
+      </c>
+      <c r="B502" t="s">
+        <v>206</v>
+      </c>
+      <c r="C502" t="s">
+        <v>29</v>
+      </c>
+      <c r="D502">
+        <v>0</v>
+      </c>
+      <c r="E502">
+        <v>0</v>
+      </c>
+      <c r="G502">
+        <v>20.5</v>
+      </c>
+      <c r="H502">
+        <v>24</v>
+      </c>
+      <c r="I502">
+        <v>24</v>
+      </c>
+      <c r="J502">
+        <v>24</v>
+      </c>
+      <c r="L502" t="s">
+        <v>207</v>
+      </c>
+      <c r="M502" t="s">
+        <v>207</v>
+      </c>
+      <c r="N502">
+        <v>175</v>
+      </c>
+      <c r="O502">
+        <v>1</v>
+      </c>
+      <c r="P502">
+        <v>1600</v>
+      </c>
+      <c r="Q502">
+        <v>1</v>
+      </c>
+      <c r="R502">
+        <v>74.190542744002229</v>
+      </c>
+      <c r="S502" t="s">
+        <v>101</v>
+      </c>
+      <c r="T502" t="s">
+        <v>210</v>
+      </c>
+      <c r="U502" s="1">
+        <v>1</v>
+      </c>
+      <c r="V502" s="1">
+        <v>2</v>
+      </c>
+      <c r="W502" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A503">
+        <v>78</v>
+      </c>
+      <c r="B503" t="s">
+        <v>206</v>
+      </c>
+      <c r="C503" t="s">
+        <v>29</v>
+      </c>
+      <c r="D503">
+        <v>0</v>
+      </c>
+      <c r="E503">
+        <v>1</v>
+      </c>
+      <c r="F503">
+        <v>1</v>
+      </c>
+      <c r="G503">
+        <v>20.5</v>
+      </c>
+      <c r="H503">
+        <v>24</v>
+      </c>
+      <c r="I503" s="5">
+        <v>21</v>
+      </c>
+      <c r="J503" s="5">
+        <v>27</v>
+      </c>
+      <c r="K503">
+        <v>24</v>
+      </c>
+      <c r="L503" t="s">
+        <v>207</v>
+      </c>
+      <c r="M503" t="s">
+        <v>207</v>
+      </c>
+      <c r="N503">
+        <v>108.962264150943</v>
+      </c>
+      <c r="O503">
+        <v>1</v>
+      </c>
+      <c r="P503">
+        <v>1600</v>
+      </c>
+      <c r="Q503">
+        <v>1</v>
+      </c>
+      <c r="R503">
+        <v>94.572559981364364</v>
+      </c>
+      <c r="S503" t="s">
+        <v>101</v>
+      </c>
+      <c r="T503" t="s">
+        <v>210</v>
+      </c>
+      <c r="U503" s="1">
+        <v>1</v>
+      </c>
+      <c r="V503" s="1">
+        <v>2</v>
+      </c>
+      <c r="W503" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="504" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A504">
+        <v>78</v>
+      </c>
+      <c r="B504" t="s">
+        <v>206</v>
+      </c>
+      <c r="C504" t="s">
+        <v>29</v>
+      </c>
+      <c r="D504">
+        <v>0</v>
+      </c>
+      <c r="E504">
+        <v>0</v>
+      </c>
+      <c r="G504">
+        <v>20.5</v>
+      </c>
+      <c r="H504">
+        <v>24</v>
+      </c>
+      <c r="I504">
+        <v>24</v>
+      </c>
+      <c r="J504">
+        <v>24</v>
+      </c>
+      <c r="L504" t="s">
+        <v>208</v>
+      </c>
+      <c r="M504" t="s">
+        <v>208</v>
+      </c>
+      <c r="N504">
+        <v>66.164162549157993</v>
+      </c>
+      <c r="O504">
+        <v>1</v>
+      </c>
+      <c r="P504">
+        <v>1600</v>
+      </c>
+      <c r="Q504">
+        <v>1</v>
+      </c>
+      <c r="R504">
+        <v>22.064617809298735</v>
+      </c>
+      <c r="S504" t="s">
+        <v>101</v>
+      </c>
+      <c r="T504" t="s">
+        <v>210</v>
+      </c>
+      <c r="U504" s="1">
+        <v>1</v>
+      </c>
+      <c r="V504" s="1">
+        <v>2</v>
+      </c>
+      <c r="W504" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="505" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A505">
+        <v>78</v>
+      </c>
+      <c r="B505" t="s">
+        <v>206</v>
+      </c>
+      <c r="C505" t="s">
+        <v>29</v>
+      </c>
+      <c r="D505">
+        <v>0</v>
+      </c>
+      <c r="E505">
+        <v>1</v>
+      </c>
+      <c r="F505">
+        <v>1</v>
+      </c>
+      <c r="G505">
+        <v>20.5</v>
+      </c>
+      <c r="H505">
+        <v>24</v>
+      </c>
+      <c r="I505" s="5">
+        <v>21</v>
+      </c>
+      <c r="J505" s="5">
+        <v>27</v>
+      </c>
+      <c r="K505">
+        <v>24</v>
+      </c>
+      <c r="L505" t="s">
+        <v>208</v>
+      </c>
+      <c r="M505" t="s">
+        <v>208</v>
+      </c>
+      <c r="N505">
+        <v>48.076535242512797</v>
+      </c>
+      <c r="O505">
+        <v>1</v>
+      </c>
+      <c r="P505">
+        <v>1600</v>
+      </c>
+      <c r="Q505">
+        <v>1</v>
+      </c>
+      <c r="R505">
+        <v>30.33884948778563</v>
+      </c>
+      <c r="S505" t="s">
+        <v>101</v>
+      </c>
+      <c r="T505" t="s">
+        <v>210</v>
+      </c>
+      <c r="U505" s="1">
+        <v>1</v>
+      </c>
+      <c r="V505" s="1">
+        <v>2</v>
+      </c>
+      <c r="W505" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="506" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A506">
+        <v>78</v>
+      </c>
+      <c r="B506" t="s">
+        <v>206</v>
+      </c>
+      <c r="C506" t="s">
+        <v>29</v>
+      </c>
+      <c r="D506">
+        <v>0</v>
+      </c>
+      <c r="E506">
+        <v>0</v>
+      </c>
+      <c r="G506">
+        <v>20.5</v>
+      </c>
+      <c r="H506">
+        <v>24</v>
+      </c>
+      <c r="I506">
+        <v>24</v>
+      </c>
+      <c r="J506">
+        <v>24</v>
+      </c>
+      <c r="L506" t="s">
+        <v>209</v>
+      </c>
+      <c r="M506" t="s">
+        <v>209</v>
+      </c>
+      <c r="N506">
+        <v>1972.5</v>
+      </c>
+      <c r="O506">
+        <v>1</v>
+      </c>
+      <c r="P506">
+        <v>1600</v>
+      </c>
+      <c r="Q506">
+        <v>1</v>
+      </c>
+      <c r="R506">
+        <v>61.111111111111107</v>
+      </c>
+      <c r="S506" t="s">
+        <v>101</v>
+      </c>
+      <c r="T506" t="s">
+        <v>210</v>
+      </c>
+      <c r="U506" s="1">
+        <v>1</v>
+      </c>
+      <c r="V506" s="1">
+        <v>2</v>
+      </c>
+      <c r="W506" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A507">
+        <v>78</v>
+      </c>
+      <c r="B507" t="s">
+        <v>206</v>
+      </c>
+      <c r="C507" t="s">
+        <v>29</v>
+      </c>
+      <c r="D507">
+        <v>0</v>
+      </c>
+      <c r="E507">
+        <v>1</v>
+      </c>
+      <c r="F507">
+        <v>1</v>
+      </c>
+      <c r="G507">
+        <v>20.5</v>
+      </c>
+      <c r="H507">
+        <v>24</v>
+      </c>
+      <c r="I507" s="5">
+        <v>21</v>
+      </c>
+      <c r="J507" s="5">
+        <v>27</v>
+      </c>
+      <c r="K507">
+        <v>24</v>
+      </c>
+      <c r="L507" t="s">
+        <v>209</v>
+      </c>
+      <c r="M507" t="s">
+        <v>209</v>
+      </c>
+      <c r="N507">
+        <v>1925</v>
+      </c>
+      <c r="O507">
+        <v>1</v>
+      </c>
+      <c r="P507">
+        <v>1600</v>
+      </c>
+      <c r="Q507">
+        <v>1</v>
+      </c>
+      <c r="R507">
+        <v>59.259259259259252</v>
+      </c>
+      <c r="S507" t="s">
+        <v>101</v>
+      </c>
+      <c r="T507" t="s">
+        <v>210</v>
+      </c>
+      <c r="U507" s="1">
+        <v>1</v>
+      </c>
+      <c r="V507" s="1">
+        <v>2</v>
+      </c>
+      <c r="W507" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="508" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A508">
+        <v>78</v>
+      </c>
+      <c r="B508" t="s">
+        <v>206</v>
+      </c>
+      <c r="C508" t="s">
+        <v>29</v>
+      </c>
+      <c r="D508">
+        <v>0</v>
+      </c>
+      <c r="E508">
+        <v>0</v>
+      </c>
+      <c r="G508">
+        <v>20.5</v>
+      </c>
+      <c r="H508">
+        <v>17</v>
+      </c>
+      <c r="I508">
+        <v>17</v>
+      </c>
+      <c r="J508">
+        <v>17</v>
+      </c>
+      <c r="L508" t="s">
+        <v>207</v>
+      </c>
+      <c r="M508" t="s">
+        <v>207</v>
+      </c>
+      <c r="N508">
+        <v>83.807526384141099</v>
+      </c>
+      <c r="O508">
+        <v>1</v>
+      </c>
+      <c r="P508">
+        <v>1600</v>
+      </c>
+      <c r="Q508">
+        <v>1</v>
+      </c>
+      <c r="R508">
+        <v>65.825868262015703</v>
+      </c>
+      <c r="S508" t="s">
+        <v>101</v>
+      </c>
+      <c r="T508" t="s">
+        <v>210</v>
+      </c>
+      <c r="U508" s="1">
+        <v>1</v>
+      </c>
+      <c r="V508" s="1">
+        <v>2</v>
+      </c>
+      <c r="W508" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A509">
+        <v>78</v>
+      </c>
+      <c r="B509" t="s">
+        <v>206</v>
+      </c>
+      <c r="C509" t="s">
+        <v>29</v>
+      </c>
+      <c r="D509">
+        <v>0</v>
+      </c>
+      <c r="E509">
+        <v>1</v>
+      </c>
+      <c r="F509">
+        <v>1</v>
+      </c>
+      <c r="G509">
+        <v>20.5</v>
+      </c>
+      <c r="H509">
+        <v>17</v>
+      </c>
+      <c r="I509" s="5">
+        <v>14</v>
+      </c>
+      <c r="J509" s="5">
+        <v>20</v>
+      </c>
+      <c r="K509">
+        <v>24</v>
+      </c>
+      <c r="L509" t="s">
+        <v>207</v>
+      </c>
+      <c r="M509" t="s">
+        <v>207</v>
+      </c>
+      <c r="N509">
+        <v>81.6027526085593</v>
+      </c>
+      <c r="O509">
+        <v>1</v>
+      </c>
+      <c r="P509">
+        <v>1600</v>
+      </c>
+      <c r="Q509">
+        <v>1</v>
+      </c>
+      <c r="R509">
+        <v>72.331440873483203</v>
+      </c>
+      <c r="S509" t="s">
+        <v>101</v>
+      </c>
+      <c r="T509" t="s">
+        <v>210</v>
+      </c>
+      <c r="U509" s="1">
+        <v>1</v>
+      </c>
+      <c r="V509" s="1">
+        <v>2</v>
+      </c>
+      <c r="W509" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A510">
+        <v>78</v>
+      </c>
+      <c r="B510" t="s">
+        <v>206</v>
+      </c>
+      <c r="C510" t="s">
+        <v>29</v>
+      </c>
+      <c r="D510">
+        <v>0</v>
+      </c>
+      <c r="E510">
+        <v>0</v>
+      </c>
+      <c r="G510">
+        <v>20.5</v>
+      </c>
+      <c r="H510">
+        <v>17</v>
+      </c>
+      <c r="I510">
+        <v>17</v>
+      </c>
+      <c r="J510">
+        <v>17</v>
+      </c>
+      <c r="L510" t="s">
+        <v>208</v>
+      </c>
+      <c r="M510" t="s">
+        <v>208</v>
+      </c>
+      <c r="N510">
+        <v>54.993025561736303</v>
+      </c>
+      <c r="O510">
+        <v>1</v>
+      </c>
+      <c r="P510">
+        <v>1600</v>
+      </c>
+      <c r="Q510">
+        <v>1</v>
+      </c>
+      <c r="R510">
+        <v>32.306494350424884</v>
+      </c>
+      <c r="S510" t="s">
+        <v>101</v>
+      </c>
+      <c r="T510" t="s">
+        <v>210</v>
+      </c>
+      <c r="U510" s="1">
+        <v>1</v>
+      </c>
+      <c r="V510" s="1">
+        <v>2</v>
+      </c>
+      <c r="W510" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A511">
+        <v>78</v>
+      </c>
+      <c r="B511" t="s">
+        <v>206</v>
+      </c>
+      <c r="C511" t="s">
+        <v>29</v>
+      </c>
+      <c r="D511">
+        <v>0</v>
+      </c>
+      <c r="E511">
+        <v>1</v>
+      </c>
+      <c r="F511">
+        <v>1</v>
+      </c>
+      <c r="G511">
+        <v>20.5</v>
+      </c>
+      <c r="H511">
+        <v>17</v>
+      </c>
+      <c r="I511" s="5">
+        <v>14</v>
+      </c>
+      <c r="J511" s="5">
+        <v>20</v>
+      </c>
+      <c r="K511">
+        <v>24</v>
+      </c>
+      <c r="L511" t="s">
+        <v>208</v>
+      </c>
+      <c r="M511" t="s">
+        <v>208</v>
+      </c>
+      <c r="N511">
+        <v>54.995546443036403</v>
+      </c>
+      <c r="O511">
+        <v>1</v>
+      </c>
+      <c r="P511">
+        <v>1600</v>
+      </c>
+      <c r="Q511">
+        <v>1</v>
+      </c>
+      <c r="R511">
+        <v>37.036414597209856</v>
+      </c>
+      <c r="S511" t="s">
+        <v>101</v>
+      </c>
+      <c r="T511" t="s">
+        <v>210</v>
+      </c>
+      <c r="U511" s="1">
+        <v>1</v>
+      </c>
+      <c r="V511" s="1">
+        <v>2</v>
+      </c>
+      <c r="W511" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="512" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A512">
+        <v>78</v>
+      </c>
+      <c r="B512" t="s">
+        <v>206</v>
+      </c>
+      <c r="C512" t="s">
+        <v>29</v>
+      </c>
+      <c r="D512">
+        <v>0</v>
+      </c>
+      <c r="E512">
+        <v>0</v>
+      </c>
+      <c r="G512">
+        <v>20.5</v>
+      </c>
+      <c r="H512">
+        <v>17</v>
+      </c>
+      <c r="I512">
+        <v>17</v>
+      </c>
+      <c r="J512">
+        <v>17</v>
+      </c>
+      <c r="L512" t="s">
+        <v>209</v>
+      </c>
+      <c r="M512" t="s">
+        <v>209</v>
+      </c>
+      <c r="N512">
+        <v>2252.5</v>
+      </c>
+      <c r="O512">
+        <v>1</v>
+      </c>
+      <c r="P512">
+        <v>1600</v>
+      </c>
+      <c r="Q512">
+        <v>1</v>
+      </c>
+      <c r="R512">
+        <v>70.370370370370367</v>
+      </c>
+      <c r="S512" t="s">
+        <v>101</v>
+      </c>
+      <c r="T512" t="s">
+        <v>210</v>
+      </c>
+      <c r="U512" s="1">
+        <v>1</v>
+      </c>
+      <c r="V512" s="1">
+        <v>2</v>
+      </c>
+      <c r="W512" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A513">
+        <v>78</v>
+      </c>
+      <c r="B513" t="s">
+        <v>206</v>
+      </c>
+      <c r="C513" t="s">
+        <v>29</v>
+      </c>
+      <c r="D513">
+        <v>0</v>
+      </c>
+      <c r="E513">
+        <v>1</v>
+      </c>
+      <c r="F513">
+        <v>1</v>
+      </c>
+      <c r="G513">
+        <v>20.5</v>
+      </c>
+      <c r="H513">
+        <v>17</v>
+      </c>
+      <c r="I513" s="5">
+        <v>14</v>
+      </c>
+      <c r="J513" s="5">
+        <v>20</v>
+      </c>
+      <c r="K513">
+        <v>24</v>
+      </c>
+      <c r="L513" t="s">
+        <v>209</v>
+      </c>
+      <c r="M513" t="s">
+        <v>209</v>
+      </c>
+      <c r="N513">
+        <v>2207.5</v>
+      </c>
+      <c r="O513">
+        <v>1</v>
+      </c>
+      <c r="P513">
+        <v>1600</v>
+      </c>
+      <c r="Q513">
+        <v>1</v>
+      </c>
+      <c r="R513">
+        <v>79.629629629629619</v>
+      </c>
+      <c r="S513" t="s">
+        <v>101</v>
+      </c>
+      <c r="T513" t="s">
+        <v>210</v>
+      </c>
+      <c r="U513" s="1">
+        <v>1</v>
+      </c>
+      <c r="V513" s="1">
+        <v>2</v>
+      </c>
+      <c r="W513" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="514" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A514">
+        <v>79</v>
+      </c>
+      <c r="B514" t="s">
+        <v>206</v>
+      </c>
+      <c r="C514" t="s">
+        <v>52</v>
+      </c>
+      <c r="D514">
+        <v>0</v>
+      </c>
+      <c r="E514">
+        <v>0</v>
+      </c>
+      <c r="G514">
+        <v>20.5</v>
+      </c>
+      <c r="H514">
+        <v>21</v>
+      </c>
+      <c r="I514">
+        <v>21</v>
+      </c>
+      <c r="J514">
+        <v>21</v>
+      </c>
+      <c r="L514" t="s">
+        <v>209</v>
+      </c>
+      <c r="M514" t="s">
+        <v>209</v>
+      </c>
+      <c r="N514">
+        <v>2242.07650273224</v>
+      </c>
+      <c r="O514">
+        <v>1</v>
+      </c>
+      <c r="P514">
+        <v>480</v>
+      </c>
+      <c r="Q514">
+        <v>1</v>
+      </c>
+      <c r="R514">
+        <v>64.764217769681494</v>
+      </c>
+      <c r="S514" t="s">
+        <v>101</v>
+      </c>
+      <c r="T514" t="s">
+        <v>210</v>
+      </c>
+      <c r="U514" s="1">
+        <v>1</v>
+      </c>
+      <c r="V514" s="1">
+        <v>2</v>
+      </c>
+      <c r="W514" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A515">
+        <v>79</v>
+      </c>
+      <c r="B515" t="s">
+        <v>206</v>
+      </c>
+      <c r="C515" t="s">
+        <v>52</v>
+      </c>
+      <c r="D515">
+        <v>0</v>
+      </c>
+      <c r="E515">
+        <v>1</v>
+      </c>
+      <c r="F515">
+        <v>1</v>
+      </c>
+      <c r="G515">
+        <v>20.5</v>
+      </c>
+      <c r="H515">
+        <v>24</v>
+      </c>
+      <c r="I515" s="5">
+        <v>21</v>
+      </c>
+      <c r="J515" s="5">
+        <v>27</v>
+      </c>
+      <c r="K515">
+        <v>24</v>
+      </c>
+      <c r="L515" t="s">
+        <v>209</v>
+      </c>
+      <c r="M515" t="s">
+        <v>209</v>
+      </c>
+      <c r="N515">
+        <v>2006.0109289617401</v>
+      </c>
+      <c r="O515">
+        <v>1</v>
+      </c>
+      <c r="P515">
+        <v>480</v>
+      </c>
+      <c r="Q515">
+        <v>1</v>
+      </c>
+      <c r="R515">
+        <v>74.478850435133509</v>
+      </c>
+      <c r="S515" t="s">
+        <v>101</v>
+      </c>
+      <c r="T515" t="s">
+        <v>210</v>
+      </c>
+      <c r="U515" s="1">
+        <v>1</v>
+      </c>
+      <c r="V515" s="1">
+        <v>2</v>
+      </c>
+      <c r="W515" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A516">
+        <v>79</v>
+      </c>
+      <c r="B516" t="s">
+        <v>206</v>
+      </c>
+      <c r="C516" t="s">
+        <v>52</v>
+      </c>
+      <c r="D516">
+        <v>0</v>
+      </c>
+      <c r="E516">
+        <v>0</v>
+      </c>
+      <c r="G516">
+        <v>20.5</v>
+      </c>
+      <c r="H516">
+        <v>27</v>
+      </c>
+      <c r="I516">
+        <v>27</v>
+      </c>
+      <c r="J516">
+        <v>27</v>
+      </c>
+      <c r="L516" t="s">
+        <v>209</v>
+      </c>
+      <c r="M516" t="s">
+        <v>209</v>
+      </c>
+      <c r="N516">
+        <v>1936.0655737704899</v>
+      </c>
+      <c r="O516">
+        <v>1</v>
+      </c>
+      <c r="P516">
+        <v>480</v>
+      </c>
+      <c r="Q516">
+        <v>1</v>
+      </c>
+      <c r="R516">
+        <v>84.193483100592587</v>
+      </c>
+      <c r="S516" t="s">
+        <v>101</v>
+      </c>
+      <c r="T516" t="s">
+        <v>210</v>
+      </c>
+      <c r="U516" s="1">
+        <v>1</v>
+      </c>
+      <c r="V516" s="1">
+        <v>2</v>
+      </c>
+      <c r="W516" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="517" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B517" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finishing up all extractiosn including duncan, kern and their corresponding raw files
</commit_message>
<xml_diff>
--- a/data extraction /extraction /data/metanaly_fulldataset.xlsx
+++ b/data extraction /extraction /data/metanaly_fulldataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maslein/Desktop/thesis/data extraction /extraction /data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588EF591-C0B7-244A-8132-C6763BABB014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D07183-EA0D-0346-A4B4-816AF2C6BC80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28840" yWindow="-7060" windowWidth="23540" windowHeight="11100" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="27400" windowHeight="15160" xr2:uid="{91BB1903-1808-2647-B602-9ADB3433B97D}"/>
   </bookViews>
   <sheets>
     <sheet name="metanaly_fulldataset" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4048" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4113" uniqueCount="219">
   <si>
     <t>study_id</t>
   </si>
@@ -659,12 +659,36 @@
   <si>
     <t>birchii</t>
   </si>
+  <si>
+    <t>figure 5a</t>
+  </si>
+  <si>
+    <t>figure 5b</t>
+  </si>
+  <si>
+    <t>figure 5c</t>
+  </si>
+  <si>
+    <t>duncan2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phage density </t>
+  </si>
+  <si>
+    <t>ml^-1</t>
+  </si>
+  <si>
+    <t>lytic phage</t>
+  </si>
+  <si>
+    <t>SBWΦ2.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -684,6 +708,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -706,13 +736,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1027,11 +1058,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ADBDD29-FB0D-9242-849C-099DCE2463A5}">
-  <dimension ref="A1:AG517"/>
+  <dimension ref="A1:AG527"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A511" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D520" sqref="D520"/>
+      <pane ySplit="1" topLeftCell="A498" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C531" sqref="C531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7560,6 +7591,9 @@
       <c r="O90">
         <v>0</v>
       </c>
+      <c r="P90">
+        <v>7</v>
+      </c>
       <c r="Q90">
         <v>0</v>
       </c>
@@ -7625,6 +7659,9 @@
       <c r="O91">
         <v>0</v>
       </c>
+      <c r="P91">
+        <v>7</v>
+      </c>
       <c r="Q91">
         <v>0</v>
       </c>
@@ -7684,6 +7721,9 @@
       <c r="O92">
         <v>0</v>
       </c>
+      <c r="P92">
+        <v>7</v>
+      </c>
       <c r="Q92">
         <v>0</v>
       </c>
@@ -7749,6 +7789,9 @@
       <c r="O93">
         <v>0</v>
       </c>
+      <c r="P93">
+        <v>7</v>
+      </c>
       <c r="Q93">
         <v>0</v>
       </c>
@@ -7808,6 +7851,9 @@
       <c r="O94">
         <v>0</v>
       </c>
+      <c r="P94">
+        <v>7</v>
+      </c>
       <c r="Q94">
         <v>0</v>
       </c>
@@ -7873,6 +7919,9 @@
       <c r="O95">
         <v>0</v>
       </c>
+      <c r="P95">
+        <v>7</v>
+      </c>
       <c r="Q95">
         <v>0</v>
       </c>
@@ -7932,6 +7981,9 @@
       <c r="O96">
         <v>0</v>
       </c>
+      <c r="P96">
+        <v>7</v>
+      </c>
       <c r="Q96">
         <v>0</v>
       </c>
@@ -7997,6 +8049,9 @@
       <c r="O97">
         <v>0</v>
       </c>
+      <c r="P97">
+        <v>7</v>
+      </c>
       <c r="Q97">
         <v>0</v>
       </c>
@@ -8056,6 +8111,9 @@
       <c r="O98">
         <v>0</v>
       </c>
+      <c r="P98">
+        <v>7</v>
+      </c>
       <c r="Q98">
         <v>0</v>
       </c>
@@ -8121,6 +8179,9 @@
       <c r="O99">
         <v>0</v>
       </c>
+      <c r="P99">
+        <v>7</v>
+      </c>
       <c r="Q99">
         <v>0</v>
       </c>
@@ -8180,6 +8241,9 @@
       <c r="O100">
         <v>0</v>
       </c>
+      <c r="P100">
+        <v>7</v>
+      </c>
       <c r="Q100">
         <v>0</v>
       </c>
@@ -8245,6 +8309,9 @@
       <c r="O101">
         <v>0</v>
       </c>
+      <c r="P101">
+        <v>7</v>
+      </c>
       <c r="Q101">
         <v>0</v>
       </c>
@@ -8304,6 +8371,9 @@
       <c r="O102">
         <v>0</v>
       </c>
+      <c r="P102">
+        <v>7</v>
+      </c>
       <c r="Q102">
         <v>0</v>
       </c>
@@ -8369,6 +8439,9 @@
       <c r="O103">
         <v>0</v>
       </c>
+      <c r="P103">
+        <v>7</v>
+      </c>
       <c r="Q103">
         <v>0</v>
       </c>
@@ -8428,6 +8501,9 @@
       <c r="O104">
         <v>0</v>
       </c>
+      <c r="P104">
+        <v>7</v>
+      </c>
       <c r="Q104">
         <v>0</v>
       </c>
@@ -8493,6 +8569,9 @@
       <c r="O105">
         <v>0</v>
       </c>
+      <c r="P105">
+        <v>7</v>
+      </c>
       <c r="Q105">
         <v>0</v>
       </c>
@@ -8552,6 +8631,9 @@
       <c r="O106">
         <v>0</v>
       </c>
+      <c r="P106">
+        <v>7</v>
+      </c>
       <c r="Q106">
         <v>0</v>
       </c>
@@ -8617,6 +8699,9 @@
       <c r="O107">
         <v>0</v>
       </c>
+      <c r="P107">
+        <v>7</v>
+      </c>
       <c r="Q107">
         <v>0</v>
       </c>
@@ -8682,6 +8767,9 @@
       <c r="O108">
         <v>0</v>
       </c>
+      <c r="P108">
+        <v>7</v>
+      </c>
       <c r="Q108">
         <v>0</v>
       </c>
@@ -8741,6 +8829,9 @@
       <c r="O109">
         <v>0</v>
       </c>
+      <c r="P109">
+        <v>7</v>
+      </c>
       <c r="Q109">
         <v>0</v>
       </c>
@@ -8806,6 +8897,9 @@
       <c r="O110">
         <v>0</v>
       </c>
+      <c r="P110">
+        <v>7</v>
+      </c>
       <c r="Q110">
         <v>0</v>
       </c>
@@ -8871,6 +8965,9 @@
       <c r="O111">
         <v>0</v>
       </c>
+      <c r="P111">
+        <v>7</v>
+      </c>
       <c r="Q111">
         <v>0</v>
       </c>
@@ -8930,6 +9027,9 @@
       <c r="O112">
         <v>0</v>
       </c>
+      <c r="P112">
+        <v>7</v>
+      </c>
       <c r="Q112">
         <v>0</v>
       </c>
@@ -8995,6 +9095,9 @@
       <c r="O113">
         <v>0</v>
       </c>
+      <c r="P113">
+        <v>7</v>
+      </c>
       <c r="Q113">
         <v>0</v>
       </c>
@@ -9060,6 +9163,9 @@
       <c r="O114">
         <v>0</v>
       </c>
+      <c r="P114">
+        <v>7</v>
+      </c>
       <c r="Q114">
         <v>0</v>
       </c>
@@ -9119,6 +9225,9 @@
       <c r="O115">
         <v>0</v>
       </c>
+      <c r="P115">
+        <v>7</v>
+      </c>
       <c r="Q115">
         <v>0</v>
       </c>
@@ -9184,6 +9293,9 @@
       <c r="O116">
         <v>0</v>
       </c>
+      <c r="P116">
+        <v>7</v>
+      </c>
       <c r="Q116">
         <v>0</v>
       </c>
@@ -9249,6 +9361,9 @@
       <c r="O117">
         <v>0</v>
       </c>
+      <c r="P117">
+        <v>7</v>
+      </c>
       <c r="Q117">
         <v>0</v>
       </c>
@@ -37985,8 +38100,715 @@
       </c>
     </row>
     <row r="517" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A517">
+        <v>80</v>
+      </c>
       <c r="B517" t="s">
         <v>69</v>
+      </c>
+      <c r="C517" t="s">
+        <v>211</v>
+      </c>
+      <c r="D517">
+        <v>0</v>
+      </c>
+      <c r="E517">
+        <v>0</v>
+      </c>
+      <c r="H517">
+        <v>24</v>
+      </c>
+      <c r="I517">
+        <v>24</v>
+      </c>
+      <c r="J517">
+        <v>24</v>
+      </c>
+      <c r="L517" t="s">
+        <v>85</v>
+      </c>
+      <c r="M517" t="s">
+        <v>86</v>
+      </c>
+      <c r="N517">
+        <v>39.721402927368104</v>
+      </c>
+      <c r="O517">
+        <v>1</v>
+      </c>
+      <c r="P517">
+        <v>7</v>
+      </c>
+      <c r="Q517">
+        <v>0</v>
+      </c>
+      <c r="R517">
+        <v>7.5117370891998547E-2</v>
+      </c>
+      <c r="S517" t="s">
+        <v>74</v>
+      </c>
+      <c r="T517" t="s">
+        <v>75</v>
+      </c>
+      <c r="U517" s="6">
+        <v>1</v>
+      </c>
+      <c r="V517" s="6">
+        <v>1</v>
+      </c>
+      <c r="W517" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="518" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A518">
+        <v>80</v>
+      </c>
+      <c r="B518" t="s">
+        <v>69</v>
+      </c>
+      <c r="C518" t="s">
+        <v>211</v>
+      </c>
+      <c r="D518">
+        <v>0</v>
+      </c>
+      <c r="E518">
+        <v>1</v>
+      </c>
+      <c r="F518">
+        <v>1</v>
+      </c>
+      <c r="H518">
+        <v>25</v>
+      </c>
+      <c r="I518">
+        <v>20</v>
+      </c>
+      <c r="J518">
+        <v>30</v>
+      </c>
+      <c r="K518">
+        <v>24</v>
+      </c>
+      <c r="L518" t="s">
+        <v>85</v>
+      </c>
+      <c r="M518" t="s">
+        <v>86</v>
+      </c>
+      <c r="N518">
+        <v>40.514995857497901</v>
+      </c>
+      <c r="O518">
+        <v>1</v>
+      </c>
+      <c r="P518">
+        <v>7</v>
+      </c>
+      <c r="Q518">
+        <v>0</v>
+      </c>
+      <c r="R518">
+        <v>0.16901408450705091</v>
+      </c>
+      <c r="S518" t="s">
+        <v>74</v>
+      </c>
+      <c r="T518" t="s">
+        <v>75</v>
+      </c>
+      <c r="U518" s="6">
+        <v>1</v>
+      </c>
+      <c r="V518" s="6">
+        <v>1</v>
+      </c>
+      <c r="W518" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="519" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A519">
+        <v>80</v>
+      </c>
+      <c r="B519" t="s">
+        <v>69</v>
+      </c>
+      <c r="C519" t="s">
+        <v>212</v>
+      </c>
+      <c r="D519">
+        <v>0</v>
+      </c>
+      <c r="E519">
+        <v>0</v>
+      </c>
+      <c r="H519">
+        <v>24</v>
+      </c>
+      <c r="I519">
+        <v>24</v>
+      </c>
+      <c r="J519">
+        <v>24</v>
+      </c>
+      <c r="L519" t="s">
+        <v>85</v>
+      </c>
+      <c r="M519" t="s">
+        <v>86</v>
+      </c>
+      <c r="N519">
+        <v>40.488262910798099</v>
+      </c>
+      <c r="O519">
+        <v>1</v>
+      </c>
+      <c r="P519">
+        <v>7</v>
+      </c>
+      <c r="Q519">
+        <v>0</v>
+      </c>
+      <c r="R519">
+        <v>0.11267605633804934</v>
+      </c>
+      <c r="S519" t="s">
+        <v>74</v>
+      </c>
+      <c r="T519" t="s">
+        <v>76</v>
+      </c>
+      <c r="U519" s="6">
+        <v>1</v>
+      </c>
+      <c r="V519" s="6">
+        <v>1</v>
+      </c>
+      <c r="W519" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="520" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A520">
+        <v>80</v>
+      </c>
+      <c r="B520" t="s">
+        <v>69</v>
+      </c>
+      <c r="C520" t="s">
+        <v>212</v>
+      </c>
+      <c r="D520">
+        <v>0</v>
+      </c>
+      <c r="E520">
+        <v>1</v>
+      </c>
+      <c r="F520">
+        <v>1</v>
+      </c>
+      <c r="H520">
+        <v>25</v>
+      </c>
+      <c r="I520">
+        <v>20</v>
+      </c>
+      <c r="J520">
+        <v>30</v>
+      </c>
+      <c r="K520">
+        <v>24</v>
+      </c>
+      <c r="L520" t="s">
+        <v>85</v>
+      </c>
+      <c r="M520" t="s">
+        <v>86</v>
+      </c>
+      <c r="N520">
+        <v>41.577227075533301</v>
+      </c>
+      <c r="O520">
+        <v>1</v>
+      </c>
+      <c r="P520">
+        <v>7</v>
+      </c>
+      <c r="Q520">
+        <v>0</v>
+      </c>
+      <c r="R520">
+        <v>9.389671361504881E-2</v>
+      </c>
+      <c r="S520" t="s">
+        <v>74</v>
+      </c>
+      <c r="T520" t="s">
+        <v>76</v>
+      </c>
+      <c r="U520" s="6">
+        <v>1</v>
+      </c>
+      <c r="V520" s="6">
+        <v>1</v>
+      </c>
+      <c r="W520" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="521" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A521">
+        <v>80</v>
+      </c>
+      <c r="B521" t="s">
+        <v>69</v>
+      </c>
+      <c r="C521" t="s">
+        <v>213</v>
+      </c>
+      <c r="D521">
+        <v>0</v>
+      </c>
+      <c r="E521">
+        <v>0</v>
+      </c>
+      <c r="H521">
+        <v>24</v>
+      </c>
+      <c r="I521">
+        <v>24</v>
+      </c>
+      <c r="J521">
+        <v>24</v>
+      </c>
+      <c r="L521" t="s">
+        <v>85</v>
+      </c>
+      <c r="M521" t="s">
+        <v>86</v>
+      </c>
+      <c r="N521">
+        <v>41.735849056603698</v>
+      </c>
+      <c r="O521">
+        <v>1</v>
+      </c>
+      <c r="P521">
+        <v>7</v>
+      </c>
+      <c r="Q521">
+        <v>0</v>
+      </c>
+      <c r="R521">
+        <v>0.15094339622639907</v>
+      </c>
+      <c r="S521" t="s">
+        <v>77</v>
+      </c>
+      <c r="T521" t="s">
+        <v>78</v>
+      </c>
+      <c r="U521" s="6">
+        <v>1</v>
+      </c>
+      <c r="V521" s="6">
+        <v>1</v>
+      </c>
+      <c r="W521" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="522" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A522">
+        <v>80</v>
+      </c>
+      <c r="B522" t="s">
+        <v>69</v>
+      </c>
+      <c r="C522" t="s">
+        <v>213</v>
+      </c>
+      <c r="D522">
+        <v>0</v>
+      </c>
+      <c r="E522">
+        <v>1</v>
+      </c>
+      <c r="F522">
+        <v>1</v>
+      </c>
+      <c r="H522">
+        <v>25</v>
+      </c>
+      <c r="I522">
+        <v>20</v>
+      </c>
+      <c r="J522">
+        <v>30</v>
+      </c>
+      <c r="K522">
+        <v>24</v>
+      </c>
+      <c r="L522" t="s">
+        <v>85</v>
+      </c>
+      <c r="M522" t="s">
+        <v>86</v>
+      </c>
+      <c r="N522">
+        <v>42.905660377358402</v>
+      </c>
+      <c r="O522">
+        <v>1</v>
+      </c>
+      <c r="P522">
+        <v>7</v>
+      </c>
+      <c r="Q522">
+        <v>0</v>
+      </c>
+      <c r="R522">
+        <v>0.1320754716981476</v>
+      </c>
+      <c r="S522" t="s">
+        <v>77</v>
+      </c>
+      <c r="T522" t="s">
+        <v>78</v>
+      </c>
+      <c r="U522" s="6">
+        <v>1</v>
+      </c>
+      <c r="V522" s="6">
+        <v>1</v>
+      </c>
+      <c r="W522" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="523" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A523">
+        <v>80</v>
+      </c>
+      <c r="B523" t="s">
+        <v>69</v>
+      </c>
+      <c r="C523" t="s">
+        <v>213</v>
+      </c>
+      <c r="D523">
+        <v>0</v>
+      </c>
+      <c r="E523">
+        <v>1</v>
+      </c>
+      <c r="F523">
+        <v>1</v>
+      </c>
+      <c r="H523">
+        <v>28</v>
+      </c>
+      <c r="I523">
+        <v>18</v>
+      </c>
+      <c r="J523">
+        <v>38</v>
+      </c>
+      <c r="K523">
+        <v>24</v>
+      </c>
+      <c r="L523" t="s">
+        <v>85</v>
+      </c>
+      <c r="M523" t="s">
+        <v>86</v>
+      </c>
+      <c r="N523">
+        <v>43.358490566037702</v>
+      </c>
+      <c r="O523">
+        <v>1</v>
+      </c>
+      <c r="P523">
+        <v>7</v>
+      </c>
+      <c r="Q523">
+        <v>0</v>
+      </c>
+      <c r="R523">
+        <v>0.13207547169809786</v>
+      </c>
+      <c r="S523" t="s">
+        <v>77</v>
+      </c>
+      <c r="T523" t="s">
+        <v>78</v>
+      </c>
+      <c r="U523" s="6">
+        <v>1</v>
+      </c>
+      <c r="V523" s="6">
+        <v>1</v>
+      </c>
+      <c r="W523" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="524" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A524">
+        <v>81</v>
+      </c>
+      <c r="B524" t="s">
+        <v>214</v>
+      </c>
+      <c r="C524" t="s">
+        <v>52</v>
+      </c>
+      <c r="D524">
+        <v>0</v>
+      </c>
+      <c r="E524">
+        <v>0</v>
+      </c>
+      <c r="H524">
+        <v>28</v>
+      </c>
+      <c r="I524">
+        <v>28</v>
+      </c>
+      <c r="J524">
+        <v>28</v>
+      </c>
+      <c r="K524">
+        <v>48</v>
+      </c>
+      <c r="L524" t="s">
+        <v>215</v>
+      </c>
+      <c r="M524" t="s">
+        <v>216</v>
+      </c>
+      <c r="N524">
+        <v>0.548371234564345</v>
+      </c>
+      <c r="O524">
+        <v>1</v>
+      </c>
+      <c r="Q524">
+        <v>0</v>
+      </c>
+      <c r="R524">
+        <v>0.1222824233956695</v>
+      </c>
+      <c r="S524" t="s">
+        <v>217</v>
+      </c>
+      <c r="T524" t="s">
+        <v>218</v>
+      </c>
+      <c r="U524" s="6">
+        <v>3</v>
+      </c>
+      <c r="V524" s="6">
+        <v>1</v>
+      </c>
+      <c r="W524" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="525" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A525">
+        <v>81</v>
+      </c>
+      <c r="B525" t="s">
+        <v>214</v>
+      </c>
+      <c r="C525" t="s">
+        <v>52</v>
+      </c>
+      <c r="D525">
+        <v>0</v>
+      </c>
+      <c r="E525">
+        <v>4</v>
+      </c>
+      <c r="F525">
+        <v>0</v>
+      </c>
+      <c r="H525">
+        <v>30</v>
+      </c>
+      <c r="I525">
+        <v>28</v>
+      </c>
+      <c r="J525">
+        <v>32</v>
+      </c>
+      <c r="K525">
+        <v>48</v>
+      </c>
+      <c r="L525" t="s">
+        <v>215</v>
+      </c>
+      <c r="M525" t="s">
+        <v>216</v>
+      </c>
+      <c r="N525">
+        <v>-0.845099459477481</v>
+      </c>
+      <c r="O525">
+        <v>1</v>
+      </c>
+      <c r="Q525">
+        <v>0</v>
+      </c>
+      <c r="R525">
+        <v>0.11956503620909947</v>
+      </c>
+      <c r="S525" t="s">
+        <v>217</v>
+      </c>
+      <c r="T525" t="s">
+        <v>218</v>
+      </c>
+      <c r="U525" s="6">
+        <v>3</v>
+      </c>
+      <c r="V525" s="6">
+        <v>1</v>
+      </c>
+      <c r="W525" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="526" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A526">
+        <v>81</v>
+      </c>
+      <c r="B526" t="s">
+        <v>214</v>
+      </c>
+      <c r="C526" t="s">
+        <v>52</v>
+      </c>
+      <c r="D526">
+        <v>0</v>
+      </c>
+      <c r="E526">
+        <v>0</v>
+      </c>
+      <c r="H526">
+        <v>32</v>
+      </c>
+      <c r="I526">
+        <v>32</v>
+      </c>
+      <c r="J526">
+        <v>32</v>
+      </c>
+      <c r="K526">
+        <v>48</v>
+      </c>
+      <c r="L526" t="s">
+        <v>215</v>
+      </c>
+      <c r="M526" t="s">
+        <v>216</v>
+      </c>
+      <c r="N526">
+        <v>-0.59619088461124703</v>
+      </c>
+      <c r="O526">
+        <v>1</v>
+      </c>
+      <c r="Q526">
+        <v>0</v>
+      </c>
+      <c r="R526">
+        <v>0.11413026183595801</v>
+      </c>
+      <c r="S526" t="s">
+        <v>217</v>
+      </c>
+      <c r="T526" t="s">
+        <v>218</v>
+      </c>
+      <c r="U526" s="6">
+        <v>3</v>
+      </c>
+      <c r="V526" s="6">
+        <v>1</v>
+      </c>
+      <c r="W526" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="527" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A527">
+        <v>81</v>
+      </c>
+      <c r="B527" t="s">
+        <v>214</v>
+      </c>
+      <c r="C527" t="s">
+        <v>52</v>
+      </c>
+      <c r="D527">
+        <v>0</v>
+      </c>
+      <c r="E527">
+        <v>4</v>
+      </c>
+      <c r="F527">
+        <v>0</v>
+      </c>
+      <c r="H527">
+        <v>30</v>
+      </c>
+      <c r="I527">
+        <v>28</v>
+      </c>
+      <c r="J527">
+        <v>32</v>
+      </c>
+      <c r="K527">
+        <v>48</v>
+      </c>
+      <c r="L527" t="s">
+        <v>215</v>
+      </c>
+      <c r="M527" t="s">
+        <v>216</v>
+      </c>
+      <c r="N527">
+        <v>2.4135967098892701</v>
+      </c>
+      <c r="O527">
+        <v>1</v>
+      </c>
+      <c r="Q527">
+        <v>0</v>
+      </c>
+      <c r="R527">
+        <v>0.28260826740332501</v>
+      </c>
+      <c r="S527" t="s">
+        <v>217</v>
+      </c>
+      <c r="T527" t="s">
+        <v>218</v>
+      </c>
+      <c r="U527" s="6">
+        <v>3</v>
+      </c>
+      <c r="V527" s="6">
+        <v>1</v>
+      </c>
+      <c r="W527" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>